<commit_message>
new blood type and element type to replace elment card
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/ItemConsumer.xlsx
+++ b/ConfigData/Xlsx/ItemConsumer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fish\Trunk\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="118">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -402,6 +402,10 @@
   </si>
   <si>
     <t>随机卡牌类型</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>金币</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1137,17 +1141,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color auto="1"/>
@@ -1183,74 +1177,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1263,8 +1189,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:O85" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A3:O85"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:O86" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A3:O86"/>
   <sortState ref="A4:O111">
     <sortCondition ref="A3:A111"/>
   </sortState>
@@ -1297,7 +1223,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1576,14 +1502,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O85"/>
+  <dimension ref="A1:O86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.375" customWidth="1"/>
     <col min="3" max="3" width="8.875" customWidth="1"/>
     <col min="4" max="4" width="7.625" customWidth="1"/>
@@ -1837,737 +1764,737 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11">
-        <v>22033001</v>
+        <v>22032008</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="L11">
-        <v>2</v>
+        <v>117</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12">
-        <v>22033002</v>
+        <v>22033001</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L12">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13">
-        <v>22033003</v>
+        <v>22033002</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L13">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14">
-        <v>22033004</v>
+        <v>22033003</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="K14">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="L14">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15">
-        <v>22033005</v>
+        <v>22033004</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L15">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16">
-        <v>22033006</v>
+        <v>22033005</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K16">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L16">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17">
-        <v>22033007</v>
+        <v>22033006</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K17">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="L17">
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:15">
       <c r="A18">
-        <v>22033008</v>
+        <v>22033007</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K18">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:15">
       <c r="A19">
-        <v>22033009</v>
+        <v>22033008</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K19">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:15">
       <c r="A20">
-        <v>22033013</v>
+        <v>22033009</v>
       </c>
       <c r="B20" t="s">
-        <v>103</v>
-      </c>
-      <c r="O20">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="K20">
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:15">
       <c r="A21">
-        <v>22033014</v>
+        <v>22033013</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="O21">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:15">
       <c r="A22">
-        <v>22033015</v>
+        <v>22033014</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O22">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:15">
       <c r="A23">
-        <v>22033016</v>
+        <v>22033015</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
-      </c>
-      <c r="N23">
-        <v>9999</v>
+        <v>23</v>
+      </c>
+      <c r="O23">
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:15">
       <c r="A24">
-        <v>22033017</v>
+        <v>22033016</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N24">
-        <v>100</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="25" spans="1:15">
       <c r="A25">
-        <v>22033018</v>
+        <v>22033017</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="N25">
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:15">
       <c r="A26">
-        <v>22033030</v>
+        <v>22033018</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:15">
       <c r="A27">
-        <v>22033031</v>
+        <v>22033030</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:15">
       <c r="A28">
-        <v>22033032</v>
+        <v>22033031</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:15">
       <c r="A29">
-        <v>22034001</v>
+        <v>22033032</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29">
-        <v>50</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:15">
       <c r="A30">
-        <v>22034002</v>
+        <v>22034001</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30">
-        <v>300</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:15">
       <c r="A31">
-        <v>22034003</v>
+        <v>22034002</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="C31">
+        <v>300</v>
       </c>
     </row>
     <row r="32" spans="1:15">
       <c r="A32">
-        <v>22034004</v>
+        <v>22034003</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33">
-        <v>22034005</v>
+        <v>22034004</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34">
-        <v>22034006</v>
+        <v>22034005</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35">
-        <v>22034007</v>
+        <v>22034006</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36">
-        <v>22034008</v>
+        <v>22034007</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37">
-        <v>22034009</v>
+        <v>22034008</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38">
-        <v>22034010</v>
+        <v>22034009</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39">
-        <v>22034011</v>
+        <v>22034010</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40">
-        <v>22035001</v>
+        <v>22034011</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
-      </c>
-      <c r="H40" t="s">
-        <v>104</v>
+        <v>42</v>
+      </c>
+      <c r="D40">
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41">
-        <v>22035002</v>
+        <v>22035001</v>
       </c>
       <c r="B41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H41" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42">
-        <v>22035003</v>
+        <v>22035002</v>
       </c>
       <c r="B42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H42" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43">
-        <v>22036101</v>
+        <v>22035003</v>
       </c>
       <c r="B43" t="s">
-        <v>51</v>
-      </c>
-      <c r="G43">
-        <v>43000101</v>
+        <v>88</v>
+      </c>
+      <c r="H43" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44">
-        <v>22036102</v>
+        <v>22036101</v>
       </c>
       <c r="B44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G44">
-        <v>43000102</v>
+        <v>43000101</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45">
-        <v>22036103</v>
+        <v>22036102</v>
       </c>
       <c r="B45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G45">
-        <v>43000103</v>
+        <v>43000102</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46">
-        <v>22036104</v>
+        <v>22036103</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G46">
-        <v>43000104</v>
+        <v>43000103</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47">
-        <v>22036105</v>
+        <v>22036104</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G47">
-        <v>43000105</v>
+        <v>43000104</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48">
-        <v>22036106</v>
+        <v>22036105</v>
       </c>
       <c r="B48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G48">
-        <v>43000106</v>
+        <v>43000105</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49">
-        <v>22036107</v>
+        <v>22036106</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G49">
-        <v>43000107</v>
+        <v>43000106</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50">
-        <v>22036108</v>
+        <v>22036107</v>
       </c>
       <c r="B50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G50">
-        <v>43000108</v>
+        <v>43000107</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51">
-        <v>22036109</v>
+        <v>22036108</v>
       </c>
       <c r="B51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G51">
-        <v>43000109</v>
+        <v>43000108</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52">
-        <v>22036110</v>
+        <v>22036109</v>
       </c>
       <c r="B52" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G52">
-        <v>43000110</v>
+        <v>43000109</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53">
-        <v>22036201</v>
+        <v>22036110</v>
       </c>
       <c r="B53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G53">
-        <v>43000201</v>
+        <v>43000110</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54">
-        <v>22036202</v>
+        <v>22036201</v>
       </c>
       <c r="B54" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G54">
-        <v>43000202</v>
+        <v>43000201</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55">
-        <v>22036203</v>
+        <v>22036202</v>
       </c>
       <c r="B55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G55">
-        <v>43000203</v>
+        <v>43000202</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56">
-        <v>22036301</v>
+        <v>22036203</v>
       </c>
       <c r="B56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G56">
-        <v>43000301</v>
+        <v>43000203</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57">
-        <v>22036302</v>
+        <v>22036301</v>
       </c>
       <c r="B57" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G57">
-        <v>43000302</v>
+        <v>43000301</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58">
-        <v>22036303</v>
+        <v>22036302</v>
       </c>
       <c r="B58" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G58">
-        <v>43000303</v>
+        <v>43000302</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59">
-        <v>22036304</v>
+        <v>22036303</v>
       </c>
       <c r="B59" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G59">
-        <v>43000304</v>
+        <v>43000303</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60">
-        <v>22036305</v>
+        <v>22036304</v>
       </c>
       <c r="B60" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G60">
-        <v>43000305</v>
+        <v>43000304</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61">
-        <v>22036306</v>
+        <v>22036305</v>
       </c>
       <c r="B61" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G61">
-        <v>43000306</v>
+        <v>43000305</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62">
-        <v>22036307</v>
+        <v>22036306</v>
       </c>
       <c r="B62" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G62">
-        <v>43000307</v>
+        <v>43000306</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63">
-        <v>22036308</v>
+        <v>22036307</v>
       </c>
       <c r="B63" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G63">
-        <v>43000308</v>
+        <v>43000307</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64">
-        <v>22036309</v>
+        <v>22036308</v>
       </c>
       <c r="B64" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G64">
-        <v>43000309</v>
+        <v>43000308</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65">
-        <v>22036310</v>
+        <v>22036309</v>
       </c>
       <c r="B65" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G65">
-        <v>43000310</v>
+        <v>43000309</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66">
-        <v>22036311</v>
+        <v>22036310</v>
       </c>
       <c r="B66" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G66">
-        <v>43000311</v>
+        <v>43000310</v>
       </c>
     </row>
     <row r="67" spans="1:10">
       <c r="A67">
-        <v>22036312</v>
+        <v>22036311</v>
       </c>
       <c r="B67" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G67">
-        <v>43000312</v>
+        <v>43000311</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68">
-        <v>22036401</v>
+        <v>22036312</v>
       </c>
       <c r="B68" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G68">
-        <v>43000401</v>
+        <v>43000312</v>
       </c>
     </row>
     <row r="69" spans="1:10">
       <c r="A69">
-        <v>22036402</v>
+        <v>22036401</v>
       </c>
       <c r="B69" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G69">
-        <v>43000402</v>
+        <v>43000401</v>
       </c>
     </row>
     <row r="70" spans="1:10">
       <c r="A70">
-        <v>22036403</v>
+        <v>22036402</v>
       </c>
       <c r="B70" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G70">
-        <v>43000403</v>
+        <v>43000402</v>
       </c>
     </row>
     <row r="71" spans="1:10">
       <c r="A71">
-        <v>22036404</v>
+        <v>22036403</v>
       </c>
       <c r="B71" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G71">
-        <v>43000404</v>
+        <v>43000403</v>
       </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72">
-        <v>22036405</v>
+        <v>22036404</v>
       </c>
       <c r="B72" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G72">
-        <v>43000405</v>
+        <v>43000404</v>
       </c>
     </row>
     <row r="73" spans="1:10">
       <c r="A73">
-        <v>22036406</v>
+        <v>22036405</v>
       </c>
       <c r="B73" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G73">
-        <v>43000406</v>
+        <v>43000405</v>
       </c>
     </row>
     <row r="74" spans="1:10">
       <c r="A74">
-        <v>22036407</v>
+        <v>22036406</v>
       </c>
       <c r="B74" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G74">
-        <v>43000407</v>
+        <v>43000406</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="A75">
-        <v>22036408</v>
+        <v>22036407</v>
       </c>
       <c r="B75" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G75">
-        <v>43000408</v>
+        <v>43000407</v>
       </c>
     </row>
     <row r="76" spans="1:10">
       <c r="A76">
-        <v>22036501</v>
+        <v>22036408</v>
       </c>
       <c r="B76" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G76">
-        <v>43000501</v>
+        <v>43000408</v>
       </c>
     </row>
     <row r="77" spans="1:10">
       <c r="A77">
-        <v>22036502</v>
+        <v>22036501</v>
       </c>
       <c r="B77" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G77">
-        <v>43000502</v>
+        <v>43000501</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78">
-        <v>22037001</v>
+        <v>22036502</v>
       </c>
       <c r="B78" t="s">
-        <v>89</v>
-      </c>
-      <c r="I78">
-        <v>22037101</v>
-      </c>
-      <c r="J78">
-        <v>10800</v>
+        <v>85</v>
+      </c>
+      <c r="G78">
+        <v>43000502</v>
       </c>
     </row>
     <row r="79" spans="1:10">
       <c r="A79">
-        <v>22037002</v>
+        <v>22037001</v>
       </c>
       <c r="B79" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I79">
-        <v>22037102</v>
+        <v>22037101</v>
       </c>
       <c r="J79">
         <v>10800</v>
@@ -2575,13 +2502,13 @@
     </row>
     <row r="80" spans="1:10">
       <c r="A80">
-        <v>22037003</v>
+        <v>22037002</v>
       </c>
       <c r="B80" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I80">
-        <v>22037103</v>
+        <v>22037102</v>
       </c>
       <c r="J80">
         <v>10800</v>
@@ -2589,13 +2516,13 @@
     </row>
     <row r="81" spans="1:12">
       <c r="A81">
-        <v>22037004</v>
+        <v>22037003</v>
       </c>
       <c r="B81" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I81">
-        <v>22037104</v>
+        <v>22037103</v>
       </c>
       <c r="J81">
         <v>10800</v>
@@ -2603,55 +2530,69 @@
     </row>
     <row r="82" spans="1:12">
       <c r="A82">
-        <v>22037101</v>
+        <v>22037004</v>
       </c>
       <c r="B82" t="s">
-        <v>43</v>
-      </c>
-      <c r="C82">
-        <v>5</v>
+        <v>92</v>
+      </c>
+      <c r="I82">
+        <v>22037104</v>
+      </c>
+      <c r="J82">
+        <v>10800</v>
       </c>
     </row>
     <row r="83" spans="1:12">
       <c r="A83">
-        <v>22037102</v>
+        <v>22037101</v>
       </c>
       <c r="B83" t="s">
         <v>43</v>
       </c>
-      <c r="E83">
-        <v>1</v>
-      </c>
-      <c r="F83">
-        <v>20</v>
+      <c r="C83">
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:12">
       <c r="A84">
-        <v>22037103</v>
+        <v>22037102</v>
       </c>
       <c r="B84" t="s">
-        <v>30</v>
-      </c>
-      <c r="K84">
-        <v>2</v>
+        <v>43</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
+      <c r="F84">
+        <v>20</v>
       </c>
     </row>
     <row r="85" spans="1:12">
       <c r="A85">
+        <v>22037103</v>
+      </c>
+      <c r="B85" t="s">
+        <v>30</v>
+      </c>
+      <c r="K85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
+      <c r="A86">
         <v>22037104</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B86" t="s">
         <v>31</v>
       </c>
-      <c r="L85">
+      <c r="L86">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="A4:O85">
-    <cfRule type="containsBlanks" dxfId="1" priority="3">
+  <conditionalFormatting sqref="A4:O86">
+    <cfRule type="containsBlanks" dxfId="0" priority="3">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
#43 item given initial
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/ItemConsumer.xlsx
+++ b/ConfigData/Xlsx/ItemConsumer.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1505,7 +1505,7 @@
   <dimension ref="A1:O86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1675,7 +1675,7 @@
         <v>2</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1689,7 +1689,7 @@
         <v>3</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -1703,7 +1703,7 @@
         <v>4</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1717,7 +1717,7 @@
         <v>5</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1731,7 +1731,7 @@
         <v>6</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1745,7 +1745,7 @@
         <v>7</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:15">

</xml_diff>

<commit_message>
#42 cardbag rate via quality of card
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/ItemConsumer.xlsx
+++ b/ConfigData/Xlsx/ItemConsumer.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="134">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -344,123 +344,124 @@
     <t>随机幻兽卡</t>
   </si>
   <si>
+    <t>1;1;2;3;5</t>
+  </si>
+  <si>
+    <t>1;1;1;2;3</t>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int[]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Id</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PeopleId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得lp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得mp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得pp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>直接伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机卡牌类型</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>金币</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FightRandomCardType</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机卡牌（无）</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机卡牌（水）</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机卡牌（风）</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机卡牌（地）</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机卡牌（火）</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机卡牌（光）</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机卡牌（暗）</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机卡包概率</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机单卡</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RandomCardRate2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;1</t>
+  </si>
+  <si>
+    <t>1;2</t>
+  </si>
+  <si>
+    <t>1;3</t>
+  </si>
+  <si>
+    <t>1;4</t>
+  </si>
+  <si>
+    <t>1;5</t>
+  </si>
+  <si>
+    <t>1;6</t>
+  </si>
+  <si>
     <t>1;3;5;7;9</t>
-  </si>
-  <si>
-    <t>1;1;2;3;5</t>
-  </si>
-  <si>
-    <t>1;1;1;2;3</t>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int[]</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Id</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Name</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>PeopleId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>获得lp</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>获得mp</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>获得pp</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>直接伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机卡牌类型</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>金币</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>FightRandomCardType</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机卡牌（无）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机卡牌（水）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机卡牌（风）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机卡牌（地）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机卡牌（火）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机卡牌（光）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机卡牌（暗）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机卡包概率</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机单卡</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RandomCardRate2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;1</t>
-  </si>
-  <si>
-    <t>1;2</t>
-  </si>
-  <si>
-    <t>1;3</t>
-  </si>
-  <si>
-    <t>1;4</t>
-  </si>
-  <si>
-    <t>1;5</t>
-  </si>
-  <si>
-    <t>1;6</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>RandomCardRate</t>
@@ -1205,7 +1206,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
     <dxf>
       <font>
         <color auto="1"/>
@@ -1236,6 +1237,16 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1570,7 +1581,7 @@
   <dimension ref="A1:P93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H4" sqref="H4:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1579,8 +1590,7 @@
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
     <col min="3" max="3" width="8.88671875" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" customWidth="1"/>
-    <col min="6" max="6" width="8.21875" customWidth="1"/>
+    <col min="5" max="6" width="4.21875" customWidth="1"/>
     <col min="7" max="7" width="10.77734375" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" customWidth="1"/>
     <col min="9" max="9" width="6.88671875" customWidth="1"/>
@@ -1612,10 +1622,10 @@
         <v>97</v>
       </c>
       <c r="H1" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>123</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>124</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>98</v>
@@ -1624,19 +1634,19 @@
         <v>99</v>
       </c>
       <c r="L1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="M1" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>112</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -1644,7 +1654,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -1662,10 +1672,10 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>0</v>
@@ -1691,10 +1701,10 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>107</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -1709,13 +1719,13 @@
         <v>4</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>133</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>5</v>
@@ -1736,7 +1746,7 @@
         <v>10</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1744,10 +1754,13 @@
         <v>22031002</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
+      </c>
+      <c r="H4" t="s">
+        <v>132</v>
       </c>
       <c r="I4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1755,10 +1768,13 @@
         <v>22031003</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
+      </c>
+      <c r="H5" t="s">
+        <v>132</v>
       </c>
       <c r="I5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1766,10 +1782,13 @@
         <v>22031004</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
+      </c>
+      <c r="H6" t="s">
+        <v>132</v>
       </c>
       <c r="I6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1777,10 +1796,13 @@
         <v>22031005</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
+      </c>
+      <c r="H7" t="s">
+        <v>132</v>
       </c>
       <c r="I7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1788,10 +1810,13 @@
         <v>22031006</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
+      </c>
+      <c r="H8" t="s">
+        <v>132</v>
       </c>
       <c r="I8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1799,10 +1824,13 @@
         <v>22031007</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
+      </c>
+      <c r="H9" t="s">
+        <v>132</v>
       </c>
       <c r="I9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1810,10 +1838,13 @@
         <v>22031008</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="H10" t="s">
+        <v>132</v>
       </c>
       <c r="I10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1919,7 +1950,7 @@
         <v>22032008</v>
       </c>
       <c r="B18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -2228,7 +2259,7 @@
         <v>84</v>
       </c>
       <c r="H48" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -2239,7 +2270,7 @@
         <v>85</v>
       </c>
       <c r="H49" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -2250,7 +2281,7 @@
         <v>86</v>
       </c>
       <c r="H50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -2744,7 +2775,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="A4:P93">
-    <cfRule type="containsBlanks" dxfId="0" priority="3">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
#42 card package method redo
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/ItemConsumer.xlsx
+++ b/ConfigData/Xlsx/ItemConsumer.xlsx
@@ -344,12 +344,6 @@
     <t>随机幻兽卡</t>
   </si>
   <si>
-    <t>1;1;2;3;5</t>
-  </si>
-  <si>
-    <t>1;1;1;2;3</t>
-  </si>
-  <si>
     <t>string</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -460,11 +454,19 @@
     <t>1;6</t>
   </si>
   <si>
-    <t>1;3;5;7;9</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>RandomCardRate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0;250;120;50;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0;220;120;50;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0;120;80;50;30</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1206,7 +1208,37 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -1264,7 +1296,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:P93" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:P93" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A3:P93"/>
   <sortState ref="A4:O93">
     <sortCondition ref="A3:A93"/>
@@ -1580,8 +1612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H10"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1622,10 +1654,10 @@
         <v>97</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>98</v>
@@ -1634,19 +1666,19 @@
         <v>99</v>
       </c>
       <c r="L1" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="N1" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>110</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -1654,7 +1686,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -1672,10 +1704,10 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>0</v>
@@ -1701,10 +1733,10 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -1719,13 +1751,13 @@
         <v>4</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>5</v>
@@ -1746,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1754,13 +1786,13 @@
         <v>22031002</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1768,13 +1800,13 @@
         <v>22031003</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1782,13 +1814,13 @@
         <v>22031004</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1796,13 +1828,13 @@
         <v>22031005</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1810,13 +1842,13 @@
         <v>22031006</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1824,13 +1856,13 @@
         <v>22031007</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1838,13 +1870,13 @@
         <v>22031008</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1950,7 +1982,7 @@
         <v>22032008</v>
       </c>
       <c r="B18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -2259,7 +2291,7 @@
         <v>84</v>
       </c>
       <c r="H48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -2270,7 +2302,7 @@
         <v>85</v>
       </c>
       <c r="H49" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -2281,7 +2313,7 @@
         <v>86</v>
       </c>
       <c r="H50" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -2775,7 +2807,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="A4:P93">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+    <cfRule type="containsBlanks" dxfId="5" priority="3">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
new cardbag random by card type
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/ItemConsumer.xlsx
+++ b/ConfigData/Xlsx/ItemConsumer.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="141">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -392,34 +392,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>随机卡牌（无）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机卡牌（水）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机卡牌（风）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机卡牌（地）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机卡牌（火）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机卡牌（光）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机卡牌（暗）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>随机卡包概率</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -428,55 +400,100 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>1;1;0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;1;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;1;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;1;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;1;4</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;1;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;1;6</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>5;0;0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RandomCardCatalog</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0;840;150;10;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0;720;250;30;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0;600;350;50;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡牌补给包（生物）</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡牌补给包（武器）</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡牌补给包（法术）</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>RandomCardRate</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>1;1;0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;1;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;1;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;1;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;1;4</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;1;5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;1;6</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>5;0;0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RandomCardCatalog</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0;840;150;10;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0;720;250;30;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0;600;350;50;10</t>
+    <t>卡牌补给包（无）</t>
+  </si>
+  <si>
+    <t>卡牌补给包（水）</t>
+  </si>
+  <si>
+    <t>卡牌补给包（风）</t>
+  </si>
+  <si>
+    <t>卡牌补给包（地）</t>
+  </si>
+  <si>
+    <t>卡牌补给包（火）</t>
+  </si>
+  <si>
+    <t>卡牌补给包（光）</t>
+  </si>
+  <si>
+    <t>卡牌补给包（暗）</t>
+  </si>
+  <si>
+    <t>1;2;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;2;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;2;3</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1167,10 +1184,10 @@
     <xf numFmtId="0" fontId="21" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1218,7 +1235,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="5">
     <dxf>
       <font>
         <color auto="1"/>
@@ -1282,16 +1299,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1306,8 +1313,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:P93" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A3:P93"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:P96" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A3:P96"/>
   <sortState ref="A4:O93">
     <sortCondition ref="A3:A93"/>
   </sortState>
@@ -1620,10 +1627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P93"/>
+  <dimension ref="A1:P96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1664,10 +1671,10 @@
         <v>97</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>98</v>
@@ -1764,10 +1771,10 @@
         <v>105</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>5</v>
@@ -1795,179 +1802,179 @@
       <c r="A4">
         <v>22031002</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>113</v>
+      <c r="B4" s="12" t="s">
+        <v>131</v>
       </c>
       <c r="H4" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="I4" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5">
         <v>22031003</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>114</v>
+      <c r="B5" s="12" t="s">
+        <v>132</v>
       </c>
       <c r="H5" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="I5" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6">
         <v>22031004</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>115</v>
+      <c r="B6" s="12" t="s">
+        <v>133</v>
       </c>
       <c r="H6" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="I6" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7">
         <v>22031005</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>116</v>
+      <c r="B7" s="12" t="s">
+        <v>134</v>
       </c>
       <c r="H7" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="I7" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8">
         <v>22031006</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>117</v>
+      <c r="B8" s="12" t="s">
+        <v>135</v>
       </c>
       <c r="H8" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="I8" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9">
         <v>22031007</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>118</v>
+      <c r="B9" s="12" t="s">
+        <v>136</v>
       </c>
       <c r="H9" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="I9" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10">
         <v>22031008</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>119</v>
+      <c r="B10" s="12" t="s">
+        <v>137</v>
       </c>
       <c r="H10" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="I10" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11">
-        <v>22032001</v>
-      </c>
-      <c r="B11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <v>30</v>
+        <v>22031011</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="H11" t="s">
+        <v>124</v>
+      </c>
+      <c r="I11" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:16">
       <c r="A12">
-        <v>22032002</v>
-      </c>
-      <c r="B12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12">
-        <v>3</v>
-      </c>
-      <c r="F12">
-        <v>30</v>
+        <v>22031012</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="H12" t="s">
+        <v>124</v>
+      </c>
+      <c r="I12" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13">
-        <v>22032003</v>
-      </c>
-      <c r="B13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13">
-        <v>4</v>
-      </c>
-      <c r="F13">
-        <v>10</v>
+        <v>22031013</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="H13" t="s">
+        <v>124</v>
+      </c>
+      <c r="I13" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14">
-        <v>22032004</v>
+        <v>22032001</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F14">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15">
-        <v>22032005</v>
+        <v>22032002</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E15">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F15">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16">
-        <v>22032006</v>
+        <v>22032003</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E16">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F16">
         <v>10</v>
@@ -1975,802 +1982,802 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17">
-        <v>22032007</v>
+        <v>22032004</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F17">
-        <v>300</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:16">
       <c r="A18">
-        <v>22032008</v>
+        <v>22032005</v>
       </c>
       <c r="B18" t="s">
-        <v>111</v>
+        <v>46</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F18">
-        <v>50</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:16">
       <c r="A19">
-        <v>22033001</v>
+        <v>22032006</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="M19">
-        <v>2</v>
+        <v>47</v>
+      </c>
+      <c r="E19">
+        <v>7</v>
+      </c>
+      <c r="F19">
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:16">
       <c r="A20">
-        <v>22033002</v>
+        <v>22032007</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
-      </c>
-      <c r="M20">
-        <v>5</v>
+        <v>48</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>300</v>
       </c>
     </row>
     <row r="21" spans="1:16">
       <c r="A21">
-        <v>22033003</v>
+        <v>22032008</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
-      </c>
-      <c r="M21">
-        <v>10</v>
+        <v>111</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:16">
       <c r="A22">
-        <v>22033004</v>
+        <v>22033001</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="L22">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="M22">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:16">
       <c r="A23">
-        <v>22033005</v>
+        <v>22033002</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
-      </c>
-      <c r="L23">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="M23">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:16">
       <c r="A24">
-        <v>22033006</v>
+        <v>22033003</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
-      </c>
-      <c r="L24">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="M24">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:16">
       <c r="A25">
-        <v>22033007</v>
+        <v>22033004</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="L25">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:16">
       <c r="A26">
-        <v>22033008</v>
+        <v>22033005</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="L26">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="M26">
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:16">
       <c r="A27">
-        <v>22033009</v>
+        <v>22033006</v>
       </c>
       <c r="B27" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L27">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="M27">
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:16">
       <c r="A28">
-        <v>22033013</v>
+        <v>22033007</v>
       </c>
       <c r="B28" t="s">
-        <v>100</v>
-      </c>
-      <c r="P28">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="L28">
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:16">
       <c r="A29">
-        <v>22033014</v>
+        <v>22033008</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
-      </c>
-      <c r="P29">
-        <v>2</v>
+        <v>18</v>
+      </c>
+      <c r="L29">
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:16">
       <c r="A30">
-        <v>22033015</v>
+        <v>22033009</v>
       </c>
       <c r="B30" t="s">
-        <v>21</v>
-      </c>
-      <c r="P30">
-        <v>3</v>
+        <v>19</v>
+      </c>
+      <c r="L30">
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:16">
       <c r="A31">
-        <v>22033016</v>
+        <v>22033013</v>
       </c>
       <c r="B31" t="s">
-        <v>22</v>
-      </c>
-      <c r="O31">
-        <v>9999</v>
+        <v>100</v>
+      </c>
+      <c r="P31">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:16">
       <c r="A32">
+        <v>22033014</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="P32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33">
+        <v>22033015</v>
+      </c>
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="P33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34">
+        <v>22033016</v>
+      </c>
+      <c r="B34" t="s">
+        <v>22</v>
+      </c>
+      <c r="O34">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35">
         <v>22033017</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B35" t="s">
         <v>23</v>
       </c>
-      <c r="O32">
+      <c r="O35">
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
-      <c r="A33">
+    <row r="36" spans="1:16">
+      <c r="A36">
         <v>22033018</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B36" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
-      <c r="A34">
+    <row r="37" spans="1:16">
+      <c r="A37">
         <v>22033030</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B37" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
-      <c r="A35">
+    <row r="38" spans="1:16">
+      <c r="A38">
         <v>22033031</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B38" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
-      <c r="A36">
+    <row r="39" spans="1:16">
+      <c r="A39">
         <v>22033032</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B39" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
-      <c r="A37">
+    <row r="40" spans="1:16">
+      <c r="A40">
         <v>22034001</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B40" t="s">
         <v>30</v>
       </c>
-      <c r="C37">
+      <c r="C40">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
-      <c r="A38">
+    <row r="41" spans="1:16">
+      <c r="A41">
         <v>22034002</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B41" t="s">
         <v>31</v>
       </c>
-      <c r="C38">
+      <c r="C41">
         <v>300</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
-      <c r="A39">
+    <row r="42" spans="1:16">
+      <c r="A42">
         <v>22034003</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B42" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
-      <c r="A40">
+    <row r="43" spans="1:16">
+      <c r="A43">
         <v>22034004</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B43" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
-      <c r="A41">
+    <row r="44" spans="1:16">
+      <c r="A44">
         <v>22034005</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B44" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
-      <c r="A42">
+    <row r="45" spans="1:16">
+      <c r="A45">
         <v>22034006</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B45" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
-      <c r="A43">
+    <row r="46" spans="1:16">
+      <c r="A46">
         <v>22034007</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B46" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
-      <c r="A44">
+    <row r="47" spans="1:16">
+      <c r="A47">
         <v>22034008</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B47" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
-      <c r="A45">
+    <row r="48" spans="1:16">
+      <c r="A48">
         <v>22034009</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B48" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46">
-        <v>22034010</v>
-      </c>
-      <c r="B46" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47">
-        <v>22034011</v>
-      </c>
-      <c r="B47" t="s">
-        <v>40</v>
-      </c>
-      <c r="D47">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48">
-        <v>22035001</v>
-      </c>
-      <c r="B48" t="s">
-        <v>84</v>
-      </c>
-      <c r="H48" t="s">
-        <v>132</v>
-      </c>
-      <c r="I48" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49">
-        <v>22035002</v>
+        <v>22034010</v>
       </c>
       <c r="B49" t="s">
-        <v>85</v>
-      </c>
-      <c r="H49" t="s">
-        <v>133</v>
-      </c>
-      <c r="I49" t="s">
-        <v>130</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50">
-        <v>22035003</v>
+        <v>22034011</v>
       </c>
       <c r="B50" t="s">
-        <v>86</v>
-      </c>
-      <c r="H50" t="s">
-        <v>134</v>
-      </c>
-      <c r="I50" t="s">
-        <v>130</v>
+        <v>40</v>
+      </c>
+      <c r="D50">
+        <v>20</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51">
-        <v>22036101</v>
+        <v>22035001</v>
       </c>
       <c r="B51" t="s">
-        <v>49</v>
-      </c>
-      <c r="G51">
-        <v>43000101</v>
+        <v>84</v>
+      </c>
+      <c r="H51" t="s">
+        <v>124</v>
+      </c>
+      <c r="I51" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52">
-        <v>22036102</v>
+        <v>22035002</v>
       </c>
       <c r="B52" t="s">
-        <v>50</v>
-      </c>
-      <c r="G52">
-        <v>43000102</v>
+        <v>85</v>
+      </c>
+      <c r="H52" t="s">
+        <v>125</v>
+      </c>
+      <c r="I52" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53">
-        <v>22036103</v>
+        <v>22035003</v>
       </c>
       <c r="B53" t="s">
-        <v>51</v>
-      </c>
-      <c r="G53">
-        <v>43000103</v>
+        <v>86</v>
+      </c>
+      <c r="H53" t="s">
+        <v>126</v>
+      </c>
+      <c r="I53" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54">
-        <v>22036104</v>
+        <v>22036101</v>
       </c>
       <c r="B54" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G54">
-        <v>43000104</v>
+        <v>43000101</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55">
-        <v>22036105</v>
+        <v>22036102</v>
       </c>
       <c r="B55" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G55">
-        <v>43000105</v>
+        <v>43000102</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56">
-        <v>22036106</v>
+        <v>22036103</v>
       </c>
       <c r="B56" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G56">
-        <v>43000106</v>
+        <v>43000103</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57">
-        <v>22036107</v>
+        <v>22036104</v>
       </c>
       <c r="B57" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G57">
-        <v>43000107</v>
+        <v>43000104</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58">
-        <v>22036108</v>
+        <v>22036105</v>
       </c>
       <c r="B58" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G58">
-        <v>43000108</v>
+        <v>43000105</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59">
-        <v>22036109</v>
+        <v>22036106</v>
       </c>
       <c r="B59" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G59">
-        <v>43000109</v>
+        <v>43000106</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60">
-        <v>22036110</v>
+        <v>22036107</v>
       </c>
       <c r="B60" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G60">
-        <v>43000110</v>
+        <v>43000107</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61">
-        <v>22036201</v>
+        <v>22036108</v>
       </c>
       <c r="B61" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G61">
-        <v>43000201</v>
+        <v>43000108</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62">
-        <v>22036202</v>
+        <v>22036109</v>
       </c>
       <c r="B62" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G62">
-        <v>43000202</v>
+        <v>43000109</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63">
-        <v>22036203</v>
+        <v>22036110</v>
       </c>
       <c r="B63" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G63">
-        <v>43000203</v>
+        <v>43000110</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64">
-        <v>22036301</v>
+        <v>22036201</v>
       </c>
       <c r="B64" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G64">
-        <v>43000301</v>
+        <v>43000201</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65">
-        <v>22036302</v>
+        <v>22036202</v>
       </c>
       <c r="B65" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G65">
-        <v>43000302</v>
+        <v>43000202</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66">
-        <v>22036303</v>
+        <v>22036203</v>
       </c>
       <c r="B66" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G66">
-        <v>43000303</v>
+        <v>43000203</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67">
-        <v>22036304</v>
+        <v>22036301</v>
       </c>
       <c r="B67" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G67">
-        <v>43000304</v>
+        <v>43000301</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68">
-        <v>22036305</v>
+        <v>22036302</v>
       </c>
       <c r="B68" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G68">
-        <v>43000305</v>
+        <v>43000302</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69">
-        <v>22036306</v>
+        <v>22036303</v>
       </c>
       <c r="B69" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G69">
-        <v>43000306</v>
+        <v>43000303</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70">
-        <v>22036307</v>
+        <v>22036304</v>
       </c>
       <c r="B70" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G70">
-        <v>43000307</v>
+        <v>43000304</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71">
-        <v>22036308</v>
+        <v>22036305</v>
       </c>
       <c r="B71" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G71">
-        <v>43000308</v>
+        <v>43000305</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72">
-        <v>22036309</v>
+        <v>22036306</v>
       </c>
       <c r="B72" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G72">
-        <v>43000309</v>
+        <v>43000306</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73">
-        <v>22036310</v>
+        <v>22036307</v>
       </c>
       <c r="B73" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G73">
-        <v>43000310</v>
+        <v>43000307</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74">
-        <v>22036311</v>
+        <v>22036308</v>
       </c>
       <c r="B74" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G74">
-        <v>43000311</v>
+        <v>43000308</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75">
-        <v>22036312</v>
+        <v>22036309</v>
       </c>
       <c r="B75" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G75">
-        <v>43000312</v>
+        <v>43000309</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76">
-        <v>22036401</v>
+        <v>22036310</v>
       </c>
       <c r="B76" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G76">
-        <v>43000401</v>
+        <v>43000310</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77">
-        <v>22036402</v>
+        <v>22036311</v>
       </c>
       <c r="B77" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G77">
-        <v>43000402</v>
+        <v>43000311</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78">
-        <v>22036403</v>
+        <v>22036312</v>
       </c>
       <c r="B78" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G78">
-        <v>43000403</v>
+        <v>43000312</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79">
-        <v>22036404</v>
+        <v>22036401</v>
       </c>
       <c r="B79" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G79">
-        <v>43000404</v>
+        <v>43000401</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80">
-        <v>22036405</v>
+        <v>22036402</v>
       </c>
       <c r="B80" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G80">
-        <v>43000405</v>
+        <v>43000402</v>
       </c>
     </row>
     <row r="81" spans="1:13">
       <c r="A81">
-        <v>22036406</v>
+        <v>22036403</v>
       </c>
       <c r="B81" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G81">
-        <v>43000406</v>
+        <v>43000403</v>
       </c>
     </row>
     <row r="82" spans="1:13">
       <c r="A82">
-        <v>22036407</v>
+        <v>22036404</v>
       </c>
       <c r="B82" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G82">
-        <v>43000407</v>
+        <v>43000404</v>
       </c>
     </row>
     <row r="83" spans="1:13">
       <c r="A83">
-        <v>22036408</v>
+        <v>22036405</v>
       </c>
       <c r="B83" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G83">
-        <v>43000408</v>
+        <v>43000405</v>
       </c>
     </row>
     <row r="84" spans="1:13">
       <c r="A84">
-        <v>22036501</v>
+        <v>22036406</v>
       </c>
       <c r="B84" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G84">
-        <v>43000501</v>
+        <v>43000406</v>
       </c>
     </row>
     <row r="85" spans="1:13">
       <c r="A85">
-        <v>22036502</v>
+        <v>22036407</v>
       </c>
       <c r="B85" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G85">
-        <v>43000502</v>
+        <v>43000407</v>
       </c>
     </row>
     <row r="86" spans="1:13">
       <c r="A86">
-        <v>22037001</v>
+        <v>22036408</v>
       </c>
       <c r="B86" t="s">
-        <v>87</v>
-      </c>
-      <c r="J86">
-        <v>22037101</v>
-      </c>
-      <c r="K86">
-        <v>10800</v>
+        <v>81</v>
+      </c>
+      <c r="G86">
+        <v>43000408</v>
       </c>
     </row>
     <row r="87" spans="1:13">
       <c r="A87">
-        <v>22037002</v>
-      </c>
-      <c r="B87" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="J87">
-        <v>22037102</v>
-      </c>
-      <c r="K87">
-        <v>10800</v>
+        <v>22036501</v>
+      </c>
+      <c r="B87" t="s">
+        <v>82</v>
+      </c>
+      <c r="G87">
+        <v>43000501</v>
       </c>
     </row>
     <row r="88" spans="1:13">
       <c r="A88">
-        <v>22037003</v>
-      </c>
-      <c r="B88" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="J88">
-        <v>22037103</v>
-      </c>
-      <c r="K88">
-        <v>10800</v>
+        <v>22036502</v>
+      </c>
+      <c r="B88" t="s">
+        <v>83</v>
+      </c>
+      <c r="G88">
+        <v>43000502</v>
       </c>
     </row>
     <row r="89" spans="1:13">
       <c r="A89">
-        <v>22037004</v>
-      </c>
-      <c r="B89" s="12" t="s">
-        <v>90</v>
+        <v>22037001</v>
+      </c>
+      <c r="B89" t="s">
+        <v>87</v>
       </c>
       <c r="J89">
-        <v>22037104</v>
+        <v>22037101</v>
       </c>
       <c r="K89">
         <v>10800</v>
@@ -2778,55 +2785,97 @@
     </row>
     <row r="90" spans="1:13">
       <c r="A90">
-        <v>22037101</v>
-      </c>
-      <c r="B90" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C90">
-        <v>5</v>
+        <v>22037002</v>
+      </c>
+      <c r="B90" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="J90">
+        <v>22037102</v>
+      </c>
+      <c r="K90">
+        <v>10800</v>
       </c>
     </row>
     <row r="91" spans="1:13">
       <c r="A91">
-        <v>22037102</v>
-      </c>
-      <c r="B91" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E91">
-        <v>1</v>
-      </c>
-      <c r="F91">
-        <v>20</v>
+        <v>22037003</v>
+      </c>
+      <c r="B91" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="J91">
+        <v>22037103</v>
+      </c>
+      <c r="K91">
+        <v>10800</v>
       </c>
     </row>
     <row r="92" spans="1:13">
       <c r="A92">
-        <v>22037103</v>
-      </c>
-      <c r="B92" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L92">
-        <v>2</v>
+        <v>22037004</v>
+      </c>
+      <c r="B92" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="J92">
+        <v>22037104</v>
+      </c>
+      <c r="K92">
+        <v>10800</v>
       </c>
     </row>
     <row r="93" spans="1:13">
       <c r="A93">
+        <v>22037101</v>
+      </c>
+      <c r="B93" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C93">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13">
+      <c r="A94">
+        <v>22037102</v>
+      </c>
+      <c r="B94" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E94">
+        <v>1</v>
+      </c>
+      <c r="F94">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13">
+      <c r="A95">
+        <v>22037103</v>
+      </c>
+      <c r="B95" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13">
+      <c r="A96">
         <v>22037104</v>
       </c>
-      <c r="B93" s="12" t="s">
+      <c r="B96" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="M93">
+      <c r="M96">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="A4:P93">
-    <cfRule type="containsBlanks" dxfId="5" priority="3">
+  <conditionalFormatting sqref="A4:A10 A14:P96 C4:P13">
+    <cfRule type="containsBlanks" dxfId="3" priority="3">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
new effect of witch eye #87
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/ItemConsumer.xlsx
+++ b/ConfigData/Xlsx/ItemConsumer.xlsx
@@ -14,12 +14,15 @@
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -65,246 +68,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>小型魔法药剂</t>
-  </si>
-  <si>
-    <t>中型魔法药剂</t>
-  </si>
-  <si>
-    <t>大型魔法药剂</t>
-  </si>
-  <si>
-    <t>小型恢复药剂</t>
-  </si>
-  <si>
-    <t>中型恢复药剂</t>
-  </si>
-  <si>
-    <t>大型恢复药剂</t>
-  </si>
-  <si>
-    <t>小型活力药剂</t>
-  </si>
-  <si>
-    <t>中型活力药剂</t>
-  </si>
-  <si>
-    <t>大型活力药剂</t>
-  </si>
-  <si>
-    <t>随机武器卡</t>
-  </si>
-  <si>
-    <t>随机魔法卡</t>
-  </si>
-  <si>
-    <t>符文-查姆</t>
-  </si>
-  <si>
-    <t>符文-普尔</t>
-  </si>
-  <si>
-    <t>符文-艾尔</t>
-  </si>
-  <si>
-    <t>小型药剂-命</t>
-  </si>
-  <si>
-    <t>药剂-命</t>
-  </si>
-  <si>
-    <t>大型药剂-命</t>
-  </si>
-  <si>
-    <t>作物-苹果</t>
-  </si>
-  <si>
-    <t>作物-蓝莓</t>
-  </si>
-  <si>
-    <t>经验之书</t>
-  </si>
-  <si>
-    <t>能量之书</t>
-  </si>
-  <si>
-    <t>战斗药水</t>
-  </si>
-  <si>
-    <t>守护药水</t>
-  </si>
-  <si>
-    <t>法术药水</t>
-  </si>
-  <si>
-    <t>技巧药水</t>
-  </si>
-  <si>
-    <t>速度药水</t>
-  </si>
-  <si>
-    <t>幸运药水</t>
-  </si>
-  <si>
-    <t>体质药水</t>
-  </si>
-  <si>
-    <t>生存药水</t>
-  </si>
-  <si>
-    <t>体力药水</t>
-  </si>
-  <si>
-    <t>作物-豌豆</t>
-  </si>
-  <si>
-    <t>木材补给车</t>
-  </si>
-  <si>
-    <t>矿石补给车</t>
-  </si>
-  <si>
-    <t>水银补给车</t>
-  </si>
-  <si>
-    <t>红宝石补给车</t>
-  </si>
-  <si>
-    <t>硫磺补给车</t>
-  </si>
-  <si>
-    <t>水晶补给车</t>
-  </si>
-  <si>
-    <t>初始资源包</t>
-  </si>
-  <si>
-    <t>名片-塞尼斯</t>
-  </si>
-  <si>
-    <t>名片-塞巴斯恰恩</t>
-  </si>
-  <si>
-    <t>名片-科迪</t>
-  </si>
-  <si>
-    <t>名片-威阿伊丁</t>
-  </si>
-  <si>
-    <t>名片-奥莱伊李</t>
-  </si>
-  <si>
-    <t>名片-米兰达</t>
-  </si>
-  <si>
-    <t>名片-盖露贝尔</t>
-  </si>
-  <si>
-    <t>名片-贝露凯伊鲁</t>
-  </si>
-  <si>
-    <t>名片-雷洛比克</t>
-  </si>
-  <si>
-    <t>名片-巴鲁迪亚斯</t>
-  </si>
-  <si>
-    <t>名片-武藤游戏</t>
-  </si>
-  <si>
-    <t>名片-城之内</t>
-  </si>
-  <si>
-    <t>名片-海马懒人</t>
-  </si>
-  <si>
-    <t>名片-内芙妮</t>
-  </si>
-  <si>
-    <t>名片-塔妮丝</t>
-  </si>
-  <si>
-    <t>名片-卢卡</t>
-  </si>
-  <si>
-    <t>名片-艾斯特尔</t>
-  </si>
-  <si>
-    <t>名片-萨恩</t>
-  </si>
-  <si>
-    <t>名片-玛莎</t>
-  </si>
-  <si>
-    <t>名片-阿特罗姆</t>
-  </si>
-  <si>
-    <t>名片-泽诺</t>
-  </si>
-  <si>
-    <t>名片-拉凯尔</t>
-  </si>
-  <si>
-    <t>名片-纳尔萨斯</t>
-  </si>
-  <si>
-    <t>名片-纳隆</t>
-  </si>
-  <si>
-    <t>名片-维加</t>
-  </si>
-  <si>
-    <t>名片-诺德</t>
-  </si>
-  <si>
-    <t>名片-那那美</t>
-  </si>
-  <si>
-    <t>名片-弗兰克</t>
-  </si>
-  <si>
-    <t>名片-维克托</t>
-  </si>
-  <si>
-    <t>名片-洛克</t>
-  </si>
-  <si>
-    <t>名片-谢拉</t>
-  </si>
-  <si>
-    <t>名片-克莱布</t>
-  </si>
-  <si>
-    <t>名片-蔡</t>
-  </si>
-  <si>
-    <t>名片-约修亚</t>
-  </si>
-  <si>
-    <t>名片-艾斯蒂尔</t>
-  </si>
-  <si>
-    <t>猛兽卡片</t>
-  </si>
-  <si>
-    <t>战斧卡片</t>
-  </si>
-  <si>
-    <t>火焰卡片</t>
-  </si>
-  <si>
-    <t>种子-豌豆</t>
-  </si>
-  <si>
-    <t>种子-玉米</t>
-  </si>
-  <si>
-    <t>种子-苹果</t>
-  </si>
-  <si>
-    <t>种子-蓝莓</t>
-  </si>
-  <si>
     <t>序列</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -341,9 +104,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>随机幻兽卡</t>
-  </si>
-  <si>
     <t>string</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -384,10 +144,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>金币</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>FightRandomCardType</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -448,43 +204,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>卡牌补给包（生物）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>卡牌补给包（武器）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>卡牌补给包（法术）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>RandomCardRate</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>卡牌补给包（无）</t>
-  </si>
-  <si>
-    <t>卡牌补给包（水）</t>
-  </si>
-  <si>
-    <t>卡牌补给包（风）</t>
-  </si>
-  <si>
-    <t>卡牌补给包（地）</t>
-  </si>
-  <si>
-    <t>卡牌补给包（火）</t>
-  </si>
-  <si>
-    <t>卡牌补给包（光）</t>
-  </si>
-  <si>
-    <t>卡牌补给包（暗）</t>
-  </si>
-  <si>
     <t>1;2;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -494,6 +217,22 @@
   </si>
   <si>
     <t>1;2;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>圣言</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>HolyWord</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>witcheye</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1150,7 +889,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1182,9 +921,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
@@ -1235,7 +971,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="4">
     <dxf>
       <font>
         <color auto="1"/>
@@ -1248,33 +984,30 @@
     </dxf>
     <dxf>
       <font>
-        <color auto="1"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1299,6 +1032,16 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1312,15 +1055,859 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="材料"/>
+      <sheetName val="任务"/>
+      <sheetName val="其他"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>序列</v>
+          </cell>
+          <cell r="B1" t="str">
+            <v>名字</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>int</v>
+          </cell>
+          <cell r="B2" t="str">
+            <v>string</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>Id</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>Name</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>22031001</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>新手礼包</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>22031002</v>
+          </cell>
+          <cell r="B5" t="str">
+            <v>卡牌补给包（无）</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>22031003</v>
+          </cell>
+          <cell r="B6" t="str">
+            <v>卡牌补给包（水）</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>22031004</v>
+          </cell>
+          <cell r="B7" t="str">
+            <v>卡牌补给包（风）</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>22031005</v>
+          </cell>
+          <cell r="B8" t="str">
+            <v>卡牌补给包（地）</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>22031006</v>
+          </cell>
+          <cell r="B9" t="str">
+            <v>卡牌补给包（火）</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>22031007</v>
+          </cell>
+          <cell r="B10" t="str">
+            <v>卡牌补给包（光）</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>22031008</v>
+          </cell>
+          <cell r="B11" t="str">
+            <v>卡牌补给包（暗）</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>22031011</v>
+          </cell>
+          <cell r="B12" t="str">
+            <v>卡牌补给包（生物）</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>22031012</v>
+          </cell>
+          <cell r="B13" t="str">
+            <v>卡牌补给包（武器）</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>22031013</v>
+          </cell>
+          <cell r="B14" t="str">
+            <v>卡牌补给包（法术）</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>22031101</v>
+          </cell>
+          <cell r="B15" t="str">
+            <v>资源袋(植物)</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16">
+            <v>22031102</v>
+          </cell>
+          <cell r="B16" t="str">
+            <v>资源袋(鱼)</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17">
+            <v>22031103</v>
+          </cell>
+          <cell r="B17" t="str">
+            <v>资源袋(矿石)</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18">
+            <v>22031201</v>
+          </cell>
+          <cell r="B18" t="str">
+            <v>蓝色卡包</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>22031202</v>
+          </cell>
+          <cell r="B19" t="str">
+            <v>黄色卡包</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>22031203</v>
+          </cell>
+          <cell r="B20" t="str">
+            <v>红色卡包</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>22032001</v>
+          </cell>
+          <cell r="B21" t="str">
+            <v>木材补给车</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>22032002</v>
+          </cell>
+          <cell r="B22" t="str">
+            <v>矿石补给车</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23">
+            <v>22032003</v>
+          </cell>
+          <cell r="B23" t="str">
+            <v>水银补给车</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24">
+            <v>22032004</v>
+          </cell>
+          <cell r="B24" t="str">
+            <v>红宝石补给车</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25">
+            <v>22032005</v>
+          </cell>
+          <cell r="B25" t="str">
+            <v>硫磺补给车</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26">
+            <v>22032006</v>
+          </cell>
+          <cell r="B26" t="str">
+            <v>水晶补给车</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27">
+            <v>22032007</v>
+          </cell>
+          <cell r="B27" t="str">
+            <v>初始资源包</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28">
+            <v>22032008</v>
+          </cell>
+          <cell r="B28" t="str">
+            <v>金币</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29">
+            <v>22033001</v>
+          </cell>
+          <cell r="B29" t="str">
+            <v>小型魔法药剂</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30">
+            <v>22033002</v>
+          </cell>
+          <cell r="B30" t="str">
+            <v>中型魔法药剂</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31">
+            <v>22033003</v>
+          </cell>
+          <cell r="B31" t="str">
+            <v>大型魔法药剂</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32">
+            <v>22033004</v>
+          </cell>
+          <cell r="B32" t="str">
+            <v>小型恢复药剂</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33">
+            <v>22033005</v>
+          </cell>
+          <cell r="B33" t="str">
+            <v>中型恢复药剂</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34">
+            <v>22033006</v>
+          </cell>
+          <cell r="B34" t="str">
+            <v>大型恢复药剂</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35">
+            <v>22033007</v>
+          </cell>
+          <cell r="B35" t="str">
+            <v>小型活力药剂</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36">
+            <v>22033008</v>
+          </cell>
+          <cell r="B36" t="str">
+            <v>中型活力药剂</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37">
+            <v>22033009</v>
+          </cell>
+          <cell r="B37" t="str">
+            <v>大型活力药剂</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38">
+            <v>22033013</v>
+          </cell>
+          <cell r="B38" t="str">
+            <v>随机幻兽卡</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39">
+            <v>22033014</v>
+          </cell>
+          <cell r="B39" t="str">
+            <v>随机武器卡</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40">
+            <v>22033015</v>
+          </cell>
+          <cell r="B40" t="str">
+            <v>随机魔法卡</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41">
+            <v>22033016</v>
+          </cell>
+          <cell r="B41" t="str">
+            <v>符文-查姆</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42">
+            <v>22033017</v>
+          </cell>
+          <cell r="B42" t="str">
+            <v>符文-普尔</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43">
+            <v>22033018</v>
+          </cell>
+          <cell r="B43" t="str">
+            <v>符文-艾尔</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44">
+            <v>22033030</v>
+          </cell>
+          <cell r="B44" t="str">
+            <v>小型药剂-命</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45">
+            <v>22033031</v>
+          </cell>
+          <cell r="B45" t="str">
+            <v>药剂-命</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46">
+            <v>22033032</v>
+          </cell>
+          <cell r="B46" t="str">
+            <v>大型药剂-命</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47">
+            <v>22034001</v>
+          </cell>
+          <cell r="B47" t="str">
+            <v>经验之书</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48">
+            <v>22034002</v>
+          </cell>
+          <cell r="B48" t="str">
+            <v>能量之书</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49">
+            <v>22034003</v>
+          </cell>
+          <cell r="B49" t="str">
+            <v>战斗药水</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50">
+            <v>22034004</v>
+          </cell>
+          <cell r="B50" t="str">
+            <v>守护药水</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51">
+            <v>22034005</v>
+          </cell>
+          <cell r="B51" t="str">
+            <v>法术药水</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="A52">
+            <v>22034006</v>
+          </cell>
+          <cell r="B52" t="str">
+            <v>技巧药水</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="A53">
+            <v>22034007</v>
+          </cell>
+          <cell r="B53" t="str">
+            <v>速度药水</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="A54">
+            <v>22034008</v>
+          </cell>
+          <cell r="B54" t="str">
+            <v>幸运药水</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="A55">
+            <v>22034009</v>
+          </cell>
+          <cell r="B55" t="str">
+            <v>体质药水</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="A56">
+            <v>22034010</v>
+          </cell>
+          <cell r="B56" t="str">
+            <v>生存药水</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="A57">
+            <v>22034011</v>
+          </cell>
+          <cell r="B57" t="str">
+            <v>体力药水</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="A58">
+            <v>22035001</v>
+          </cell>
+          <cell r="B58" t="str">
+            <v>猛兽卡片</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="A59">
+            <v>22035002</v>
+          </cell>
+          <cell r="B59" t="str">
+            <v>战斧卡片</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="A60">
+            <v>22035003</v>
+          </cell>
+          <cell r="B60" t="str">
+            <v>火焰卡片</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="A61">
+            <v>22036101</v>
+          </cell>
+          <cell r="B61" t="str">
+            <v>名片-塞尼斯</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="A62">
+            <v>22036102</v>
+          </cell>
+          <cell r="B62" t="str">
+            <v>名片-塞巴斯恰恩</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="A63">
+            <v>22036103</v>
+          </cell>
+          <cell r="B63" t="str">
+            <v>名片-科迪</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="A64">
+            <v>22036104</v>
+          </cell>
+          <cell r="B64" t="str">
+            <v>名片-威阿伊丁</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="A65">
+            <v>22036105</v>
+          </cell>
+          <cell r="B65" t="str">
+            <v>名片-奥莱伊李</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="A66">
+            <v>22036106</v>
+          </cell>
+          <cell r="B66" t="str">
+            <v>名片-米兰达</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="A67">
+            <v>22036107</v>
+          </cell>
+          <cell r="B67" t="str">
+            <v>名片-盖露贝尔</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="A68">
+            <v>22036108</v>
+          </cell>
+          <cell r="B68" t="str">
+            <v>名片-贝露凯伊鲁</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="A69">
+            <v>22036109</v>
+          </cell>
+          <cell r="B69" t="str">
+            <v>名片-雷洛比克</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="A70">
+            <v>22036110</v>
+          </cell>
+          <cell r="B70" t="str">
+            <v>名片-巴鲁迪亚斯</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="A71">
+            <v>22036201</v>
+          </cell>
+          <cell r="B71" t="str">
+            <v>名片-武藤游戏</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="A72">
+            <v>22036202</v>
+          </cell>
+          <cell r="B72" t="str">
+            <v>名片-城之内</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="A73">
+            <v>22036203</v>
+          </cell>
+          <cell r="B73" t="str">
+            <v>名片-海马懒人</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="A74">
+            <v>22036301</v>
+          </cell>
+          <cell r="B74" t="str">
+            <v>名片-内芙妮</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="A75">
+            <v>22036302</v>
+          </cell>
+          <cell r="B75" t="str">
+            <v>名片-塔妮丝</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="A76">
+            <v>22036303</v>
+          </cell>
+          <cell r="B76" t="str">
+            <v>名片-卢卡</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="A77">
+            <v>22036304</v>
+          </cell>
+          <cell r="B77" t="str">
+            <v>名片-艾斯特尔</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="A78">
+            <v>22036305</v>
+          </cell>
+          <cell r="B78" t="str">
+            <v>名片-萨恩</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="A79">
+            <v>22036306</v>
+          </cell>
+          <cell r="B79" t="str">
+            <v>名片-玛莎</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="A80">
+            <v>22036307</v>
+          </cell>
+          <cell r="B80" t="str">
+            <v>名片-阿特罗姆</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="A81">
+            <v>22036308</v>
+          </cell>
+          <cell r="B81" t="str">
+            <v>名片-泽诺</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="A82">
+            <v>22036309</v>
+          </cell>
+          <cell r="B82" t="str">
+            <v>名片-拉凯尔</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="A83">
+            <v>22036310</v>
+          </cell>
+          <cell r="B83" t="str">
+            <v>名片-纳尔萨斯</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="A84">
+            <v>22036311</v>
+          </cell>
+          <cell r="B84" t="str">
+            <v>名片-纳隆</v>
+          </cell>
+        </row>
+        <row r="85">
+          <cell r="A85">
+            <v>22036312</v>
+          </cell>
+          <cell r="B85" t="str">
+            <v>名片-维加</v>
+          </cell>
+        </row>
+        <row r="86">
+          <cell r="A86">
+            <v>22036401</v>
+          </cell>
+          <cell r="B86" t="str">
+            <v>名片-诺德</v>
+          </cell>
+        </row>
+        <row r="87">
+          <cell r="A87">
+            <v>22036402</v>
+          </cell>
+          <cell r="B87" t="str">
+            <v>名片-那那美</v>
+          </cell>
+        </row>
+        <row r="88">
+          <cell r="A88">
+            <v>22036403</v>
+          </cell>
+          <cell r="B88" t="str">
+            <v>名片-弗兰克</v>
+          </cell>
+        </row>
+        <row r="89">
+          <cell r="A89">
+            <v>22036404</v>
+          </cell>
+          <cell r="B89" t="str">
+            <v>名片-维克托</v>
+          </cell>
+        </row>
+        <row r="90">
+          <cell r="A90">
+            <v>22036405</v>
+          </cell>
+          <cell r="B90" t="str">
+            <v>名片-洛克</v>
+          </cell>
+        </row>
+        <row r="91">
+          <cell r="A91">
+            <v>22036406</v>
+          </cell>
+          <cell r="B91" t="str">
+            <v>名片-谢拉</v>
+          </cell>
+        </row>
+        <row r="92">
+          <cell r="A92">
+            <v>22036407</v>
+          </cell>
+          <cell r="B92" t="str">
+            <v>名片-克莱布</v>
+          </cell>
+        </row>
+        <row r="93">
+          <cell r="A93">
+            <v>22036408</v>
+          </cell>
+          <cell r="B93" t="str">
+            <v>名片-蔡</v>
+          </cell>
+        </row>
+        <row r="94">
+          <cell r="A94">
+            <v>22036501</v>
+          </cell>
+          <cell r="B94" t="str">
+            <v>名片-约修亚</v>
+          </cell>
+        </row>
+        <row r="95">
+          <cell r="A95">
+            <v>22036502</v>
+          </cell>
+          <cell r="B95" t="str">
+            <v>名片-艾斯蒂尔</v>
+          </cell>
+        </row>
+        <row r="96">
+          <cell r="A96">
+            <v>22037001</v>
+          </cell>
+          <cell r="B96" t="str">
+            <v>种子-豌豆</v>
+          </cell>
+        </row>
+        <row r="97">
+          <cell r="A97">
+            <v>22037002</v>
+          </cell>
+          <cell r="B97" t="str">
+            <v>种子-玉米</v>
+          </cell>
+        </row>
+        <row r="98">
+          <cell r="A98">
+            <v>22037003</v>
+          </cell>
+          <cell r="B98" t="str">
+            <v>种子-苹果</v>
+          </cell>
+        </row>
+        <row r="99">
+          <cell r="A99">
+            <v>22037004</v>
+          </cell>
+          <cell r="B99" t="str">
+            <v>种子-蓝莓</v>
+          </cell>
+        </row>
+        <row r="100">
+          <cell r="A100">
+            <v>22037101</v>
+          </cell>
+          <cell r="B100" t="str">
+            <v>作物-豌豆</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="A101">
+            <v>22037102</v>
+          </cell>
+          <cell r="B101" t="str">
+            <v>作物-豌豆</v>
+          </cell>
+        </row>
+        <row r="102">
+          <cell r="A102">
+            <v>22037103</v>
+          </cell>
+          <cell r="B102" t="str">
+            <v>作物-苹果</v>
+          </cell>
+        </row>
+        <row r="103">
+          <cell r="A103">
+            <v>22037104</v>
+          </cell>
+          <cell r="B103" t="str">
+            <v>作物-蓝莓</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:P96" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A3:P96"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:Q96" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A3:Q96"/>
   <sortState ref="A4:O93">
     <sortCondition ref="A3:A93"/>
   </sortState>
-  <tableColumns count="16">
+  <tableColumns count="17">
     <tableColumn id="1" name="Id"/>
-    <tableColumn id="2" name="Name"/>
+    <tableColumn id="2" name="Name" dataDxfId="1">
+      <calculatedColumnFormula>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="3" name="GainExp"/>
     <tableColumn id="4" name="GainAp"/>
     <tableColumn id="5" name="ResourceId"/>
@@ -1335,6 +1922,7 @@
     <tableColumn id="13" name="GainPp"/>
     <tableColumn id="14" name="DirectDamage"/>
     <tableColumn id="15" name="FightRandomCardType"/>
+    <tableColumn id="17" name="HolyWord"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1627,10 +2215,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P96"/>
+  <dimension ref="A1:Q96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1645,65 +2233,68 @@
     <col min="9" max="9" width="6.88671875" customWidth="1"/>
     <col min="10" max="10" width="12.77734375" customWidth="1"/>
     <col min="11" max="11" width="10.77734375" customWidth="1"/>
-    <col min="12" max="16" width="7.33203125" customWidth="1"/>
+    <col min="12" max="17" width="7.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" s="9" t="s">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>92</v>
+        <v>12</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>93</v>
+        <v>13</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>94</v>
+        <v>14</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>95</v>
+        <v>15</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>96</v>
+        <v>16</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>97</v>
+        <v>17</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>113</v>
+        <v>31</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>114</v>
+        <v>32</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>98</v>
+        <v>18</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>106</v>
+        <v>25</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>107</v>
+        <v>26</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>108</v>
+        <v>27</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>109</v>
+        <v>28</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>101</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -1721,10 +2312,10 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>0</v>
@@ -1747,13 +2338,16 @@
       <c r="P2" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="Q2" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="4" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>104</v>
+        <v>23</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -1768,13 +2362,13 @@
         <v>4</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>105</v>
+        <v>24</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>130</v>
+        <v>45</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>123</v>
+        <v>41</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>5</v>
@@ -1795,155 +2389,169 @@
         <v>10</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>22031002</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>131</v>
+      <c r="B4" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>卡牌补给包（无）</v>
       </c>
       <c r="H4" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="I4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>22031003</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>132</v>
+      <c r="B5" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>卡牌补给包（水）</v>
       </c>
       <c r="H5" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="I5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>22031004</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>133</v>
+      <c r="B6" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>卡牌补给包（风）</v>
       </c>
       <c r="H6" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="I6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>22031005</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>134</v>
+      <c r="B7" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>卡牌补给包（地）</v>
       </c>
       <c r="H7" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="I7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8">
         <v>22031006</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>135</v>
+      <c r="B8" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>卡牌补给包（火）</v>
       </c>
       <c r="H8" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="I8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9">
         <v>22031007</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>136</v>
+      <c r="B9" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>卡牌补给包（光）</v>
       </c>
       <c r="H9" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="I9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10">
         <v>22031008</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>137</v>
+      <c r="B10" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>卡牌补给包（暗）</v>
       </c>
       <c r="H10" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="I10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11">
         <v>22031011</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>127</v>
+      <c r="B11" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>卡牌补给包（生物）</v>
       </c>
       <c r="H11" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="I11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12">
         <v>22031012</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>128</v>
+      <c r="B12" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>卡牌补给包（武器）</v>
       </c>
       <c r="H12" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="I12" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13">
         <v>22031013</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>129</v>
+      <c r="B13" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>卡牌补给包（法术）</v>
       </c>
       <c r="H13" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="I13" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14">
         <v>22032001</v>
       </c>
-      <c r="B14" t="s">
-        <v>42</v>
+      <c r="B14" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>木材补给车</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -1952,12 +2560,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:17">
       <c r="A15">
         <v>22032002</v>
       </c>
-      <c r="B15" t="s">
-        <v>43</v>
+      <c r="B15" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>矿石补给车</v>
       </c>
       <c r="E15">
         <v>3</v>
@@ -1966,12 +2575,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:17">
       <c r="A16">
         <v>22032003</v>
       </c>
-      <c r="B16" t="s">
-        <v>44</v>
+      <c r="B16" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>水银补给车</v>
       </c>
       <c r="E16">
         <v>4</v>
@@ -1984,8 +2594,9 @@
       <c r="A17">
         <v>22032004</v>
       </c>
-      <c r="B17" t="s">
-        <v>45</v>
+      <c r="B17" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>红宝石补给车</v>
       </c>
       <c r="E17">
         <v>5</v>
@@ -1998,8 +2609,9 @@
       <c r="A18">
         <v>22032005</v>
       </c>
-      <c r="B18" t="s">
-        <v>46</v>
+      <c r="B18" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>硫磺补给车</v>
       </c>
       <c r="E18">
         <v>6</v>
@@ -2012,8 +2624,9 @@
       <c r="A19">
         <v>22032006</v>
       </c>
-      <c r="B19" t="s">
-        <v>47</v>
+      <c r="B19" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>水晶补给车</v>
       </c>
       <c r="E19">
         <v>7</v>
@@ -2026,8 +2639,9 @@
       <c r="A20">
         <v>22032007</v>
       </c>
-      <c r="B20" t="s">
-        <v>48</v>
+      <c r="B20" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>初始资源包</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -2040,8 +2654,9 @@
       <c r="A21">
         <v>22032008</v>
       </c>
-      <c r="B21" t="s">
-        <v>111</v>
+      <c r="B21" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>金币</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -2054,8 +2669,9 @@
       <c r="A22">
         <v>22033001</v>
       </c>
-      <c r="B22" t="s">
-        <v>11</v>
+      <c r="B22" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>小型魔法药剂</v>
       </c>
       <c r="M22">
         <v>2</v>
@@ -2065,8 +2681,9 @@
       <c r="A23">
         <v>22033002</v>
       </c>
-      <c r="B23" t="s">
-        <v>12</v>
+      <c r="B23" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>中型魔法药剂</v>
       </c>
       <c r="M23">
         <v>5</v>
@@ -2076,8 +2693,9 @@
       <c r="A24">
         <v>22033003</v>
       </c>
-      <c r="B24" t="s">
-        <v>13</v>
+      <c r="B24" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>大型魔法药剂</v>
       </c>
       <c r="M24">
         <v>10</v>
@@ -2087,8 +2705,9 @@
       <c r="A25">
         <v>22033004</v>
       </c>
-      <c r="B25" t="s">
-        <v>14</v>
+      <c r="B25" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>小型恢复药剂</v>
       </c>
       <c r="L25">
         <v>1</v>
@@ -2101,8 +2720,9 @@
       <c r="A26">
         <v>22033005</v>
       </c>
-      <c r="B26" t="s">
-        <v>15</v>
+      <c r="B26" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>中型恢复药剂</v>
       </c>
       <c r="L26">
         <v>3</v>
@@ -2115,8 +2735,9 @@
       <c r="A27">
         <v>22033006</v>
       </c>
-      <c r="B27" t="s">
-        <v>16</v>
+      <c r="B27" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>大型恢复药剂</v>
       </c>
       <c r="L27">
         <v>5</v>
@@ -2129,8 +2750,9 @@
       <c r="A28">
         <v>22033007</v>
       </c>
-      <c r="B28" t="s">
-        <v>17</v>
+      <c r="B28" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>小型活力药剂</v>
       </c>
       <c r="L28">
         <v>2</v>
@@ -2140,8 +2762,9 @@
       <c r="A29">
         <v>22033008</v>
       </c>
-      <c r="B29" t="s">
-        <v>18</v>
+      <c r="B29" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>中型活力药剂</v>
       </c>
       <c r="L29">
         <v>5</v>
@@ -2151,8 +2774,9 @@
       <c r="A30">
         <v>22033009</v>
       </c>
-      <c r="B30" t="s">
-        <v>19</v>
+      <c r="B30" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>大型活力药剂</v>
       </c>
       <c r="L30">
         <v>10</v>
@@ -2162,8 +2786,9 @@
       <c r="A31">
         <v>22033013</v>
       </c>
-      <c r="B31" t="s">
-        <v>100</v>
+      <c r="B31" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>随机幻兽卡</v>
       </c>
       <c r="P31">
         <v>1</v>
@@ -2173,170 +2798,192 @@
       <c r="A32">
         <v>22033014</v>
       </c>
-      <c r="B32" t="s">
-        <v>20</v>
+      <c r="B32" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>随机武器卡</v>
       </c>
       <c r="P32">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:17">
       <c r="A33">
         <v>22033015</v>
       </c>
-      <c r="B33" t="s">
-        <v>21</v>
+      <c r="B33" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>随机魔法卡</v>
       </c>
       <c r="P33">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:17">
       <c r="A34">
         <v>22033016</v>
       </c>
-      <c r="B34" t="s">
-        <v>22</v>
+      <c r="B34" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>符文-查姆</v>
       </c>
       <c r="O34">
         <v>9999</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:17">
       <c r="A35">
         <v>22033017</v>
       </c>
-      <c r="B35" t="s">
-        <v>23</v>
+      <c r="B35" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>符文-普尔</v>
       </c>
       <c r="O35">
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:17">
       <c r="A36">
         <v>22033018</v>
       </c>
-      <c r="B36" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16">
+      <c r="B36" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>符文-艾尔</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
       <c r="A37">
         <v>22033030</v>
       </c>
-      <c r="B37" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16">
+      <c r="B37" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>小型药剂-命</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
       <c r="A38">
         <v>22033031</v>
       </c>
-      <c r="B38" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16">
+      <c r="B38" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>药剂-命</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
       <c r="A39">
         <v>22033032</v>
       </c>
-      <c r="B39" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16">
+      <c r="B39" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>大型药剂-命</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17">
       <c r="A40">
         <v>22034001</v>
       </c>
-      <c r="B40" t="s">
-        <v>30</v>
+      <c r="B40" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>经验之书</v>
       </c>
       <c r="C40">
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:17">
       <c r="A41">
         <v>22034002</v>
       </c>
-      <c r="B41" t="s">
-        <v>31</v>
+      <c r="B41" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>能量之书</v>
       </c>
       <c r="C41">
         <v>300</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:17">
       <c r="A42">
         <v>22034003</v>
       </c>
-      <c r="B42" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16">
+      <c r="B42" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>战斗药水</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
       <c r="A43">
         <v>22034004</v>
       </c>
-      <c r="B43" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16">
+      <c r="B43" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>守护药水</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17">
       <c r="A44">
         <v>22034005</v>
       </c>
-      <c r="B44" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16">
+      <c r="B44" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>法术药水</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17">
       <c r="A45">
         <v>22034006</v>
       </c>
-      <c r="B45" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16">
+      <c r="B45" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>技巧药水</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17">
       <c r="A46">
         <v>22034007</v>
       </c>
-      <c r="B46" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16">
+      <c r="B46" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>速度药水</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17">
       <c r="A47">
         <v>22034008</v>
       </c>
-      <c r="B47" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16">
+      <c r="B47" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>幸运药水</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17">
       <c r="A48">
         <v>22034009</v>
       </c>
-      <c r="B48" t="s">
-        <v>38</v>
+      <c r="B48" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>体质药水</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49">
         <v>22034010</v>
       </c>
-      <c r="B49" t="s">
-        <v>39</v>
+      <c r="B49" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>生存药水</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50">
         <v>22034011</v>
       </c>
-      <c r="B50" t="s">
-        <v>40</v>
+      <c r="B50" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>体力药水</v>
       </c>
       <c r="D50">
         <v>20</v>
@@ -2346,50 +2993,54 @@
       <c r="A51">
         <v>22035001</v>
       </c>
-      <c r="B51" t="s">
-        <v>84</v>
+      <c r="B51" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>猛兽卡片</v>
       </c>
       <c r="H51" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="I51" t="s">
-        <v>122</v>
+        <v>40</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52">
         <v>22035002</v>
       </c>
-      <c r="B52" t="s">
-        <v>85</v>
+      <c r="B52" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>战斧卡片</v>
       </c>
       <c r="H52" t="s">
-        <v>125</v>
+        <v>43</v>
       </c>
       <c r="I52" t="s">
-        <v>122</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53">
         <v>22035003</v>
       </c>
-      <c r="B53" t="s">
-        <v>86</v>
+      <c r="B53" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>火焰卡片</v>
       </c>
       <c r="H53" t="s">
-        <v>126</v>
+        <v>44</v>
       </c>
       <c r="I53" t="s">
-        <v>122</v>
+        <v>40</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54">
         <v>22036101</v>
       </c>
-      <c r="B54" t="s">
-        <v>49</v>
+      <c r="B54" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-塞尼斯</v>
       </c>
       <c r="G54">
         <v>43000101</v>
@@ -2399,8 +3050,9 @@
       <c r="A55">
         <v>22036102</v>
       </c>
-      <c r="B55" t="s">
-        <v>50</v>
+      <c r="B55" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-塞巴斯恰恩</v>
       </c>
       <c r="G55">
         <v>43000102</v>
@@ -2410,8 +3062,9 @@
       <c r="A56">
         <v>22036103</v>
       </c>
-      <c r="B56" t="s">
-        <v>51</v>
+      <c r="B56" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-科迪</v>
       </c>
       <c r="G56">
         <v>43000103</v>
@@ -2421,8 +3074,9 @@
       <c r="A57">
         <v>22036104</v>
       </c>
-      <c r="B57" t="s">
-        <v>52</v>
+      <c r="B57" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-威阿伊丁</v>
       </c>
       <c r="G57">
         <v>43000104</v>
@@ -2432,8 +3086,9 @@
       <c r="A58">
         <v>22036105</v>
       </c>
-      <c r="B58" t="s">
-        <v>53</v>
+      <c r="B58" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-奥莱伊李</v>
       </c>
       <c r="G58">
         <v>43000105</v>
@@ -2443,8 +3098,9 @@
       <c r="A59">
         <v>22036106</v>
       </c>
-      <c r="B59" t="s">
-        <v>54</v>
+      <c r="B59" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-米兰达</v>
       </c>
       <c r="G59">
         <v>43000106</v>
@@ -2454,8 +3110,9 @@
       <c r="A60">
         <v>22036107</v>
       </c>
-      <c r="B60" t="s">
-        <v>55</v>
+      <c r="B60" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-盖露贝尔</v>
       </c>
       <c r="G60">
         <v>43000107</v>
@@ -2465,8 +3122,9 @@
       <c r="A61">
         <v>22036108</v>
       </c>
-      <c r="B61" t="s">
-        <v>56</v>
+      <c r="B61" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-贝露凯伊鲁</v>
       </c>
       <c r="G61">
         <v>43000108</v>
@@ -2476,8 +3134,9 @@
       <c r="A62">
         <v>22036109</v>
       </c>
-      <c r="B62" t="s">
-        <v>57</v>
+      <c r="B62" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-雷洛比克</v>
       </c>
       <c r="G62">
         <v>43000109</v>
@@ -2487,8 +3146,9 @@
       <c r="A63">
         <v>22036110</v>
       </c>
-      <c r="B63" t="s">
-        <v>58</v>
+      <c r="B63" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-巴鲁迪亚斯</v>
       </c>
       <c r="G63">
         <v>43000110</v>
@@ -2498,8 +3158,9 @@
       <c r="A64">
         <v>22036201</v>
       </c>
-      <c r="B64" t="s">
-        <v>59</v>
+      <c r="B64" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-武藤游戏</v>
       </c>
       <c r="G64">
         <v>43000201</v>
@@ -2509,8 +3170,9 @@
       <c r="A65">
         <v>22036202</v>
       </c>
-      <c r="B65" t="s">
-        <v>60</v>
+      <c r="B65" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-城之内</v>
       </c>
       <c r="G65">
         <v>43000202</v>
@@ -2520,8 +3182,9 @@
       <c r="A66">
         <v>22036203</v>
       </c>
-      <c r="B66" t="s">
-        <v>61</v>
+      <c r="B66" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-海马懒人</v>
       </c>
       <c r="G66">
         <v>43000203</v>
@@ -2531,8 +3194,9 @@
       <c r="A67">
         <v>22036301</v>
       </c>
-      <c r="B67" t="s">
-        <v>62</v>
+      <c r="B67" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-内芙妮</v>
       </c>
       <c r="G67">
         <v>43000301</v>
@@ -2542,8 +3206,9 @@
       <c r="A68">
         <v>22036302</v>
       </c>
-      <c r="B68" t="s">
-        <v>63</v>
+      <c r="B68" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-塔妮丝</v>
       </c>
       <c r="G68">
         <v>43000302</v>
@@ -2553,8 +3218,9 @@
       <c r="A69">
         <v>22036303</v>
       </c>
-      <c r="B69" t="s">
-        <v>64</v>
+      <c r="B69" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-卢卡</v>
       </c>
       <c r="G69">
         <v>43000303</v>
@@ -2564,8 +3230,9 @@
       <c r="A70">
         <v>22036304</v>
       </c>
-      <c r="B70" t="s">
-        <v>65</v>
+      <c r="B70" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-艾斯特尔</v>
       </c>
       <c r="G70">
         <v>43000304</v>
@@ -2575,8 +3242,9 @@
       <c r="A71">
         <v>22036305</v>
       </c>
-      <c r="B71" t="s">
-        <v>66</v>
+      <c r="B71" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-萨恩</v>
       </c>
       <c r="G71">
         <v>43000305</v>
@@ -2586,8 +3254,9 @@
       <c r="A72">
         <v>22036306</v>
       </c>
-      <c r="B72" t="s">
-        <v>67</v>
+      <c r="B72" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-玛莎</v>
       </c>
       <c r="G72">
         <v>43000306</v>
@@ -2597,8 +3266,9 @@
       <c r="A73">
         <v>22036307</v>
       </c>
-      <c r="B73" t="s">
-        <v>68</v>
+      <c r="B73" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-阿特罗姆</v>
       </c>
       <c r="G73">
         <v>43000307</v>
@@ -2608,8 +3278,9 @@
       <c r="A74">
         <v>22036308</v>
       </c>
-      <c r="B74" t="s">
-        <v>69</v>
+      <c r="B74" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-泽诺</v>
       </c>
       <c r="G74">
         <v>43000308</v>
@@ -2619,8 +3290,9 @@
       <c r="A75">
         <v>22036309</v>
       </c>
-      <c r="B75" t="s">
-        <v>70</v>
+      <c r="B75" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-拉凯尔</v>
       </c>
       <c r="G75">
         <v>43000309</v>
@@ -2630,8 +3302,9 @@
       <c r="A76">
         <v>22036310</v>
       </c>
-      <c r="B76" t="s">
-        <v>71</v>
+      <c r="B76" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-纳尔萨斯</v>
       </c>
       <c r="G76">
         <v>43000310</v>
@@ -2641,8 +3314,9 @@
       <c r="A77">
         <v>22036311</v>
       </c>
-      <c r="B77" t="s">
-        <v>72</v>
+      <c r="B77" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-纳隆</v>
       </c>
       <c r="G77">
         <v>43000311</v>
@@ -2652,8 +3326,9 @@
       <c r="A78">
         <v>22036312</v>
       </c>
-      <c r="B78" t="s">
-        <v>73</v>
+      <c r="B78" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-维加</v>
       </c>
       <c r="G78">
         <v>43000312</v>
@@ -2663,8 +3338,9 @@
       <c r="A79">
         <v>22036401</v>
       </c>
-      <c r="B79" t="s">
-        <v>74</v>
+      <c r="B79" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-诺德</v>
       </c>
       <c r="G79">
         <v>43000401</v>
@@ -2674,8 +3350,9 @@
       <c r="A80">
         <v>22036402</v>
       </c>
-      <c r="B80" t="s">
-        <v>75</v>
+      <c r="B80" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-那那美</v>
       </c>
       <c r="G80">
         <v>43000402</v>
@@ -2685,8 +3362,9 @@
       <c r="A81">
         <v>22036403</v>
       </c>
-      <c r="B81" t="s">
-        <v>76</v>
+      <c r="B81" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-弗兰克</v>
       </c>
       <c r="G81">
         <v>43000403</v>
@@ -2696,8 +3374,9 @@
       <c r="A82">
         <v>22036404</v>
       </c>
-      <c r="B82" t="s">
-        <v>77</v>
+      <c r="B82" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-维克托</v>
       </c>
       <c r="G82">
         <v>43000404</v>
@@ -2707,8 +3386,9 @@
       <c r="A83">
         <v>22036405</v>
       </c>
-      <c r="B83" t="s">
-        <v>78</v>
+      <c r="B83" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-洛克</v>
       </c>
       <c r="G83">
         <v>43000405</v>
@@ -2718,8 +3398,9 @@
       <c r="A84">
         <v>22036406</v>
       </c>
-      <c r="B84" t="s">
-        <v>79</v>
+      <c r="B84" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-谢拉</v>
       </c>
       <c r="G84">
         <v>43000406</v>
@@ -2729,8 +3410,9 @@
       <c r="A85">
         <v>22036407</v>
       </c>
-      <c r="B85" t="s">
-        <v>80</v>
+      <c r="B85" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-克莱布</v>
       </c>
       <c r="G85">
         <v>43000407</v>
@@ -2740,8 +3422,9 @@
       <c r="A86">
         <v>22036408</v>
       </c>
-      <c r="B86" t="s">
-        <v>81</v>
+      <c r="B86" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-蔡</v>
       </c>
       <c r="G86">
         <v>43000408</v>
@@ -2751,8 +3434,9 @@
       <c r="A87">
         <v>22036501</v>
       </c>
-      <c r="B87" t="s">
-        <v>82</v>
+      <c r="B87" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-约修亚</v>
       </c>
       <c r="G87">
         <v>43000501</v>
@@ -2762,8 +3446,9 @@
       <c r="A88">
         <v>22036502</v>
       </c>
-      <c r="B88" t="s">
-        <v>83</v>
+      <c r="B88" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>名片-艾斯蒂尔</v>
       </c>
       <c r="G88">
         <v>43000502</v>
@@ -2773,8 +3458,9 @@
       <c r="A89">
         <v>22037001</v>
       </c>
-      <c r="B89" t="s">
-        <v>87</v>
+      <c r="B89" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>种子-豌豆</v>
       </c>
       <c r="J89">
         <v>22037101</v>
@@ -2787,8 +3473,9 @@
       <c r="A90">
         <v>22037002</v>
       </c>
-      <c r="B90" s="11" t="s">
-        <v>88</v>
+      <c r="B90" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>种子-玉米</v>
       </c>
       <c r="J90">
         <v>22037102</v>
@@ -2801,8 +3488,9 @@
       <c r="A91">
         <v>22037003</v>
       </c>
-      <c r="B91" s="11" t="s">
-        <v>89</v>
+      <c r="B91" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>种子-苹果</v>
       </c>
       <c r="J91">
         <v>22037103</v>
@@ -2815,8 +3503,9 @@
       <c r="A92">
         <v>22037004</v>
       </c>
-      <c r="B92" s="11" t="s">
-        <v>90</v>
+      <c r="B92" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>种子-蓝莓</v>
       </c>
       <c r="J92">
         <v>22037104</v>
@@ -2829,8 +3518,9 @@
       <c r="A93">
         <v>22037101</v>
       </c>
-      <c r="B93" s="11" t="s">
-        <v>41</v>
+      <c r="B93" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>作物-豌豆</v>
       </c>
       <c r="C93">
         <v>5</v>
@@ -2840,8 +3530,9 @@
       <c r="A94">
         <v>22037102</v>
       </c>
-      <c r="B94" s="11" t="s">
-        <v>41</v>
+      <c r="B94" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>作物-豌豆</v>
       </c>
       <c r="E94">
         <v>1</v>
@@ -2854,8 +3545,9 @@
       <c r="A95">
         <v>22037103</v>
       </c>
-      <c r="B95" s="11" t="s">
-        <v>28</v>
+      <c r="B95" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>作物-苹果</v>
       </c>
       <c r="L95">
         <v>2</v>
@@ -2865,8 +3557,9 @@
       <c r="A96">
         <v>22037104</v>
       </c>
-      <c r="B96" s="11" t="s">
-        <v>29</v>
+      <c r="B96" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>作物-蓝莓</v>
       </c>
       <c r="M96">
         <v>2</v>
@@ -2875,8 +3568,13 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="A4:A10 A14:P96 C4:P13">
-    <cfRule type="containsBlanks" dxfId="3" priority="3">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(A4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q4:Q96">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(Q4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
check some deck  cards
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/ItemConsumer.xlsx
+++ b/ConfigData/Xlsx/ItemConsumer.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -291,8 +291,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1026,26 +1026,6 @@
   <dxfs count="4">
     <dxf>
       <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1094,6 +1074,26 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1950,14 +1950,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:S95" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:S95" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A3:S95"/>
   <sortState ref="A4:O93">
     <sortCondition ref="A3:A93"/>
   </sortState>
   <tableColumns count="19">
     <tableColumn id="1" name="Id"/>
-    <tableColumn id="2" name="~Name" dataDxfId="2">
+    <tableColumn id="2" name="~Name" dataDxfId="0">
       <calculatedColumnFormula>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="GainExp"/>
@@ -1983,7 +1983,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2058,6 +2058,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2093,6 +2110,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2271,26 +2305,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="V54" sqref="V54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" customWidth="1"/>
-    <col min="5" max="6" width="4.21875" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
-    <col min="9" max="9" width="6.88671875" customWidth="1"/>
-    <col min="10" max="10" width="12.77734375" customWidth="1"/>
-    <col min="11" max="11" width="10.77734375" customWidth="1"/>
-    <col min="12" max="19" width="7.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" customWidth="1"/>
+    <col min="3" max="3" width="8.875" customWidth="1"/>
+    <col min="4" max="4" width="7.625" customWidth="1"/>
+    <col min="5" max="6" width="4.25" customWidth="1"/>
+    <col min="7" max="7" width="10.75" customWidth="1"/>
+    <col min="8" max="8" width="12.625" customWidth="1"/>
+    <col min="9" max="9" width="6.875" customWidth="1"/>
+    <col min="10" max="10" width="12.75" customWidth="1"/>
+    <col min="11" max="11" width="10.75" customWidth="1"/>
+    <col min="12" max="19" width="7.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -2349,7 +2383,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2408,7 +2442,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>22</v>
       </c>
@@ -2467,7 +2501,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>22031002</v>
       </c>
@@ -2482,7 +2516,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>22031003</v>
       </c>
@@ -2497,7 +2531,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>22031004</v>
       </c>
@@ -2512,7 +2546,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>22031005</v>
       </c>
@@ -2527,7 +2561,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>22031006</v>
       </c>
@@ -2542,7 +2576,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>22031007</v>
       </c>
@@ -2557,7 +2591,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>22031008</v>
       </c>
@@ -2572,7 +2606,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>22031011</v>
       </c>
@@ -2587,7 +2621,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>22031012</v>
       </c>
@@ -2602,7 +2636,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>22031013</v>
       </c>
@@ -2617,7 +2651,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>22032001</v>
       </c>
@@ -2632,7 +2666,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>22032002</v>
       </c>
@@ -2647,7 +2681,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>22032003</v>
       </c>
@@ -2662,7 +2696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>22032004</v>
       </c>
@@ -2677,7 +2711,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>22032005</v>
       </c>
@@ -2692,7 +2726,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>22032006</v>
       </c>
@@ -2707,7 +2741,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>22032007</v>
       </c>
@@ -2722,7 +2756,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>22032008</v>
       </c>
@@ -2737,7 +2771,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>22033001</v>
       </c>
@@ -2749,7 +2783,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>22033002</v>
       </c>
@@ -2761,7 +2795,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>22033003</v>
       </c>
@@ -2773,7 +2807,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>22033004</v>
       </c>
@@ -2785,7 +2819,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>22033005</v>
       </c>
@@ -2797,7 +2831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>22033006</v>
       </c>
@@ -2809,7 +2843,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>22033007</v>
       </c>
@@ -2821,7 +2855,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>22033008</v>
       </c>
@@ -2833,7 +2867,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>22033009</v>
       </c>
@@ -2845,7 +2879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>22033013</v>
       </c>
@@ -2857,7 +2891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>22033014</v>
       </c>
@@ -2869,7 +2903,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:19">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>22033015</v>
       </c>
@@ -2881,7 +2915,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:19">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>22033016</v>
       </c>
@@ -2893,7 +2927,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="35" spans="1:19">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>22033017</v>
       </c>
@@ -2905,7 +2939,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:19">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>22033018</v>
       </c>
@@ -2917,7 +2951,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:19">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>22033030</v>
       </c>
@@ -2929,7 +2963,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:19">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>22033031</v>
       </c>
@@ -2941,7 +2975,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="39" spans="1:19">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>22033032</v>
       </c>
@@ -2953,7 +2987,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="40" spans="1:19">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>22034001</v>
       </c>
@@ -2965,7 +2999,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:19">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>22034002</v>
       </c>
@@ -2977,7 +3011,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="42" spans="1:19">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>22034003</v>
       </c>
@@ -2989,7 +3023,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:19">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>22034004</v>
       </c>
@@ -3001,7 +3035,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:19">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>22034005</v>
       </c>
@@ -3013,7 +3047,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:19">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>22034006</v>
       </c>
@@ -3025,7 +3059,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:19">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>22034007</v>
       </c>
@@ -3037,7 +3071,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="1:19">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>22034008</v>
       </c>
@@ -3049,7 +3083,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="1:19">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>22034009</v>
       </c>
@@ -3061,7 +3095,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>22034011</v>
       </c>
@@ -3073,7 +3107,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>22035001</v>
       </c>
@@ -3088,7 +3122,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>22035002</v>
       </c>
@@ -3103,7 +3137,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>22035003</v>
       </c>
@@ -3118,7 +3152,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>22036101</v>
       </c>
@@ -3127,10 +3161,10 @@
         <v>名片-塞尼斯</v>
       </c>
       <c r="G53">
-        <v>43000101</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
+        <v>43020101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>22036102</v>
       </c>
@@ -3139,10 +3173,10 @@
         <v>名片-塞巴斯恰恩</v>
       </c>
       <c r="G54">
-        <v>43000102</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
+        <v>43020102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>22036103</v>
       </c>
@@ -3151,10 +3185,10 @@
         <v>名片-科迪</v>
       </c>
       <c r="G55">
-        <v>43000103</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
+        <v>43020103</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>22036104</v>
       </c>
@@ -3163,10 +3197,10 @@
         <v>名片-威阿伊丁</v>
       </c>
       <c r="G56">
-        <v>43000104</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
+        <v>43020104</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>22036105</v>
       </c>
@@ -3175,10 +3209,10 @@
         <v>名片-奥莱伊李</v>
       </c>
       <c r="G57">
-        <v>43000105</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
+        <v>43020105</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>22036106</v>
       </c>
@@ -3187,10 +3221,10 @@
         <v>名片-米兰达</v>
       </c>
       <c r="G58">
-        <v>43000106</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
+        <v>43020106</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>22036107</v>
       </c>
@@ -3199,10 +3233,10 @@
         <v>名片-盖露贝尔</v>
       </c>
       <c r="G59">
-        <v>43000107</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
+        <v>43020107</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A60">
         <v>22036108</v>
       </c>
@@ -3211,10 +3245,10 @@
         <v>名片-贝露凯伊鲁</v>
       </c>
       <c r="G60">
-        <v>43000108</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
+        <v>43020108</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>22036109</v>
       </c>
@@ -3223,10 +3257,10 @@
         <v>名片-雷洛比克</v>
       </c>
       <c r="G61">
-        <v>43000109</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9">
+        <v>43020109</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>22036110</v>
       </c>
@@ -3235,10 +3269,10 @@
         <v>名片-巴鲁迪亚斯</v>
       </c>
       <c r="G62">
-        <v>43000110</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
+        <v>43020110</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>22036201</v>
       </c>
@@ -3247,10 +3281,10 @@
         <v>名片-武藤游戏</v>
       </c>
       <c r="G63">
-        <v>43000201</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
+        <v>43020201</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>22036202</v>
       </c>
@@ -3259,10 +3293,10 @@
         <v>名片-城之内</v>
       </c>
       <c r="G64">
-        <v>43000202</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
+        <v>43020202</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A65">
         <v>22036203</v>
       </c>
@@ -3271,10 +3305,10 @@
         <v>名片-海马懒人</v>
       </c>
       <c r="G65">
-        <v>43000203</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
+        <v>43020203</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A66">
         <v>22036301</v>
       </c>
@@ -3283,10 +3317,10 @@
         <v>名片-内芙妮</v>
       </c>
       <c r="G66">
-        <v>43000301</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
+        <v>43020301</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>22036302</v>
       </c>
@@ -3295,10 +3329,10 @@
         <v>名片-塔妮丝</v>
       </c>
       <c r="G67">
-        <v>43000302</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
+        <v>43020302</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A68">
         <v>22036303</v>
       </c>
@@ -3307,10 +3341,10 @@
         <v>名片-卢卡</v>
       </c>
       <c r="G68">
-        <v>43000303</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
+        <v>43020303</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A69">
         <v>22036304</v>
       </c>
@@ -3319,10 +3353,10 @@
         <v>名片-艾斯特尔</v>
       </c>
       <c r="G69">
-        <v>43000304</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7">
+        <v>43020304</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A70">
         <v>22036305</v>
       </c>
@@ -3331,10 +3365,10 @@
         <v>名片-萨恩</v>
       </c>
       <c r="G70">
-        <v>43000305</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7">
+        <v>43020305</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>22036306</v>
       </c>
@@ -3343,10 +3377,10 @@
         <v>名片-玛莎</v>
       </c>
       <c r="G71">
-        <v>43000306</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7">
+        <v>43020306</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A72">
         <v>22036307</v>
       </c>
@@ -3355,10 +3389,10 @@
         <v>名片-阿特罗姆</v>
       </c>
       <c r="G72">
-        <v>43000307</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7">
+        <v>43020307</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A73">
         <v>22036308</v>
       </c>
@@ -3367,10 +3401,10 @@
         <v>名片-泽诺</v>
       </c>
       <c r="G73">
-        <v>43000308</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7">
+        <v>43020308</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A74">
         <v>22036309</v>
       </c>
@@ -3379,10 +3413,10 @@
         <v>名片-拉凯尔</v>
       </c>
       <c r="G74">
-        <v>43000309</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7">
+        <v>43020309</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A75">
         <v>22036310</v>
       </c>
@@ -3391,10 +3425,10 @@
         <v>名片-纳尔萨斯</v>
       </c>
       <c r="G75">
-        <v>43000310</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7">
+        <v>43020310</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A76">
         <v>22036311</v>
       </c>
@@ -3403,10 +3437,10 @@
         <v>名片-纳隆</v>
       </c>
       <c r="G76">
-        <v>43000311</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7">
+        <v>43020311</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A77">
         <v>22036312</v>
       </c>
@@ -3415,10 +3449,10 @@
         <v>名片-维加</v>
       </c>
       <c r="G77">
-        <v>43000312</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
+        <v>43020312</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A78">
         <v>22036401</v>
       </c>
@@ -3427,10 +3461,10 @@
         <v>名片-诺德</v>
       </c>
       <c r="G78">
-        <v>43000401</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
+        <v>43020401</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A79">
         <v>22036402</v>
       </c>
@@ -3439,10 +3473,10 @@
         <v>名片-那那美</v>
       </c>
       <c r="G79">
-        <v>43000402</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7">
+        <v>43020402</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A80">
         <v>22036403</v>
       </c>
@@ -3451,10 +3485,10 @@
         <v>名片-弗兰克</v>
       </c>
       <c r="G80">
-        <v>43000403</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13">
+        <v>43020403</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A81">
         <v>22036404</v>
       </c>
@@ -3463,10 +3497,10 @@
         <v>名片-维克托</v>
       </c>
       <c r="G81">
-        <v>43000404</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13">
+        <v>43020404</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A82">
         <v>22036405</v>
       </c>
@@ -3475,10 +3509,10 @@
         <v>名片-洛克</v>
       </c>
       <c r="G82">
-        <v>43000405</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13">
+        <v>43020405</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A83">
         <v>22036406</v>
       </c>
@@ -3487,10 +3521,10 @@
         <v>名片-谢拉</v>
       </c>
       <c r="G83">
-        <v>43000406</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13">
+        <v>43020406</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A84">
         <v>22036407</v>
       </c>
@@ -3499,10 +3533,10 @@
         <v>名片-克莱布</v>
       </c>
       <c r="G84">
-        <v>43000407</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13">
+        <v>43020407</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A85">
         <v>22036408</v>
       </c>
@@ -3511,10 +3545,10 @@
         <v>名片-蔡</v>
       </c>
       <c r="G85">
-        <v>43000408</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13">
+        <v>43020408</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A86">
         <v>22036501</v>
       </c>
@@ -3523,10 +3557,10 @@
         <v>名片-约修亚</v>
       </c>
       <c r="G86">
-        <v>43000501</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13">
+        <v>43020501</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A87">
         <v>22036502</v>
       </c>
@@ -3535,10 +3569,10 @@
         <v>名片-艾斯蒂尔</v>
       </c>
       <c r="G87">
-        <v>43000502</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13">
+        <v>43020502</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A88">
         <v>22037001</v>
       </c>
@@ -3553,7 +3587,7 @@
         <v>10800</v>
       </c>
     </row>
-    <row r="89" spans="1:13">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A89">
         <v>22037002</v>
       </c>
@@ -3568,7 +3602,7 @@
         <v>10800</v>
       </c>
     </row>
-    <row r="90" spans="1:13">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A90">
         <v>22037003</v>
       </c>
@@ -3583,7 +3617,7 @@
         <v>10800</v>
       </c>
     </row>
-    <row r="91" spans="1:13">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A91">
         <v>22037004</v>
       </c>
@@ -3598,7 +3632,7 @@
         <v>10800</v>
       </c>
     </row>
-    <row r="92" spans="1:13">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A92">
         <v>22037101</v>
       </c>
@@ -3610,7 +3644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:13">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A93">
         <v>22037102</v>
       </c>
@@ -3625,7 +3659,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="94" spans="1:13">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A94">
         <v>22037103</v>
       </c>
@@ -3637,7 +3671,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:13">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A95">
         <v>22037104</v>
       </c>
@@ -3651,13 +3685,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="A4:A10 C4:P13 Q4:R95 S95 S4:S46 S48 A14:P95">
-    <cfRule type="containsBlanks" dxfId="1" priority="5">
+  <conditionalFormatting sqref="A4:A10 C4:P13 Q4:R95 S95 S4:S46 S48 A14:P52 A88:P95 A53:F87 H53:P87">
+    <cfRule type="containsBlanks" dxfId="3" priority="5">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S49:S94">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
       <formula>LEN(TRIM(S49))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
remove all people item
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/ItemConsumer.xlsx
+++ b/ConfigData/Xlsx/ItemConsumer.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="64">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -92,10 +92,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>角色id</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>产出物</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -113,10 +109,6 @@
   </si>
   <si>
     <t>Id</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>PeopleId</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1023,7 +1015,17 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1074,26 +1076,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1601,345 +1583,65 @@
         </row>
         <row r="61">
           <cell r="A61">
-            <v>22036101</v>
+            <v>22037001</v>
           </cell>
           <cell r="B61" t="str">
-            <v>名片-塞尼斯</v>
+            <v>种子-豌豆</v>
           </cell>
         </row>
         <row r="62">
           <cell r="A62">
-            <v>22036102</v>
+            <v>22037002</v>
           </cell>
           <cell r="B62" t="str">
-            <v>名片-塞巴斯恰恩</v>
+            <v>种子-玉米</v>
           </cell>
         </row>
         <row r="63">
           <cell r="A63">
-            <v>22036103</v>
+            <v>22037003</v>
           </cell>
           <cell r="B63" t="str">
-            <v>名片-科迪</v>
+            <v>种子-苹果</v>
           </cell>
         </row>
         <row r="64">
           <cell r="A64">
-            <v>22036104</v>
+            <v>22037004</v>
           </cell>
           <cell r="B64" t="str">
-            <v>名片-威阿伊丁</v>
+            <v>种子-蓝莓</v>
           </cell>
         </row>
         <row r="65">
           <cell r="A65">
-            <v>22036105</v>
+            <v>22037101</v>
           </cell>
           <cell r="B65" t="str">
-            <v>名片-奥莱伊李</v>
+            <v>作物-豌豆</v>
           </cell>
         </row>
         <row r="66">
           <cell r="A66">
-            <v>22036106</v>
+            <v>22037102</v>
           </cell>
           <cell r="B66" t="str">
-            <v>名片-米兰达</v>
+            <v>作物-豌豆</v>
           </cell>
         </row>
         <row r="67">
           <cell r="A67">
-            <v>22036107</v>
+            <v>22037103</v>
           </cell>
           <cell r="B67" t="str">
-            <v>名片-盖露贝尔</v>
+            <v>作物-苹果</v>
           </cell>
         </row>
         <row r="68">
           <cell r="A68">
-            <v>22036108</v>
+            <v>22037104</v>
           </cell>
           <cell r="B68" t="str">
-            <v>名片-贝露凯伊鲁</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="A69">
-            <v>22036109</v>
-          </cell>
-          <cell r="B69" t="str">
-            <v>名片-雷洛比克</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="A70">
-            <v>22036110</v>
-          </cell>
-          <cell r="B70" t="str">
-            <v>名片-巴鲁迪亚斯</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="A71">
-            <v>22036201</v>
-          </cell>
-          <cell r="B71" t="str">
-            <v>名片-武藤游戏</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="A72">
-            <v>22036202</v>
-          </cell>
-          <cell r="B72" t="str">
-            <v>名片-城之内</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="A73">
-            <v>22036203</v>
-          </cell>
-          <cell r="B73" t="str">
-            <v>名片-海马懒人</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="A74">
-            <v>22036301</v>
-          </cell>
-          <cell r="B74" t="str">
-            <v>名片-内芙妮</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="A75">
-            <v>22036302</v>
-          </cell>
-          <cell r="B75" t="str">
-            <v>名片-塔妮丝</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="A76">
-            <v>22036303</v>
-          </cell>
-          <cell r="B76" t="str">
-            <v>名片-卢卡</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="A77">
-            <v>22036304</v>
-          </cell>
-          <cell r="B77" t="str">
-            <v>名片-艾斯特尔</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="A78">
-            <v>22036305</v>
-          </cell>
-          <cell r="B78" t="str">
-            <v>名片-萨恩</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="A79">
-            <v>22036306</v>
-          </cell>
-          <cell r="B79" t="str">
-            <v>名片-玛莎</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="A80">
-            <v>22036307</v>
-          </cell>
-          <cell r="B80" t="str">
-            <v>名片-阿特罗姆</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="A81">
-            <v>22036308</v>
-          </cell>
-          <cell r="B81" t="str">
-            <v>名片-泽诺</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="A82">
-            <v>22036309</v>
-          </cell>
-          <cell r="B82" t="str">
-            <v>名片-拉凯尔</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="A83">
-            <v>22036310</v>
-          </cell>
-          <cell r="B83" t="str">
-            <v>名片-纳尔萨斯</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="A84">
-            <v>22036311</v>
-          </cell>
-          <cell r="B84" t="str">
-            <v>名片-纳隆</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="A85">
-            <v>22036312</v>
-          </cell>
-          <cell r="B85" t="str">
-            <v>名片-维加</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="A86">
-            <v>22036401</v>
-          </cell>
-          <cell r="B86" t="str">
-            <v>名片-诺德</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="A87">
-            <v>22036402</v>
-          </cell>
-          <cell r="B87" t="str">
-            <v>名片-那那美</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="A88">
-            <v>22036403</v>
-          </cell>
-          <cell r="B88" t="str">
-            <v>名片-弗兰克</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="A89">
-            <v>22036404</v>
-          </cell>
-          <cell r="B89" t="str">
-            <v>名片-维克托</v>
-          </cell>
-        </row>
-        <row r="90">
-          <cell r="A90">
-            <v>22036405</v>
-          </cell>
-          <cell r="B90" t="str">
-            <v>名片-洛克</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="A91">
-            <v>22036406</v>
-          </cell>
-          <cell r="B91" t="str">
-            <v>名片-谢拉</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="A92">
-            <v>22036407</v>
-          </cell>
-          <cell r="B92" t="str">
-            <v>名片-克莱布</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="A93">
-            <v>22036408</v>
-          </cell>
-          <cell r="B93" t="str">
-            <v>名片-蔡</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="A94">
-            <v>22036501</v>
-          </cell>
-          <cell r="B94" t="str">
-            <v>名片-约修亚</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="A95">
-            <v>22036502</v>
-          </cell>
-          <cell r="B95" t="str">
-            <v>名片-艾斯蒂尔</v>
-          </cell>
-        </row>
-        <row r="96">
-          <cell r="A96">
-            <v>22037001</v>
-          </cell>
-          <cell r="B96" t="str">
-            <v>种子-豌豆</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="A97">
-            <v>22037002</v>
-          </cell>
-          <cell r="B97" t="str">
-            <v>种子-玉米</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="A98">
-            <v>22037003</v>
-          </cell>
-          <cell r="B98" t="str">
-            <v>种子-苹果</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="A99">
-            <v>22037004</v>
-          </cell>
-          <cell r="B99" t="str">
-            <v>种子-蓝莓</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="A100">
-            <v>22037101</v>
-          </cell>
-          <cell r="B100" t="str">
-            <v>作物-豌豆</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="A101">
-            <v>22037102</v>
-          </cell>
-          <cell r="B101" t="str">
-            <v>作物-豌豆</v>
-          </cell>
-        </row>
-        <row r="102">
-          <cell r="A102">
-            <v>22037103</v>
-          </cell>
-          <cell r="B102" t="str">
-            <v>作物-苹果</v>
-          </cell>
-        </row>
-        <row r="103">
-          <cell r="A103">
-            <v>22037104</v>
-          </cell>
-          <cell r="B103" t="str">
             <v>作物-蓝莓</v>
           </cell>
         </row>
@@ -1950,21 +1652,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:S95" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A3:S95"/>
-  <sortState ref="A4:O93">
-    <sortCondition ref="A3:A93"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:R60" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A3:R60"/>
+  <sortState ref="A4:N58">
+    <sortCondition ref="A3:A58"/>
   </sortState>
-  <tableColumns count="19">
+  <tableColumns count="18">
     <tableColumn id="1" name="Id"/>
-    <tableColumn id="2" name="~Name" dataDxfId="0">
+    <tableColumn id="2" name="~Name" dataDxfId="1">
       <calculatedColumnFormula>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="GainExp"/>
     <tableColumn id="4" name="GainAp"/>
     <tableColumn id="5" name="ResourceId"/>
     <tableColumn id="6" name="ResourceCount"/>
-    <tableColumn id="7" name="PeopleId"/>
     <tableColumn id="8" name="RandomCardRate"/>
     <tableColumn id="16" name="RandomCardCatalog"/>
     <tableColumn id="9" name="FarmItemId"/>
@@ -2303,10 +2004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S95"/>
+  <dimension ref="A1:R60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="V54" sqref="V54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2316,15 +2017,14 @@
     <col min="3" max="3" width="8.875" customWidth="1"/>
     <col min="4" max="4" width="7.625" customWidth="1"/>
     <col min="5" max="6" width="4.25" customWidth="1"/>
-    <col min="7" max="7" width="10.75" customWidth="1"/>
-    <col min="8" max="8" width="12.625" customWidth="1"/>
-    <col min="9" max="9" width="6.875" customWidth="1"/>
-    <col min="10" max="10" width="12.75" customWidth="1"/>
-    <col min="11" max="11" width="10.75" customWidth="1"/>
-    <col min="12" max="19" width="7.375" customWidth="1"/>
+    <col min="7" max="7" width="12.625" customWidth="1"/>
+    <col min="8" max="8" width="6.875" customWidth="1"/>
+    <col min="9" max="9" width="12.75" customWidth="1"/>
+    <col min="10" max="10" width="10.75" customWidth="1"/>
+    <col min="11" max="18" width="7.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -2344,51 +2044,48 @@
         <v>16</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>17</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>31</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="9" t="s">
-        <v>19</v>
+      <c r="K1" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="L1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="10" t="s">
-        <v>27</v>
-      </c>
       <c r="P1" s="10" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="Q1" s="10" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -2403,21 +2100,21 @@
         <v>0</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="M2" s="3" t="s">
@@ -2430,24 +2127,21 @@
         <v>0</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="R2" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -2462,46 +2156,43 @@
         <v>4</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="L3" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="M3" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="S3" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>22031002</v>
       </c>
@@ -2509,14 +2200,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包（无）</v>
       </c>
+      <c r="G4" t="s">
+        <v>39</v>
+      </c>
       <c r="H4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>22031003</v>
       </c>
@@ -2524,14 +2215,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包（水）</v>
       </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
       <c r="H5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>22031004</v>
       </c>
@@ -2539,14 +2230,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包（风）</v>
       </c>
+      <c r="G6" t="s">
+        <v>39</v>
+      </c>
       <c r="H6" t="s">
-        <v>41</v>
-      </c>
-      <c r="I6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>22031005</v>
       </c>
@@ -2554,14 +2245,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包（地）</v>
       </c>
+      <c r="G7" t="s">
+        <v>39</v>
+      </c>
       <c r="H7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>22031006</v>
       </c>
@@ -2569,14 +2260,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包（火）</v>
       </c>
+      <c r="G8" t="s">
+        <v>39</v>
+      </c>
       <c r="H8" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>22031007</v>
       </c>
@@ -2584,14 +2275,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包（光）</v>
       </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
       <c r="H9" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>22031008</v>
       </c>
@@ -2599,14 +2290,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包（暗）</v>
       </c>
+      <c r="G10" t="s">
+        <v>39</v>
+      </c>
       <c r="H10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>22031011</v>
       </c>
@@ -2614,14 +2305,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包（生物）</v>
       </c>
+      <c r="G11" t="s">
+        <v>39</v>
+      </c>
       <c r="H11" t="s">
-        <v>41</v>
-      </c>
-      <c r="I11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>22031012</v>
       </c>
@@ -2629,14 +2320,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包（武器）</v>
       </c>
+      <c r="G12" t="s">
+        <v>39</v>
+      </c>
       <c r="H12" t="s">
-        <v>41</v>
-      </c>
-      <c r="I12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>22031013</v>
       </c>
@@ -2644,14 +2335,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包（法术）</v>
       </c>
+      <c r="G13" t="s">
+        <v>39</v>
+      </c>
       <c r="H13" t="s">
-        <v>41</v>
-      </c>
-      <c r="I13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>22032001</v>
       </c>
@@ -2666,7 +2357,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>22032002</v>
       </c>
@@ -2681,7 +2372,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>22032003</v>
       </c>
@@ -2696,7 +2387,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>22032004</v>
       </c>
@@ -2711,7 +2402,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>22032005</v>
       </c>
@@ -2726,7 +2417,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>22032006</v>
       </c>
@@ -2741,7 +2432,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>22032007</v>
       </c>
@@ -2756,7 +2447,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>22032008</v>
       </c>
@@ -2771,7 +2462,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>22033001</v>
       </c>
@@ -2779,11 +2470,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>小型魔法药剂</v>
       </c>
-      <c r="M22">
+      <c r="L22">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>22033002</v>
       </c>
@@ -2791,11 +2482,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>中型魔法药剂</v>
       </c>
-      <c r="M23">
+      <c r="L23">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>22033003</v>
       </c>
@@ -2803,11 +2494,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>大型魔法药剂</v>
       </c>
-      <c r="M24">
+      <c r="L24">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>22033004</v>
       </c>
@@ -2815,11 +2506,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>小型活力药剂</v>
       </c>
-      <c r="L25">
+      <c r="K25">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>22033005</v>
       </c>
@@ -2827,11 +2518,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>中型活力药剂</v>
       </c>
-      <c r="L26">
+      <c r="K26">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>22033006</v>
       </c>
@@ -2839,11 +2530,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>大型活力药剂</v>
       </c>
-      <c r="L27">
+      <c r="K27">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>22033007</v>
       </c>
@@ -2851,11 +2542,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>小型体力药剂</v>
       </c>
-      <c r="N28">
+      <c r="M28">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>22033008</v>
       </c>
@@ -2863,11 +2554,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>中型体力药剂</v>
       </c>
-      <c r="N29">
+      <c r="M29">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>22033009</v>
       </c>
@@ -2875,11 +2566,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>大型体力药剂</v>
       </c>
-      <c r="N30">
+      <c r="M30">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>22033013</v>
       </c>
@@ -2887,11 +2578,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>随机幻兽卡</v>
       </c>
-      <c r="P31">
+      <c r="O31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>22033014</v>
       </c>
@@ -2899,11 +2590,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>随机武器卡</v>
       </c>
-      <c r="P32">
+      <c r="O32">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>22033015</v>
       </c>
@@ -2911,11 +2602,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>随机魔法卡</v>
       </c>
-      <c r="P33">
+      <c r="O33">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>22033016</v>
       </c>
@@ -2923,11 +2614,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>符文-查姆</v>
       </c>
-      <c r="O34">
+      <c r="N34">
         <v>9999</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>22033017</v>
       </c>
@@ -2935,11 +2626,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>符文-普尔</v>
       </c>
-      <c r="O35">
+      <c r="N35">
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>22033018</v>
       </c>
@@ -2947,11 +2638,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>符文-艾尔</v>
       </c>
-      <c r="Q36" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="P36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>22033030</v>
       </c>
@@ -2959,11 +2650,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>木质修理锤</v>
       </c>
-      <c r="R37">
+      <c r="Q37">
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>22033031</v>
       </c>
@@ -2971,11 +2662,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>钢铁修理锤</v>
       </c>
-      <c r="R38">
+      <c r="Q38">
         <v>500</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>22033032</v>
       </c>
@@ -2983,11 +2674,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>神圣修理锤</v>
       </c>
-      <c r="R39">
+      <c r="Q39">
         <v>1000</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>22034001</v>
       </c>
@@ -2999,7 +2690,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>22034002</v>
       </c>
@@ -3011,7 +2702,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>22034003</v>
       </c>
@@ -3019,11 +2710,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>攻速药水</v>
       </c>
-      <c r="S42" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="R42" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>22034004</v>
       </c>
@@ -3031,11 +2722,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>守护药水</v>
       </c>
-      <c r="S43" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="R43" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>22034005</v>
       </c>
@@ -3043,11 +2734,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>法术药水</v>
       </c>
-      <c r="S44" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="R44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>22034006</v>
       </c>
@@ -3055,11 +2746,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>技巧药水</v>
       </c>
-      <c r="S45" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="R45" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>22034007</v>
       </c>
@@ -3067,11 +2758,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>速度药水</v>
       </c>
-      <c r="S46" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="R46" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>22034008</v>
       </c>
@@ -3079,11 +2770,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>幸运药水</v>
       </c>
-      <c r="S47" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="R47" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>22034009</v>
       </c>
@@ -3091,11 +2782,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>暴击药水</v>
       </c>
-      <c r="S48" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="R48" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>22034011</v>
       </c>
@@ -3107,7 +2798,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>22035001</v>
       </c>
@@ -3115,14 +2806,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>猛兽卡片</v>
       </c>
+      <c r="G50" t="s">
+        <v>39</v>
+      </c>
       <c r="H50" t="s">
-        <v>41</v>
-      </c>
-      <c r="I50" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>22035002</v>
       </c>
@@ -3130,14 +2821,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>战斧卡片</v>
       </c>
+      <c r="G51" t="s">
+        <v>40</v>
+      </c>
       <c r="H51" t="s">
-        <v>42</v>
-      </c>
-      <c r="I51" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>22035003</v>
       </c>
@@ -3145,554 +2836,129 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>火焰卡片</v>
       </c>
+      <c r="G52" t="s">
+        <v>41</v>
+      </c>
       <c r="H52" t="s">
-        <v>43</v>
-      </c>
-      <c r="I52" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A53">
-        <v>22036101</v>
+        <v>22037001</v>
       </c>
       <c r="B53" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-塞尼斯</v>
-      </c>
-      <c r="G53">
-        <v>43020101</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.15">
+        <v>种子-豌豆</v>
+      </c>
+      <c r="I53">
+        <v>22037101</v>
+      </c>
+      <c r="J53">
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A54">
-        <v>22036102</v>
+        <v>22037002</v>
       </c>
       <c r="B54" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-塞巴斯恰恩</v>
-      </c>
-      <c r="G54">
-        <v>43020102</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.15">
+        <v>种子-玉米</v>
+      </c>
+      <c r="I54">
+        <v>22037102</v>
+      </c>
+      <c r="J54">
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A55">
-        <v>22036103</v>
+        <v>22037003</v>
       </c>
       <c r="B55" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-科迪</v>
-      </c>
-      <c r="G55">
-        <v>43020103</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.15">
+        <v>种子-苹果</v>
+      </c>
+      <c r="I55">
+        <v>22037103</v>
+      </c>
+      <c r="J55">
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A56">
-        <v>22036104</v>
+        <v>22037004</v>
       </c>
       <c r="B56" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-威阿伊丁</v>
-      </c>
-      <c r="G56">
-        <v>43020104</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.15">
+        <v>种子-蓝莓</v>
+      </c>
+      <c r="I56">
+        <v>22037104</v>
+      </c>
+      <c r="J56">
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A57">
-        <v>22036105</v>
+        <v>22037101</v>
       </c>
       <c r="B57" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-奥莱伊李</v>
-      </c>
-      <c r="G57">
-        <v>43020105</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.15">
+        <v>作物-豌豆</v>
+      </c>
+      <c r="C57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A58">
-        <v>22036106</v>
+        <v>22037102</v>
       </c>
       <c r="B58" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-米兰达</v>
-      </c>
-      <c r="G58">
-        <v>43020106</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.15">
+        <v>作物-豌豆</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A59">
-        <v>22036107</v>
+        <v>22037103</v>
       </c>
       <c r="B59" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-盖露贝尔</v>
-      </c>
-      <c r="G59">
-        <v>43020107</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.15">
+        <v>作物-苹果</v>
+      </c>
+      <c r="K59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A60">
-        <v>22036108</v>
+        <v>22037104</v>
       </c>
       <c r="B60" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-贝露凯伊鲁</v>
-      </c>
-      <c r="G60">
-        <v>43020108</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A61">
-        <v>22036109</v>
-      </c>
-      <c r="B61" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-雷洛比克</v>
-      </c>
-      <c r="G61">
-        <v>43020109</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A62">
-        <v>22036110</v>
-      </c>
-      <c r="B62" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-巴鲁迪亚斯</v>
-      </c>
-      <c r="G62">
-        <v>43020110</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A63">
-        <v>22036201</v>
-      </c>
-      <c r="B63" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-武藤游戏</v>
-      </c>
-      <c r="G63">
-        <v>43020201</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A64">
-        <v>22036202</v>
-      </c>
-      <c r="B64" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-城之内</v>
-      </c>
-      <c r="G64">
-        <v>43020202</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A65">
-        <v>22036203</v>
-      </c>
-      <c r="B65" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-海马懒人</v>
-      </c>
-      <c r="G65">
-        <v>43020203</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A66">
-        <v>22036301</v>
-      </c>
-      <c r="B66" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-内芙妮</v>
-      </c>
-      <c r="G66">
-        <v>43020301</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A67">
-        <v>22036302</v>
-      </c>
-      <c r="B67" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-塔妮丝</v>
-      </c>
-      <c r="G67">
-        <v>43020302</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A68">
-        <v>22036303</v>
-      </c>
-      <c r="B68" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-卢卡</v>
-      </c>
-      <c r="G68">
-        <v>43020303</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A69">
-        <v>22036304</v>
-      </c>
-      <c r="B69" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-艾斯特尔</v>
-      </c>
-      <c r="G69">
-        <v>43020304</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A70">
-        <v>22036305</v>
-      </c>
-      <c r="B70" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-萨恩</v>
-      </c>
-      <c r="G70">
-        <v>43020305</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A71">
-        <v>22036306</v>
-      </c>
-      <c r="B71" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-玛莎</v>
-      </c>
-      <c r="G71">
-        <v>43020306</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A72">
-        <v>22036307</v>
-      </c>
-      <c r="B72" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-阿特罗姆</v>
-      </c>
-      <c r="G72">
-        <v>43020307</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A73">
-        <v>22036308</v>
-      </c>
-      <c r="B73" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-泽诺</v>
-      </c>
-      <c r="G73">
-        <v>43020308</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A74">
-        <v>22036309</v>
-      </c>
-      <c r="B74" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-拉凯尔</v>
-      </c>
-      <c r="G74">
-        <v>43020309</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A75">
-        <v>22036310</v>
-      </c>
-      <c r="B75" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-纳尔萨斯</v>
-      </c>
-      <c r="G75">
-        <v>43020310</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A76">
-        <v>22036311</v>
-      </c>
-      <c r="B76" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-纳隆</v>
-      </c>
-      <c r="G76">
-        <v>43020311</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A77">
-        <v>22036312</v>
-      </c>
-      <c r="B77" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-维加</v>
-      </c>
-      <c r="G77">
-        <v>43020312</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A78">
-        <v>22036401</v>
-      </c>
-      <c r="B78" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-诺德</v>
-      </c>
-      <c r="G78">
-        <v>43020401</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A79">
-        <v>22036402</v>
-      </c>
-      <c r="B79" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-那那美</v>
-      </c>
-      <c r="G79">
-        <v>43020402</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A80">
-        <v>22036403</v>
-      </c>
-      <c r="B80" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-弗兰克</v>
-      </c>
-      <c r="G80">
-        <v>43020403</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A81">
-        <v>22036404</v>
-      </c>
-      <c r="B81" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-维克托</v>
-      </c>
-      <c r="G81">
-        <v>43020404</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A82">
-        <v>22036405</v>
-      </c>
-      <c r="B82" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-洛克</v>
-      </c>
-      <c r="G82">
-        <v>43020405</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A83">
-        <v>22036406</v>
-      </c>
-      <c r="B83" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-谢拉</v>
-      </c>
-      <c r="G83">
-        <v>43020406</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A84">
-        <v>22036407</v>
-      </c>
-      <c r="B84" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-克莱布</v>
-      </c>
-      <c r="G84">
-        <v>43020407</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A85">
-        <v>22036408</v>
-      </c>
-      <c r="B85" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-蔡</v>
-      </c>
-      <c r="G85">
-        <v>43020408</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A86">
-        <v>22036501</v>
-      </c>
-      <c r="B86" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-约修亚</v>
-      </c>
-      <c r="G86">
-        <v>43020501</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A87">
-        <v>22036502</v>
-      </c>
-      <c r="B87" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>名片-艾斯蒂尔</v>
-      </c>
-      <c r="G87">
-        <v>43020502</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A88">
-        <v>22037001</v>
-      </c>
-      <c r="B88" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>种子-豌豆</v>
-      </c>
-      <c r="J88">
-        <v>22037101</v>
-      </c>
-      <c r="K88">
-        <v>10800</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A89">
-        <v>22037002</v>
-      </c>
-      <c r="B89" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>种子-玉米</v>
-      </c>
-      <c r="J89">
-        <v>22037102</v>
-      </c>
-      <c r="K89">
-        <v>10800</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A90">
-        <v>22037003</v>
-      </c>
-      <c r="B90" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>种子-苹果</v>
-      </c>
-      <c r="J90">
-        <v>22037103</v>
-      </c>
-      <c r="K90">
-        <v>10800</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A91">
-        <v>22037004</v>
-      </c>
-      <c r="B91" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>种子-蓝莓</v>
-      </c>
-      <c r="J91">
-        <v>22037104</v>
-      </c>
-      <c r="K91">
-        <v>10800</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A92">
-        <v>22037101</v>
-      </c>
-      <c r="B92" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>作物-豌豆</v>
-      </c>
-      <c r="C92">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A93">
-        <v>22037102</v>
-      </c>
-      <c r="B93" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>作物-豌豆</v>
-      </c>
-      <c r="E93">
-        <v>1</v>
-      </c>
-      <c r="F93">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A94">
-        <v>22037103</v>
-      </c>
-      <c r="B94" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>作物-苹果</v>
-      </c>
-      <c r="L94">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A95">
-        <v>22037104</v>
-      </c>
-      <c r="B95" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>作物-蓝莓</v>
       </c>
-      <c r="M95">
+      <c r="L60">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="A4:A10 C4:P13 Q4:R95 S95 S4:S46 S48 A14:P52 A88:P95 A53:F87 H53:P87">
-    <cfRule type="containsBlanks" dxfId="3" priority="5">
+  <conditionalFormatting sqref="A4:A10 R4:R46 C4:O13 P4:Q60 A14:O60 R48:R60">
+    <cfRule type="containsBlanks" dxfId="0" priority="5">
       <formula>LEN(TRIM(A4))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S49:S94">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
-      <formula>LEN(TRIM(S49))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
implement the new random item generate item
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/ItemConsumer.xlsx
+++ b/ConfigData/Xlsx/ItemConsumer.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,12 +17,12 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="72">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -277,14 +277,46 @@
   </si>
   <si>
     <t>~Name</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机素材概率</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机素材数量</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RandomItemRate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RandomItemCount</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>35;25;20;15;3;1;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>30;25;20;15;5;3;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>20;20;25;19;8;5;3</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -469,6 +501,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -933,7 +973,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -968,6 +1008,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1015,7 +1058,27 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -1218,7 +1281,7 @@
             <v>22031101</v>
           </cell>
           <cell r="B15" t="str">
-            <v>资源袋(植物)</v>
+            <v>资源袋(绿)</v>
           </cell>
         </row>
         <row r="16">
@@ -1226,7 +1289,7 @@
             <v>22031102</v>
           </cell>
           <cell r="B16" t="str">
-            <v>资源袋(鱼)</v>
+            <v>资源袋(蓝)</v>
           </cell>
         </row>
         <row r="17">
@@ -1234,7 +1297,7 @@
             <v>22031103</v>
           </cell>
           <cell r="B17" t="str">
-            <v>资源袋(矿石)</v>
+            <v>资源袋(灰)</v>
           </cell>
         </row>
         <row r="18">
@@ -1652,14 +1715,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:R60" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A3:R60"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:T63" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A3:T63"/>
   <sortState ref="A4:N58">
     <sortCondition ref="A3:A58"/>
   </sortState>
-  <tableColumns count="18">
+  <tableColumns count="20">
     <tableColumn id="1" name="Id"/>
-    <tableColumn id="2" name="~Name" dataDxfId="1">
+    <tableColumn id="2" name="~Name" dataDxfId="3">
       <calculatedColumnFormula>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="GainExp"/>
@@ -1668,6 +1731,8 @@
     <tableColumn id="6" name="ResourceCount"/>
     <tableColumn id="8" name="RandomCardRate"/>
     <tableColumn id="16" name="RandomCardCatalog"/>
+    <tableColumn id="7" name="RandomItemRate"/>
+    <tableColumn id="20" name="RandomItemCount"/>
     <tableColumn id="9" name="FarmItemId"/>
     <tableColumn id="10" name="FarmTime"/>
     <tableColumn id="11" name="GainLp"/>
@@ -1684,7 +1749,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1759,23 +1824,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1811,23 +1859,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2004,27 +2035,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R60"/>
+  <dimension ref="A1:T63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.375" customWidth="1"/>
-    <col min="3" max="3" width="8.875" customWidth="1"/>
-    <col min="4" max="4" width="7.625" customWidth="1"/>
+    <col min="3" max="4" width="7.125" customWidth="1"/>
     <col min="5" max="6" width="4.25" customWidth="1"/>
     <col min="7" max="7" width="12.625" customWidth="1"/>
     <col min="8" max="8" width="6.875" customWidth="1"/>
-    <col min="9" max="9" width="12.75" customWidth="1"/>
-    <col min="10" max="10" width="10.75" customWidth="1"/>
-    <col min="11" max="18" width="7.375" customWidth="1"/>
+    <col min="9" max="9" width="13.375" customWidth="1"/>
+    <col min="10" max="10" width="6.875" customWidth="1"/>
+    <col min="11" max="11" width="8.625" customWidth="1"/>
+    <col min="12" max="12" width="6.625" customWidth="1"/>
+    <col min="13" max="20" width="7.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:20">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -2050,37 +2082,43 @@
         <v>29</v>
       </c>
       <c r="I1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="Q1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="R1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:20">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2106,18 +2144,18 @@
         <v>20</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="N2" s="3" t="s">
@@ -2127,16 +2165,22 @@
         <v>0</v>
       </c>
       <c r="P2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:20">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
@@ -2162,37 +2206,43 @@
         <v>38</v>
       </c>
       <c r="I3" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="N3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="O3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="P3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="Q3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="R3" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="S3" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="T3" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:20">
       <c r="A4">
         <v>22031002</v>
       </c>
@@ -2207,7 +2257,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:20">
       <c r="A5">
         <v>22031003</v>
       </c>
@@ -2222,7 +2272,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:20">
       <c r="A6">
         <v>22031004</v>
       </c>
@@ -2237,7 +2287,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:20">
       <c r="A7">
         <v>22031005</v>
       </c>
@@ -2252,7 +2302,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:20">
       <c r="A8">
         <v>22031006</v>
       </c>
@@ -2267,7 +2317,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:20">
       <c r="A9">
         <v>22031007</v>
       </c>
@@ -2282,7 +2332,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:20">
       <c r="A10">
         <v>22031008</v>
       </c>
@@ -2297,7 +2347,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:20">
       <c r="A11">
         <v>22031011</v>
       </c>
@@ -2312,7 +2362,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:20">
       <c r="A12">
         <v>22031012</v>
       </c>
@@ -2327,7 +2377,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:20">
       <c r="A13">
         <v>22031013</v>
       </c>
@@ -2342,622 +2392,667 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:20">
       <c r="A14">
+        <v>22031101</v>
+      </c>
+      <c r="B14" s="12" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>资源袋(绿)</v>
+      </c>
+      <c r="I14" t="s">
+        <v>69</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15">
+        <v>22031102</v>
+      </c>
+      <c r="B15" s="12" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>资源袋(蓝)</v>
+      </c>
+      <c r="I15" t="s">
+        <v>70</v>
+      </c>
+      <c r="J15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16">
+        <v>22031103</v>
+      </c>
+      <c r="B16" s="12" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>资源袋(灰)</v>
+      </c>
+      <c r="I16" t="s">
+        <v>71</v>
+      </c>
+      <c r="J16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17">
         <v>22032001</v>
       </c>
-      <c r="B14" s="11" t="str">
+      <c r="B17" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>木材补给车</v>
       </c>
-      <c r="E14">
+      <c r="E17">
         <v>2</v>
       </c>
-      <c r="F14">
+      <c r="F17">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A15">
+    <row r="18" spans="1:15">
+      <c r="A18">
         <v>22032002</v>
       </c>
-      <c r="B15" s="11" t="str">
+      <c r="B18" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>矿石补给车</v>
       </c>
-      <c r="E15">
+      <c r="E18">
         <v>3</v>
       </c>
-      <c r="F15">
+      <c r="F18">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A16">
+    <row r="19" spans="1:15">
+      <c r="A19">
         <v>22032003</v>
       </c>
-      <c r="B16" s="11" t="str">
+      <c r="B19" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>水银补给车</v>
       </c>
-      <c r="E16">
+      <c r="E19">
         <v>4</v>
-      </c>
-      <c r="F16">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A17">
-        <v>22032004</v>
-      </c>
-      <c r="B17" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>红宝石补给车</v>
-      </c>
-      <c r="E17">
-        <v>5</v>
-      </c>
-      <c r="F17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A18">
-        <v>22032005</v>
-      </c>
-      <c r="B18" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>硫磺补给车</v>
-      </c>
-      <c r="E18">
-        <v>6</v>
-      </c>
-      <c r="F18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A19">
-        <v>22032006</v>
-      </c>
-      <c r="B19" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>水晶补给车</v>
-      </c>
-      <c r="E19">
-        <v>7</v>
       </c>
       <c r="F19">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15">
       <c r="A20">
+        <v>22032004</v>
+      </c>
+      <c r="B20" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>红宝石补给车</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21">
+        <v>22032005</v>
+      </c>
+      <c r="B21" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>硫磺补给车</v>
+      </c>
+      <c r="E21">
+        <v>6</v>
+      </c>
+      <c r="F21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22">
+        <v>22032006</v>
+      </c>
+      <c r="B22" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>水晶补给车</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23">
         <v>22032007</v>
       </c>
-      <c r="B20" s="11" t="str">
+      <c r="B23" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>初始资源包</v>
       </c>
-      <c r="E20">
+      <c r="E23">
         <v>1</v>
       </c>
-      <c r="F20">
+      <c r="F23">
         <v>300</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A21">
+    <row r="24" spans="1:15">
+      <c r="A24">
         <v>22032008</v>
       </c>
-      <c r="B21" s="11" t="str">
+      <c r="B24" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>金币</v>
       </c>
-      <c r="E21">
+      <c r="E24">
         <v>1</v>
       </c>
-      <c r="F21">
+      <c r="F24">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A22">
+    <row r="25" spans="1:15">
+      <c r="A25">
         <v>22033001</v>
       </c>
-      <c r="B22" s="11" t="str">
+      <c r="B25" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>小型魔法药剂</v>
       </c>
-      <c r="L22">
+      <c r="N25">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A23">
+    <row r="26" spans="1:15">
+      <c r="A26">
         <v>22033002</v>
       </c>
-      <c r="B23" s="11" t="str">
+      <c r="B26" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>中型魔法药剂</v>
       </c>
-      <c r="L23">
+      <c r="N26">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A24">
+    <row r="27" spans="1:15">
+      <c r="A27">
         <v>22033003</v>
       </c>
-      <c r="B24" s="11" t="str">
+      <c r="B27" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>大型魔法药剂</v>
       </c>
-      <c r="L24">
+      <c r="N27">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A25">
+    <row r="28" spans="1:15">
+      <c r="A28">
         <v>22033004</v>
       </c>
-      <c r="B25" s="11" t="str">
+      <c r="B28" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>小型活力药剂</v>
-      </c>
-      <c r="K25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A26">
-        <v>22033005</v>
-      </c>
-      <c r="B26" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>中型活力药剂</v>
-      </c>
-      <c r="K26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A27">
-        <v>22033006</v>
-      </c>
-      <c r="B27" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>大型活力药剂</v>
-      </c>
-      <c r="K27">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A28">
-        <v>22033007</v>
-      </c>
-      <c r="B28" s="11" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>小型体力药剂</v>
       </c>
       <c r="M28">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:15">
       <c r="A29">
-        <v>22033008</v>
+        <v>22033005</v>
       </c>
       <c r="B29" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>中型体力药剂</v>
+        <v>中型活力药剂</v>
       </c>
       <c r="M29">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:15">
       <c r="A30">
-        <v>22033009</v>
+        <v>22033006</v>
       </c>
       <c r="B30" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>大型体力药剂</v>
+        <v>大型活力药剂</v>
       </c>
       <c r="M30">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:15">
       <c r="A31">
+        <v>22033007</v>
+      </c>
+      <c r="B31" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>小型体力药剂</v>
+      </c>
+      <c r="O31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32">
+        <v>22033008</v>
+      </c>
+      <c r="B32" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>中型体力药剂</v>
+      </c>
+      <c r="O32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20">
+      <c r="A33">
+        <v>22033009</v>
+      </c>
+      <c r="B33" s="11" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>大型体力药剂</v>
+      </c>
+      <c r="O33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20">
+      <c r="A34">
         <v>22033013</v>
       </c>
-      <c r="B31" s="11" t="str">
+      <c r="B34" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>随机幻兽卡</v>
       </c>
-      <c r="O31">
+      <c r="Q34">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A32">
+    <row r="35" spans="1:20">
+      <c r="A35">
         <v>22033014</v>
       </c>
-      <c r="B32" s="11" t="str">
+      <c r="B35" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>随机武器卡</v>
       </c>
-      <c r="O32">
+      <c r="Q35">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A33">
+    <row r="36" spans="1:20">
+      <c r="A36">
         <v>22033015</v>
       </c>
-      <c r="B33" s="11" t="str">
+      <c r="B36" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>随机魔法卡</v>
       </c>
-      <c r="O33">
+      <c r="Q36">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A34">
+    <row r="37" spans="1:20">
+      <c r="A37">
         <v>22033016</v>
       </c>
-      <c r="B34" s="11" t="str">
+      <c r="B37" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>符文-查姆</v>
       </c>
-      <c r="N34">
+      <c r="P37">
         <v>9999</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A35">
+    <row r="38" spans="1:20">
+      <c r="A38">
         <v>22033017</v>
       </c>
-      <c r="B35" s="11" t="str">
+      <c r="B38" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>符文-普尔</v>
       </c>
-      <c r="N35">
+      <c r="P38">
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A36">
+    <row r="39" spans="1:20">
+      <c r="A39">
         <v>22033018</v>
       </c>
-      <c r="B36" s="11" t="str">
+      <c r="B39" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>符文-艾尔</v>
       </c>
-      <c r="P36" t="s">
+      <c r="R39" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A37">
+    <row r="40" spans="1:20">
+      <c r="A40">
         <v>22033030</v>
       </c>
-      <c r="B37" s="11" t="str">
+      <c r="B40" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>木质修理锤</v>
       </c>
-      <c r="Q37">
+      <c r="S40">
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A38">
+    <row r="41" spans="1:20">
+      <c r="A41">
         <v>22033031</v>
       </c>
-      <c r="B38" s="11" t="str">
+      <c r="B41" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>钢铁修理锤</v>
       </c>
-      <c r="Q38">
+      <c r="S41">
         <v>500</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A39">
+    <row r="42" spans="1:20">
+      <c r="A42">
         <v>22033032</v>
       </c>
-      <c r="B39" s="11" t="str">
+      <c r="B42" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>神圣修理锤</v>
       </c>
-      <c r="Q39">
+      <c r="S42">
         <v>1000</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A40">
+    <row r="43" spans="1:20">
+      <c r="A43">
         <v>22034001</v>
       </c>
-      <c r="B40" s="11" t="str">
+      <c r="B43" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>经验之书</v>
       </c>
-      <c r="C40">
+      <c r="C43">
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A41">
+    <row r="44" spans="1:20">
+      <c r="A44">
         <v>22034002</v>
       </c>
-      <c r="B41" s="11" t="str">
+      <c r="B44" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>能量之书</v>
       </c>
-      <c r="C41">
+      <c r="C44">
         <v>300</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A42">
+    <row r="45" spans="1:20">
+      <c r="A45">
         <v>22034003</v>
       </c>
-      <c r="B42" s="11" t="str">
+      <c r="B45" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>攻速药水</v>
       </c>
-      <c r="R42" t="s">
+      <c r="T45" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A43">
+    <row r="46" spans="1:20">
+      <c r="A46">
         <v>22034004</v>
       </c>
-      <c r="B43" s="11" t="str">
+      <c r="B46" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>守护药水</v>
       </c>
-      <c r="R43" t="s">
+      <c r="T46" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A44">
+    <row r="47" spans="1:20">
+      <c r="A47">
         <v>22034005</v>
       </c>
-      <c r="B44" s="11" t="str">
+      <c r="B47" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>法术药水</v>
       </c>
-      <c r="R44" t="s">
+      <c r="T47" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A45">
+    <row r="48" spans="1:20">
+      <c r="A48">
         <v>22034006</v>
       </c>
-      <c r="B45" s="11" t="str">
+      <c r="B48" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>技巧药水</v>
       </c>
-      <c r="R45" t="s">
+      <c r="T48" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A46">
+    <row r="49" spans="1:20">
+      <c r="A49">
         <v>22034007</v>
       </c>
-      <c r="B46" s="11" t="str">
+      <c r="B49" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>速度药水</v>
       </c>
-      <c r="R46" t="s">
+      <c r="T49" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A47">
+    <row r="50" spans="1:20">
+      <c r="A50">
         <v>22034008</v>
       </c>
-      <c r="B47" s="11" t="str">
+      <c r="B50" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>幸运药水</v>
       </c>
-      <c r="R47" t="s">
+      <c r="T50" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A48">
+    <row r="51" spans="1:20">
+      <c r="A51">
         <v>22034009</v>
       </c>
-      <c r="B48" s="11" t="str">
+      <c r="B51" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>暴击药水</v>
       </c>
-      <c r="R48" t="s">
+      <c r="T51" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A49">
+    <row r="52" spans="1:20">
+      <c r="A52">
         <v>22034011</v>
       </c>
-      <c r="B49" s="11" t="str">
+      <c r="B52" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>体力药水</v>
       </c>
-      <c r="D49">
+      <c r="D52">
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A50">
+    <row r="53" spans="1:20">
+      <c r="A53">
         <v>22035001</v>
       </c>
-      <c r="B50" s="11" t="str">
+      <c r="B53" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>猛兽卡片</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G53" t="s">
         <v>39</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H53" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A51">
+    <row r="54" spans="1:20">
+      <c r="A54">
         <v>22035002</v>
       </c>
-      <c r="B51" s="11" t="str">
+      <c r="B54" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>战斧卡片</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G54" t="s">
         <v>40</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H54" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A52">
+    <row r="55" spans="1:20">
+      <c r="A55">
         <v>22035003</v>
       </c>
-      <c r="B52" s="11" t="str">
+      <c r="B55" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>火焰卡片</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G55" t="s">
         <v>41</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H55" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A53">
+    <row r="56" spans="1:20">
+      <c r="A56">
         <v>22037001</v>
       </c>
-      <c r="B53" s="11" t="str">
+      <c r="B56" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>种子-豌豆</v>
       </c>
-      <c r="I53">
+      <c r="K56">
         <v>22037101</v>
       </c>
-      <c r="J53">
+      <c r="L56">
         <v>10800</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A54">
+    <row r="57" spans="1:20">
+      <c r="A57">
         <v>22037002</v>
       </c>
-      <c r="B54" s="11" t="str">
+      <c r="B57" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>种子-玉米</v>
       </c>
-      <c r="I54">
+      <c r="K57">
         <v>22037102</v>
       </c>
-      <c r="J54">
+      <c r="L57">
         <v>10800</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A55">
+    <row r="58" spans="1:20">
+      <c r="A58">
         <v>22037003</v>
       </c>
-      <c r="B55" s="11" t="str">
+      <c r="B58" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>种子-苹果</v>
       </c>
-      <c r="I55">
+      <c r="K58">
         <v>22037103</v>
       </c>
-      <c r="J55">
+      <c r="L58">
         <v>10800</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A56">
+    <row r="59" spans="1:20">
+      <c r="A59">
         <v>22037004</v>
       </c>
-      <c r="B56" s="11" t="str">
+      <c r="B59" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>种子-蓝莓</v>
       </c>
-      <c r="I56">
+      <c r="K59">
         <v>22037104</v>
       </c>
-      <c r="J56">
+      <c r="L59">
         <v>10800</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A57">
+    <row r="60" spans="1:20">
+      <c r="A60">
         <v>22037101</v>
       </c>
-      <c r="B57" s="11" t="str">
+      <c r="B60" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>作物-豌豆</v>
       </c>
-      <c r="C57">
+      <c r="C60">
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A58">
+    <row r="61" spans="1:20">
+      <c r="A61">
         <v>22037102</v>
       </c>
-      <c r="B58" s="11" t="str">
+      <c r="B61" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>作物-豌豆</v>
       </c>
-      <c r="E58">
+      <c r="E61">
         <v>1</v>
       </c>
-      <c r="F58">
+      <c r="F61">
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A59">
+    <row r="62" spans="1:20">
+      <c r="A62">
         <v>22037103</v>
       </c>
-      <c r="B59" s="11" t="str">
+      <c r="B62" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>作物-苹果</v>
       </c>
-      <c r="K59">
+      <c r="M62">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A60">
+    <row r="63" spans="1:20">
+      <c r="A63">
         <v>22037104</v>
       </c>
-      <c r="B60" s="11" t="str">
+      <c r="B63" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>作物-蓝莓</v>
       </c>
-      <c r="L60">
+      <c r="N63">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="A4:A10 R4:R46 C4:O13 P4:Q60 A14:O60 R48:R60">
-    <cfRule type="containsBlanks" dxfId="0" priority="5">
+  <conditionalFormatting sqref="A4:A10 T51:T63 T17:T49 A17:S63 C4:T16">
+    <cfRule type="containsBlanks" dxfId="2" priority="5">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
support race based cardbag
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/ItemConsumer.xlsx
+++ b/ConfigData/Xlsx/ItemConsumer.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="111">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -168,176 +168,273 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>0;840;150;10;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0;720;250;30;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0;600;350;50;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RandomCardRate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;2;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;2;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;2;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>圣言</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>HolyWord</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>witcheye</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int[]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>属性改变</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttrAddAfterSummon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>2;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>3;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>4;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>5;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>6;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>7;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>恢复塔生命</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddTowerHp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>~Name</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DropId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过掉落获取</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得食物</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GainFood</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得健康</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得精神</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GainMental</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GainHealth</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>特殊指令</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Instruction</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>detectall</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MoveAdd</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MoveRound</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>移动加长</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>移动时间</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>RandomCardCatalog</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>0;840;150;10;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0;720;250;30;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0;600;350;50;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RandomCardRate</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;2;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;2;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;2;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>圣言</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>HolyWord</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>witcheye</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int[]</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>属性改变</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>AttrAddAfterSummon</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>2;5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>3;5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>4;5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>5;5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>6;5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>7;5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>恢复塔生命</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>AddTowerHp</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>~Name</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>DropId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>通过掉落获取</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>获得食物</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>GainFood</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>获得健康</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>获得精神</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>GainMental</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>GainHealth</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>特殊指令</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Instruction</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>detectall</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>MoveAdd</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>MoveRound</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>移动加长</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>移动时间</t>
-    <phoneticPr fontId="18" type="noConversion"/>
+    <t>0;840;150;10;11</t>
+  </si>
+  <si>
+    <t>0;840;150;10;12</t>
+  </si>
+  <si>
+    <t>0;840;150;10;13</t>
+  </si>
+  <si>
+    <t>0;840;150;10;14</t>
+  </si>
+  <si>
+    <t>0;840;150;10;15</t>
+  </si>
+  <si>
+    <t>0;840;150;10;16</t>
+  </si>
+  <si>
+    <t>0;840;150;10;17</t>
+  </si>
+  <si>
+    <t>0;840;150;10;18</t>
+  </si>
+  <si>
+    <t>0;840;150;10;19</t>
+  </si>
+  <si>
+    <t>0;840;150;10;20</t>
+  </si>
+  <si>
+    <t>0;840;150;10;21</t>
+  </si>
+  <si>
+    <t>0;840;150;10;22</t>
+  </si>
+  <si>
+    <t>0;840;150;10;23</t>
+  </si>
+  <si>
+    <t>0;840;150;10;24</t>
+  </si>
+  <si>
+    <t>0;840;150;10;25</t>
+  </si>
+  <si>
+    <t>0;840;150;10;26</t>
+  </si>
+  <si>
+    <t>1;3;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;3;2</t>
+  </si>
+  <si>
+    <t>1;3;3</t>
+  </si>
+  <si>
+    <t>1;3;4</t>
+  </si>
+  <si>
+    <t>1;3;5</t>
+  </si>
+  <si>
+    <t>1;3;6</t>
+  </si>
+  <si>
+    <t>1;3;7</t>
+  </si>
+  <si>
+    <t>1;3;8</t>
+  </si>
+  <si>
+    <t>1;3;9</t>
+  </si>
+  <si>
+    <t>1;3;10</t>
+  </si>
+  <si>
+    <t>1;3;11</t>
+  </si>
+  <si>
+    <t>1;3;12</t>
+  </si>
+  <si>
+    <t>1;3;13</t>
+  </si>
+  <si>
+    <t>1;3;14</t>
+  </si>
+  <si>
+    <t>1;3;15</t>
+  </si>
+  <si>
+    <t>1;3;16</t>
   </si>
 </sst>
 </file>
@@ -1092,7 +1189,37 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -1163,46 +1290,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1225,8 +1312,8 @@
       <sheetName val="其他"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2">
         <row r="1">
           <cell r="A1" t="str">
@@ -1321,7 +1408,7 @@
             <v>22031212</v>
           </cell>
           <cell r="B12" t="str">
-            <v>卡牌补给包（无）</v>
+            <v>卡牌补给包(无)</v>
           </cell>
         </row>
         <row r="13">
@@ -1329,7 +1416,7 @@
             <v>22031213</v>
           </cell>
           <cell r="B13" t="str">
-            <v>卡牌补给包（水）</v>
+            <v>卡牌补给包(水)</v>
           </cell>
         </row>
         <row r="14">
@@ -1337,7 +1424,7 @@
             <v>22031214</v>
           </cell>
           <cell r="B14" t="str">
-            <v>卡牌补给包（风）</v>
+            <v>卡牌补给包(风)</v>
           </cell>
         </row>
         <row r="15">
@@ -1345,7 +1432,7 @@
             <v>22031215</v>
           </cell>
           <cell r="B15" t="str">
-            <v>卡牌补给包（地）</v>
+            <v>卡牌补给包(地)</v>
           </cell>
         </row>
         <row r="16">
@@ -1353,7 +1440,7 @@
             <v>22031216</v>
           </cell>
           <cell r="B16" t="str">
-            <v>卡牌补给包（火）</v>
+            <v>卡牌补给包(火)</v>
           </cell>
         </row>
         <row r="17">
@@ -1361,7 +1448,7 @@
             <v>22031217</v>
           </cell>
           <cell r="B17" t="str">
-            <v>卡牌补给包（光）</v>
+            <v>卡牌补给包(光)</v>
           </cell>
         </row>
         <row r="18">
@@ -1369,7 +1456,7 @@
             <v>22031218</v>
           </cell>
           <cell r="B18" t="str">
-            <v>卡牌补给包（暗）</v>
+            <v>卡牌补给包(暗)</v>
           </cell>
         </row>
         <row r="19">
@@ -1377,7 +1464,7 @@
             <v>22031221</v>
           </cell>
           <cell r="B19" t="str">
-            <v>卡牌补给包（生物）</v>
+            <v>卡牌补给包(生物)</v>
           </cell>
         </row>
         <row r="20">
@@ -1385,7 +1472,7 @@
             <v>22031222</v>
           </cell>
           <cell r="B20" t="str">
-            <v>卡牌补给包（武器）</v>
+            <v>卡牌补给包(武器)</v>
           </cell>
         </row>
         <row r="21">
@@ -1393,622 +1480,750 @@
             <v>22031223</v>
           </cell>
           <cell r="B21" t="str">
-            <v>卡牌补给包（法术）</v>
+            <v>卡牌补给包(法术)</v>
           </cell>
         </row>
         <row r="22">
           <cell r="A22">
-            <v>22031301</v>
+            <v>22031231</v>
           </cell>
           <cell r="B22" t="str">
-            <v>资源袋(绿)</v>
+            <v>卡牌补给包(恶魔)</v>
           </cell>
         </row>
         <row r="23">
           <cell r="A23">
-            <v>22031302</v>
+            <v>22031232</v>
           </cell>
           <cell r="B23" t="str">
-            <v>资源袋(蓝)</v>
+            <v>卡牌补给包(机械)</v>
           </cell>
         </row>
         <row r="24">
           <cell r="A24">
-            <v>22031303</v>
+            <v>22031233</v>
           </cell>
           <cell r="B24" t="str">
-            <v>资源袋(红)</v>
+            <v>卡牌补给包(精灵)</v>
           </cell>
         </row>
         <row r="25">
           <cell r="A25">
-            <v>22031304</v>
+            <v>22031234</v>
           </cell>
           <cell r="B25" t="str">
-            <v>资源袋(紫)</v>
+            <v>卡牌补给包(昆虫)</v>
           </cell>
         </row>
         <row r="26">
           <cell r="A26">
-            <v>22031305</v>
+            <v>22031235</v>
           </cell>
           <cell r="B26" t="str">
-            <v>资源袋(灰)</v>
+            <v>卡牌补给包(龙)</v>
           </cell>
         </row>
         <row r="27">
           <cell r="A27">
-            <v>22031401</v>
+            <v>22031236</v>
           </cell>
           <cell r="B27" t="str">
-            <v>素材袋(无)</v>
+            <v>卡牌补给包(鸟)</v>
           </cell>
         </row>
         <row r="28">
           <cell r="A28">
-            <v>22031402</v>
+            <v>22031237</v>
           </cell>
           <cell r="B28" t="str">
-            <v>素材袋(水)</v>
+            <v>卡牌补给包(爬行)</v>
           </cell>
         </row>
         <row r="29">
           <cell r="A29">
-            <v>22031403</v>
+            <v>22031238</v>
           </cell>
           <cell r="B29" t="str">
-            <v>素材袋(风)</v>
+            <v>卡牌补给包(人类)</v>
           </cell>
         </row>
         <row r="30">
           <cell r="A30">
-            <v>22031404</v>
+            <v>22031239</v>
           </cell>
           <cell r="B30" t="str">
-            <v>素材袋(火)</v>
+            <v>卡牌补给包(兽人)</v>
           </cell>
         </row>
         <row r="31">
           <cell r="A31">
-            <v>22031405</v>
+            <v>22031240</v>
           </cell>
           <cell r="B31" t="str">
-            <v>素材袋(地)</v>
+            <v>卡牌补给包(亡灵)</v>
           </cell>
         </row>
         <row r="32">
           <cell r="A32">
-            <v>22031406</v>
+            <v>22031241</v>
           </cell>
           <cell r="B32" t="str">
-            <v>素材袋(光)</v>
+            <v>卡牌补给包(野兽)</v>
           </cell>
         </row>
         <row r="33">
           <cell r="A33">
-            <v>22031407</v>
+            <v>22031242</v>
           </cell>
           <cell r="B33" t="str">
-            <v>素材袋(暗)</v>
+            <v>卡牌补给包(鱼)</v>
           </cell>
         </row>
         <row r="34">
           <cell r="A34">
-            <v>22031501</v>
+            <v>22031243</v>
           </cell>
           <cell r="B34" t="str">
-            <v>资源袋(恶魔)</v>
+            <v>卡牌补给包(元素)</v>
           </cell>
         </row>
         <row r="35">
           <cell r="A35">
-            <v>22031502</v>
+            <v>22031244</v>
           </cell>
           <cell r="B35" t="str">
-            <v>资源袋(机械)</v>
+            <v>卡牌补给包(植物)</v>
           </cell>
         </row>
         <row r="36">
           <cell r="A36">
-            <v>22031503</v>
+            <v>22031245</v>
           </cell>
           <cell r="B36" t="str">
-            <v>资源袋(精灵)</v>
+            <v>卡牌补给包(地精)</v>
           </cell>
         </row>
         <row r="37">
           <cell r="A37">
-            <v>22031504</v>
+            <v>22031246</v>
           </cell>
           <cell r="B37" t="str">
-            <v>资源袋(昆虫)</v>
+            <v>卡牌补给包(石像)</v>
           </cell>
         </row>
         <row r="38">
           <cell r="A38">
-            <v>22031505</v>
+            <v>22031301</v>
           </cell>
           <cell r="B38" t="str">
-            <v>资源袋(龙)</v>
+            <v>资源袋(绿)</v>
           </cell>
         </row>
         <row r="39">
           <cell r="A39">
-            <v>22031506</v>
+            <v>22031302</v>
           </cell>
           <cell r="B39" t="str">
-            <v>资源袋(鸟)</v>
+            <v>资源袋(蓝)</v>
           </cell>
         </row>
         <row r="40">
           <cell r="A40">
-            <v>22031507</v>
+            <v>22031303</v>
           </cell>
           <cell r="B40" t="str">
-            <v>资源袋(爬行)</v>
+            <v>资源袋(红)</v>
           </cell>
         </row>
         <row r="41">
           <cell r="A41">
-            <v>22031508</v>
+            <v>22031304</v>
           </cell>
           <cell r="B41" t="str">
-            <v>资源袋(人类)</v>
+            <v>资源袋(紫)</v>
           </cell>
         </row>
         <row r="42">
           <cell r="A42">
-            <v>22031509</v>
+            <v>22031305</v>
           </cell>
           <cell r="B42" t="str">
-            <v>资源袋(兽人)</v>
+            <v>资源袋(灰)</v>
           </cell>
         </row>
         <row r="43">
           <cell r="A43">
-            <v>22031510</v>
+            <v>22031401</v>
           </cell>
           <cell r="B43" t="str">
-            <v>资源袋(亡灵)</v>
+            <v>素材袋(无)</v>
           </cell>
         </row>
         <row r="44">
           <cell r="A44">
-            <v>22031511</v>
+            <v>22031402</v>
           </cell>
           <cell r="B44" t="str">
-            <v>资源袋(野兽)</v>
+            <v>素材袋(水)</v>
           </cell>
         </row>
         <row r="45">
           <cell r="A45">
-            <v>22031512</v>
+            <v>22031403</v>
           </cell>
           <cell r="B45" t="str">
-            <v>资源袋(鱼)</v>
+            <v>素材袋(风)</v>
           </cell>
         </row>
         <row r="46">
           <cell r="A46">
-            <v>22031513</v>
+            <v>22031404</v>
           </cell>
           <cell r="B46" t="str">
-            <v>资源袋(元素)</v>
+            <v>素材袋(火)</v>
           </cell>
         </row>
         <row r="47">
           <cell r="A47">
-            <v>22031514</v>
+            <v>22031405</v>
           </cell>
           <cell r="B47" t="str">
-            <v>资源袋(植物)</v>
+            <v>素材袋(地)</v>
           </cell>
         </row>
         <row r="48">
           <cell r="A48">
-            <v>22031515</v>
+            <v>22031406</v>
           </cell>
           <cell r="B48" t="str">
-            <v>资源袋(地精)</v>
+            <v>素材袋(光)</v>
           </cell>
         </row>
         <row r="49">
           <cell r="A49">
-            <v>22031516</v>
+            <v>22031407</v>
           </cell>
           <cell r="B49" t="str">
-            <v>资源袋(石像)</v>
+            <v>素材袋(暗)</v>
           </cell>
         </row>
         <row r="50">
           <cell r="A50">
-            <v>22032001</v>
+            <v>22031501</v>
           </cell>
           <cell r="B50" t="str">
-            <v>木材补给车</v>
+            <v>资源袋(恶魔)</v>
           </cell>
         </row>
         <row r="51">
           <cell r="A51">
-            <v>22032002</v>
+            <v>22031502</v>
           </cell>
           <cell r="B51" t="str">
-            <v>矿石补给车</v>
+            <v>资源袋(机械)</v>
           </cell>
         </row>
         <row r="52">
           <cell r="A52">
-            <v>22032003</v>
+            <v>22031503</v>
           </cell>
           <cell r="B52" t="str">
-            <v>水银补给车</v>
+            <v>资源袋(精灵)</v>
           </cell>
         </row>
         <row r="53">
           <cell r="A53">
-            <v>22032004</v>
+            <v>22031504</v>
           </cell>
           <cell r="B53" t="str">
-            <v>红宝石补给车</v>
+            <v>资源袋(昆虫)</v>
           </cell>
         </row>
         <row r="54">
           <cell r="A54">
-            <v>22032005</v>
+            <v>22031505</v>
           </cell>
           <cell r="B54" t="str">
-            <v>硫磺补给车</v>
+            <v>资源袋(龙)</v>
           </cell>
         </row>
         <row r="55">
           <cell r="A55">
-            <v>22032006</v>
+            <v>22031506</v>
           </cell>
           <cell r="B55" t="str">
-            <v>水晶补给车</v>
+            <v>资源袋(鸟)</v>
           </cell>
         </row>
         <row r="56">
           <cell r="A56">
-            <v>22032007</v>
+            <v>22031507</v>
           </cell>
           <cell r="B56" t="str">
-            <v>初始资源包</v>
+            <v>资源袋(爬行)</v>
           </cell>
         </row>
         <row r="57">
           <cell r="A57">
-            <v>22032008</v>
+            <v>22031508</v>
           </cell>
           <cell r="B57" t="str">
-            <v>金币</v>
+            <v>资源袋(人类)</v>
           </cell>
         </row>
         <row r="58">
           <cell r="A58">
-            <v>22033001</v>
+            <v>22031509</v>
           </cell>
           <cell r="B58" t="str">
-            <v>小型魔法药剂</v>
+            <v>资源袋(兽人)</v>
           </cell>
         </row>
         <row r="59">
           <cell r="A59">
-            <v>22033002</v>
+            <v>22031510</v>
           </cell>
           <cell r="B59" t="str">
-            <v>中型魔法药剂</v>
+            <v>资源袋(亡灵)</v>
           </cell>
         </row>
         <row r="60">
           <cell r="A60">
-            <v>22033003</v>
+            <v>22031511</v>
           </cell>
           <cell r="B60" t="str">
-            <v>大型魔法药剂</v>
+            <v>资源袋(野兽)</v>
           </cell>
         </row>
         <row r="61">
           <cell r="A61">
-            <v>22033004</v>
+            <v>22031512</v>
           </cell>
           <cell r="B61" t="str">
-            <v>小型活力药剂</v>
+            <v>资源袋(鱼)</v>
           </cell>
         </row>
         <row r="62">
           <cell r="A62">
-            <v>22033005</v>
+            <v>22031513</v>
           </cell>
           <cell r="B62" t="str">
-            <v>中型活力药剂</v>
+            <v>资源袋(元素)</v>
           </cell>
         </row>
         <row r="63">
           <cell r="A63">
-            <v>22033006</v>
+            <v>22031514</v>
           </cell>
           <cell r="B63" t="str">
-            <v>大型活力药剂</v>
+            <v>资源袋(植物)</v>
           </cell>
         </row>
         <row r="64">
           <cell r="A64">
-            <v>22033007</v>
+            <v>22031515</v>
           </cell>
           <cell r="B64" t="str">
-            <v>小型体力药剂</v>
+            <v>资源袋(地精)</v>
           </cell>
         </row>
         <row r="65">
           <cell r="A65">
-            <v>22033008</v>
+            <v>22031516</v>
           </cell>
           <cell r="B65" t="str">
-            <v>中型体力药剂</v>
+            <v>资源袋(石像)</v>
           </cell>
         </row>
         <row r="66">
           <cell r="A66">
-            <v>22033009</v>
+            <v>22032001</v>
           </cell>
           <cell r="B66" t="str">
-            <v>大型体力药剂</v>
+            <v>木材补给车</v>
           </cell>
         </row>
         <row r="67">
           <cell r="A67">
-            <v>22033013</v>
+            <v>22032002</v>
           </cell>
           <cell r="B67" t="str">
-            <v>随机幻兽卡</v>
+            <v>矿石补给车</v>
           </cell>
         </row>
         <row r="68">
           <cell r="A68">
-            <v>22033014</v>
+            <v>22032003</v>
           </cell>
           <cell r="B68" t="str">
-            <v>随机武器卡</v>
+            <v>水银补给车</v>
           </cell>
         </row>
         <row r="69">
           <cell r="A69">
-            <v>22033015</v>
+            <v>22032004</v>
           </cell>
           <cell r="B69" t="str">
-            <v>随机魔法卡</v>
+            <v>红宝石补给车</v>
           </cell>
         </row>
         <row r="70">
           <cell r="A70">
-            <v>22033016</v>
+            <v>22032005</v>
           </cell>
           <cell r="B70" t="str">
-            <v>符文-查姆</v>
+            <v>硫磺补给车</v>
           </cell>
         </row>
         <row r="71">
           <cell r="A71">
-            <v>22033017</v>
+            <v>22032006</v>
           </cell>
           <cell r="B71" t="str">
-            <v>符文-普尔</v>
+            <v>水晶补给车</v>
           </cell>
         </row>
         <row r="72">
           <cell r="A72">
-            <v>22033018</v>
+            <v>22032007</v>
           </cell>
           <cell r="B72" t="str">
-            <v>符文-艾尔</v>
+            <v>初始资源包</v>
           </cell>
         </row>
         <row r="73">
           <cell r="A73">
-            <v>22033030</v>
+            <v>22032008</v>
           </cell>
           <cell r="B73" t="str">
-            <v>木质修理锤</v>
+            <v>金币</v>
           </cell>
         </row>
         <row r="74">
           <cell r="A74">
-            <v>22033031</v>
+            <v>22033001</v>
           </cell>
           <cell r="B74" t="str">
-            <v>钢铁修理锤</v>
+            <v>小型魔法药剂</v>
           </cell>
         </row>
         <row r="75">
           <cell r="A75">
-            <v>22033032</v>
+            <v>22033002</v>
           </cell>
           <cell r="B75" t="str">
-            <v>神圣修理锤</v>
+            <v>中型魔法药剂</v>
           </cell>
         </row>
         <row r="76">
           <cell r="A76">
-            <v>22034001</v>
+            <v>22033003</v>
           </cell>
           <cell r="B76" t="str">
-            <v>经验之书</v>
+            <v>大型魔法药剂</v>
           </cell>
         </row>
         <row r="77">
           <cell r="A77">
-            <v>22034002</v>
+            <v>22033004</v>
           </cell>
           <cell r="B77" t="str">
-            <v>能量之书</v>
+            <v>小型活力药剂</v>
           </cell>
         </row>
         <row r="78">
           <cell r="A78">
-            <v>22034003</v>
+            <v>22033005</v>
           </cell>
           <cell r="B78" t="str">
-            <v>攻速药水</v>
+            <v>中型活力药剂</v>
           </cell>
         </row>
         <row r="79">
           <cell r="A79">
-            <v>22034004</v>
+            <v>22033006</v>
           </cell>
           <cell r="B79" t="str">
-            <v>守护药水</v>
+            <v>大型活力药剂</v>
           </cell>
         </row>
         <row r="80">
           <cell r="A80">
-            <v>22034005</v>
+            <v>22033007</v>
           </cell>
           <cell r="B80" t="str">
-            <v>法术药水</v>
+            <v>小型体力药剂</v>
           </cell>
         </row>
         <row r="81">
           <cell r="A81">
-            <v>22034006</v>
+            <v>22033008</v>
           </cell>
           <cell r="B81" t="str">
-            <v>技巧药水</v>
+            <v>中型体力药剂</v>
           </cell>
         </row>
         <row r="82">
           <cell r="A82">
-            <v>22034007</v>
+            <v>22033009</v>
           </cell>
           <cell r="B82" t="str">
-            <v>速度药水</v>
+            <v>大型体力药剂</v>
           </cell>
         </row>
         <row r="83">
           <cell r="A83">
-            <v>22034008</v>
+            <v>22033013</v>
           </cell>
           <cell r="B83" t="str">
-            <v>幸运药水</v>
+            <v>随机幻兽卡</v>
           </cell>
         </row>
         <row r="84">
           <cell r="A84">
-            <v>22034009</v>
+            <v>22033014</v>
           </cell>
           <cell r="B84" t="str">
-            <v>暴击药水</v>
+            <v>随机武器卡</v>
           </cell>
         </row>
         <row r="85">
           <cell r="A85">
-            <v>22034010</v>
+            <v>22033015</v>
           </cell>
           <cell r="B85" t="str">
-            <v>饼干</v>
+            <v>随机魔法卡</v>
           </cell>
         </row>
         <row r="86">
           <cell r="A86">
-            <v>22034011</v>
+            <v>22033016</v>
           </cell>
           <cell r="B86" t="str">
-            <v>红色胶囊</v>
+            <v>符文-查姆</v>
           </cell>
         </row>
         <row r="87">
           <cell r="A87">
-            <v>22034012</v>
+            <v>22033017</v>
           </cell>
           <cell r="B87" t="str">
-            <v>蓝色胶囊</v>
+            <v>符文-普尔</v>
           </cell>
         </row>
         <row r="88">
           <cell r="A88">
-            <v>22034013</v>
+            <v>22033018</v>
           </cell>
           <cell r="B88" t="str">
-            <v>水晶球</v>
+            <v>符文-艾尔</v>
           </cell>
         </row>
         <row r="89">
           <cell r="A89">
-            <v>22034014</v>
+            <v>22033030</v>
           </cell>
           <cell r="B89" t="str">
-            <v>坐骑黑豹</v>
+            <v>木质修理锤</v>
           </cell>
         </row>
         <row r="90">
           <cell r="A90">
-            <v>22034015</v>
+            <v>22033031</v>
           </cell>
           <cell r="B90" t="str">
-            <v>坐骑鹰</v>
+            <v>钢铁修理锤</v>
           </cell>
         </row>
         <row r="91">
           <cell r="A91">
-            <v>22034016</v>
+            <v>22033032</v>
           </cell>
           <cell r="B91" t="str">
-            <v>坐骑传送器</v>
+            <v>神圣修理锤</v>
           </cell>
         </row>
         <row r="92">
           <cell r="A92">
-            <v>22037001</v>
+            <v>22034001</v>
           </cell>
           <cell r="B92" t="str">
-            <v>种子-豌豆</v>
+            <v>经验之书</v>
           </cell>
         </row>
         <row r="93">
           <cell r="A93">
-            <v>22037002</v>
+            <v>22034002</v>
           </cell>
           <cell r="B93" t="str">
-            <v>种子-玉米</v>
+            <v>能量之书</v>
           </cell>
         </row>
         <row r="94">
           <cell r="A94">
-            <v>22037003</v>
+            <v>22034003</v>
           </cell>
           <cell r="B94" t="str">
-            <v>种子-苹果</v>
+            <v>攻速药水</v>
           </cell>
         </row>
         <row r="95">
           <cell r="A95">
-            <v>22037004</v>
+            <v>22034004</v>
           </cell>
           <cell r="B95" t="str">
-            <v>种子-蓝莓</v>
+            <v>守护药水</v>
           </cell>
         </row>
         <row r="96">
           <cell r="A96">
-            <v>22037101</v>
+            <v>22034005</v>
           </cell>
           <cell r="B96" t="str">
-            <v>作物-豌豆</v>
+            <v>法术药水</v>
           </cell>
         </row>
         <row r="97">
           <cell r="A97">
-            <v>22037102</v>
+            <v>22034006</v>
           </cell>
           <cell r="B97" t="str">
-            <v>作物-玉米</v>
+            <v>技巧药水</v>
           </cell>
         </row>
         <row r="98">
           <cell r="A98">
+            <v>22034007</v>
+          </cell>
+          <cell r="B98" t="str">
+            <v>速度药水</v>
+          </cell>
+        </row>
+        <row r="99">
+          <cell r="A99">
+            <v>22034008</v>
+          </cell>
+          <cell r="B99" t="str">
+            <v>幸运药水</v>
+          </cell>
+        </row>
+        <row r="100">
+          <cell r="A100">
+            <v>22034009</v>
+          </cell>
+          <cell r="B100" t="str">
+            <v>暴击药水</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="A101">
+            <v>22034010</v>
+          </cell>
+          <cell r="B101" t="str">
+            <v>饼干</v>
+          </cell>
+        </row>
+        <row r="102">
+          <cell r="A102">
+            <v>22034011</v>
+          </cell>
+          <cell r="B102" t="str">
+            <v>红色胶囊</v>
+          </cell>
+        </row>
+        <row r="103">
+          <cell r="A103">
+            <v>22034012</v>
+          </cell>
+          <cell r="B103" t="str">
+            <v>蓝色胶囊</v>
+          </cell>
+        </row>
+        <row r="104">
+          <cell r="A104">
+            <v>22034013</v>
+          </cell>
+          <cell r="B104" t="str">
+            <v>水晶球</v>
+          </cell>
+        </row>
+        <row r="105">
+          <cell r="A105">
+            <v>22034014</v>
+          </cell>
+          <cell r="B105" t="str">
+            <v>坐骑黑豹</v>
+          </cell>
+        </row>
+        <row r="106">
+          <cell r="A106">
+            <v>22034015</v>
+          </cell>
+          <cell r="B106" t="str">
+            <v>坐骑鹰</v>
+          </cell>
+        </row>
+        <row r="107">
+          <cell r="A107">
+            <v>22034016</v>
+          </cell>
+          <cell r="B107" t="str">
+            <v>坐骑传送器</v>
+          </cell>
+        </row>
+        <row r="108">
+          <cell r="A108">
+            <v>22037001</v>
+          </cell>
+          <cell r="B108" t="str">
+            <v>种子-豌豆</v>
+          </cell>
+        </row>
+        <row r="109">
+          <cell r="A109">
+            <v>22037002</v>
+          </cell>
+          <cell r="B109" t="str">
+            <v>种子-玉米</v>
+          </cell>
+        </row>
+        <row r="110">
+          <cell r="A110">
+            <v>22037003</v>
+          </cell>
+          <cell r="B110" t="str">
+            <v>种子-苹果</v>
+          </cell>
+        </row>
+        <row r="111">
+          <cell r="A111">
+            <v>22037004</v>
+          </cell>
+          <cell r="B111" t="str">
+            <v>种子-蓝莓</v>
+          </cell>
+        </row>
+        <row r="112">
+          <cell r="A112">
+            <v>22037101</v>
+          </cell>
+          <cell r="B112" t="str">
+            <v>作物-豌豆</v>
+          </cell>
+        </row>
+        <row r="113">
+          <cell r="A113">
+            <v>22037102</v>
+          </cell>
+          <cell r="B113" t="str">
+            <v>作物-玉米</v>
+          </cell>
+        </row>
+        <row r="114">
+          <cell r="A114">
             <v>22037103</v>
           </cell>
-          <cell r="B98" t="str">
+          <cell r="B114" t="str">
             <v>作物-苹果</v>
           </cell>
         </row>
@@ -2019,14 +2234,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:X98" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A3:X98"/>
-  <sortState ref="A4:X98">
-    <sortCondition ref="A3:A98"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:X114" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A3:X114"/>
+  <sortState ref="A4:X114">
+    <sortCondition ref="A3:A114"/>
   </sortState>
   <tableColumns count="24">
     <tableColumn id="1" name="Id"/>
-    <tableColumn id="2" name="~Name" dataDxfId="2">
+    <tableColumn id="2" name="~Name" dataDxfId="5">
       <calculatedColumnFormula>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="GainExp"/>
@@ -2377,10 +2592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X98"/>
+  <dimension ref="A1:X114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2410,13 +2625,13 @@
         <v>12</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>67</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>68</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>13</v>
@@ -2425,10 +2640,10 @@
         <v>14</v>
       </c>
       <c r="I1" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>77</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>78</v>
       </c>
       <c r="K1" s="11" t="s">
         <v>26</v>
@@ -2437,10 +2652,10 @@
         <v>27</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O1" s="11" t="s">
         <v>15</v>
@@ -2464,13 +2679,13 @@
         <v>24</v>
       </c>
       <c r="V1" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="W1" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="X1" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.15">
@@ -2511,10 +2726,10 @@
         <v>18</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>0</v>
@@ -2538,13 +2753,13 @@
         <v>0</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.15">
@@ -2552,19 +2767,19 @@
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>2</v>
@@ -2573,22 +2788,22 @@
         <v>3</v>
       </c>
       <c r="I3" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="K3" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>4</v>
@@ -2612,13 +2827,13 @@
         <v>25</v>
       </c>
       <c r="V3" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="W3" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="X3" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.15">
@@ -2678,7 +2893,7 @@
         <v>蓝色卡包</v>
       </c>
       <c r="K8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L8" t="s">
         <v>35</v>
@@ -2693,7 +2908,7 @@
         <v>黄色卡包</v>
       </c>
       <c r="K9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L9" t="s">
         <v>35</v>
@@ -2708,7 +2923,7 @@
         <v>红色卡包</v>
       </c>
       <c r="K10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L10" t="s">
         <v>35</v>
@@ -2720,10 +2935,10 @@
       </c>
       <c r="B11" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包（无）</v>
+        <v>卡牌补给包(无)</v>
       </c>
       <c r="K11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L11" t="s">
         <v>28</v>
@@ -2735,10 +2950,10 @@
       </c>
       <c r="B12" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包（水）</v>
+        <v>卡牌补给包(水)</v>
       </c>
       <c r="K12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L12" t="s">
         <v>29</v>
@@ -2750,10 +2965,10 @@
       </c>
       <c r="B13" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包（风）</v>
+        <v>卡牌补给包(风)</v>
       </c>
       <c r="K13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L13" t="s">
         <v>30</v>
@@ -2765,10 +2980,10 @@
       </c>
       <c r="B14" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包（地）</v>
+        <v>卡牌补给包(地)</v>
       </c>
       <c r="K14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L14" t="s">
         <v>31</v>
@@ -2780,10 +2995,10 @@
       </c>
       <c r="B15" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包（火）</v>
+        <v>卡牌补给包(火)</v>
       </c>
       <c r="K15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L15" t="s">
         <v>32</v>
@@ -2795,1079 +3010,1314 @@
       </c>
       <c r="B16" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包（光）</v>
+        <v>卡牌补给包(光)</v>
       </c>
       <c r="K16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>22031218</v>
       </c>
       <c r="B17" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包（暗）</v>
+        <v>卡牌补给包(暗)</v>
       </c>
       <c r="K17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>22031221</v>
       </c>
       <c r="B18" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包（生物）</v>
+        <v>卡牌补给包(生物)</v>
       </c>
       <c r="K18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>22031222</v>
       </c>
       <c r="B19" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包（武器）</v>
+        <v>卡牌补给包(武器)</v>
       </c>
       <c r="K19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>22031223</v>
       </c>
       <c r="B20" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包（法术）</v>
+        <v>卡牌补给包(法术)</v>
       </c>
       <c r="K20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A21">
-        <v>22031301</v>
+        <v>22031231</v>
       </c>
       <c r="B21" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(绿)</v>
-      </c>
-      <c r="M21">
-        <v>23000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
+        <v>卡牌补给包(恶魔)</v>
+      </c>
+      <c r="K21" t="s">
+        <v>79</v>
+      </c>
+      <c r="L21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A22">
-        <v>22031302</v>
+        <v>22031232</v>
       </c>
       <c r="B22" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(蓝)</v>
-      </c>
-      <c r="M22">
-        <v>23000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
+        <v>卡牌补给包(机械)</v>
+      </c>
+      <c r="K22" t="s">
+        <v>80</v>
+      </c>
+      <c r="L22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>22031303</v>
+        <v>22031233</v>
       </c>
       <c r="B23" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(红)</v>
-      </c>
-      <c r="M23">
-        <v>23000003</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
+        <v>卡牌补给包(精灵)</v>
+      </c>
+      <c r="K23" t="s">
+        <v>81</v>
+      </c>
+      <c r="L23" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A24">
-        <v>22031304</v>
+        <v>22031234</v>
       </c>
       <c r="B24" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(紫)</v>
-      </c>
-      <c r="M24">
-        <v>23000004</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
+        <v>卡牌补给包(昆虫)</v>
+      </c>
+      <c r="K24" t="s">
+        <v>82</v>
+      </c>
+      <c r="L24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>22031305</v>
+        <v>22031235</v>
       </c>
       <c r="B25" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(灰)</v>
-      </c>
-      <c r="M25">
-        <v>23000005</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
+        <v>卡牌补给包(龙)</v>
+      </c>
+      <c r="K25" t="s">
+        <v>83</v>
+      </c>
+      <c r="L25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>22031401</v>
+        <v>22031236</v>
       </c>
       <c r="B26" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>素材袋(无)</v>
-      </c>
-      <c r="M26">
-        <v>23000301</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
+        <v>卡牌补给包(鸟)</v>
+      </c>
+      <c r="K26" t="s">
+        <v>84</v>
+      </c>
+      <c r="L26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>22031402</v>
+        <v>22031237</v>
       </c>
       <c r="B27" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>素材袋(水)</v>
-      </c>
-      <c r="M27">
-        <v>23000302</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
+        <v>卡牌补给包(爬行)</v>
+      </c>
+      <c r="K27" t="s">
+        <v>85</v>
+      </c>
+      <c r="L27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>22031403</v>
+        <v>22031238</v>
       </c>
       <c r="B28" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>素材袋(风)</v>
-      </c>
-      <c r="M28">
-        <v>23000303</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
+        <v>卡牌补给包(人类)</v>
+      </c>
+      <c r="K28" t="s">
+        <v>86</v>
+      </c>
+      <c r="L28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A29">
-        <v>22031404</v>
+        <v>22031239</v>
       </c>
       <c r="B29" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>素材袋(火)</v>
-      </c>
-      <c r="M29">
-        <v>23000304</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
+        <v>卡牌补给包(兽人)</v>
+      </c>
+      <c r="K29" t="s">
+        <v>87</v>
+      </c>
+      <c r="L29" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A30">
-        <v>22031405</v>
+        <v>22031240</v>
       </c>
       <c r="B30" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>素材袋(地)</v>
-      </c>
-      <c r="M30">
-        <v>23000305</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.15">
+        <v>卡牌补给包(亡灵)</v>
+      </c>
+      <c r="K30" t="s">
+        <v>88</v>
+      </c>
+      <c r="L30" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A31">
-        <v>22031406</v>
+        <v>22031241</v>
       </c>
       <c r="B31" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>素材袋(光)</v>
-      </c>
-      <c r="M31">
-        <v>23000306</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.15">
+        <v>卡牌补给包(野兽)</v>
+      </c>
+      <c r="K31" t="s">
+        <v>89</v>
+      </c>
+      <c r="L31" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A32">
-        <v>22031407</v>
+        <v>22031242</v>
       </c>
       <c r="B32" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>素材袋(暗)</v>
-      </c>
-      <c r="M32">
-        <v>23000307</v>
+        <v>卡牌补给包(鱼)</v>
+      </c>
+      <c r="K32" t="s">
+        <v>90</v>
+      </c>
+      <c r="L32" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A33">
-        <v>22031501</v>
+        <v>22031243</v>
       </c>
       <c r="B33" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(恶魔)</v>
-      </c>
-      <c r="M33">
-        <v>23000401</v>
+        <v>卡牌补给包(元素)</v>
+      </c>
+      <c r="K33" t="s">
+        <v>91</v>
+      </c>
+      <c r="L33" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A34">
-        <v>22031502</v>
+        <v>22031244</v>
       </c>
       <c r="B34" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(机械)</v>
-      </c>
-      <c r="M34">
-        <v>23000402</v>
+        <v>卡牌补给包(植物)</v>
+      </c>
+      <c r="K34" t="s">
+        <v>92</v>
+      </c>
+      <c r="L34" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A35">
-        <v>22031503</v>
+        <v>22031245</v>
       </c>
       <c r="B35" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(精灵)</v>
-      </c>
-      <c r="M35">
-        <v>23000403</v>
+        <v>卡牌补给包(地精)</v>
+      </c>
+      <c r="K35" t="s">
+        <v>93</v>
+      </c>
+      <c r="L35" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A36">
-        <v>22031504</v>
+        <v>22031246</v>
       </c>
       <c r="B36" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(昆虫)</v>
-      </c>
-      <c r="M36">
-        <v>23000404</v>
+        <v>卡牌补给包(石像)</v>
+      </c>
+      <c r="K36" t="s">
+        <v>94</v>
+      </c>
+      <c r="L36" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A37">
-        <v>22031505</v>
+        <v>22031301</v>
       </c>
       <c r="B37" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(龙)</v>
+        <v>资源袋(绿)</v>
       </c>
       <c r="M37">
-        <v>23000405</v>
+        <v>23000001</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A38">
-        <v>22031506</v>
+        <v>22031302</v>
       </c>
       <c r="B38" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(鸟)</v>
+        <v>资源袋(蓝)</v>
       </c>
       <c r="M38">
-        <v>23000406</v>
+        <v>23000002</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A39">
-        <v>22031507</v>
+        <v>22031303</v>
       </c>
       <c r="B39" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(爬行)</v>
+        <v>资源袋(红)</v>
       </c>
       <c r="M39">
-        <v>23000407</v>
+        <v>23000003</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A40">
-        <v>22031508</v>
+        <v>22031304</v>
       </c>
       <c r="B40" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(人类)</v>
+        <v>资源袋(紫)</v>
       </c>
       <c r="M40">
-        <v>23000408</v>
+        <v>23000004</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A41">
-        <v>22031509</v>
+        <v>22031305</v>
       </c>
       <c r="B41" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(兽人)</v>
+        <v>资源袋(灰)</v>
       </c>
       <c r="M41">
-        <v>23000409</v>
+        <v>23000005</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A42">
-        <v>22031510</v>
+        <v>22031401</v>
       </c>
       <c r="B42" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(亡灵)</v>
+        <v>素材袋(无)</v>
       </c>
       <c r="M42">
-        <v>23000410</v>
+        <v>23000301</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A43">
-        <v>22031511</v>
+        <v>22031402</v>
       </c>
       <c r="B43" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(野兽)</v>
+        <v>素材袋(水)</v>
       </c>
       <c r="M43">
-        <v>23000411</v>
+        <v>23000302</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A44">
-        <v>22031512</v>
+        <v>22031403</v>
       </c>
       <c r="B44" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(鱼)</v>
+        <v>素材袋(风)</v>
       </c>
       <c r="M44">
-        <v>23000412</v>
+        <v>23000303</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A45">
-        <v>22031513</v>
+        <v>22031404</v>
       </c>
       <c r="B45" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(元素)</v>
+        <v>素材袋(火)</v>
       </c>
       <c r="M45">
-        <v>23000413</v>
+        <v>23000304</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A46">
-        <v>22031514</v>
+        <v>22031405</v>
       </c>
       <c r="B46" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(植物)</v>
+        <v>素材袋(地)</v>
       </c>
       <c r="M46">
-        <v>23000414</v>
+        <v>23000305</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A47">
-        <v>22031515</v>
+        <v>22031406</v>
       </c>
       <c r="B47" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(地精)</v>
+        <v>素材袋(光)</v>
       </c>
       <c r="M47">
-        <v>23000415</v>
+        <v>23000306</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A48">
+        <v>22031407</v>
+      </c>
+      <c r="B48" s="10" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>素材袋(暗)</v>
+      </c>
+      <c r="M48">
+        <v>23000307</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A49">
+        <v>22031501</v>
+      </c>
+      <c r="B49" s="10" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>资源袋(恶魔)</v>
+      </c>
+      <c r="M49">
+        <v>23000401</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A50">
+        <v>22031502</v>
+      </c>
+      <c r="B50" s="10" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>资源袋(机械)</v>
+      </c>
+      <c r="M50">
+        <v>23000402</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A51">
+        <v>22031503</v>
+      </c>
+      <c r="B51" s="10" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>资源袋(精灵)</v>
+      </c>
+      <c r="M51">
+        <v>23000403</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A52">
+        <v>22031504</v>
+      </c>
+      <c r="B52" s="10" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>资源袋(昆虫)</v>
+      </c>
+      <c r="M52">
+        <v>23000404</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A53">
+        <v>22031505</v>
+      </c>
+      <c r="B53" s="10" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>资源袋(龙)</v>
+      </c>
+      <c r="M53">
+        <v>23000405</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A54">
+        <v>22031506</v>
+      </c>
+      <c r="B54" s="10" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>资源袋(鸟)</v>
+      </c>
+      <c r="M54">
+        <v>23000406</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A55">
+        <v>22031507</v>
+      </c>
+      <c r="B55" s="10" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>资源袋(爬行)</v>
+      </c>
+      <c r="M55">
+        <v>23000407</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A56">
+        <v>22031508</v>
+      </c>
+      <c r="B56" s="10" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>资源袋(人类)</v>
+      </c>
+      <c r="M56">
+        <v>23000408</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A57">
+        <v>22031509</v>
+      </c>
+      <c r="B57" s="10" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>资源袋(兽人)</v>
+      </c>
+      <c r="M57">
+        <v>23000409</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A58">
+        <v>22031510</v>
+      </c>
+      <c r="B58" s="10" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>资源袋(亡灵)</v>
+      </c>
+      <c r="M58">
+        <v>23000410</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A59">
+        <v>22031511</v>
+      </c>
+      <c r="B59" s="10" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>资源袋(野兽)</v>
+      </c>
+      <c r="M59">
+        <v>23000411</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A60">
+        <v>22031512</v>
+      </c>
+      <c r="B60" s="10" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>资源袋(鱼)</v>
+      </c>
+      <c r="M60">
+        <v>23000412</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A61">
+        <v>22031513</v>
+      </c>
+      <c r="B61" s="10" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>资源袋(元素)</v>
+      </c>
+      <c r="M61">
+        <v>23000413</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A62">
+        <v>22031514</v>
+      </c>
+      <c r="B62" s="10" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>资源袋(植物)</v>
+      </c>
+      <c r="M62">
+        <v>23000414</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A63">
+        <v>22031515</v>
+      </c>
+      <c r="B63" s="10" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>资源袋(地精)</v>
+      </c>
+      <c r="M63">
+        <v>23000415</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A64">
         <v>22031516</v>
       </c>
-      <c r="B48" s="10" t="str">
+      <c r="B64" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(石像)</v>
       </c>
-      <c r="M48">
+      <c r="M64">
         <v>23000416</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A49">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A65">
         <v>22032001</v>
       </c>
-      <c r="B49" s="9" t="str">
+      <c r="B65" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>木材补给车</v>
       </c>
-      <c r="G49">
+      <c r="G65">
         <v>2</v>
       </c>
-      <c r="H49">
+      <c r="H65">
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A50">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A66">
         <v>22032002</v>
       </c>
-      <c r="B50" s="9" t="str">
+      <c r="B66" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>矿石补给车</v>
       </c>
-      <c r="G50">
+      <c r="G66">
         <v>3</v>
       </c>
-      <c r="H50">
+      <c r="H66">
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A51">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A67">
         <v>22032003</v>
       </c>
-      <c r="B51" s="9" t="str">
+      <c r="B67" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>水银补给车</v>
       </c>
-      <c r="G51">
+      <c r="G67">
         <v>4</v>
       </c>
-      <c r="H51">
+      <c r="H67">
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A52">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A68">
         <v>22032004</v>
       </c>
-      <c r="B52" s="9" t="str">
+      <c r="B68" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>红宝石补给车</v>
       </c>
-      <c r="G52">
+      <c r="G68">
         <v>5</v>
       </c>
-      <c r="H52">
+      <c r="H68">
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A53">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A69">
         <v>22032005</v>
       </c>
-      <c r="B53" s="9" t="str">
+      <c r="B69" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>硫磺补给车</v>
       </c>
-      <c r="G53">
+      <c r="G69">
         <v>6</v>
       </c>
-      <c r="H53">
+      <c r="H69">
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A54">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A70">
         <v>22032006</v>
       </c>
-      <c r="B54" s="9" t="str">
+      <c r="B70" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>水晶补给车</v>
       </c>
-      <c r="G54">
+      <c r="G70">
         <v>7</v>
       </c>
-      <c r="H54">
+      <c r="H70">
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A55">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A71">
         <v>22032007</v>
       </c>
-      <c r="B55" s="9" t="str">
+      <c r="B71" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>初始资源包</v>
       </c>
-      <c r="G55">
+      <c r="G71">
         <v>1</v>
       </c>
-      <c r="H55">
+      <c r="H71">
         <v>300</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A56">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A72">
         <v>22032008</v>
       </c>
-      <c r="B56" s="9" t="str">
+      <c r="B72" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>金币</v>
       </c>
-      <c r="G56">
+      <c r="G72">
         <v>1</v>
       </c>
-      <c r="H56">
+      <c r="H72">
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A57">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A73">
         <v>22033001</v>
       </c>
-      <c r="B57" s="9" t="str">
+      <c r="B73" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>小型魔法药剂</v>
       </c>
-      <c r="R57">
+      <c r="R73">
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A58">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A74">
         <v>22033002</v>
       </c>
-      <c r="B58" s="9" t="str">
+      <c r="B74" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>中型魔法药剂</v>
       </c>
-      <c r="R58">
+      <c r="R74">
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A59">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A75">
         <v>22033003</v>
       </c>
-      <c r="B59" s="9" t="str">
+      <c r="B75" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>大型魔法药剂</v>
       </c>
-      <c r="R59">
+      <c r="R75">
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A60">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A76">
         <v>22033004</v>
       </c>
-      <c r="B60" s="9" t="str">
+      <c r="B76" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>小型活力药剂</v>
       </c>
-      <c r="Q60">
+      <c r="Q76">
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A61">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A77">
         <v>22033005</v>
       </c>
-      <c r="B61" s="9" t="str">
+      <c r="B77" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>中型活力药剂</v>
       </c>
-      <c r="Q61">
+      <c r="Q77">
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A62">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A78">
         <v>22033006</v>
       </c>
-      <c r="B62" s="9" t="str">
+      <c r="B78" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>大型活力药剂</v>
       </c>
-      <c r="Q62">
+      <c r="Q78">
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A63">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A79">
         <v>22033007</v>
       </c>
-      <c r="B63" s="9" t="str">
+      <c r="B79" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>小型体力药剂</v>
       </c>
-      <c r="S63">
+      <c r="S79">
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A64">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A80">
         <v>22033008</v>
       </c>
-      <c r="B64" s="9" t="str">
+      <c r="B80" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>中型体力药剂</v>
       </c>
-      <c r="S64">
+      <c r="S80">
         <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A65">
-        <v>22033009</v>
-      </c>
-      <c r="B65" s="9" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>大型体力药剂</v>
-      </c>
-      <c r="S65">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A66">
-        <v>22033013</v>
-      </c>
-      <c r="B66" s="9" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>随机幻兽卡</v>
-      </c>
-      <c r="U66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A67">
-        <v>22033014</v>
-      </c>
-      <c r="B67" s="9" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>随机武器卡</v>
-      </c>
-      <c r="U67">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A68">
-        <v>22033015</v>
-      </c>
-      <c r="B68" s="9" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>随机魔法卡</v>
-      </c>
-      <c r="U68">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A69">
-        <v>22033016</v>
-      </c>
-      <c r="B69" s="9" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>符文-查姆</v>
-      </c>
-      <c r="T69">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A70">
-        <v>22033017</v>
-      </c>
-      <c r="B70" s="9" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>符文-普尔</v>
-      </c>
-      <c r="T70">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A71">
-        <v>22033018</v>
-      </c>
-      <c r="B71" s="9" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>符文-艾尔</v>
-      </c>
-      <c r="V71" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A72">
-        <v>22033030</v>
-      </c>
-      <c r="B72" s="13" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>木质修理锤</v>
-      </c>
-      <c r="W72">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A73">
-        <v>22033031</v>
-      </c>
-      <c r="B73" s="13" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>钢铁修理锤</v>
-      </c>
-      <c r="W73">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A74">
-        <v>22033032</v>
-      </c>
-      <c r="B74" s="13" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>神圣修理锤</v>
-      </c>
-      <c r="W74">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A75">
-        <v>22034001</v>
-      </c>
-      <c r="B75" s="13" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>经验之书</v>
-      </c>
-      <c r="C75">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A76">
-        <v>22034002</v>
-      </c>
-      <c r="B76" s="13" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>能量之书</v>
-      </c>
-      <c r="C76">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A77">
-        <v>22034003</v>
-      </c>
-      <c r="B77" s="13" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>攻速药水</v>
-      </c>
-      <c r="X77" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A78">
-        <v>22034004</v>
-      </c>
-      <c r="B78" s="13" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>守护药水</v>
-      </c>
-      <c r="X78" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A79">
-        <v>22034005</v>
-      </c>
-      <c r="B79" s="13" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>法术药水</v>
-      </c>
-      <c r="X79" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A80">
-        <v>22034006</v>
-      </c>
-      <c r="B80" s="13" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>技巧药水</v>
-      </c>
-      <c r="X80" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="81" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A81">
-        <v>22034007</v>
-      </c>
-      <c r="B81" s="13" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>速度药水</v>
-      </c>
-      <c r="X81" t="s">
-        <v>55</v>
+        <v>22033009</v>
+      </c>
+      <c r="B81" s="9" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>大型体力药剂</v>
+      </c>
+      <c r="S81">
+        <v>10</v>
       </c>
     </row>
     <row r="82" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A82">
-        <v>22034008</v>
-      </c>
-      <c r="B82" s="13" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>幸运药水</v>
-      </c>
-      <c r="X82" t="s">
-        <v>57</v>
+        <v>22033013</v>
+      </c>
+      <c r="B82" s="9" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>随机幻兽卡</v>
+      </c>
+      <c r="U82">
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A83">
-        <v>22034009</v>
+        <v>22033014</v>
       </c>
       <c r="B83" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>暴击药水</v>
-      </c>
-      <c r="X83" t="s">
-        <v>56</v>
+        <v>随机武器卡</v>
+      </c>
+      <c r="U83">
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A84">
-        <v>22034010</v>
+        <v>22033015</v>
       </c>
       <c r="B84" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>饼干</v>
-      </c>
-      <c r="D84">
-        <v>50</v>
+        <v>随机魔法卡</v>
+      </c>
+      <c r="U84">
+        <v>3</v>
       </c>
     </row>
     <row r="85" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A85">
-        <v>22034011</v>
-      </c>
-      <c r="B85" s="10" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>红色胶囊</v>
-      </c>
-      <c r="E85">
-        <v>50</v>
+        <v>22033016</v>
+      </c>
+      <c r="B85" s="9" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>符文-查姆</v>
+      </c>
+      <c r="T85">
+        <v>9999</v>
       </c>
     </row>
     <row r="86" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A86">
-        <v>22034012</v>
-      </c>
-      <c r="B86" s="10" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>蓝色胶囊</v>
-      </c>
-      <c r="F86">
-        <v>50</v>
+        <v>22033017</v>
+      </c>
+      <c r="B86" s="9" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>符文-普尔</v>
+      </c>
+      <c r="T86">
+        <v>100</v>
       </c>
     </row>
     <row r="87" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A87">
-        <v>22034013</v>
-      </c>
-      <c r="B87" s="10" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>水晶球</v>
-      </c>
-      <c r="N87" t="s">
-        <v>74</v>
+        <v>22033018</v>
+      </c>
+      <c r="B87" s="9" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>符文-艾尔</v>
+      </c>
+      <c r="V87" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="88" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A88">
-        <v>22034014</v>
-      </c>
-      <c r="B88" s="14" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>坐骑黑豹</v>
-      </c>
-      <c r="I88">
-        <v>2</v>
-      </c>
-      <c r="J88">
-        <v>10</v>
+        <v>22033030</v>
+      </c>
+      <c r="B88" s="13" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>木质修理锤</v>
+      </c>
+      <c r="W88">
+        <v>200</v>
       </c>
     </row>
     <row r="89" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A89">
-        <v>22034015</v>
-      </c>
-      <c r="B89" s="14" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>坐骑鹰</v>
-      </c>
-      <c r="I89">
-        <v>5</v>
-      </c>
-      <c r="J89">
-        <v>10</v>
+        <v>22033031</v>
+      </c>
+      <c r="B89" s="13" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>钢铁修理锤</v>
+      </c>
+      <c r="W89">
+        <v>500</v>
       </c>
     </row>
     <row r="90" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A90">
-        <v>22034016</v>
-      </c>
-      <c r="B90" s="14" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>坐骑传送器</v>
-      </c>
-      <c r="I90">
-        <v>99</v>
-      </c>
-      <c r="J90">
-        <v>10</v>
+        <v>22033032</v>
+      </c>
+      <c r="B90" s="13" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>神圣修理锤</v>
+      </c>
+      <c r="W90">
+        <v>1000</v>
       </c>
     </row>
     <row r="91" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A91">
-        <v>22037001</v>
+        <v>22034001</v>
       </c>
       <c r="B91" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>种子-豌豆</v>
-      </c>
-      <c r="O91">
-        <v>22037101</v>
-      </c>
-      <c r="P91">
-        <v>10800</v>
+        <v>经验之书</v>
+      </c>
+      <c r="C91">
+        <v>50</v>
       </c>
     </row>
     <row r="92" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A92">
-        <v>22037002</v>
+        <v>22034002</v>
       </c>
       <c r="B92" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>种子-玉米</v>
-      </c>
-      <c r="O92">
-        <v>22037102</v>
-      </c>
-      <c r="P92">
-        <v>10800</v>
+        <v>能量之书</v>
+      </c>
+      <c r="C92">
+        <v>300</v>
       </c>
     </row>
     <row r="93" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A93">
-        <v>22037003</v>
+        <v>22034003</v>
       </c>
       <c r="B93" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>种子-苹果</v>
-      </c>
-      <c r="O93">
-        <v>22037103</v>
-      </c>
-      <c r="P93">
-        <v>10800</v>
+        <v>攻速药水</v>
+      </c>
+      <c r="X93" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="94" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A94">
-        <v>22037004</v>
+        <v>22034004</v>
       </c>
       <c r="B94" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>种子-蓝莓</v>
-      </c>
-      <c r="O94">
-        <v>22037104</v>
-      </c>
-      <c r="P94">
-        <v>10800</v>
+        <v>守护药水</v>
+      </c>
+      <c r="X94" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="95" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A95">
-        <v>22037101</v>
+        <v>22034005</v>
       </c>
       <c r="B95" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>作物-豌豆</v>
-      </c>
-      <c r="C95">
-        <v>5</v>
+        <v>法术药水</v>
+      </c>
+      <c r="X95" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="96" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A96">
+        <v>22034006</v>
+      </c>
+      <c r="B96" s="13" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>技巧药水</v>
+      </c>
+      <c r="X96" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="97" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A97">
+        <v>22034007</v>
+      </c>
+      <c r="B97" s="13" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>速度药水</v>
+      </c>
+      <c r="X97" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="98" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A98">
+        <v>22034008</v>
+      </c>
+      <c r="B98" s="13" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>幸运药水</v>
+      </c>
+      <c r="X98" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="99" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A99">
+        <v>22034009</v>
+      </c>
+      <c r="B99" s="9" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>暴击药水</v>
+      </c>
+      <c r="X99" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="100" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A100">
+        <v>22034010</v>
+      </c>
+      <c r="B100" s="9" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>饼干</v>
+      </c>
+      <c r="D100">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="101" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A101">
+        <v>22034011</v>
+      </c>
+      <c r="B101" s="10" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>红色胶囊</v>
+      </c>
+      <c r="E101">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="102" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A102">
+        <v>22034012</v>
+      </c>
+      <c r="B102" s="10" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>蓝色胶囊</v>
+      </c>
+      <c r="F102">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="103" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A103">
+        <v>22034013</v>
+      </c>
+      <c r="B103" s="10" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>水晶球</v>
+      </c>
+      <c r="N103" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="104" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A104">
+        <v>22034014</v>
+      </c>
+      <c r="B104" s="14" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>坐骑黑豹</v>
+      </c>
+      <c r="I104">
+        <v>2</v>
+      </c>
+      <c r="J104">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A105">
+        <v>22034015</v>
+      </c>
+      <c r="B105" s="14" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>坐骑鹰</v>
+      </c>
+      <c r="I105">
+        <v>5</v>
+      </c>
+      <c r="J105">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="106" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A106">
+        <v>22034016</v>
+      </c>
+      <c r="B106" s="14" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>坐骑传送器</v>
+      </c>
+      <c r="I106">
+        <v>99</v>
+      </c>
+      <c r="J106">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A107">
+        <v>22037001</v>
+      </c>
+      <c r="B107" s="13" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>种子-豌豆</v>
+      </c>
+      <c r="O107">
+        <v>22037101</v>
+      </c>
+      <c r="P107">
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="108" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A108">
+        <v>22037002</v>
+      </c>
+      <c r="B108" s="13" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>种子-玉米</v>
+      </c>
+      <c r="O108">
         <v>22037102</v>
       </c>
-      <c r="B96" s="13" t="str">
+      <c r="P108">
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="109" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A109">
+        <v>22037003</v>
+      </c>
+      <c r="B109" s="13" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>种子-苹果</v>
+      </c>
+      <c r="O109">
+        <v>22037103</v>
+      </c>
+      <c r="P109">
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="110" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A110">
+        <v>22037004</v>
+      </c>
+      <c r="B110" s="13" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>种子-蓝莓</v>
+      </c>
+      <c r="O110">
+        <v>22037104</v>
+      </c>
+      <c r="P110">
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="111" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A111">
+        <v>22037101</v>
+      </c>
+      <c r="B111" s="13" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>作物-豌豆</v>
+      </c>
+      <c r="C111">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A112">
+        <v>22037102</v>
+      </c>
+      <c r="B112" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>作物-玉米</v>
       </c>
-      <c r="G96">
+      <c r="G112">
         <v>1</v>
       </c>
-      <c r="H96">
+      <c r="H112">
         <v>20</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A97">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A113">
         <v>22037103</v>
       </c>
-      <c r="B97" s="13" t="str">
+      <c r="B113" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>作物-苹果</v>
       </c>
-      <c r="Q97">
+      <c r="Q113">
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A98">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A114">
         <v>22037104</v>
       </c>
-      <c r="B98" s="13" t="str">
+      <c r="B114" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>作物-苹果</v>
       </c>
-      <c r="R98">
+      <c r="R114">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="X23:X55 C4:X13 C14:L22 O14:X22 A23:L45 O23:W45 X57:X70 A46:W70 C71:X86 C88:X98 K87:X87 J85:J87">
-    <cfRule type="containsBlanks" dxfId="7" priority="11">
+  <conditionalFormatting sqref="X39:X71 C4:X13 A39:L61 O39:W61 X73:X86 A62:W86 C87:X102 C104:X114 K103:X103 J101:J103 C14:L20 C37:L38 O37:X38 N14:X20 N37:N61 C21:X36">
+    <cfRule type="containsBlanks" dxfId="4" priority="11">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X56">
-    <cfRule type="containsBlanks" dxfId="6" priority="5">
-      <formula>LEN(TRIM(X56))=0</formula>
+  <conditionalFormatting sqref="X72">
+    <cfRule type="containsBlanks" dxfId="3" priority="5">
+      <formula>LEN(TRIM(X72))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N14:N45">
-    <cfRule type="containsBlanks" dxfId="5" priority="4">
-      <formula>LEN(TRIM(N14))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C87:J87">
-    <cfRule type="containsBlanks" dxfId="4" priority="3">
-      <formula>LEN(TRIM(C87))=0</formula>
+  <conditionalFormatting sqref="C103:J103">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(C103))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M18:M20">

</xml_diff>

<commit_message>
save the item cd data into db
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/ItemConsumer.xlsx
+++ b/ConfigData/Xlsx/ItemConsumer.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="150">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -547,6 +547,26 @@
   </si>
   <si>
     <t>0;0;350;650;0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cd时间</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CdTime</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CdGroup</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cd组</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -748,7 +768,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -946,6 +966,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -1211,7 +1243,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1255,6 +1287,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1302,7 +1343,28 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -1397,6 +1459,25 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -2377,16 +2458,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:X115" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A3:X115"/>
-  <sortState ref="A4:X115">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:Z115" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:Z115"/>
+  <sortState ref="A4:Z115">
     <sortCondition ref="A3:A115"/>
   </sortState>
-  <tableColumns count="24">
+  <tableColumns count="26">
     <tableColumn id="1" name="Id"/>
-    <tableColumn id="2" name="~Name" dataDxfId="8">
+    <tableColumn id="2" name="~Name" dataDxfId="12">
       <calculatedColumnFormula>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="16" name="CdGroup" dataDxfId="11"/>
+    <tableColumn id="25" name="CdTime"/>
     <tableColumn id="3" name="GainExp"/>
     <tableColumn id="4" name="GainFood"/>
     <tableColumn id="21" name="GainHealth"/>
@@ -2735,114 +2818,121 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X115"/>
+  <dimension ref="A1:Z115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.375" customWidth="1"/>
-    <col min="3" max="3" width="4.625" customWidth="1"/>
-    <col min="4" max="6" width="3.75" customWidth="1"/>
-    <col min="7" max="10" width="4.25" customWidth="1"/>
-    <col min="11" max="11" width="6.875" customWidth="1"/>
-    <col min="12" max="12" width="12.625" customWidth="1"/>
-    <col min="13" max="13" width="9.75" customWidth="1"/>
-    <col min="14" max="14" width="6.75" customWidth="1"/>
-    <col min="15" max="15" width="8.625" customWidth="1"/>
-    <col min="16" max="16" width="6.625" customWidth="1"/>
-    <col min="17" max="24" width="7.375" customWidth="1"/>
+    <col min="3" max="4" width="6" customWidth="1"/>
+    <col min="5" max="5" width="4.625" customWidth="1"/>
+    <col min="6" max="8" width="3.75" customWidth="1"/>
+    <col min="9" max="12" width="4.25" customWidth="1"/>
+    <col min="13" max="13" width="6.875" customWidth="1"/>
+    <col min="14" max="14" width="12.625" customWidth="1"/>
+    <col min="15" max="15" width="9.75" customWidth="1"/>
+    <col min="16" max="16" width="6.75" customWidth="1"/>
+    <col min="17" max="17" width="8.625" customWidth="1"/>
+    <col min="18" max="18" width="6.625" customWidth="1"/>
+    <col min="19" max="26" width="7.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="77.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:26" ht="77.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="R1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="S1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="T1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="U1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="V1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="W1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="X1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="Y1" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="Z1" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>0</v>
+      <c r="C2" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>148</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
@@ -2863,30 +2953,30 @@
         <v>0</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="T2" s="3" t="s">
@@ -2896,90 +2986,102 @@
         <v>0</v>
       </c>
       <c r="V2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="X2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="Q3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="R3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="S3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="T3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="U3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="8" t="s">
+      <c r="V3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="U3" s="8" t="s">
+      <c r="W3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="V3" s="8" t="s">
+      <c r="X3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="W3" s="8" t="s">
+      <c r="Y3" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="X3" s="8" t="s">
+      <c r="Z3" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>22020001</v>
       </c>
@@ -2987,14 +3089,20 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>#N/A</v>
       </c>
-      <c r="K4" t="s">
+      <c r="C4" s="14">
+        <v>4</v>
+      </c>
+      <c r="D4" s="14">
+        <v>15</v>
+      </c>
+      <c r="M4" t="s">
         <v>143</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>22031101</v>
       </c>
@@ -3002,11 +3110,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>素材袋</v>
       </c>
-      <c r="M5" s="13" t="s">
+      <c r="O5" s="13" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>22031102</v>
       </c>
@@ -3014,11 +3122,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>高级素材袋</v>
       </c>
-      <c r="M6" s="13" t="s">
+      <c r="O6" s="13" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>22031103</v>
       </c>
@@ -3026,11 +3134,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>特级素材袋</v>
       </c>
-      <c r="M7" s="13" t="s">
+      <c r="O7" s="13" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>22031104</v>
       </c>
@@ -3038,11 +3146,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>极品素材袋</v>
       </c>
-      <c r="M8" s="13" t="s">
+      <c r="O8" s="13" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>22031201</v>
       </c>
@@ -3050,14 +3158,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>蓝色卡包</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>34</v>
       </c>
-      <c r="L9" t="s">
+      <c r="N9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>22031202</v>
       </c>
@@ -3065,14 +3173,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>黄色卡包</v>
       </c>
-      <c r="K10" t="s">
+      <c r="M10" t="s">
         <v>34</v>
       </c>
-      <c r="L10" t="s">
+      <c r="N10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>22031203</v>
       </c>
@@ -3080,14 +3188,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>红色卡包</v>
       </c>
-      <c r="K11" t="s">
+      <c r="M11" t="s">
         <v>34</v>
       </c>
-      <c r="L11" t="s">
+      <c r="N11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>22031212</v>
       </c>
@@ -3095,14 +3203,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(无)</v>
       </c>
-      <c r="K12" t="s">
+      <c r="M12" t="s">
         <v>27</v>
       </c>
-      <c r="L12" t="s">
+      <c r="N12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>22031213</v>
       </c>
@@ -3110,14 +3218,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(水)</v>
       </c>
-      <c r="K13" t="s">
+      <c r="M13" t="s">
         <v>28</v>
       </c>
-      <c r="L13" t="s">
+      <c r="N13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>22031214</v>
       </c>
@@ -3125,14 +3233,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(风)</v>
       </c>
-      <c r="K14" t="s">
+      <c r="M14" t="s">
         <v>29</v>
       </c>
-      <c r="L14" t="s">
+      <c r="N14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>22031215</v>
       </c>
@@ -3140,14 +3248,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(地)</v>
       </c>
-      <c r="K15" t="s">
+      <c r="M15" t="s">
         <v>30</v>
       </c>
-      <c r="L15" t="s">
+      <c r="N15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>22031216</v>
       </c>
@@ -3155,14 +3263,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(火)</v>
       </c>
-      <c r="K16" t="s">
+      <c r="M16" t="s">
         <v>31</v>
       </c>
-      <c r="L16" t="s">
+      <c r="N16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>22031217</v>
       </c>
@@ -3170,14 +3278,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(光)</v>
       </c>
-      <c r="K17" t="s">
+      <c r="M17" t="s">
         <v>32</v>
       </c>
-      <c r="L17" t="s">
+      <c r="N17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>22031218</v>
       </c>
@@ -3185,14 +3293,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(暗)</v>
       </c>
-      <c r="K18" t="s">
+      <c r="M18" t="s">
         <v>33</v>
       </c>
-      <c r="L18" t="s">
+      <c r="N18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>22031221</v>
       </c>
@@ -3200,14 +3308,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(生物)</v>
       </c>
-      <c r="K19" t="s">
+      <c r="M19" t="s">
         <v>39</v>
       </c>
-      <c r="L19" t="s">
+      <c r="N19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>22031222</v>
       </c>
@@ -3215,14 +3323,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(武器)</v>
       </c>
-      <c r="K20" t="s">
+      <c r="M20" t="s">
         <v>40</v>
       </c>
-      <c r="L20" t="s">
+      <c r="N20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>22031223</v>
       </c>
@@ -3230,14 +3338,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(法术)</v>
       </c>
-      <c r="K21" t="s">
+      <c r="M21" t="s">
         <v>41</v>
       </c>
-      <c r="L21" t="s">
+      <c r="N21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>22031231</v>
       </c>
@@ -3245,14 +3353,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(恶魔)</v>
       </c>
-      <c r="K22" t="s">
+      <c r="M22" t="s">
         <v>92</v>
       </c>
-      <c r="L22" t="s">
+      <c r="N22" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>22031232</v>
       </c>
@@ -3260,14 +3368,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(机械)</v>
       </c>
-      <c r="K23" t="s">
+      <c r="M23" t="s">
         <v>93</v>
       </c>
-      <c r="L23" t="s">
+      <c r="N23" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>22031233</v>
       </c>
@@ -3275,14 +3383,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(精灵)</v>
       </c>
-      <c r="K24" t="s">
+      <c r="M24" t="s">
         <v>94</v>
       </c>
-      <c r="L24" t="s">
+      <c r="N24" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>22031234</v>
       </c>
@@ -3290,14 +3398,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(昆虫)</v>
       </c>
-      <c r="K25" t="s">
+      <c r="M25" t="s">
         <v>95</v>
       </c>
-      <c r="L25" t="s">
+      <c r="N25" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>22031235</v>
       </c>
@@ -3305,14 +3413,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(龙)</v>
       </c>
-      <c r="K26" t="s">
+      <c r="M26" t="s">
         <v>96</v>
       </c>
-      <c r="L26" t="s">
+      <c r="N26" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>22031236</v>
       </c>
@@ -3320,14 +3428,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(鸟)</v>
       </c>
-      <c r="K27" t="s">
+      <c r="M27" t="s">
         <v>97</v>
       </c>
-      <c r="L27" t="s">
+      <c r="N27" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>22031237</v>
       </c>
@@ -3335,14 +3443,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(爬行)</v>
       </c>
-      <c r="K28" t="s">
+      <c r="M28" t="s">
         <v>98</v>
       </c>
-      <c r="L28" t="s">
+      <c r="N28" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>22031238</v>
       </c>
@@ -3350,14 +3458,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(人类)</v>
       </c>
-      <c r="K29" t="s">
+      <c r="M29" t="s">
         <v>99</v>
       </c>
-      <c r="L29" t="s">
+      <c r="N29" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>22031239</v>
       </c>
@@ -3365,14 +3473,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(兽人)</v>
       </c>
-      <c r="K30" t="s">
+      <c r="M30" t="s">
         <v>100</v>
       </c>
-      <c r="L30" t="s">
+      <c r="N30" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>22031240</v>
       </c>
@@ -3380,14 +3488,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(亡灵)</v>
       </c>
-      <c r="K31" t="s">
+      <c r="M31" t="s">
         <v>101</v>
       </c>
-      <c r="L31" t="s">
+      <c r="N31" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>22031241</v>
       </c>
@@ -3395,14 +3503,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(野兽)</v>
       </c>
-      <c r="K32" t="s">
+      <c r="M32" t="s">
         <v>102</v>
       </c>
-      <c r="L32" t="s">
+      <c r="N32" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>22031242</v>
       </c>
@@ -3410,14 +3518,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(鱼)</v>
       </c>
-      <c r="K33" t="s">
+      <c r="M33" t="s">
         <v>103</v>
       </c>
-      <c r="L33" t="s">
+      <c r="N33" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>22031243</v>
       </c>
@@ -3425,14 +3533,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(元素)</v>
       </c>
-      <c r="K34" t="s">
+      <c r="M34" t="s">
         <v>104</v>
       </c>
-      <c r="L34" t="s">
+      <c r="N34" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>22031244</v>
       </c>
@@ -3440,14 +3548,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(植物)</v>
       </c>
-      <c r="K35" t="s">
+      <c r="M35" t="s">
         <v>105</v>
       </c>
-      <c r="L35" t="s">
+      <c r="N35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>22031245</v>
       </c>
@@ -3455,14 +3563,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(地精)</v>
       </c>
-      <c r="K36" t="s">
+      <c r="M36" t="s">
         <v>106</v>
       </c>
-      <c r="L36" t="s">
+      <c r="N36" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>22031246</v>
       </c>
@@ -3470,14 +3578,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(石像)</v>
       </c>
-      <c r="K37" t="s">
+      <c r="M37" t="s">
         <v>107</v>
       </c>
-      <c r="L37" t="s">
+      <c r="N37" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>22031301</v>
       </c>
@@ -3485,11 +3593,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(绿)</v>
       </c>
-      <c r="M38" s="13" t="s">
+      <c r="O38" s="13" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>22031302</v>
       </c>
@@ -3497,11 +3605,13 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(蓝)</v>
       </c>
-      <c r="M39" s="9" t="s">
+      <c r="C39" s="10"/>
+      <c r="D39" s="14"/>
+      <c r="O39" s="9" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>22031303</v>
       </c>
@@ -3509,11 +3619,13 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(红)</v>
       </c>
-      <c r="M40" t="s">
+      <c r="C40" s="10"/>
+      <c r="D40" s="14"/>
+      <c r="O40" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>22031304</v>
       </c>
@@ -3521,11 +3633,13 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(紫)</v>
       </c>
-      <c r="M41" t="s">
+      <c r="C41" s="10"/>
+      <c r="D41" s="14"/>
+      <c r="O41" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>22031305</v>
       </c>
@@ -3533,11 +3647,13 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(灰)</v>
       </c>
-      <c r="M42" t="s">
+      <c r="C42" s="10"/>
+      <c r="D42" s="14"/>
+      <c r="O42" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>22031401</v>
       </c>
@@ -3545,11 +3661,13 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>素材袋(无)</v>
       </c>
-      <c r="M43" s="14" t="s">
+      <c r="C43" s="10"/>
+      <c r="D43" s="14"/>
+      <c r="O43" s="14" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>22031402</v>
       </c>
@@ -3557,11 +3675,13 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>素材袋(水)</v>
       </c>
-      <c r="M44" s="14" t="s">
+      <c r="C44" s="10"/>
+      <c r="D44" s="14"/>
+      <c r="O44" s="14" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>22031403</v>
       </c>
@@ -3569,11 +3689,13 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>素材袋(风)</v>
       </c>
-      <c r="M45" s="14" t="s">
+      <c r="C45" s="10"/>
+      <c r="D45" s="14"/>
+      <c r="O45" s="14" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>22031404</v>
       </c>
@@ -3581,11 +3703,13 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>素材袋(火)</v>
       </c>
-      <c r="M46" s="14" t="s">
+      <c r="C46" s="10"/>
+      <c r="D46" s="14"/>
+      <c r="O46" s="14" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>22031405</v>
       </c>
@@ -3593,11 +3717,13 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>素材袋(地)</v>
       </c>
-      <c r="M47" s="14" t="s">
+      <c r="C47" s="10"/>
+      <c r="D47" s="14"/>
+      <c r="O47" s="14" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>22031406</v>
       </c>
@@ -3605,11 +3731,13 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>素材袋(光)</v>
       </c>
-      <c r="M48" s="14" t="s">
+      <c r="C48" s="10"/>
+      <c r="D48" s="14"/>
+      <c r="O48" s="14" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>22031407</v>
       </c>
@@ -3617,11 +3745,13 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>素材袋(暗)</v>
       </c>
-      <c r="M49" s="10" t="s">
+      <c r="C49" s="10"/>
+      <c r="D49" s="14"/>
+      <c r="O49" s="10" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>22031501</v>
       </c>
@@ -3629,11 +3759,13 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(恶魔)</v>
       </c>
-      <c r="M50" s="9" t="s">
+      <c r="C50" s="10"/>
+      <c r="D50" s="14"/>
+      <c r="O50" s="9" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>22031502</v>
       </c>
@@ -3641,11 +3773,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(机械)</v>
       </c>
-      <c r="M51" s="9" t="s">
+      <c r="O51" s="9" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>22031503</v>
       </c>
@@ -3653,11 +3785,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(精灵)</v>
       </c>
-      <c r="M52" s="9" t="s">
+      <c r="O52" s="9" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>22031504</v>
       </c>
@@ -3665,11 +3797,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(昆虫)</v>
       </c>
-      <c r="M53" s="9" t="s">
+      <c r="O53" s="9" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>22031505</v>
       </c>
@@ -3677,11 +3809,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(龙)</v>
       </c>
-      <c r="M54" s="9" t="s">
+      <c r="O54" s="9" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>22031506</v>
       </c>
@@ -3689,11 +3821,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(鸟)</v>
       </c>
-      <c r="M55" s="9" t="s">
+      <c r="O55" s="9" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>22031507</v>
       </c>
@@ -3701,11 +3833,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(爬行)</v>
       </c>
-      <c r="M56" s="9" t="s">
+      <c r="O56" s="9" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>22031508</v>
       </c>
@@ -3713,11 +3845,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(人类)</v>
       </c>
-      <c r="M57" s="9" t="s">
+      <c r="O57" s="9" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>22031509</v>
       </c>
@@ -3725,11 +3857,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(兽人)</v>
       </c>
-      <c r="M58" s="9" t="s">
+      <c r="O58" s="9" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>22031510</v>
       </c>
@@ -3737,11 +3869,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(亡灵)</v>
       </c>
-      <c r="M59" s="9" t="s">
+      <c r="O59" s="9" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A60">
         <v>22031511</v>
       </c>
@@ -3749,11 +3881,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(野兽)</v>
       </c>
-      <c r="M60" s="9" t="s">
+      <c r="O60" s="9" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>22031512</v>
       </c>
@@ -3761,11 +3893,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(鱼)</v>
       </c>
-      <c r="M61" s="9" t="s">
+      <c r="O61" s="9" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>22031513</v>
       </c>
@@ -3773,11 +3905,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(元素)</v>
       </c>
-      <c r="M62" s="9" t="s">
+      <c r="O62" s="9" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>22031514</v>
       </c>
@@ -3785,11 +3917,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(植物)</v>
       </c>
-      <c r="M63" s="9" t="s">
+      <c r="O63" s="9" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>22031515</v>
       </c>
@@ -3797,11 +3929,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(地精)</v>
       </c>
-      <c r="M64" s="9" t="s">
+      <c r="O64" s="9" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A65">
         <v>22031516</v>
       </c>
@@ -3809,11 +3941,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(石像)</v>
       </c>
-      <c r="M65" s="9" t="s">
+      <c r="O65" s="9" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A66">
         <v>22032001</v>
       </c>
@@ -3821,14 +3953,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>木材补给车</v>
       </c>
-      <c r="G66">
+      <c r="I66">
         <v>2</v>
       </c>
-      <c r="H66">
+      <c r="J66">
         <v>30</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>22032002</v>
       </c>
@@ -3836,14 +3968,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>矿石补给车</v>
       </c>
-      <c r="G67">
+      <c r="I67">
         <v>3</v>
       </c>
-      <c r="H67">
+      <c r="J67">
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A68">
         <v>22032003</v>
       </c>
@@ -3851,14 +3983,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>水银补给车</v>
       </c>
-      <c r="G68">
+      <c r="I68">
         <v>4</v>
       </c>
-      <c r="H68">
+      <c r="J68">
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A69">
         <v>22032004</v>
       </c>
@@ -3866,14 +3998,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>红宝石补给车</v>
       </c>
-      <c r="G69">
+      <c r="I69">
         <v>5</v>
       </c>
-      <c r="H69">
+      <c r="J69">
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A70">
         <v>22032005</v>
       </c>
@@ -3881,14 +4013,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>硫磺补给车</v>
       </c>
-      <c r="G70">
+      <c r="I70">
         <v>6</v>
       </c>
-      <c r="H70">
+      <c r="J70">
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>22032006</v>
       </c>
@@ -3896,14 +4028,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>水晶补给车</v>
       </c>
-      <c r="G71">
+      <c r="I71">
         <v>7</v>
       </c>
-      <c r="H71">
+      <c r="J71">
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A72">
         <v>22032007</v>
       </c>
@@ -3911,14 +4043,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>初始资源包</v>
       </c>
-      <c r="G72">
+      <c r="I72">
         <v>1</v>
       </c>
-      <c r="H72">
+      <c r="J72">
         <v>300</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A73">
         <v>22032008</v>
       </c>
@@ -3926,14 +4058,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>金币</v>
       </c>
-      <c r="G73">
+      <c r="I73">
         <v>1</v>
       </c>
-      <c r="H73">
+      <c r="J73">
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A74">
         <v>22033001</v>
       </c>
@@ -3941,11 +4073,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>小型魔法药剂</v>
       </c>
-      <c r="R74">
+      <c r="T74">
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A75">
         <v>22033002</v>
       </c>
@@ -3953,11 +4085,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>中型魔法药剂</v>
       </c>
-      <c r="R75">
+      <c r="C75">
+        <v>2</v>
+      </c>
+      <c r="D75">
+        <v>15</v>
+      </c>
+      <c r="T75">
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A76">
         <v>22033003</v>
       </c>
@@ -3965,11 +4103,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>大型魔法药剂</v>
       </c>
-      <c r="R76">
+      <c r="C76">
+        <v>2</v>
+      </c>
+      <c r="D76">
+        <v>15</v>
+      </c>
+      <c r="T76">
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A77">
         <v>22033004</v>
       </c>
@@ -3977,11 +4121,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>小型活力药剂</v>
       </c>
-      <c r="Q77">
+      <c r="C77">
         <v>2</v>
       </c>
-    </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="D77">
+        <v>15</v>
+      </c>
+      <c r="S77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A78">
         <v>22033005</v>
       </c>
@@ -3989,11 +4139,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>中型活力药剂</v>
       </c>
-      <c r="Q78">
+      <c r="C78">
+        <v>3</v>
+      </c>
+      <c r="D78">
+        <v>15</v>
+      </c>
+      <c r="S78">
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A79">
         <v>22033006</v>
       </c>
@@ -4001,11 +4157,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>大型活力药剂</v>
       </c>
-      <c r="Q79">
+      <c r="C79">
+        <v>3</v>
+      </c>
+      <c r="D79">
+        <v>15</v>
+      </c>
+      <c r="S79">
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A80">
         <v>22033007</v>
       </c>
@@ -4013,11 +4175,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>小型体力药剂</v>
       </c>
-      <c r="S80">
+      <c r="C80">
+        <v>3</v>
+      </c>
+      <c r="D80">
+        <v>15</v>
+      </c>
+      <c r="U80">
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A81">
         <v>22033008</v>
       </c>
@@ -4025,11 +4193,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>中型体力药剂</v>
       </c>
-      <c r="S81">
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <v>15</v>
+      </c>
+      <c r="U81">
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A82">
         <v>22033009</v>
       </c>
@@ -4037,11 +4211,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>大型体力药剂</v>
       </c>
-      <c r="S82">
+      <c r="C82">
+        <v>1</v>
+      </c>
+      <c r="D82">
+        <v>15</v>
+      </c>
+      <c r="U82">
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A83">
         <v>22033013</v>
       </c>
@@ -4049,11 +4229,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>随机幻兽卡</v>
       </c>
-      <c r="U83">
+      <c r="C83">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="D83">
+        <v>15</v>
+      </c>
+      <c r="W83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A84">
         <v>22033014</v>
       </c>
@@ -4061,11 +4247,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>随机武器卡</v>
       </c>
-      <c r="U84">
+      <c r="C84">
+        <v>1</v>
+      </c>
+      <c r="D84">
+        <v>15</v>
+      </c>
+      <c r="W84">
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A85">
         <v>22033015</v>
       </c>
@@ -4073,11 +4265,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>随机魔法卡</v>
       </c>
-      <c r="U85">
+      <c r="C85">
+        <v>4</v>
+      </c>
+      <c r="D85">
+        <v>15</v>
+      </c>
+      <c r="W85">
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A86">
         <v>22033016</v>
       </c>
@@ -4085,11 +4283,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>符文-查姆</v>
       </c>
-      <c r="T86">
+      <c r="C86">
+        <v>4</v>
+      </c>
+      <c r="D86">
+        <v>15</v>
+      </c>
+      <c r="V86">
         <v>9999</v>
       </c>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A87">
         <v>22033017</v>
       </c>
@@ -4097,11 +4301,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>符文-普尔</v>
       </c>
-      <c r="T87">
+      <c r="C87">
+        <v>4</v>
+      </c>
+      <c r="D87">
+        <v>15</v>
+      </c>
+      <c r="V87">
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A88">
         <v>22033018</v>
       </c>
@@ -4109,11 +4319,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>符文-艾尔</v>
       </c>
-      <c r="V88" t="s">
+      <c r="C88">
+        <v>4</v>
+      </c>
+      <c r="D88">
+        <v>15</v>
+      </c>
+      <c r="X88" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A89">
         <v>22033030</v>
       </c>
@@ -4121,11 +4337,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>木质修理锤</v>
       </c>
-      <c r="W89">
+      <c r="C89">
+        <v>4</v>
+      </c>
+      <c r="D89">
+        <v>15</v>
+      </c>
+      <c r="Y89">
         <v>200</v>
       </c>
     </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A90">
         <v>22033031</v>
       </c>
@@ -4133,11 +4355,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>钢铁修理锤</v>
       </c>
-      <c r="W90">
+      <c r="C90">
+        <v>1</v>
+      </c>
+      <c r="D90">
+        <v>15</v>
+      </c>
+      <c r="Y90">
         <v>500</v>
       </c>
     </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A91">
         <v>22033032</v>
       </c>
@@ -4145,11 +4373,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>神圣修理锤</v>
       </c>
-      <c r="W91">
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="D91">
+        <v>15</v>
+      </c>
+      <c r="Y91">
         <v>1000</v>
       </c>
     </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A92">
         <v>22034001</v>
       </c>
@@ -4158,10 +4392,16 @@
         <v>经验之书</v>
       </c>
       <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="D92">
+        <v>15</v>
+      </c>
+      <c r="E92">
         <v>50</v>
       </c>
     </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A93">
         <v>22034002</v>
       </c>
@@ -4169,11 +4409,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>能量之书</v>
       </c>
-      <c r="C93">
+      <c r="E93">
         <v>300</v>
       </c>
     </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A94">
         <v>22034003</v>
       </c>
@@ -4181,11 +4421,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>攻速药水</v>
       </c>
-      <c r="X94" t="s">
+      <c r="Z94" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A95">
         <v>22034004</v>
       </c>
@@ -4193,11 +4433,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>守护药水</v>
       </c>
-      <c r="X95" t="s">
+      <c r="C95">
+        <v>4</v>
+      </c>
+      <c r="D95">
+        <v>15</v>
+      </c>
+      <c r="Z95" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A96">
         <v>22034005</v>
       </c>
@@ -4205,11 +4451,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>法术药水</v>
       </c>
-      <c r="X96" t="s">
+      <c r="C96">
+        <v>4</v>
+      </c>
+      <c r="D96">
+        <v>15</v>
+      </c>
+      <c r="Z96" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A97">
         <v>22034006</v>
       </c>
@@ -4217,11 +4469,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>技巧药水</v>
       </c>
-      <c r="X97" t="s">
+      <c r="C97">
+        <v>4</v>
+      </c>
+      <c r="D97">
+        <v>15</v>
+      </c>
+      <c r="Z97" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A98">
         <v>22034007</v>
       </c>
@@ -4229,11 +4487,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>速度药水</v>
       </c>
-      <c r="X98" t="s">
+      <c r="C98">
+        <v>4</v>
+      </c>
+      <c r="D98">
+        <v>15</v>
+      </c>
+      <c r="Z98" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A99">
         <v>22034008</v>
       </c>
@@ -4241,11 +4505,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>幸运药水</v>
       </c>
-      <c r="X99" t="s">
+      <c r="C99">
+        <v>4</v>
+      </c>
+      <c r="D99">
+        <v>15</v>
+      </c>
+      <c r="Z99" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A100">
         <v>22034009</v>
       </c>
@@ -4253,11 +4523,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>暴击药水</v>
       </c>
-      <c r="X100" t="s">
+      <c r="C100">
+        <v>4</v>
+      </c>
+      <c r="D100">
+        <v>15</v>
+      </c>
+      <c r="Z100" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A101">
         <v>22034010</v>
       </c>
@@ -4265,11 +4541,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>饼干</v>
       </c>
+      <c r="C101">
+        <v>4</v>
+      </c>
       <c r="D101">
+        <v>15</v>
+      </c>
+      <c r="F101">
         <v>50</v>
       </c>
     </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A102">
         <v>22034011</v>
       </c>
@@ -4277,11 +4559,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>红色胶囊</v>
       </c>
-      <c r="E102">
+      <c r="C102">
+        <v>4</v>
+      </c>
+      <c r="D102">
+        <v>15</v>
+      </c>
+      <c r="G102">
         <v>50</v>
       </c>
     </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A103">
         <v>22034012</v>
       </c>
@@ -4289,11 +4577,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>蓝色胶囊</v>
       </c>
-      <c r="F103">
+      <c r="H103">
         <v>50</v>
       </c>
     </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A104">
         <v>22034013</v>
       </c>
@@ -4301,11 +4589,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>水晶球</v>
       </c>
-      <c r="N104" t="s">
+      <c r="P104" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A105">
         <v>22034014</v>
       </c>
@@ -4313,14 +4601,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>坐骑黑豹</v>
       </c>
-      <c r="I105">
+      <c r="K105">
         <v>2</v>
       </c>
-      <c r="J105">
+      <c r="L105">
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A106">
         <v>22034015</v>
       </c>
@@ -4328,14 +4616,15 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>坐骑鹰</v>
       </c>
-      <c r="I106">
+      <c r="D106" s="14"/>
+      <c r="K106">
         <v>5</v>
       </c>
-      <c r="J106">
+      <c r="L106">
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A107">
         <v>22034016</v>
       </c>
@@ -4343,14 +4632,15 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>坐骑传送器</v>
       </c>
-      <c r="I107">
+      <c r="D107" s="14"/>
+      <c r="K107">
         <v>99</v>
       </c>
-      <c r="J107">
+      <c r="L107">
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A108">
         <v>22037001</v>
       </c>
@@ -4358,14 +4648,15 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>种子-豌豆</v>
       </c>
-      <c r="O108">
+      <c r="D108" s="14"/>
+      <c r="Q108">
         <v>22037101</v>
       </c>
-      <c r="P108">
+      <c r="R108">
         <v>10800</v>
       </c>
     </row>
-    <row r="109" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A109">
         <v>22037002</v>
       </c>
@@ -4373,14 +4664,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>种子-玉米</v>
       </c>
-      <c r="O109">
+      <c r="Q109">
         <v>22037102</v>
       </c>
-      <c r="P109">
+      <c r="R109">
         <v>10800</v>
       </c>
     </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A110">
         <v>22037003</v>
       </c>
@@ -4388,14 +4679,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>种子-苹果</v>
       </c>
-      <c r="O110">
+      <c r="Q110">
         <v>22037103</v>
       </c>
-      <c r="P110">
+      <c r="R110">
         <v>10800</v>
       </c>
     </row>
-    <row r="111" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A111">
         <v>22037004</v>
       </c>
@@ -4403,14 +4694,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>种子-蓝莓</v>
       </c>
-      <c r="O111">
+      <c r="Q111">
         <v>22037104</v>
       </c>
-      <c r="P111">
+      <c r="R111">
         <v>10800</v>
       </c>
     </row>
-    <row r="112" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A112">
         <v>22037101</v>
       </c>
@@ -4418,11 +4709,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>作物-豌豆</v>
       </c>
-      <c r="C112">
+      <c r="E112">
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A113">
         <v>22037102</v>
       </c>
@@ -4430,14 +4721,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>作物-玉米</v>
       </c>
-      <c r="G113">
+      <c r="I113">
         <v>1</v>
       </c>
-      <c r="H113">
+      <c r="J113">
         <v>20</v>
       </c>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A114">
         <v>22037103</v>
       </c>
@@ -4445,11 +4736,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>作物-苹果</v>
       </c>
-      <c r="Q114">
+      <c r="S114">
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A115">
         <v>22037104</v>
       </c>
@@ -4457,50 +4748,71 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>作物-苹果</v>
       </c>
-      <c r="R115">
+      <c r="C115">
+        <v>1</v>
+      </c>
+      <c r="D115">
+        <v>15</v>
+      </c>
+      <c r="T115">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="X40:X72 O40:W62 X74:X87 J102:K104 O38:X39 N15:X21 N38:N62 M9:X14 A40:J87 M66:W87 C88:J103 C105:J115 M88:X115 M22:X37 N5:X8 N63:W65 K40:L115 C5:L39">
-    <cfRule type="containsBlanks" dxfId="7" priority="14">
+  <conditionalFormatting sqref="Z40:Z72 Q40:Y62 Z74:Z87 L102:M104 Q38:Z39 P15:Z21 P38:P62 O9:Z14 A40:B87 O66:Y87 E105:L115 O88:Z115 O22:Z37 P5:Z8 P63:Y65 M40:N115 E5:N39 E40:L103">
+    <cfRule type="containsBlanks" dxfId="10" priority="17">
       <formula>LEN(TRIM(A5))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X73">
-    <cfRule type="containsBlanks" dxfId="6" priority="8">
-      <formula>LEN(TRIM(X73))=0</formula>
+  <conditionalFormatting sqref="Z73">
+    <cfRule type="containsBlanks" dxfId="9" priority="11">
+      <formula>LEN(TRIM(Z73))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C104:K104">
-    <cfRule type="containsBlanks" dxfId="5" priority="6">
-      <formula>LEN(TRIM(C104))=0</formula>
+  <conditionalFormatting sqref="E104:M104">
+    <cfRule type="containsBlanks" dxfId="8" priority="9">
+      <formula>LEN(TRIM(E104))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M19:M21">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
-      <formula>LEN(TRIM(M19))=0</formula>
+  <conditionalFormatting sqref="O19:O21">
+    <cfRule type="containsBlanks" dxfId="7" priority="8">
+      <formula>LEN(TRIM(O19))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M15:M18">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
-      <formula>LEN(TRIM(M15))=0</formula>
+  <conditionalFormatting sqref="O15:O18">
+    <cfRule type="containsBlanks" dxfId="6" priority="7">
+      <formula>LEN(TRIM(O15))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N4:X4 C4:J4">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
-      <formula>LEN(TRIM(C4))=0</formula>
+  <conditionalFormatting sqref="P4:Z4 E4:L4">
+    <cfRule type="containsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M4">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+  <conditionalFormatting sqref="O4">
+    <cfRule type="containsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(O4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M4:N4">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(M4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4:L4">
+  <conditionalFormatting sqref="C5:D12 C16:D22 C39:D115">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(C5))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13:D15">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(C13))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23:D38">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(K4))=0</formula>
+      <formula>LEN(TRIM(C23))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
check the code of itemtypes
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/ItemConsumer.xlsx
+++ b/ConfigData/Xlsx/ItemConsumer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -1345,6 +1345,75 @@
   </cellStyles>
   <dxfs count="14">
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
@@ -1445,75 +1514,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1573,889 +1573,881 @@
         </row>
         <row r="5">
           <cell r="A5">
-            <v>22300002</v>
+            <v>22301201</v>
           </cell>
           <cell r="B5" t="str">
-            <v>穷奇召唤</v>
+            <v>蓝色卡包</v>
           </cell>
         </row>
         <row r="6">
           <cell r="A6">
-            <v>22301201</v>
+            <v>22301202</v>
           </cell>
           <cell r="B6" t="str">
-            <v>蓝色卡包</v>
+            <v>黄色卡包</v>
           </cell>
         </row>
         <row r="7">
           <cell r="A7">
-            <v>22301202</v>
+            <v>22301203</v>
           </cell>
           <cell r="B7" t="str">
-            <v>黄色卡包</v>
+            <v>红色卡包</v>
           </cell>
         </row>
         <row r="8">
           <cell r="A8">
-            <v>22301203</v>
+            <v>22301212</v>
           </cell>
           <cell r="B8" t="str">
-            <v>红色卡包</v>
+            <v>卡牌补给包(无)</v>
           </cell>
         </row>
         <row r="9">
           <cell r="A9">
-            <v>22301212</v>
+            <v>22301213</v>
           </cell>
           <cell r="B9" t="str">
-            <v>卡牌补给包(无)</v>
+            <v>卡牌补给包(水)</v>
           </cell>
         </row>
         <row r="10">
           <cell r="A10">
-            <v>22301213</v>
+            <v>22301214</v>
           </cell>
           <cell r="B10" t="str">
-            <v>卡牌补给包(水)</v>
+            <v>卡牌补给包(风)</v>
           </cell>
         </row>
         <row r="11">
           <cell r="A11">
-            <v>22301214</v>
+            <v>22301215</v>
           </cell>
           <cell r="B11" t="str">
-            <v>卡牌补给包(风)</v>
+            <v>卡牌补给包(地)</v>
           </cell>
         </row>
         <row r="12">
           <cell r="A12">
-            <v>22301215</v>
+            <v>22301216</v>
           </cell>
           <cell r="B12" t="str">
-            <v>卡牌补给包(地)</v>
+            <v>卡牌补给包(火)</v>
           </cell>
         </row>
         <row r="13">
           <cell r="A13">
-            <v>22301216</v>
+            <v>22301217</v>
           </cell>
           <cell r="B13" t="str">
-            <v>卡牌补给包(火)</v>
+            <v>卡牌补给包(光)</v>
           </cell>
         </row>
         <row r="14">
           <cell r="A14">
-            <v>22301217</v>
+            <v>22301218</v>
           </cell>
           <cell r="B14" t="str">
-            <v>卡牌补给包(光)</v>
+            <v>卡牌补给包(暗)</v>
           </cell>
         </row>
         <row r="15">
           <cell r="A15">
-            <v>22301218</v>
+            <v>22301221</v>
           </cell>
           <cell r="B15" t="str">
-            <v>卡牌补给包(暗)</v>
+            <v>卡牌补给包(生物)</v>
           </cell>
         </row>
         <row r="16">
           <cell r="A16">
-            <v>22301221</v>
+            <v>22301222</v>
           </cell>
           <cell r="B16" t="str">
-            <v>卡牌补给包(生物)</v>
+            <v>卡牌补给包(武器)</v>
           </cell>
         </row>
         <row r="17">
           <cell r="A17">
-            <v>22301222</v>
+            <v>22301223</v>
           </cell>
           <cell r="B17" t="str">
-            <v>卡牌补给包(武器)</v>
+            <v>卡牌补给包(法术)</v>
           </cell>
         </row>
         <row r="18">
           <cell r="A18">
-            <v>22301223</v>
+            <v>22301231</v>
           </cell>
           <cell r="B18" t="str">
-            <v>卡牌补给包(法术)</v>
+            <v>卡牌补给包(恶魔)</v>
           </cell>
         </row>
         <row r="19">
           <cell r="A19">
-            <v>22301231</v>
+            <v>22301232</v>
           </cell>
           <cell r="B19" t="str">
-            <v>卡牌补给包(恶魔)</v>
+            <v>卡牌补给包(机械)</v>
           </cell>
         </row>
         <row r="20">
           <cell r="A20">
-            <v>22301232</v>
+            <v>22301233</v>
           </cell>
           <cell r="B20" t="str">
-            <v>卡牌补给包(机械)</v>
+            <v>卡牌补给包(精灵)</v>
           </cell>
         </row>
         <row r="21">
           <cell r="A21">
-            <v>22301233</v>
+            <v>22301234</v>
           </cell>
           <cell r="B21" t="str">
-            <v>卡牌补给包(精灵)</v>
+            <v>卡牌补给包(昆虫)</v>
           </cell>
         </row>
         <row r="22">
           <cell r="A22">
-            <v>22301234</v>
+            <v>22301235</v>
           </cell>
           <cell r="B22" t="str">
-            <v>卡牌补给包(昆虫)</v>
+            <v>卡牌补给包(龙)</v>
           </cell>
         </row>
         <row r="23">
           <cell r="A23">
-            <v>22301235</v>
+            <v>22301236</v>
           </cell>
           <cell r="B23" t="str">
-            <v>卡牌补给包(龙)</v>
+            <v>卡牌补给包(鸟)</v>
           </cell>
         </row>
         <row r="24">
           <cell r="A24">
-            <v>22301236</v>
+            <v>22301237</v>
           </cell>
           <cell r="B24" t="str">
-            <v>卡牌补给包(鸟)</v>
+            <v>卡牌补给包(爬行)</v>
           </cell>
         </row>
         <row r="25">
           <cell r="A25">
-            <v>22301237</v>
+            <v>22301238</v>
           </cell>
           <cell r="B25" t="str">
-            <v>卡牌补给包(爬行)</v>
+            <v>卡牌补给包(人类)</v>
           </cell>
         </row>
         <row r="26">
           <cell r="A26">
-            <v>22301238</v>
+            <v>22301239</v>
           </cell>
           <cell r="B26" t="str">
-            <v>卡牌补给包(人类)</v>
+            <v>卡牌补给包(兽人)</v>
           </cell>
         </row>
         <row r="27">
           <cell r="A27">
-            <v>22301239</v>
+            <v>22301240</v>
           </cell>
           <cell r="B27" t="str">
-            <v>卡牌补给包(兽人)</v>
+            <v>卡牌补给包(亡灵)</v>
           </cell>
         </row>
         <row r="28">
           <cell r="A28">
-            <v>22301240</v>
+            <v>22301241</v>
           </cell>
           <cell r="B28" t="str">
-            <v>卡牌补给包(亡灵)</v>
+            <v>卡牌补给包(野兽)</v>
           </cell>
         </row>
         <row r="29">
           <cell r="A29">
-            <v>22301241</v>
+            <v>22301242</v>
           </cell>
           <cell r="B29" t="str">
-            <v>卡牌补给包(野兽)</v>
+            <v>卡牌补给包(鱼)</v>
           </cell>
         </row>
         <row r="30">
           <cell r="A30">
-            <v>22301242</v>
+            <v>22301243</v>
           </cell>
           <cell r="B30" t="str">
-            <v>卡牌补给包(鱼)</v>
+            <v>卡牌补给包(元素)</v>
           </cell>
         </row>
         <row r="31">
           <cell r="A31">
-            <v>22301243</v>
+            <v>22301244</v>
           </cell>
           <cell r="B31" t="str">
-            <v>卡牌补给包(元素)</v>
+            <v>卡牌补给包(植物)</v>
           </cell>
         </row>
         <row r="32">
           <cell r="A32">
-            <v>22301244</v>
+            <v>22301245</v>
           </cell>
           <cell r="B32" t="str">
-            <v>卡牌补给包(植物)</v>
+            <v>卡牌补给包(地精)</v>
           </cell>
         </row>
         <row r="33">
           <cell r="A33">
-            <v>22301245</v>
+            <v>22301246</v>
           </cell>
           <cell r="B33" t="str">
-            <v>卡牌补给包(地精)</v>
+            <v>卡牌补给包(石像)</v>
           </cell>
         </row>
         <row r="34">
           <cell r="A34">
-            <v>22301246</v>
+            <v>22301301</v>
           </cell>
           <cell r="B34" t="str">
-            <v>卡牌补给包(石像)</v>
+            <v>资源袋(绿)</v>
           </cell>
         </row>
         <row r="35">
           <cell r="A35">
-            <v>22301301</v>
+            <v>22301302</v>
           </cell>
           <cell r="B35" t="str">
-            <v>资源袋(绿)</v>
+            <v>资源袋(蓝)</v>
           </cell>
         </row>
         <row r="36">
           <cell r="A36">
-            <v>22301302</v>
+            <v>22301303</v>
           </cell>
           <cell r="B36" t="str">
-            <v>资源袋(蓝)</v>
+            <v>资源袋(红)</v>
           </cell>
         </row>
         <row r="37">
           <cell r="A37">
-            <v>22301303</v>
+            <v>22301304</v>
           </cell>
           <cell r="B37" t="str">
-            <v>资源袋(红)</v>
+            <v>资源袋(紫)</v>
           </cell>
         </row>
         <row r="38">
           <cell r="A38">
-            <v>22301304</v>
+            <v>22301305</v>
           </cell>
           <cell r="B38" t="str">
-            <v>资源袋(紫)</v>
+            <v>资源袋(灰)</v>
           </cell>
         </row>
         <row r="39">
           <cell r="A39">
-            <v>22301305</v>
+            <v>22301311</v>
           </cell>
           <cell r="B39" t="str">
-            <v>资源袋(灰)</v>
+            <v>素材袋</v>
           </cell>
         </row>
         <row r="40">
           <cell r="A40">
-            <v>22301311</v>
+            <v>22301312</v>
           </cell>
           <cell r="B40" t="str">
-            <v>素材袋</v>
+            <v>高级素材袋</v>
           </cell>
         </row>
         <row r="41">
           <cell r="A41">
-            <v>22301312</v>
+            <v>22301313</v>
           </cell>
           <cell r="B41" t="str">
-            <v>高级素材袋</v>
+            <v>特级素材袋</v>
           </cell>
         </row>
         <row r="42">
           <cell r="A42">
-            <v>22301313</v>
+            <v>22301314</v>
           </cell>
           <cell r="B42" t="str">
-            <v>特级素材袋</v>
+            <v>极品素材袋</v>
           </cell>
         </row>
         <row r="43">
           <cell r="A43">
-            <v>22301314</v>
+            <v>22301321</v>
           </cell>
           <cell r="B43" t="str">
-            <v>极品素材袋</v>
+            <v>素材袋(无)</v>
           </cell>
         </row>
         <row r="44">
           <cell r="A44">
-            <v>22301321</v>
+            <v>22301322</v>
           </cell>
           <cell r="B44" t="str">
-            <v>素材袋(无)</v>
+            <v>素材袋(水)</v>
           </cell>
         </row>
         <row r="45">
           <cell r="A45">
-            <v>22301322</v>
+            <v>22301323</v>
           </cell>
           <cell r="B45" t="str">
-            <v>素材袋(水)</v>
+            <v>素材袋(风)</v>
           </cell>
         </row>
         <row r="46">
           <cell r="A46">
-            <v>22301323</v>
+            <v>22301324</v>
           </cell>
           <cell r="B46" t="str">
-            <v>素材袋(风)</v>
+            <v>素材袋(火)</v>
           </cell>
         </row>
         <row r="47">
           <cell r="A47">
-            <v>22301324</v>
+            <v>22301325</v>
           </cell>
           <cell r="B47" t="str">
-            <v>素材袋(火)</v>
+            <v>素材袋(地)</v>
           </cell>
         </row>
         <row r="48">
           <cell r="A48">
-            <v>22301325</v>
+            <v>22301326</v>
           </cell>
           <cell r="B48" t="str">
-            <v>素材袋(地)</v>
+            <v>素材袋(光)</v>
           </cell>
         </row>
         <row r="49">
           <cell r="A49">
-            <v>22301326</v>
+            <v>22301327</v>
           </cell>
           <cell r="B49" t="str">
-            <v>素材袋(光)</v>
+            <v>素材袋(暗)</v>
           </cell>
         </row>
         <row r="50">
           <cell r="A50">
-            <v>22301327</v>
+            <v>22301331</v>
           </cell>
           <cell r="B50" t="str">
-            <v>素材袋(暗)</v>
+            <v>资源袋(恶魔)</v>
           </cell>
         </row>
         <row r="51">
           <cell r="A51">
-            <v>22301331</v>
+            <v>22301332</v>
           </cell>
           <cell r="B51" t="str">
-            <v>资源袋(恶魔)</v>
+            <v>资源袋(机械)</v>
           </cell>
         </row>
         <row r="52">
           <cell r="A52">
-            <v>22301332</v>
+            <v>22301333</v>
           </cell>
           <cell r="B52" t="str">
-            <v>资源袋(机械)</v>
+            <v>资源袋(精灵)</v>
           </cell>
         </row>
         <row r="53">
           <cell r="A53">
-            <v>22301333</v>
+            <v>22301334</v>
           </cell>
           <cell r="B53" t="str">
-            <v>资源袋(精灵)</v>
+            <v>资源袋(昆虫)</v>
           </cell>
         </row>
         <row r="54">
           <cell r="A54">
-            <v>22301334</v>
+            <v>22301335</v>
           </cell>
           <cell r="B54" t="str">
-            <v>资源袋(昆虫)</v>
+            <v>资源袋(龙)</v>
           </cell>
         </row>
         <row r="55">
           <cell r="A55">
-            <v>22301335</v>
+            <v>22301336</v>
           </cell>
           <cell r="B55" t="str">
-            <v>资源袋(龙)</v>
+            <v>资源袋(鸟)</v>
           </cell>
         </row>
         <row r="56">
           <cell r="A56">
-            <v>22301336</v>
+            <v>22301337</v>
           </cell>
           <cell r="B56" t="str">
-            <v>资源袋(鸟)</v>
+            <v>资源袋(爬行)</v>
           </cell>
         </row>
         <row r="57">
           <cell r="A57">
-            <v>22301337</v>
+            <v>22301338</v>
           </cell>
           <cell r="B57" t="str">
-            <v>资源袋(爬行)</v>
+            <v>资源袋(人类)</v>
           </cell>
         </row>
         <row r="58">
           <cell r="A58">
-            <v>22301338</v>
+            <v>22301339</v>
           </cell>
           <cell r="B58" t="str">
-            <v>资源袋(人类)</v>
+            <v>资源袋(兽人)</v>
           </cell>
         </row>
         <row r="59">
           <cell r="A59">
-            <v>22301339</v>
+            <v>22301340</v>
           </cell>
           <cell r="B59" t="str">
-            <v>资源袋(兽人)</v>
+            <v>资源袋(亡灵)</v>
           </cell>
         </row>
         <row r="60">
           <cell r="A60">
-            <v>22301340</v>
+            <v>22301341</v>
           </cell>
           <cell r="B60" t="str">
-            <v>资源袋(亡灵)</v>
+            <v>资源袋(野兽)</v>
           </cell>
         </row>
         <row r="61">
           <cell r="A61">
-            <v>22301341</v>
+            <v>22301342</v>
           </cell>
           <cell r="B61" t="str">
-            <v>资源袋(野兽)</v>
+            <v>资源袋(鱼)</v>
           </cell>
         </row>
         <row r="62">
           <cell r="A62">
-            <v>22301342</v>
+            <v>22301343</v>
           </cell>
           <cell r="B62" t="str">
-            <v>资源袋(鱼)</v>
+            <v>资源袋(元素)</v>
           </cell>
         </row>
         <row r="63">
           <cell r="A63">
-            <v>22301343</v>
+            <v>22301344</v>
           </cell>
           <cell r="B63" t="str">
-            <v>资源袋(元素)</v>
+            <v>资源袋(植物)</v>
           </cell>
         </row>
         <row r="64">
           <cell r="A64">
-            <v>22301344</v>
+            <v>22301345</v>
           </cell>
           <cell r="B64" t="str">
-            <v>资源袋(植物)</v>
+            <v>资源袋(地精)</v>
           </cell>
         </row>
         <row r="65">
           <cell r="A65">
-            <v>22301345</v>
+            <v>22301346</v>
           </cell>
           <cell r="B65" t="str">
-            <v>资源袋(地精)</v>
+            <v>资源袋(石像)</v>
           </cell>
         </row>
         <row r="66">
           <cell r="A66">
-            <v>22301346</v>
+            <v>22301401</v>
           </cell>
           <cell r="B66" t="str">
-            <v>资源袋(石像)</v>
+            <v>木材补给车</v>
           </cell>
         </row>
         <row r="67">
           <cell r="A67">
-            <v>22301401</v>
+            <v>22301402</v>
           </cell>
           <cell r="B67" t="str">
-            <v>木材补给车</v>
+            <v>矿石补给车</v>
           </cell>
         </row>
         <row r="68">
           <cell r="A68">
-            <v>22301402</v>
+            <v>22301403</v>
           </cell>
           <cell r="B68" t="str">
-            <v>矿石补给车</v>
+            <v>水银补给车</v>
           </cell>
         </row>
         <row r="69">
           <cell r="A69">
-            <v>22301403</v>
+            <v>22301404</v>
           </cell>
           <cell r="B69" t="str">
-            <v>水银补给车</v>
+            <v>红宝石补给车</v>
           </cell>
         </row>
         <row r="70">
           <cell r="A70">
-            <v>22301404</v>
+            <v>22301405</v>
           </cell>
           <cell r="B70" t="str">
-            <v>红宝石补给车</v>
+            <v>硫磺补给车</v>
           </cell>
         </row>
         <row r="71">
           <cell r="A71">
-            <v>22301405</v>
+            <v>22301406</v>
           </cell>
           <cell r="B71" t="str">
-            <v>硫磺补给车</v>
+            <v>水晶补给车</v>
           </cell>
         </row>
         <row r="72">
           <cell r="A72">
-            <v>22301406</v>
+            <v>22301407</v>
           </cell>
           <cell r="B72" t="str">
-            <v>水晶补给车</v>
+            <v>初始资源包</v>
           </cell>
         </row>
         <row r="73">
           <cell r="A73">
-            <v>22301407</v>
+            <v>22301408</v>
           </cell>
           <cell r="B73" t="str">
-            <v>初始资源包</v>
+            <v>金币</v>
           </cell>
         </row>
         <row r="74">
           <cell r="A74">
-            <v>22301408</v>
+            <v>22301501</v>
           </cell>
           <cell r="B74" t="str">
-            <v>金币</v>
+            <v>种子-豌豆</v>
           </cell>
         </row>
         <row r="75">
           <cell r="A75">
-            <v>22301501</v>
+            <v>22301502</v>
           </cell>
           <cell r="B75" t="str">
-            <v>种子-豌豆</v>
+            <v>种子-玉米</v>
           </cell>
         </row>
         <row r="76">
           <cell r="A76">
-            <v>22301502</v>
+            <v>22301503</v>
           </cell>
           <cell r="B76" t="str">
-            <v>种子-玉米</v>
+            <v>种子-苹果</v>
           </cell>
         </row>
         <row r="77">
           <cell r="A77">
-            <v>22301503</v>
+            <v>22301504</v>
           </cell>
           <cell r="B77" t="str">
-            <v>种子-苹果</v>
+            <v>种子-蓝莓</v>
           </cell>
         </row>
         <row r="78">
           <cell r="A78">
-            <v>22301504</v>
+            <v>22301605</v>
           </cell>
           <cell r="B78" t="str">
-            <v>种子-蓝莓</v>
+            <v>作物-豌豆</v>
           </cell>
         </row>
         <row r="79">
           <cell r="A79">
-            <v>22301605</v>
+            <v>22301606</v>
           </cell>
           <cell r="B79" t="str">
-            <v>作物-豌豆</v>
+            <v>作物-玉米</v>
           </cell>
         </row>
         <row r="80">
           <cell r="A80">
-            <v>22301606</v>
+            <v>22301607</v>
           </cell>
           <cell r="B80" t="str">
-            <v>作物-玉米</v>
+            <v>作物-苹果</v>
           </cell>
         </row>
         <row r="81">
           <cell r="A81">
-            <v>22301607</v>
+            <v>22302001</v>
           </cell>
           <cell r="B81" t="str">
-            <v>作物-苹果</v>
+            <v>小型魔法药剂</v>
           </cell>
         </row>
         <row r="82">
           <cell r="A82">
-            <v>22302001</v>
+            <v>22302002</v>
           </cell>
           <cell r="B82" t="str">
-            <v>小型魔法药剂</v>
+            <v>中型魔法药剂</v>
           </cell>
         </row>
         <row r="83">
           <cell r="A83">
-            <v>22302002</v>
+            <v>22302003</v>
           </cell>
           <cell r="B83" t="str">
-            <v>中型魔法药剂</v>
+            <v>大型魔法药剂</v>
           </cell>
         </row>
         <row r="84">
           <cell r="A84">
-            <v>22302003</v>
+            <v>22302004</v>
           </cell>
           <cell r="B84" t="str">
-            <v>大型魔法药剂</v>
+            <v>小型活力药剂</v>
           </cell>
         </row>
         <row r="85">
           <cell r="A85">
-            <v>22302004</v>
+            <v>22302005</v>
           </cell>
           <cell r="B85" t="str">
-            <v>小型活力药剂</v>
+            <v>中型活力药剂</v>
           </cell>
         </row>
         <row r="86">
           <cell r="A86">
-            <v>22302005</v>
+            <v>22302006</v>
           </cell>
           <cell r="B86" t="str">
-            <v>中型活力药剂</v>
+            <v>大型活力药剂</v>
           </cell>
         </row>
         <row r="87">
           <cell r="A87">
-            <v>22302006</v>
+            <v>22302007</v>
           </cell>
           <cell r="B87" t="str">
-            <v>大型活力药剂</v>
+            <v>小型体力药剂</v>
           </cell>
         </row>
         <row r="88">
           <cell r="A88">
-            <v>22302007</v>
+            <v>22302008</v>
           </cell>
           <cell r="B88" t="str">
-            <v>小型体力药剂</v>
+            <v>中型体力药剂</v>
           </cell>
         </row>
         <row r="89">
           <cell r="A89">
-            <v>22302008</v>
+            <v>22302009</v>
           </cell>
           <cell r="B89" t="str">
-            <v>中型体力药剂</v>
+            <v>大型体力药剂</v>
           </cell>
         </row>
         <row r="90">
           <cell r="A90">
-            <v>22302009</v>
+            <v>22302013</v>
           </cell>
           <cell r="B90" t="str">
-            <v>大型体力药剂</v>
+            <v>随机幻兽卡</v>
           </cell>
         </row>
         <row r="91">
           <cell r="A91">
-            <v>22302013</v>
+            <v>22302014</v>
           </cell>
           <cell r="B91" t="str">
-            <v>随机幻兽卡</v>
+            <v>随机武器卡</v>
           </cell>
         </row>
         <row r="92">
           <cell r="A92">
-            <v>22302014</v>
+            <v>22302015</v>
           </cell>
           <cell r="B92" t="str">
-            <v>随机武器卡</v>
+            <v>随机魔法卡</v>
           </cell>
         </row>
         <row r="93">
           <cell r="A93">
-            <v>22302015</v>
+            <v>22302016</v>
           </cell>
           <cell r="B93" t="str">
-            <v>随机魔法卡</v>
+            <v>符文-查姆</v>
           </cell>
         </row>
         <row r="94">
           <cell r="A94">
-            <v>22302016</v>
+            <v>22302017</v>
           </cell>
           <cell r="B94" t="str">
-            <v>符文-查姆</v>
+            <v>符文-普尔</v>
           </cell>
         </row>
         <row r="95">
           <cell r="A95">
-            <v>22302017</v>
+            <v>22302018</v>
           </cell>
           <cell r="B95" t="str">
-            <v>符文-普尔</v>
+            <v>符文-艾尔</v>
           </cell>
         </row>
         <row r="96">
           <cell r="A96">
-            <v>22302018</v>
+            <v>22302030</v>
           </cell>
           <cell r="B96" t="str">
-            <v>符文-艾尔</v>
+            <v>木质修理锤</v>
           </cell>
         </row>
         <row r="97">
           <cell r="A97">
-            <v>22302030</v>
+            <v>22302031</v>
           </cell>
           <cell r="B97" t="str">
-            <v>木质修理锤</v>
+            <v>钢铁修理锤</v>
           </cell>
         </row>
         <row r="98">
           <cell r="A98">
-            <v>22302031</v>
+            <v>22302032</v>
           </cell>
           <cell r="B98" t="str">
-            <v>钢铁修理锤</v>
+            <v>神圣修理锤</v>
           </cell>
         </row>
         <row r="99">
           <cell r="A99">
-            <v>22302032</v>
+            <v>22302101</v>
           </cell>
           <cell r="B99" t="str">
-            <v>神圣修理锤</v>
+            <v>经验之书</v>
           </cell>
         </row>
         <row r="100">
           <cell r="A100">
-            <v>22302101</v>
+            <v>22302102</v>
           </cell>
           <cell r="B100" t="str">
-            <v>经验之书</v>
+            <v>能量之书</v>
           </cell>
         </row>
         <row r="101">
           <cell r="A101">
-            <v>22302102</v>
+            <v>22302103</v>
           </cell>
           <cell r="B101" t="str">
-            <v>能量之书</v>
+            <v>攻速药水</v>
           </cell>
         </row>
         <row r="102">
           <cell r="A102">
-            <v>22302103</v>
+            <v>22302104</v>
           </cell>
           <cell r="B102" t="str">
-            <v>攻速药水</v>
+            <v>守护药水</v>
           </cell>
         </row>
         <row r="103">
           <cell r="A103">
-            <v>22302104</v>
+            <v>22302105</v>
           </cell>
           <cell r="B103" t="str">
-            <v>守护药水</v>
+            <v>法术药水</v>
           </cell>
         </row>
         <row r="104">
           <cell r="A104">
-            <v>22302105</v>
+            <v>22302106</v>
           </cell>
           <cell r="B104" t="str">
-            <v>法术药水</v>
+            <v>技巧药水</v>
           </cell>
         </row>
         <row r="105">
           <cell r="A105">
-            <v>22302106</v>
+            <v>22302107</v>
           </cell>
           <cell r="B105" t="str">
-            <v>技巧药水</v>
+            <v>速度药水</v>
           </cell>
         </row>
         <row r="106">
           <cell r="A106">
-            <v>22302107</v>
+            <v>22302108</v>
           </cell>
           <cell r="B106" t="str">
-            <v>速度药水</v>
+            <v>幸运药水</v>
           </cell>
         </row>
         <row r="107">
           <cell r="A107">
-            <v>22302108</v>
+            <v>22302109</v>
           </cell>
           <cell r="B107" t="str">
-            <v>幸运药水</v>
+            <v>暴击药水</v>
           </cell>
         </row>
         <row r="108">
           <cell r="A108">
-            <v>22302109</v>
+            <v>22302110</v>
           </cell>
           <cell r="B108" t="str">
-            <v>暴击药水</v>
+            <v>饼干</v>
           </cell>
         </row>
         <row r="109">
           <cell r="A109">
-            <v>22302110</v>
+            <v>22302111</v>
           </cell>
           <cell r="B109" t="str">
-            <v>饼干</v>
+            <v>红色胶囊</v>
           </cell>
         </row>
         <row r="110">
           <cell r="A110">
-            <v>22302111</v>
+            <v>22302112</v>
           </cell>
           <cell r="B110" t="str">
-            <v>红色胶囊</v>
+            <v>蓝色胶囊</v>
           </cell>
         </row>
         <row r="111">
           <cell r="A111">
-            <v>22302112</v>
+            <v>22302113</v>
           </cell>
           <cell r="B111" t="str">
-            <v>蓝色胶囊</v>
+            <v>水晶球</v>
           </cell>
         </row>
         <row r="112">
           <cell r="A112">
-            <v>22302113</v>
+            <v>22302114</v>
           </cell>
           <cell r="B112" t="str">
-            <v>水晶球</v>
+            <v>坐骑黑豹</v>
           </cell>
         </row>
         <row r="113">
           <cell r="A113">
-            <v>22302114</v>
+            <v>22302115</v>
           </cell>
           <cell r="B113" t="str">
-            <v>坐骑黑豹</v>
+            <v>坐骑鹰</v>
           </cell>
         </row>
         <row r="114">
           <cell r="A114">
-            <v>22302115</v>
+            <v>22302116</v>
           </cell>
           <cell r="B114" t="str">
-            <v>坐骑鹰</v>
-          </cell>
-        </row>
-        <row r="115">
-          <cell r="A115">
-            <v>22302116</v>
-          </cell>
-          <cell r="B115" t="str">
             <v>坐骑传送器</v>
           </cell>
         </row>
@@ -2466,17 +2458,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:Z114" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:Z114" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A3:Z114"/>
   <sortState ref="A4:Z114">
     <sortCondition ref="A3:A114"/>
   </sortState>
   <tableColumns count="26">
     <tableColumn id="1" name="Id"/>
-    <tableColumn id="2" name="~Name" dataDxfId="12">
+    <tableColumn id="2" name="~Name" dataDxfId="1">
       <calculatedColumnFormula>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="CdGroup" dataDxfId="11"/>
+    <tableColumn id="16" name="CdGroup" dataDxfId="0"/>
     <tableColumn id="25" name="CdTime"/>
     <tableColumn id="3" name="GainExp"/>
     <tableColumn id="4" name="GainFood"/>
@@ -2828,8 +2820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="O109" sqref="O109"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3091,11 +3083,11 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A4">
-        <v>22300002</v>
-      </c>
-      <c r="B4" s="10" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>穷奇召唤</v>
+        <v>22200001</v>
+      </c>
+      <c r="B4" s="10" t="e">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>#N/A</v>
       </c>
       <c r="C4" s="14">
         <v>4</v>
@@ -4739,57 +4731,57 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="Z40:Z72 Q40:Y62 Z74:Z87 L102:M104 Q38:Z39 P15:Z21 P38:P62 O9:Z14 O66:Y87 E105:L114 O88:Z114 O22:Z37 P5:Z8 P63:Y65 M40:N114 E5:N39 E40:L103 B40:B87">
-    <cfRule type="containsBlanks" dxfId="10" priority="17">
+    <cfRule type="containsBlanks" dxfId="13" priority="17">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z73">
-    <cfRule type="containsBlanks" dxfId="9" priority="11">
+    <cfRule type="containsBlanks" dxfId="12" priority="11">
       <formula>LEN(TRIM(Z73))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E104:M104">
-    <cfRule type="containsBlanks" dxfId="8" priority="9">
+    <cfRule type="containsBlanks" dxfId="11" priority="9">
       <formula>LEN(TRIM(E104))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O19:O21">
-    <cfRule type="containsBlanks" dxfId="7" priority="8">
+    <cfRule type="containsBlanks" dxfId="10" priority="8">
       <formula>LEN(TRIM(O19))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O15:O18">
-    <cfRule type="containsBlanks" dxfId="6" priority="7">
+    <cfRule type="containsBlanks" dxfId="9" priority="7">
       <formula>LEN(TRIM(O15))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:Z4 E4:L4">
-    <cfRule type="containsBlanks" dxfId="5" priority="6">
+    <cfRule type="containsBlanks" dxfId="8" priority="6">
       <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
+    <cfRule type="containsBlanks" dxfId="7" priority="5">
       <formula>LEN(TRIM(O4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:N4">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="6" priority="4">
       <formula>LEN(TRIM(M4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:D12 C16:D22 C39:D114">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+    <cfRule type="containsBlanks" dxfId="5" priority="3">
       <formula>LEN(TRIM(C5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:D15">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="4" priority="2">
       <formula>LEN(TRIM(C13))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:D52">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="3" priority="1">
       <formula>LEN(TRIM(C23))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
remove npc and gift relative codes
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/ItemConsumer.xlsx
+++ b/ConfigData/Xlsx/ItemConsumer.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="158">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -567,6 +567,37 @@
   </si>
   <si>
     <t>cd组</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t>礼包内物品</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemCount</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string[]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int[]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>道具数量</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>xiaoxingmofayaoji;zhongxingmofayaoji;chushiziyuanbao;suijihuanshouka;suijiwuqika;suijimofaka</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>5;5;1;5;3;3</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -574,7 +605,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -760,6 +791,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -979,7 +1019,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1114,6 +1154,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1243,7 +1294,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1297,6 +1348,18 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1344,75 +1407,6 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="14">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1514,6 +1508,75 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2458,17 +2521,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:Z114" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A3:Z114"/>
-  <sortState ref="A4:Z114">
-    <sortCondition ref="A3:A114"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:AB115" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A3:AB115"/>
+  <sortState ref="A4:Z115">
+    <sortCondition ref="A3:A115"/>
   </sortState>
-  <tableColumns count="26">
+  <tableColumns count="28">
     <tableColumn id="1" name="Id"/>
-    <tableColumn id="2" name="~Name" dataDxfId="1">
+    <tableColumn id="2" name="~Name" dataDxfId="12">
       <calculatedColumnFormula>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="CdGroup" dataDxfId="0"/>
+    <tableColumn id="16" name="CdGroup" dataDxfId="11"/>
     <tableColumn id="25" name="CdTime"/>
     <tableColumn id="3" name="GainExp"/>
     <tableColumn id="4" name="GainFood"/>
@@ -2492,6 +2555,8 @@
     <tableColumn id="17" name="HolyWord"/>
     <tableColumn id="19" name="AddTowerHp"/>
     <tableColumn id="18" name="AttrAddAfterSummon"/>
+    <tableColumn id="27" name="Items"/>
+    <tableColumn id="28" name="ItemCount"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2818,10 +2883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z114"/>
+  <dimension ref="A1:AB115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="AA5" sqref="AA5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2839,9 +2904,10 @@
     <col min="17" max="17" width="8.625" customWidth="1"/>
     <col min="18" max="18" width="6.625" customWidth="1"/>
     <col min="19" max="26" width="7.375" customWidth="1"/>
+    <col min="27" max="27" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="77.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:28" ht="77.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
@@ -2920,8 +2986,14 @@
       <c r="Z1" s="12" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="AA1" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB1" s="21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3000,8 +3072,14 @@
       <c r="Z2" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="AA2" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB2" s="18" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -3080,8 +3158,14 @@
       <c r="Z3" s="8" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="AA3" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="AB3" s="19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>22200001</v>
       </c>
@@ -3102,169 +3186,171 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A5">
+        <v>22300001</v>
+      </c>
+      <c r="B5" s="10" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>新手礼包</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="AA5" t="s">
+        <v>156</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A6">
         <v>22301311</v>
       </c>
-      <c r="B5" s="10" t="str">
+      <c r="B6" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>素材袋</v>
       </c>
-      <c r="O5" s="13" t="s">
+      <c r="O6" s="13" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A6">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A7">
         <v>22301312</v>
       </c>
-      <c r="B6" s="10" t="str">
+      <c r="B7" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>高级素材袋</v>
       </c>
-      <c r="O6" s="13" t="s">
+      <c r="O7" s="13" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A7">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A8">
         <v>22301313</v>
       </c>
-      <c r="B7" s="10" t="str">
+      <c r="B8" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>特级素材袋</v>
       </c>
-      <c r="O7" s="13" t="s">
+      <c r="O8" s="13" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A8">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A9">
         <v>22301314</v>
       </c>
-      <c r="B8" s="10" t="str">
+      <c r="B9" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>极品素材袋</v>
       </c>
-      <c r="O8" s="13" t="s">
+      <c r="O9" s="13" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A9">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A10">
         <v>22301201</v>
       </c>
-      <c r="B9" s="9" t="str">
+      <c r="B10" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>蓝色卡包</v>
-      </c>
-      <c r="M9" t="s">
-        <v>34</v>
-      </c>
-      <c r="N9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A10">
-        <v>22301202</v>
-      </c>
-      <c r="B10" s="9" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>黄色卡包</v>
       </c>
       <c r="M10" t="s">
         <v>34</v>
       </c>
       <c r="N10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.15">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A11">
-        <v>22301203</v>
+        <v>22301202</v>
       </c>
       <c r="B11" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>红色卡包</v>
+        <v>黄色卡包</v>
       </c>
       <c r="M11" t="s">
         <v>34</v>
       </c>
       <c r="N11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>22301203</v>
+      </c>
+      <c r="B12" s="9" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>红色卡包</v>
+      </c>
+      <c r="M12" t="s">
+        <v>34</v>
+      </c>
+      <c r="N12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A12">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A13">
         <v>22301212</v>
       </c>
-      <c r="B12" s="9" t="str">
+      <c r="B13" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(无)</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M13" t="s">
         <v>27</v>
-      </c>
-      <c r="N12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A13">
-        <v>22301213</v>
-      </c>
-      <c r="B13" s="9" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(水)</v>
-      </c>
-      <c r="M13" t="s">
-        <v>28</v>
       </c>
       <c r="N13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>22301214</v>
+        <v>22301213</v>
       </c>
       <c r="B14" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(风)</v>
+        <v>卡牌补给包(水)</v>
       </c>
       <c r="M14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>22301215</v>
+        <v>22301214</v>
       </c>
       <c r="B15" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(地)</v>
+        <v>卡牌补给包(风)</v>
       </c>
       <c r="M15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>22301216</v>
+        <v>22301215</v>
       </c>
       <c r="B16" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(火)</v>
+        <v>卡牌补给包(地)</v>
       </c>
       <c r="M16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N16" t="s">
         <v>35</v>
@@ -3272,14 +3358,14 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>22301217</v>
+        <v>22301216</v>
       </c>
       <c r="B17" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(光)</v>
+        <v>卡牌补给包(火)</v>
       </c>
       <c r="M17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N17" t="s">
         <v>35</v>
@@ -3287,14 +3373,14 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>22301218</v>
+        <v>22301217</v>
       </c>
       <c r="B18" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(暗)</v>
+        <v>卡牌补给包(光)</v>
       </c>
       <c r="M18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N18" t="s">
         <v>35</v>
@@ -3302,14 +3388,14 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>22301221</v>
+        <v>22301218</v>
       </c>
       <c r="B19" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(生物)</v>
+        <v>卡牌补给包(暗)</v>
       </c>
       <c r="M19" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="N19" t="s">
         <v>35</v>
@@ -3317,14 +3403,14 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>22301222</v>
+        <v>22301221</v>
       </c>
       <c r="B20" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(武器)</v>
+        <v>卡牌补给包(生物)</v>
       </c>
       <c r="M20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N20" t="s">
         <v>35</v>
@@ -3332,14 +3418,14 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A21">
-        <v>22301223</v>
+        <v>22301222</v>
       </c>
       <c r="B21" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(法术)</v>
+        <v>卡牌补给包(武器)</v>
       </c>
       <c r="M21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N21" t="s">
         <v>35</v>
@@ -3347,737 +3433,734 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A22">
-        <v>22301231</v>
-      </c>
-      <c r="B22" s="10" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(恶魔)</v>
+        <v>22301223</v>
+      </c>
+      <c r="B22" s="9" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>卡牌补给包(法术)</v>
       </c>
       <c r="M22" t="s">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="N22" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>22301232</v>
+        <v>22301231</v>
       </c>
       <c r="B23" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(机械)</v>
+        <v>卡牌补给包(恶魔)</v>
       </c>
       <c r="M23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A24">
-        <v>22301233</v>
+        <v>22301232</v>
       </c>
       <c r="B24" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(精灵)</v>
+        <v>卡牌补给包(机械)</v>
       </c>
       <c r="M24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>22301234</v>
+        <v>22301233</v>
       </c>
       <c r="B25" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(昆虫)</v>
+        <v>卡牌补给包(精灵)</v>
       </c>
       <c r="M25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>22301235</v>
+        <v>22301234</v>
       </c>
       <c r="B26" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(龙)</v>
+        <v>卡牌补给包(昆虫)</v>
       </c>
       <c r="M26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>22301236</v>
+        <v>22301235</v>
       </c>
       <c r="B27" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(鸟)</v>
+        <v>卡牌补给包(龙)</v>
       </c>
       <c r="M27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>22301237</v>
+        <v>22301236</v>
       </c>
       <c r="B28" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(爬行)</v>
+        <v>卡牌补给包(鸟)</v>
       </c>
       <c r="M28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A29">
-        <v>22301238</v>
+        <v>22301237</v>
       </c>
       <c r="B29" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(人类)</v>
+        <v>卡牌补给包(爬行)</v>
       </c>
       <c r="M29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A30">
-        <v>22301239</v>
+        <v>22301238</v>
       </c>
       <c r="B30" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(兽人)</v>
+        <v>卡牌补给包(人类)</v>
       </c>
       <c r="M30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A31">
-        <v>22301240</v>
+        <v>22301239</v>
       </c>
       <c r="B31" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(亡灵)</v>
+        <v>卡牌补给包(兽人)</v>
       </c>
       <c r="M31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A32">
-        <v>22301241</v>
+        <v>22301240</v>
       </c>
       <c r="B32" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(野兽)</v>
+        <v>卡牌补给包(亡灵)</v>
       </c>
       <c r="M32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A33">
-        <v>22301242</v>
+        <v>22301241</v>
       </c>
       <c r="B33" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(鱼)</v>
+        <v>卡牌补给包(野兽)</v>
       </c>
       <c r="M33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A34">
-        <v>22301243</v>
+        <v>22301242</v>
       </c>
       <c r="B34" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(元素)</v>
+        <v>卡牌补给包(鱼)</v>
       </c>
       <c r="M34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A35">
-        <v>22301244</v>
+        <v>22301243</v>
       </c>
       <c r="B35" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(植物)</v>
+        <v>卡牌补给包(元素)</v>
       </c>
       <c r="M35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A36">
-        <v>22301245</v>
+        <v>22301244</v>
       </c>
       <c r="B36" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(地精)</v>
+        <v>卡牌补给包(植物)</v>
       </c>
       <c r="M36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A37">
-        <v>22301246</v>
+        <v>22301245</v>
       </c>
       <c r="B37" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>卡牌补给包(石像)</v>
+        <v>卡牌补给包(地精)</v>
       </c>
       <c r="M37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A38">
-        <v>22301301</v>
+        <v>22301246</v>
       </c>
       <c r="B38" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(绿)</v>
-      </c>
-      <c r="O38" s="13" t="s">
-        <v>115</v>
+        <v>卡牌补给包(石像)</v>
+      </c>
+      <c r="M38" t="s">
+        <v>107</v>
+      </c>
+      <c r="N38" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A39">
-        <v>22301302</v>
+        <v>22301301</v>
       </c>
       <c r="B39" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(蓝)</v>
-      </c>
-      <c r="O39" s="9" t="s">
-        <v>116</v>
+        <v>资源袋(绿)</v>
+      </c>
+      <c r="O39" s="13" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A40">
-        <v>22301303</v>
+        <v>22301302</v>
       </c>
       <c r="B40" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(红)</v>
-      </c>
-      <c r="O40" t="s">
-        <v>117</v>
+        <v>资源袋(蓝)</v>
+      </c>
+      <c r="O40" s="9" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A41">
-        <v>22301304</v>
+        <v>22301303</v>
       </c>
       <c r="B41" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(紫)</v>
+        <v>资源袋(红)</v>
       </c>
       <c r="O41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A42">
-        <v>22301305</v>
+        <v>22301304</v>
       </c>
       <c r="B42" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(灰)</v>
+        <v>资源袋(紫)</v>
       </c>
       <c r="O42" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A43">
-        <v>22301321</v>
+        <v>22301305</v>
       </c>
       <c r="B43" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>素材袋(无)</v>
-      </c>
-      <c r="O43" s="14" t="s">
-        <v>120</v>
+        <v>资源袋(灰)</v>
+      </c>
+      <c r="O43" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A44">
-        <v>22301322</v>
+        <v>22301321</v>
       </c>
       <c r="B44" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>素材袋(水)</v>
+        <v>素材袋(无)</v>
       </c>
       <c r="O44" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A45">
-        <v>22301323</v>
+        <v>22301322</v>
       </c>
       <c r="B45" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>素材袋(风)</v>
+        <v>素材袋(水)</v>
       </c>
       <c r="O45" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A46">
-        <v>22301324</v>
+        <v>22301323</v>
       </c>
       <c r="B46" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>素材袋(火)</v>
+        <v>素材袋(风)</v>
       </c>
       <c r="O46" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A47">
-        <v>22301325</v>
+        <v>22301324</v>
       </c>
       <c r="B47" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>素材袋(地)</v>
+        <v>素材袋(火)</v>
       </c>
       <c r="O47" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A48">
-        <v>22301326</v>
+        <v>22301325</v>
       </c>
       <c r="B48" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>素材袋(光)</v>
+        <v>素材袋(地)</v>
       </c>
       <c r="O48" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A49">
-        <v>22301327</v>
+        <v>22301326</v>
       </c>
       <c r="B49" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>素材袋(暗)</v>
-      </c>
-      <c r="O49" s="10" t="s">
-        <v>126</v>
+        <v>素材袋(光)</v>
+      </c>
+      <c r="O49" s="14" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A50">
-        <v>22301331</v>
+        <v>22301327</v>
       </c>
       <c r="B50" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(恶魔)</v>
-      </c>
-      <c r="O50" s="9" t="s">
-        <v>127</v>
+        <v>素材袋(暗)</v>
+      </c>
+      <c r="O50" s="10" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A51">
-        <v>22301332</v>
+        <v>22301331</v>
       </c>
       <c r="B51" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(机械)</v>
+        <v>资源袋(恶魔)</v>
       </c>
       <c r="O51" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A52">
-        <v>22301333</v>
+        <v>22301332</v>
       </c>
       <c r="B52" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(精灵)</v>
+        <v>资源袋(机械)</v>
       </c>
       <c r="O52" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A53">
-        <v>22301334</v>
+        <v>22301333</v>
       </c>
       <c r="B53" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(昆虫)</v>
+        <v>资源袋(精灵)</v>
       </c>
       <c r="O53" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A54">
-        <v>22301335</v>
+        <v>22301334</v>
       </c>
       <c r="B54" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(龙)</v>
+        <v>资源袋(昆虫)</v>
       </c>
       <c r="O54" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A55">
-        <v>22301336</v>
+        <v>22301335</v>
       </c>
       <c r="B55" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(鸟)</v>
+        <v>资源袋(龙)</v>
       </c>
       <c r="O55" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A56">
-        <v>22301337</v>
+        <v>22301336</v>
       </c>
       <c r="B56" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(爬行)</v>
+        <v>资源袋(鸟)</v>
       </c>
       <c r="O56" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A57">
-        <v>22301338</v>
+        <v>22301337</v>
       </c>
       <c r="B57" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(人类)</v>
+        <v>资源袋(爬行)</v>
       </c>
       <c r="O57" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A58">
-        <v>22301339</v>
+        <v>22301338</v>
       </c>
       <c r="B58" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(兽人)</v>
+        <v>资源袋(人类)</v>
       </c>
       <c r="O58" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A59">
-        <v>22301340</v>
+        <v>22301339</v>
       </c>
       <c r="B59" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(亡灵)</v>
+        <v>资源袋(兽人)</v>
       </c>
       <c r="O59" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A60">
-        <v>22301341</v>
+        <v>22301340</v>
       </c>
       <c r="B60" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(野兽)</v>
+        <v>资源袋(亡灵)</v>
       </c>
       <c r="O60" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A61">
-        <v>22301342</v>
+        <v>22301341</v>
       </c>
       <c r="B61" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(鱼)</v>
+        <v>资源袋(野兽)</v>
       </c>
       <c r="O61" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A62">
-        <v>22301343</v>
+        <v>22301342</v>
       </c>
       <c r="B62" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(元素)</v>
+        <v>资源袋(鱼)</v>
       </c>
       <c r="O62" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A63">
-        <v>22301344</v>
+        <v>22301343</v>
       </c>
       <c r="B63" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>资源袋(植物)</v>
+        <v>资源袋(元素)</v>
       </c>
       <c r="O63" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A64">
+        <v>22301344</v>
+      </c>
+      <c r="B64" s="10" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>资源袋(植物)</v>
+      </c>
+      <c r="O64" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A65">
         <v>22301345</v>
       </c>
-      <c r="B64" s="10" t="str">
+      <c r="B65" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(地精)</v>
       </c>
-      <c r="O64" s="9" t="s">
+      <c r="O65" s="9" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A65">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A66">
         <v>22301346</v>
       </c>
-      <c r="B65" s="10" t="str">
+      <c r="B66" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(石像)</v>
       </c>
-      <c r="O65" s="9" t="s">
+      <c r="O66" s="9" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A66">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A67">
         <v>22301401</v>
       </c>
-      <c r="B66" s="9" t="str">
+      <c r="B67" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>木材补给车</v>
       </c>
-      <c r="I66">
+      <c r="I67">
         <v>2</v>
-      </c>
-      <c r="J66">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A67">
-        <v>22301402</v>
-      </c>
-      <c r="B67" s="9" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>矿石补给车</v>
-      </c>
-      <c r="I67">
-        <v>3</v>
       </c>
       <c r="J67">
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A68">
+        <v>22301402</v>
+      </c>
+      <c r="B68" s="9" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>矿石补给车</v>
+      </c>
+      <c r="I68">
+        <v>3</v>
+      </c>
+      <c r="J68">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A69">
         <v>22301403</v>
       </c>
-      <c r="B68" s="9" t="str">
+      <c r="B69" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>水银补给车</v>
       </c>
-      <c r="I68">
+      <c r="I69">
         <v>4</v>
-      </c>
-      <c r="J68">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A69">
-        <v>22301404</v>
-      </c>
-      <c r="B69" s="9" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>红宝石补给车</v>
-      </c>
-      <c r="I69">
-        <v>5</v>
       </c>
       <c r="J69">
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A70">
-        <v>22301405</v>
+        <v>22301404</v>
       </c>
       <c r="B70" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>硫磺补给车</v>
+        <v>红宝石补给车</v>
       </c>
       <c r="I70">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J70">
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A71">
-        <v>22301406</v>
+        <v>22301405</v>
       </c>
       <c r="B71" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>水晶补给车</v>
+        <v>硫磺补给车</v>
       </c>
       <c r="I71">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J71">
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A72">
+        <v>22301406</v>
+      </c>
+      <c r="B72" s="9" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>水晶补给车</v>
+      </c>
+      <c r="I72">
+        <v>7</v>
+      </c>
+      <c r="J72">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A73">
         <v>22301407</v>
       </c>
-      <c r="B72" s="9" t="str">
+      <c r="B73" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>初始资源包</v>
-      </c>
-      <c r="I72">
-        <v>1</v>
-      </c>
-      <c r="J72">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A73">
-        <v>22301408</v>
-      </c>
-      <c r="B73" s="9" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>金币</v>
       </c>
       <c r="I73">
         <v>1</v>
       </c>
       <c r="J73">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A74">
+        <v>22301408</v>
+      </c>
+      <c r="B74" s="9" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>金币</v>
+      </c>
+      <c r="I74">
+        <v>1</v>
+      </c>
+      <c r="J74">
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A74">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A75">
         <v>22302001</v>
       </c>
-      <c r="B74" s="9" t="str">
+      <c r="B75" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>小型魔法药剂</v>
       </c>
-      <c r="T74">
+      <c r="T75">
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A75">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A76">
         <v>22302002</v>
       </c>
-      <c r="B75" s="9" t="str">
+      <c r="B76" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>中型魔法药剂</v>
-      </c>
-      <c r="C75">
-        <v>2</v>
-      </c>
-      <c r="D75">
-        <v>15</v>
-      </c>
-      <c r="T75">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A76">
-        <v>22302003</v>
-      </c>
-      <c r="B76" s="9" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>大型魔法药剂</v>
       </c>
       <c r="C76">
         <v>2</v>
@@ -4086,16 +4169,16 @@
         <v>15</v>
       </c>
       <c r="T76">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A77">
-        <v>22302004</v>
+        <v>22302003</v>
       </c>
       <c r="B77" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>小型活力药剂</v>
+        <v>大型魔法药剂</v>
       </c>
       <c r="C77">
         <v>2</v>
@@ -4103,35 +4186,35 @@
       <c r="D77">
         <v>15</v>
       </c>
-      <c r="S77">
+      <c r="T77">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A78">
+        <v>22302004</v>
+      </c>
+      <c r="B78" s="9" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>小型活力药剂</v>
+      </c>
+      <c r="C78">
         <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A78">
-        <v>22302005</v>
-      </c>
-      <c r="B78" s="9" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>中型活力药剂</v>
-      </c>
-      <c r="C78">
-        <v>3</v>
       </c>
       <c r="D78">
         <v>15</v>
       </c>
       <c r="S78">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A79">
-        <v>22302006</v>
+        <v>22302005</v>
       </c>
       <c r="B79" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>大型活力药剂</v>
+        <v>中型活力药剂</v>
       </c>
       <c r="C79">
         <v>3</v>
@@ -4140,16 +4223,16 @@
         <v>15</v>
       </c>
       <c r="S79">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A80">
-        <v>22302007</v>
+        <v>22302006</v>
       </c>
       <c r="B80" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>小型体力药剂</v>
+        <v>大型活力药剂</v>
       </c>
       <c r="C80">
         <v>3</v>
@@ -4157,35 +4240,35 @@
       <c r="D80">
         <v>15</v>
       </c>
-      <c r="U80">
-        <v>2</v>
+      <c r="S80">
+        <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A81">
-        <v>22302008</v>
+        <v>22302007</v>
       </c>
       <c r="B81" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>中型体力药剂</v>
+        <v>小型体力药剂</v>
       </c>
       <c r="C81">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D81">
         <v>15</v>
       </c>
       <c r="U81">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A82">
-        <v>22302009</v>
+        <v>22302008</v>
       </c>
       <c r="B82" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>大型体力药剂</v>
+        <v>中型体力药剂</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -4194,16 +4277,16 @@
         <v>15</v>
       </c>
       <c r="U82">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A83">
-        <v>22302013</v>
+        <v>22302009</v>
       </c>
       <c r="B83" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>随机幻兽卡</v>
+        <v>大型体力药剂</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -4211,17 +4294,17 @@
       <c r="D83">
         <v>15</v>
       </c>
-      <c r="W83">
-        <v>1</v>
+      <c r="U83">
+        <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A84">
-        <v>22302014</v>
+        <v>22302013</v>
       </c>
       <c r="B84" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>随机武器卡</v>
+        <v>随机幻兽卡</v>
       </c>
       <c r="C84">
         <v>1</v>
@@ -4230,34 +4313,34 @@
         <v>15</v>
       </c>
       <c r="W84">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A85">
-        <v>22302015</v>
+        <v>22302014</v>
       </c>
       <c r="B85" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>随机魔法卡</v>
+        <v>随机武器卡</v>
       </c>
       <c r="C85">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D85">
         <v>15</v>
       </c>
       <c r="W85">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A86">
-        <v>22302016</v>
+        <v>22302015</v>
       </c>
       <c r="B86" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>符文-查姆</v>
+        <v>随机魔法卡</v>
       </c>
       <c r="C86">
         <v>4</v>
@@ -4265,17 +4348,17 @@
       <c r="D86">
         <v>15</v>
       </c>
-      <c r="V86">
-        <v>9999</v>
+      <c r="W86">
+        <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A87">
-        <v>22302017</v>
+        <v>22302016</v>
       </c>
       <c r="B87" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>符文-普尔</v>
+        <v>符文-查姆</v>
       </c>
       <c r="C87">
         <v>4</v>
@@ -4284,16 +4367,16 @@
         <v>15</v>
       </c>
       <c r="V87">
-        <v>100</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A88">
-        <v>22302018</v>
+        <v>22302017</v>
       </c>
       <c r="B88" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>符文-艾尔</v>
+        <v>符文-普尔</v>
       </c>
       <c r="C88">
         <v>4</v>
@@ -4301,17 +4384,17 @@
       <c r="D88">
         <v>15</v>
       </c>
-      <c r="X88" t="s">
-        <v>45</v>
+      <c r="V88">
+        <v>100</v>
       </c>
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A89">
-        <v>22302030</v>
-      </c>
-      <c r="B89" s="13" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>木质修理锤</v>
+        <v>22302018</v>
+      </c>
+      <c r="B89" s="9" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>符文-艾尔</v>
       </c>
       <c r="C89">
         <v>4</v>
@@ -4319,35 +4402,35 @@
       <c r="D89">
         <v>15</v>
       </c>
-      <c r="Y89">
-        <v>200</v>
+      <c r="X89" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A90">
-        <v>22302031</v>
+        <v>22302030</v>
       </c>
       <c r="B90" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>钢铁修理锤</v>
+        <v>木质修理锤</v>
       </c>
       <c r="C90">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D90">
         <v>15</v>
       </c>
       <c r="Y90">
-        <v>500</v>
+        <v>200</v>
       </c>
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A91">
-        <v>22302032</v>
+        <v>22302031</v>
       </c>
       <c r="B91" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>神圣修理锤</v>
+        <v>钢铁修理锤</v>
       </c>
       <c r="C91">
         <v>1</v>
@@ -4356,16 +4439,16 @@
         <v>15</v>
       </c>
       <c r="Y91">
-        <v>1000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="92" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A92">
-        <v>22302101</v>
+        <v>22302032</v>
       </c>
       <c r="B92" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>经验之书</v>
+        <v>神圣修理锤</v>
       </c>
       <c r="C92">
         <v>1</v>
@@ -4373,17 +4456,17 @@
       <c r="D92">
         <v>15</v>
       </c>
-      <c r="E92">
-        <v>50</v>
+      <c r="Y92">
+        <v>1000</v>
       </c>
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A93">
-        <v>22302102</v>
+        <v>22302101</v>
       </c>
       <c r="B93" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>能量之书</v>
+        <v>经验之书</v>
       </c>
       <c r="C93">
         <v>1</v>
@@ -4392,34 +4475,34 @@
         <v>15</v>
       </c>
       <c r="E93">
-        <v>300</v>
+        <v>50</v>
       </c>
     </row>
     <row r="94" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A94">
-        <v>22302103</v>
+        <v>22302102</v>
       </c>
       <c r="B94" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>攻速药水</v>
+        <v>能量之书</v>
       </c>
       <c r="C94">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D94">
         <v>15</v>
       </c>
-      <c r="Z94" t="s">
-        <v>51</v>
+      <c r="E94">
+        <v>300</v>
       </c>
     </row>
     <row r="95" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A95">
-        <v>22302104</v>
+        <v>22302103</v>
       </c>
       <c r="B95" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>守护药水</v>
+        <v>攻速药水</v>
       </c>
       <c r="C95">
         <v>4</v>
@@ -4428,16 +4511,16 @@
         <v>15</v>
       </c>
       <c r="Z95" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="96" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A96">
-        <v>22302105</v>
+        <v>22302104</v>
       </c>
       <c r="B96" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>法术药水</v>
+        <v>守护药水</v>
       </c>
       <c r="C96">
         <v>4</v>
@@ -4446,16 +4529,16 @@
         <v>15</v>
       </c>
       <c r="Z96" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="97" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A97">
-        <v>22302106</v>
+        <v>22302105</v>
       </c>
       <c r="B97" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>技巧药水</v>
+        <v>法术药水</v>
       </c>
       <c r="C97">
         <v>4</v>
@@ -4464,16 +4547,16 @@
         <v>15</v>
       </c>
       <c r="Z97" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="98" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A98">
-        <v>22302107</v>
+        <v>22302106</v>
       </c>
       <c r="B98" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>速度药水</v>
+        <v>技巧药水</v>
       </c>
       <c r="C98">
         <v>4</v>
@@ -4482,16 +4565,16 @@
         <v>15</v>
       </c>
       <c r="Z98" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="99" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A99">
-        <v>22302108</v>
+        <v>22302107</v>
       </c>
       <c r="B99" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>幸运药水</v>
+        <v>速度药水</v>
       </c>
       <c r="C99">
         <v>4</v>
@@ -4500,16 +4583,16 @@
         <v>15</v>
       </c>
       <c r="Z99" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="100" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A100">
-        <v>22302109</v>
-      </c>
-      <c r="B100" s="9" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>暴击药水</v>
+        <v>22302108</v>
+      </c>
+      <c r="B100" s="13" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>幸运药水</v>
       </c>
       <c r="C100">
         <v>4</v>
@@ -4518,16 +4601,16 @@
         <v>15</v>
       </c>
       <c r="Z100" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="101" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A101">
-        <v>22302110</v>
+        <v>22302109</v>
       </c>
       <c r="B101" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>饼干</v>
+        <v>暴击药水</v>
       </c>
       <c r="C101">
         <v>4</v>
@@ -4535,17 +4618,17 @@
       <c r="D101">
         <v>15</v>
       </c>
-      <c r="F101">
-        <v>50</v>
+      <c r="Z101" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="102" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A102">
-        <v>22302111</v>
-      </c>
-      <c r="B102" s="10" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>红色胶囊</v>
+        <v>22302110</v>
+      </c>
+      <c r="B102" s="9" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>饼干</v>
       </c>
       <c r="C102">
         <v>4</v>
@@ -4553,60 +4636,62 @@
       <c r="D102">
         <v>15</v>
       </c>
-      <c r="G102">
+      <c r="F102">
         <v>50</v>
       </c>
     </row>
     <row r="103" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A103">
-        <v>22302112</v>
+        <v>22302111</v>
       </c>
       <c r="B103" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>蓝色胶囊</v>
-      </c>
-      <c r="H103">
+        <v>红色胶囊</v>
+      </c>
+      <c r="C103">
+        <v>4</v>
+      </c>
+      <c r="D103">
+        <v>15</v>
+      </c>
+      <c r="G103">
         <v>50</v>
       </c>
     </row>
     <row r="104" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A104">
-        <v>22302113</v>
+        <v>22302112</v>
       </c>
       <c r="B104" s="10" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>水晶球</v>
-      </c>
-      <c r="P104" t="s">
-        <v>70</v>
+        <v>蓝色胶囊</v>
+      </c>
+      <c r="H104">
+        <v>50</v>
       </c>
     </row>
     <row r="105" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A105">
-        <v>22302114</v>
-      </c>
-      <c r="B105" s="14" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>坐骑黑豹</v>
-      </c>
-      <c r="K105">
-        <v>2</v>
-      </c>
-      <c r="L105">
-        <v>10</v>
+        <v>22302113</v>
+      </c>
+      <c r="B105" s="10" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>水晶球</v>
+      </c>
+      <c r="P105" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="106" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A106">
-        <v>22302115</v>
+        <v>22302114</v>
       </c>
       <c r="B106" s="14" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>坐骑鹰</v>
-      </c>
-      <c r="D106" s="14"/>
+        <v>坐骑黑豹</v>
+      </c>
       <c r="K106">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L106">
         <v>10</v>
@@ -4614,15 +4699,15 @@
     </row>
     <row r="107" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A107">
-        <v>22302116</v>
+        <v>22302115</v>
       </c>
       <c r="B107" s="14" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>坐骑传送器</v>
+        <v>坐骑鹰</v>
       </c>
       <c r="D107" s="14"/>
       <c r="K107">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="L107">
         <v>10</v>
@@ -4630,30 +4715,31 @@
     </row>
     <row r="108" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A108">
-        <v>22301501</v>
-      </c>
-      <c r="B108" s="13" t="str">
-        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>种子-豌豆</v>
+        <v>22302116</v>
+      </c>
+      <c r="B108" s="14" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>坐骑传送器</v>
       </c>
       <c r="D108" s="14"/>
-      <c r="Q108">
-        <v>22037101</v>
-      </c>
-      <c r="R108">
-        <v>10800</v>
+      <c r="K108">
+        <v>99</v>
+      </c>
+      <c r="L108">
+        <v>10</v>
       </c>
     </row>
     <row r="109" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A109">
-        <v>22301502</v>
+        <v>22301501</v>
       </c>
       <c r="B109" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>种子-玉米</v>
-      </c>
+        <v>种子-豌豆</v>
+      </c>
+      <c r="D109" s="14"/>
       <c r="Q109">
-        <v>22037102</v>
+        <v>22037101</v>
       </c>
       <c r="R109">
         <v>10800</v>
@@ -4661,14 +4747,14 @@
     </row>
     <row r="110" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A110">
-        <v>22301503</v>
+        <v>22301502</v>
       </c>
       <c r="B110" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>种子-苹果</v>
+        <v>种子-玉米</v>
       </c>
       <c r="Q110">
-        <v>22037103</v>
+        <v>22037102</v>
       </c>
       <c r="R110">
         <v>10800</v>
@@ -4676,14 +4762,14 @@
     </row>
     <row r="111" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A111">
-        <v>22301504</v>
+        <v>22301503</v>
       </c>
       <c r="B111" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>种子-蓝莓</v>
+        <v>种子-苹果</v>
       </c>
       <c r="Q111">
-        <v>22037104</v>
+        <v>22037103</v>
       </c>
       <c r="R111">
         <v>10800</v>
@@ -4691,98 +4777,113 @@
     </row>
     <row r="112" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A112">
-        <v>22301605</v>
+        <v>22301504</v>
       </c>
       <c r="B112" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>作物-豌豆</v>
-      </c>
-      <c r="E112">
-        <v>5</v>
+        <v>种子-蓝莓</v>
+      </c>
+      <c r="Q112">
+        <v>22037104</v>
+      </c>
+      <c r="R112">
+        <v>10800</v>
       </c>
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A113">
-        <v>22301606</v>
+        <v>22301605</v>
       </c>
       <c r="B113" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>作物-玉米</v>
-      </c>
-      <c r="I113">
-        <v>1</v>
-      </c>
-      <c r="J113">
-        <v>20</v>
+        <v>作物-豌豆</v>
+      </c>
+      <c r="E113">
+        <v>5</v>
       </c>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A114">
+        <v>22301606</v>
+      </c>
+      <c r="B114" s="13" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>作物-玉米</v>
+      </c>
+      <c r="I114">
+        <v>1</v>
+      </c>
+      <c r="J114">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A115">
         <v>22301607</v>
       </c>
-      <c r="B114" s="13" t="str">
+      <c r="B115" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>作物-苹果</v>
       </c>
-      <c r="S114">
+      <c r="S115">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="Z40:Z72 Q40:Y62 Z74:Z87 L102:M104 Q38:Z39 P15:Z21 P38:P62 O9:Z14 O66:Y87 E105:L114 O88:Z114 O22:Z37 P5:Z8 P63:Y65 M40:N114 E5:N39 E40:L103 B40:B87">
-    <cfRule type="containsBlanks" dxfId="13" priority="17">
-      <formula>LEN(TRIM(B5))=0</formula>
+  <conditionalFormatting sqref="Z41:Z73 Q41:Y63 Z75:Z88 L103:M105 Q39:Z40 P16:Z22 P39:P63 O10:Z15 O67:Y88 E106:L115 O89:Z115 O23:Z38 P6:Z9 P64:Y66 M41:N115 E6:N40 E41:L104 B41:B88 E5:Z5 AA4:AB115">
+    <cfRule type="containsBlanks" dxfId="10" priority="18">
+      <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z73">
-    <cfRule type="containsBlanks" dxfId="12" priority="11">
-      <formula>LEN(TRIM(Z73))=0</formula>
+  <conditionalFormatting sqref="Z74">
+    <cfRule type="containsBlanks" dxfId="9" priority="12">
+      <formula>LEN(TRIM(Z74))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E104:M104">
-    <cfRule type="containsBlanks" dxfId="11" priority="9">
-      <formula>LEN(TRIM(E104))=0</formula>
+  <conditionalFormatting sqref="E105:M105">
+    <cfRule type="containsBlanks" dxfId="8" priority="10">
+      <formula>LEN(TRIM(E105))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O19:O21">
-    <cfRule type="containsBlanks" dxfId="10" priority="8">
-      <formula>LEN(TRIM(O19))=0</formula>
+  <conditionalFormatting sqref="O20:O22">
+    <cfRule type="containsBlanks" dxfId="7" priority="9">
+      <formula>LEN(TRIM(O20))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O15:O18">
-    <cfRule type="containsBlanks" dxfId="9" priority="7">
-      <formula>LEN(TRIM(O15))=0</formula>
+  <conditionalFormatting sqref="O16:O19">
+    <cfRule type="containsBlanks" dxfId="6" priority="8">
+      <formula>LEN(TRIM(O16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:Z4 E4:L4">
-    <cfRule type="containsBlanks" dxfId="8" priority="6">
+    <cfRule type="containsBlanks" dxfId="5" priority="7">
       <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4">
-    <cfRule type="containsBlanks" dxfId="7" priority="5">
+    <cfRule type="containsBlanks" dxfId="4" priority="6">
       <formula>LEN(TRIM(O4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:N4">
-    <cfRule type="containsBlanks" dxfId="6" priority="4">
+    <cfRule type="containsBlanks" dxfId="3" priority="5">
       <formula>LEN(TRIM(M4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:D12 C16:D22 C39:D114">
-    <cfRule type="containsBlanks" dxfId="5" priority="3">
-      <formula>LEN(TRIM(C5))=0</formula>
+  <conditionalFormatting sqref="C6:D13 C17:D23 C40:D115">
+    <cfRule type="containsBlanks" dxfId="2" priority="4">
+      <formula>LEN(TRIM(C6))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:D15">
-    <cfRule type="containsBlanks" dxfId="4" priority="2">
-      <formula>LEN(TRIM(C13))=0</formula>
+  <conditionalFormatting sqref="C14:D16">
+    <cfRule type="containsBlanks" dxfId="1" priority="3">
+      <formula>LEN(TRIM(C14))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C23:D52">
-    <cfRule type="containsBlanks" dxfId="3" priority="1">
-      <formula>LEN(TRIM(C23))=0</formula>
+  <conditionalFormatting sqref="C24:D53">
+    <cfRule type="containsBlanks" dxfId="0" priority="2">
+      <formula>LEN(TRIM(C24))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix gem icons show bug
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/ItemConsumer.xlsx
+++ b/ConfigData/Xlsx/ItemConsumer.xlsx
@@ -1406,7 +1406,86 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1508,75 +1587,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2521,17 +2531,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:AB115" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:AB115" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A3:AB115"/>
   <sortState ref="A4:Z115">
     <sortCondition ref="A3:A115"/>
   </sortState>
   <tableColumns count="28">
     <tableColumn id="1" name="Id"/>
-    <tableColumn id="2" name="~Name" dataDxfId="12">
+    <tableColumn id="2" name="~Name" dataDxfId="2">
       <calculatedColumnFormula>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="CdGroup" dataDxfId="11"/>
+    <tableColumn id="16" name="CdGroup" dataDxfId="1"/>
     <tableColumn id="25" name="CdTime"/>
     <tableColumn id="3" name="GainExp"/>
     <tableColumn id="4" name="GainFood"/>
@@ -2886,7 +2896,7 @@
   <dimension ref="A1:AB115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA5" sqref="AA5"/>
+      <selection activeCell="D5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3194,8 +3204,6 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>新手礼包</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
       <c r="AA5" t="s">
         <v>156</v>
       </c>
@@ -4150,6 +4158,12 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>小型魔法药剂</v>
       </c>
+      <c r="C75">
+        <v>2</v>
+      </c>
+      <c r="D75">
+        <v>15</v>
+      </c>
       <c r="T75">
         <v>2</v>
       </c>
@@ -4253,7 +4267,7 @@
         <v>小型体力药剂</v>
       </c>
       <c r="C81">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D81">
         <v>15</v>
@@ -4343,7 +4357,7 @@
         <v>随机魔法卡</v>
       </c>
       <c r="C86">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D86">
         <v>15</v>
@@ -4415,7 +4429,7 @@
         <v>木质修理锤</v>
       </c>
       <c r="C90">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D90">
         <v>15</v>
@@ -4666,6 +4680,12 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>蓝色胶囊</v>
       </c>
+      <c r="C104">
+        <v>4</v>
+      </c>
+      <c r="D104">
+        <v>15</v>
+      </c>
       <c r="H104">
         <v>50</v>
       </c>
@@ -4832,58 +4852,63 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="Z41:Z73 Q41:Y63 Z75:Z88 L103:M105 Q39:Z40 P16:Z22 P39:P63 O10:Z15 O67:Y88 E106:L115 O89:Z115 O23:Z38 P6:Z9 P64:Y66 M41:N115 E6:N40 E41:L104 B41:B88 E5:Z5 AA4:AB115">
-    <cfRule type="containsBlanks" dxfId="10" priority="18">
+    <cfRule type="containsBlanks" dxfId="14" priority="19">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z74">
-    <cfRule type="containsBlanks" dxfId="9" priority="12">
+    <cfRule type="containsBlanks" dxfId="13" priority="13">
       <formula>LEN(TRIM(Z74))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E105:M105">
-    <cfRule type="containsBlanks" dxfId="8" priority="10">
+    <cfRule type="containsBlanks" dxfId="12" priority="11">
       <formula>LEN(TRIM(E105))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O20:O22">
-    <cfRule type="containsBlanks" dxfId="7" priority="9">
+    <cfRule type="containsBlanks" dxfId="11" priority="10">
       <formula>LEN(TRIM(O20))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O16:O19">
-    <cfRule type="containsBlanks" dxfId="6" priority="8">
+    <cfRule type="containsBlanks" dxfId="10" priority="9">
       <formula>LEN(TRIM(O16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:Z4 E4:L4">
-    <cfRule type="containsBlanks" dxfId="5" priority="7">
+    <cfRule type="containsBlanks" dxfId="9" priority="8">
       <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4">
-    <cfRule type="containsBlanks" dxfId="4" priority="6">
+    <cfRule type="containsBlanks" dxfId="8" priority="7">
       <formula>LEN(TRIM(O4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:N4">
-    <cfRule type="containsBlanks" dxfId="3" priority="5">
+    <cfRule type="containsBlanks" dxfId="7" priority="6">
       <formula>LEN(TRIM(M4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:D13 C17:D23 C40:D115">
-    <cfRule type="containsBlanks" dxfId="2" priority="4">
+    <cfRule type="containsBlanks" dxfId="6" priority="5">
       <formula>LEN(TRIM(C6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:D16">
-    <cfRule type="containsBlanks" dxfId="1" priority="3">
+    <cfRule type="containsBlanks" dxfId="5" priority="4">
       <formula>LEN(TRIM(C14))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:D53">
-    <cfRule type="containsBlanks" dxfId="0" priority="2">
+    <cfRule type="containsBlanks" dxfId="4" priority="3">
       <formula>LEN(TRIM(C24))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:D5">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(C5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
support item required base quest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/ItemConsumer.xlsx
+++ b/ConfigData/Xlsx/ItemConsumer.xlsx
@@ -1406,7 +1406,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="16">
     <dxf>
       <font>
         <color auto="1"/>
@@ -1483,6 +1483,16 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2233,7 +2243,7 @@
             <v>22301605</v>
           </cell>
           <cell r="B78" t="str">
-            <v>作物-豌豆</v>
+            <v>豌豆</v>
           </cell>
         </row>
         <row r="79">
@@ -2241,7 +2251,7 @@
             <v>22301606</v>
           </cell>
           <cell r="B79" t="str">
-            <v>作物-玉米</v>
+            <v>玉米</v>
           </cell>
         </row>
         <row r="80">
@@ -2249,278 +2259,286 @@
             <v>22301607</v>
           </cell>
           <cell r="B80" t="str">
-            <v>作物-苹果</v>
+            <v>苹果</v>
           </cell>
         </row>
         <row r="81">
           <cell r="A81">
-            <v>22302001</v>
+            <v>22301608</v>
           </cell>
           <cell r="B81" t="str">
-            <v>小型魔法药剂</v>
+            <v>蓝莓</v>
           </cell>
         </row>
         <row r="82">
           <cell r="A82">
-            <v>22302002</v>
+            <v>22302001</v>
           </cell>
           <cell r="B82" t="str">
-            <v>中型魔法药剂</v>
+            <v>小型魔法药剂</v>
           </cell>
         </row>
         <row r="83">
           <cell r="A83">
-            <v>22302003</v>
+            <v>22302002</v>
           </cell>
           <cell r="B83" t="str">
-            <v>大型魔法药剂</v>
+            <v>中型魔法药剂</v>
           </cell>
         </row>
         <row r="84">
           <cell r="A84">
-            <v>22302004</v>
+            <v>22302003</v>
           </cell>
           <cell r="B84" t="str">
-            <v>小型活力药剂</v>
+            <v>大型魔法药剂</v>
           </cell>
         </row>
         <row r="85">
           <cell r="A85">
-            <v>22302005</v>
+            <v>22302004</v>
           </cell>
           <cell r="B85" t="str">
-            <v>中型活力药剂</v>
+            <v>小型活力药剂</v>
           </cell>
         </row>
         <row r="86">
           <cell r="A86">
-            <v>22302006</v>
+            <v>22302005</v>
           </cell>
           <cell r="B86" t="str">
-            <v>大型活力药剂</v>
+            <v>中型活力药剂</v>
           </cell>
         </row>
         <row r="87">
           <cell r="A87">
-            <v>22302007</v>
+            <v>22302006</v>
           </cell>
           <cell r="B87" t="str">
-            <v>小型体力药剂</v>
+            <v>大型活力药剂</v>
           </cell>
         </row>
         <row r="88">
           <cell r="A88">
-            <v>22302008</v>
+            <v>22302007</v>
           </cell>
           <cell r="B88" t="str">
-            <v>中型体力药剂</v>
+            <v>小型体力药剂</v>
           </cell>
         </row>
         <row r="89">
           <cell r="A89">
-            <v>22302009</v>
+            <v>22302008</v>
           </cell>
           <cell r="B89" t="str">
-            <v>大型体力药剂</v>
+            <v>中型体力药剂</v>
           </cell>
         </row>
         <row r="90">
           <cell r="A90">
-            <v>22302013</v>
+            <v>22302009</v>
           </cell>
           <cell r="B90" t="str">
-            <v>随机幻兽卡</v>
+            <v>大型体力药剂</v>
           </cell>
         </row>
         <row r="91">
           <cell r="A91">
-            <v>22302014</v>
+            <v>22302013</v>
           </cell>
           <cell r="B91" t="str">
-            <v>随机武器卡</v>
+            <v>随机幻兽卡</v>
           </cell>
         </row>
         <row r="92">
           <cell r="A92">
-            <v>22302015</v>
+            <v>22302014</v>
           </cell>
           <cell r="B92" t="str">
-            <v>随机魔法卡</v>
+            <v>随机武器卡</v>
           </cell>
         </row>
         <row r="93">
           <cell r="A93">
-            <v>22302016</v>
+            <v>22302015</v>
           </cell>
           <cell r="B93" t="str">
-            <v>符文-查姆</v>
+            <v>随机魔法卡</v>
           </cell>
         </row>
         <row r="94">
           <cell r="A94">
-            <v>22302017</v>
+            <v>22302016</v>
           </cell>
           <cell r="B94" t="str">
-            <v>符文-普尔</v>
+            <v>符文-查姆</v>
           </cell>
         </row>
         <row r="95">
           <cell r="A95">
-            <v>22302018</v>
+            <v>22302017</v>
           </cell>
           <cell r="B95" t="str">
-            <v>符文-艾尔</v>
+            <v>符文-普尔</v>
           </cell>
         </row>
         <row r="96">
           <cell r="A96">
-            <v>22302030</v>
+            <v>22302018</v>
           </cell>
           <cell r="B96" t="str">
-            <v>木质修理锤</v>
+            <v>符文-艾尔</v>
           </cell>
         </row>
         <row r="97">
           <cell r="A97">
-            <v>22302031</v>
+            <v>22302030</v>
           </cell>
           <cell r="B97" t="str">
-            <v>钢铁修理锤</v>
+            <v>木质修理锤</v>
           </cell>
         </row>
         <row r="98">
           <cell r="A98">
-            <v>22302032</v>
+            <v>22302031</v>
           </cell>
           <cell r="B98" t="str">
-            <v>神圣修理锤</v>
+            <v>钢铁修理锤</v>
           </cell>
         </row>
         <row r="99">
           <cell r="A99">
-            <v>22302101</v>
+            <v>22302032</v>
           </cell>
           <cell r="B99" t="str">
-            <v>经验之书</v>
+            <v>神圣修理锤</v>
           </cell>
         </row>
         <row r="100">
           <cell r="A100">
-            <v>22302102</v>
+            <v>22302101</v>
           </cell>
           <cell r="B100" t="str">
-            <v>能量之书</v>
+            <v>经验之书</v>
           </cell>
         </row>
         <row r="101">
           <cell r="A101">
-            <v>22302103</v>
+            <v>22302102</v>
           </cell>
           <cell r="B101" t="str">
-            <v>攻速药水</v>
+            <v>能量之书</v>
           </cell>
         </row>
         <row r="102">
           <cell r="A102">
-            <v>22302104</v>
+            <v>22302103</v>
           </cell>
           <cell r="B102" t="str">
-            <v>守护药水</v>
+            <v>攻速药水</v>
           </cell>
         </row>
         <row r="103">
           <cell r="A103">
-            <v>22302105</v>
+            <v>22302104</v>
           </cell>
           <cell r="B103" t="str">
-            <v>法术药水</v>
+            <v>守护药水</v>
           </cell>
         </row>
         <row r="104">
           <cell r="A104">
-            <v>22302106</v>
+            <v>22302105</v>
           </cell>
           <cell r="B104" t="str">
-            <v>技巧药水</v>
+            <v>法术药水</v>
           </cell>
         </row>
         <row r="105">
           <cell r="A105">
-            <v>22302107</v>
+            <v>22302106</v>
           </cell>
           <cell r="B105" t="str">
-            <v>速度药水</v>
+            <v>技巧药水</v>
           </cell>
         </row>
         <row r="106">
           <cell r="A106">
-            <v>22302108</v>
+            <v>22302107</v>
           </cell>
           <cell r="B106" t="str">
-            <v>幸运药水</v>
+            <v>速度药水</v>
           </cell>
         </row>
         <row r="107">
           <cell r="A107">
-            <v>22302109</v>
+            <v>22302108</v>
           </cell>
           <cell r="B107" t="str">
-            <v>暴击药水</v>
+            <v>幸运药水</v>
           </cell>
         </row>
         <row r="108">
           <cell r="A108">
-            <v>22302110</v>
+            <v>22302109</v>
           </cell>
           <cell r="B108" t="str">
-            <v>饼干</v>
+            <v>暴击药水</v>
           </cell>
         </row>
         <row r="109">
           <cell r="A109">
-            <v>22302111</v>
+            <v>22302110</v>
           </cell>
           <cell r="B109" t="str">
-            <v>红色胶囊</v>
+            <v>饼干</v>
           </cell>
         </row>
         <row r="110">
           <cell r="A110">
-            <v>22302112</v>
+            <v>22302111</v>
           </cell>
           <cell r="B110" t="str">
-            <v>蓝色胶囊</v>
+            <v>红色胶囊</v>
           </cell>
         </row>
         <row r="111">
           <cell r="A111">
-            <v>22302113</v>
+            <v>22302112</v>
           </cell>
           <cell r="B111" t="str">
-            <v>水晶球</v>
+            <v>蓝色胶囊</v>
           </cell>
         </row>
         <row r="112">
           <cell r="A112">
-            <v>22302114</v>
+            <v>22302113</v>
           </cell>
           <cell r="B112" t="str">
-            <v>坐骑黑豹</v>
+            <v>水晶球</v>
           </cell>
         </row>
         <row r="113">
           <cell r="A113">
-            <v>22302115</v>
+            <v>22302114</v>
           </cell>
           <cell r="B113" t="str">
-            <v>坐骑鹰</v>
+            <v>坐骑黑豹</v>
           </cell>
         </row>
         <row r="114">
           <cell r="A114">
+            <v>22302115</v>
+          </cell>
+          <cell r="B114" t="str">
+            <v>坐骑鹰</v>
+          </cell>
+        </row>
+        <row r="115">
+          <cell r="A115">
             <v>22302116</v>
           </cell>
-          <cell r="B114" t="str">
+          <cell r="B115" t="str">
             <v>坐骑传送器</v>
           </cell>
         </row>
@@ -2531,8 +2549,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:AB115" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A3:AB115"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:AB116" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A3:AB116"/>
   <sortState ref="A4:Z115">
     <sortCondition ref="A3:A115"/>
   </sortState>
@@ -2893,10 +2911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB115"/>
+  <dimension ref="A1:AB116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="C5:D5"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="Q110" sqref="Q110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4759,10 +4777,10 @@
       </c>
       <c r="D109" s="14"/>
       <c r="Q109">
-        <v>22037101</v>
+        <v>22301605</v>
       </c>
       <c r="R109">
-        <v>10800</v>
+        <v>900</v>
       </c>
     </row>
     <row r="110" spans="1:26" x14ac:dyDescent="0.15">
@@ -4774,10 +4792,10 @@
         <v>种子-玉米</v>
       </c>
       <c r="Q110">
-        <v>22037102</v>
+        <v>22301606</v>
       </c>
       <c r="R110">
-        <v>10800</v>
+        <v>900</v>
       </c>
     </row>
     <row r="111" spans="1:26" x14ac:dyDescent="0.15">
@@ -4789,10 +4807,10 @@
         <v>种子-苹果</v>
       </c>
       <c r="Q111">
-        <v>22037103</v>
+        <v>22301607</v>
       </c>
       <c r="R111">
-        <v>10800</v>
+        <v>900</v>
       </c>
     </row>
     <row r="112" spans="1:26" x14ac:dyDescent="0.15">
@@ -4804,10 +4822,10 @@
         <v>种子-蓝莓</v>
       </c>
       <c r="Q112">
-        <v>22037104</v>
+        <v>22301608</v>
       </c>
       <c r="R112">
-        <v>10800</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.15">
@@ -4816,7 +4834,7 @@
       </c>
       <c r="B113" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>作物-豌豆</v>
+        <v>豌豆</v>
       </c>
       <c r="E113">
         <v>5</v>
@@ -4828,7 +4846,7 @@
       </c>
       <c r="B114" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>作物-玉米</v>
+        <v>玉米</v>
       </c>
       <c r="I114">
         <v>1</v>
@@ -4843,71 +4861,86 @@
       </c>
       <c r="B115" s="13" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>作物-苹果</v>
+        <v>苹果</v>
       </c>
       <c r="S115">
         <v>2</v>
       </c>
     </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A116">
+        <v>22301608</v>
+      </c>
+      <c r="B116" s="13" t="str">
+        <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
+        <v>蓝莓</v>
+      </c>
+      <c r="I116">
+        <v>1</v>
+      </c>
+      <c r="J116">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="Z41:Z73 Q41:Y63 Z75:Z88 L103:M105 Q39:Z40 P16:Z22 P39:P63 O10:Z15 O67:Y88 E106:L115 O89:Z115 O23:Z38 P6:Z9 P64:Y66 M41:N115 E6:N40 E41:L104 B41:B88 E5:Z5 AA4:AB115">
-    <cfRule type="containsBlanks" dxfId="14" priority="19">
+  <conditionalFormatting sqref="Z41:Z73 Q41:Y63 Z75:Z88 L103:M105 Q39:Z40 P16:Z22 P39:P63 O10:Z15 O67:Y88 E106:L115 O89:Z108 O23:Z38 P6:Z9 P64:Y66 M41:N115 E6:N40 E41:L104 B41:B88 E5:Z5 AA4:AB116 E116:AB116 O113:Z115 O109:P112 R109:Z112">
+    <cfRule type="containsBlanks" dxfId="15" priority="19">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z74">
-    <cfRule type="containsBlanks" dxfId="13" priority="13">
+    <cfRule type="containsBlanks" dxfId="14" priority="13">
       <formula>LEN(TRIM(Z74))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E105:M105">
-    <cfRule type="containsBlanks" dxfId="12" priority="11">
+    <cfRule type="containsBlanks" dxfId="13" priority="11">
       <formula>LEN(TRIM(E105))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O20:O22">
-    <cfRule type="containsBlanks" dxfId="11" priority="10">
+    <cfRule type="containsBlanks" dxfId="12" priority="10">
       <formula>LEN(TRIM(O20))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O16:O19">
-    <cfRule type="containsBlanks" dxfId="10" priority="9">
+    <cfRule type="containsBlanks" dxfId="11" priority="9">
       <formula>LEN(TRIM(O16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:Z4 E4:L4">
-    <cfRule type="containsBlanks" dxfId="9" priority="8">
+    <cfRule type="containsBlanks" dxfId="10" priority="8">
       <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4">
-    <cfRule type="containsBlanks" dxfId="8" priority="7">
+    <cfRule type="containsBlanks" dxfId="9" priority="7">
       <formula>LEN(TRIM(O4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:N4">
-    <cfRule type="containsBlanks" dxfId="7" priority="6">
+    <cfRule type="containsBlanks" dxfId="8" priority="6">
       <formula>LEN(TRIM(M4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:D13 C17:D23 C40:D115">
-    <cfRule type="containsBlanks" dxfId="6" priority="5">
+  <conditionalFormatting sqref="C6:D13 C17:D23 C40:D116">
+    <cfRule type="containsBlanks" dxfId="7" priority="5">
       <formula>LEN(TRIM(C6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:D16">
-    <cfRule type="containsBlanks" dxfId="5" priority="4">
+    <cfRule type="containsBlanks" dxfId="6" priority="4">
       <formula>LEN(TRIM(C14))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:D53">
-    <cfRule type="containsBlanks" dxfId="4" priority="3">
+    <cfRule type="containsBlanks" dxfId="5" priority="3">
       <formula>LEN(TRIM(C24))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:D5">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="4" priority="1">
       <formula>LEN(TRIM(C5))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
finish pay based on item atrributes.
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/ItemConsumer.xlsx
+++ b/ConfigData/Xlsx/ItemConsumer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -1401,6 +1401,75 @@
   <dxfs count="14">
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color auto="1"/>
       </font>
       <fill>
@@ -1500,75 +1569,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1589,6 +1589,7 @@
       <sheetName val="材料"/>
       <sheetName val="任务"/>
       <sheetName val="其他"/>
+      <sheetName val="~素材类型分析"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -2515,23 +2516,24 @@
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="3"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:AA116" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:AA116" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A3:AA116"/>
   <sortState ref="A4:Y115">
     <sortCondition ref="A3:A115"/>
   </sortState>
   <tableColumns count="27">
     <tableColumn id="1" name="Id"/>
-    <tableColumn id="2" name="~Name" dataDxfId="12">
+    <tableColumn id="2" name="~Name" dataDxfId="1">
       <calculatedColumnFormula>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="CdGroup" dataDxfId="11"/>
+    <tableColumn id="16" name="CdGroup" dataDxfId="0"/>
     <tableColumn id="25" name="CdTime"/>
     <tableColumn id="3" name="GainExp"/>
     <tableColumn id="4" name="GainFood"/>
@@ -2884,8 +2886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="K103" sqref="K103"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4839,57 +4841,57 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="Y41:Y73 P41:X63 Y75:Y88 P39:Y40 O16:Y22 O39:O63 N10:Y15 N67:X88 E106:K106 N89:Y108 N23:Y38 O6:Y9 O64:X66 E41:K104 B41:B88 Z4:AA116 N113:Y115 N109:O112 Q109:Y112 L41:M115 E6:M40 E5:Y5 E116:AA116 E105:L105 E109:K115 E107:J108">
-    <cfRule type="containsBlanks" dxfId="10" priority="19">
+    <cfRule type="containsBlanks" dxfId="13" priority="19">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y74">
-    <cfRule type="containsBlanks" dxfId="9" priority="13">
+    <cfRule type="containsBlanks" dxfId="12" priority="13">
       <formula>LEN(TRIM(Y74))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N20:N22">
-    <cfRule type="containsBlanks" dxfId="8" priority="10">
+    <cfRule type="containsBlanks" dxfId="11" priority="10">
       <formula>LEN(TRIM(N20))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16:N19">
-    <cfRule type="containsBlanks" dxfId="7" priority="9">
+    <cfRule type="containsBlanks" dxfId="10" priority="9">
       <formula>LEN(TRIM(N16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:Y4 E4:K4">
-    <cfRule type="containsBlanks" dxfId="6" priority="8">
+    <cfRule type="containsBlanks" dxfId="9" priority="8">
       <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4">
-    <cfRule type="containsBlanks" dxfId="5" priority="7">
+    <cfRule type="containsBlanks" dxfId="8" priority="7">
       <formula>LEN(TRIM(N4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:M4">
-    <cfRule type="containsBlanks" dxfId="4" priority="6">
+    <cfRule type="containsBlanks" dxfId="7" priority="6">
       <formula>LEN(TRIM(L4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:D13 C17:D23 C40:D116">
-    <cfRule type="containsBlanks" dxfId="3" priority="5">
+    <cfRule type="containsBlanks" dxfId="6" priority="5">
       <formula>LEN(TRIM(C6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:D16">
-    <cfRule type="containsBlanks" dxfId="2" priority="4">
+    <cfRule type="containsBlanks" dxfId="5" priority="4">
       <formula>LEN(TRIM(C14))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:D53">
-    <cfRule type="containsBlanks" dxfId="1" priority="3">
+    <cfRule type="containsBlanks" dxfId="4" priority="3">
       <formula>LEN(TRIM(C24))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:D5">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="3" priority="1">
       <formula>LEN(TRIM(C5))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
optimise the card random method
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/ItemConsumer.xlsx
+++ b/ConfigData/Xlsx/ItemConsumer.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -17,12 +17,12 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="159">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -96,103 +96,155 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>Id</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得lp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得mp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得pp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>直接伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机卡牌类型</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FightRandomCardType</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机卡包概率</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0;840;150;10;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0;720;250;30;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0;600;350;50;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RandomCardRate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>圣言</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>HolyWord</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>witcheye</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>int[]</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Id</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>获得lp</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>获得mp</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>获得pp</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>直接伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机卡牌类型</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>FightRandomCardType</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机卡包概率</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;1;0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;1;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;1;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;1;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;1;4</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;1;5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;1;6</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>5;0;0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0;840;150;10;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0;720;250;30;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0;600;350;50;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RandomCardRate</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;2;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;2;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;2;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>圣言</t>
+    <t>属性改变</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttrAddAfterSummon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>2;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>3;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>4;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>5;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>6;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>7;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>恢复塔生命</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddTowerHp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>~Name</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过掉落获取</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得食物</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GainFood</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得健康</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得精神</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GainMental</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GainHealth</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>特殊指令</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -200,11 +252,215 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>HolyWord</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>witcheye</t>
+    <t>Instruction</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>detectall</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>0;840;150;10;11</t>
+  </si>
+  <si>
+    <t>0;840;150;10;12</t>
+  </si>
+  <si>
+    <t>0;840;150;10;13</t>
+  </si>
+  <si>
+    <t>0;840;150;10;14</t>
+  </si>
+  <si>
+    <t>0;840;150;10;15</t>
+  </si>
+  <si>
+    <t>0;840;150;10;16</t>
+  </si>
+  <si>
+    <t>0;840;150;10;17</t>
+  </si>
+  <si>
+    <t>0;840;150;10;18</t>
+  </si>
+  <si>
+    <t>0;840;150;10;19</t>
+  </si>
+  <si>
+    <t>0;840;150;10;20</t>
+  </si>
+  <si>
+    <t>0;840;150;10;21</t>
+  </si>
+  <si>
+    <t>0;840;150;10;22</t>
+  </si>
+  <si>
+    <t>0;840;150;10;23</t>
+  </si>
+  <si>
+    <t>0;840;150;10;24</t>
+  </si>
+  <si>
+    <t>0;840;150;10;25</t>
+  </si>
+  <si>
+    <t>0;840;150;10;26</t>
+  </si>
+  <si>
+    <t>随机卡规则</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DropItem</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlsucaidai</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlsucaidaigaoji</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlsucaidaiteji</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlsucaidaijipin</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlcao</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlyu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlshi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlgu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlmu</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlsucaidai(wu)</t>
+  </si>
+  <si>
+    <t>dlsucaidai(shui)</t>
+  </si>
+  <si>
+    <t>dlsucaidai(feng)</t>
+  </si>
+  <si>
+    <t>dlsucaidai(huo)</t>
+  </si>
+  <si>
+    <t>dlsucaidai(di)</t>
+  </si>
+  <si>
+    <t>dlsucaidai(guang)</t>
+  </si>
+  <si>
+    <t>dlsucaidai(an)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(emo)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(jixie)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(jingling)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(kunchong)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(long)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(niao)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(paxing)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(renlei)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(shouren)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(wangling)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(yeshou)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(yu)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(yuansu)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(zhiwu)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(dijing)</t>
+  </si>
+  <si>
+    <t>dlziyuandai(shixiang)</t>
+  </si>
+  <si>
+    <t>0;0;350;650;0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cd时间</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CdTime</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CdGroup</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cd组</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t>礼包内物品</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemCount</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string[]</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -212,402 +468,139 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>属性改变</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>AttrAddAfterSummon</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>2;5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>3;5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>4;5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>5;5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>6;5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>7;5</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>恢复塔生命</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>AddTowerHp</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>~Name</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>通过掉落获取</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>获得食物</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>GainFood</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>获得健康</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>获得精神</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>GainMental</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>GainHealth</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>特殊指令</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Instruction</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>detectall</t>
+    <t>道具数量</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>xiaoxingmofayaoji;zhongxingmofayaoji;chushiziyuanbao;suijihuanshouka;suijiwuqika;suijimofaka</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>5;5;1;5;3;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得祝福</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BlessId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>穷奇召唤</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>漂流瓶的信</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dlpiaoliuping</t>
+  </si>
+  <si>
+    <t>RandomCardCount</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机卡计数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>attr.0</t>
+  </si>
+  <si>
+    <t>attr.1</t>
+  </si>
+  <si>
+    <t>attr.2</t>
+  </si>
+  <si>
+    <t>attr.3</t>
+  </si>
+  <si>
+    <t>attr.4</t>
+  </si>
+  <si>
+    <t>attr.5</t>
+  </si>
+  <si>
+    <t>attr.6</t>
+  </si>
+  <si>
+    <t>type.1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>type.2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>type.3</t>
+  </si>
+  <si>
+    <t>race.1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>race.2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>race.3</t>
+  </si>
+  <si>
+    <t>race.4</t>
+  </si>
+  <si>
+    <t>race.5</t>
+  </si>
+  <si>
+    <t>race.6</t>
+  </si>
+  <si>
+    <t>race.7</t>
+  </si>
+  <si>
+    <t>race.8</t>
+  </si>
+  <si>
+    <t>race.9</t>
+  </si>
+  <si>
+    <t>race.10</t>
+  </si>
+  <si>
+    <t>race.11</t>
+  </si>
+  <si>
+    <t>race.12</t>
+  </si>
+  <si>
+    <t>race.13</t>
+  </si>
+  <si>
+    <t>race.14</t>
+  </si>
+  <si>
+    <t>race.15</t>
+  </si>
+  <si>
+    <t>race.16</t>
+  </si>
+  <si>
+    <t>all.0</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>RandomCardCatalog</t>
     <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0;840;150;10;11</t>
-  </si>
-  <si>
-    <t>0;840;150;10;12</t>
-  </si>
-  <si>
-    <t>0;840;150;10;13</t>
-  </si>
-  <si>
-    <t>0;840;150;10;14</t>
-  </si>
-  <si>
-    <t>0;840;150;10;15</t>
-  </si>
-  <si>
-    <t>0;840;150;10;16</t>
-  </si>
-  <si>
-    <t>0;840;150;10;17</t>
-  </si>
-  <si>
-    <t>0;840;150;10;18</t>
-  </si>
-  <si>
-    <t>0;840;150;10;19</t>
-  </si>
-  <si>
-    <t>0;840;150;10;20</t>
-  </si>
-  <si>
-    <t>0;840;150;10;21</t>
-  </si>
-  <si>
-    <t>0;840;150;10;22</t>
-  </si>
-  <si>
-    <t>0;840;150;10;23</t>
-  </si>
-  <si>
-    <t>0;840;150;10;24</t>
-  </si>
-  <si>
-    <t>0;840;150;10;25</t>
-  </si>
-  <si>
-    <t>0;840;150;10;26</t>
-  </si>
-  <si>
-    <t>1;3;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1;3;2</t>
-  </si>
-  <si>
-    <t>1;3;3</t>
-  </si>
-  <si>
-    <t>1;3;4</t>
-  </si>
-  <si>
-    <t>1;3;5</t>
-  </si>
-  <si>
-    <t>1;3;6</t>
-  </si>
-  <si>
-    <t>1;3;7</t>
-  </si>
-  <si>
-    <t>1;3;8</t>
-  </si>
-  <si>
-    <t>1;3;9</t>
-  </si>
-  <si>
-    <t>1;3;10</t>
-  </si>
-  <si>
-    <t>1;3;11</t>
-  </si>
-  <si>
-    <t>1;3;12</t>
-  </si>
-  <si>
-    <t>1;3;13</t>
-  </si>
-  <si>
-    <t>1;3;14</t>
-  </si>
-  <si>
-    <t>1;3;15</t>
-  </si>
-  <si>
-    <t>1;3;16</t>
-  </si>
-  <si>
-    <t>随机卡规则</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>DropItem</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dlsucaidai</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dlsucaidaigaoji</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dlsucaidaiteji</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dlsucaidaijipin</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dlcao</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dlyu</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dlshi</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dlgu</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dlmu</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dlsucaidai(wu)</t>
-  </si>
-  <si>
-    <t>dlsucaidai(shui)</t>
-  </si>
-  <si>
-    <t>dlsucaidai(feng)</t>
-  </si>
-  <si>
-    <t>dlsucaidai(huo)</t>
-  </si>
-  <si>
-    <t>dlsucaidai(di)</t>
-  </si>
-  <si>
-    <t>dlsucaidai(guang)</t>
-  </si>
-  <si>
-    <t>dlsucaidai(an)</t>
-  </si>
-  <si>
-    <t>dlziyuandai(emo)</t>
-  </si>
-  <si>
-    <t>dlziyuandai(jixie)</t>
-  </si>
-  <si>
-    <t>dlziyuandai(jingling)</t>
-  </si>
-  <si>
-    <t>dlziyuandai(kunchong)</t>
-  </si>
-  <si>
-    <t>dlziyuandai(long)</t>
-  </si>
-  <si>
-    <t>dlziyuandai(niao)</t>
-  </si>
-  <si>
-    <t>dlziyuandai(paxing)</t>
-  </si>
-  <si>
-    <t>dlziyuandai(renlei)</t>
-  </si>
-  <si>
-    <t>dlziyuandai(shouren)</t>
-  </si>
-  <si>
-    <t>dlziyuandai(wangling)</t>
-  </si>
-  <si>
-    <t>dlziyuandai(yeshou)</t>
-  </si>
-  <si>
-    <t>dlziyuandai(yu)</t>
-  </si>
-  <si>
-    <t>dlziyuandai(yuansu)</t>
-  </si>
-  <si>
-    <t>dlziyuandai(zhiwu)</t>
-  </si>
-  <si>
-    <t>dlziyuandai(dijing)</t>
-  </si>
-  <si>
-    <t>dlziyuandai(shixiang)</t>
-  </si>
-  <si>
-    <t>1;3;11</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0;0;350;650;0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>cd时间</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>CdTime</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>CdGroup</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>cd组</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Items</t>
-  </si>
-  <si>
-    <t>礼包内物品</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ItemCount</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string[]</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int[]</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>道具数量</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>xiaoxingmofayaoji;zhongxingmofayaoji;chushiziyuanbao;suijihuanshouka;suijiwuqika;suijimofaka</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>5;5;1;5;3;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>获得祝福</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>BlessId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>穷奇召唤</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>漂流瓶的信</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dlpiaoliuping</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1331,41 +1324,41 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1412,7 +1405,17 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -1609,6 +1612,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2609,41 +2680,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表2" displayName="表2" ref="A3:AA123" totalsRowShown="0" headerRowDxfId="16">
-  <autoFilter ref="A3:AA123" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState ref="A4:Y122">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:AB123" totalsRowShown="0" headerRowDxfId="17">
+  <autoFilter ref="A3:AB123"/>
+  <sortState ref="A4:Z122">
     <sortCondition ref="A3:A122"/>
   </sortState>
-  <tableColumns count="27">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="~Name" dataDxfId="15">
+  <tableColumns count="28">
+    <tableColumn id="1" name="Id"/>
+    <tableColumn id="2" name="~Name" dataDxfId="16">
       <calculatedColumnFormula>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="CdGroup" dataDxfId="14"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="CdTime"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="GainExp"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="GainFood"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="GainHealth"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="GainMental"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="ResourceId"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="ResourceCount"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="BlessId"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="RandomCardCatalog"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="RandomCardRate"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="DropItem"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Instruction"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="FarmItemId"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="FarmTime"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="GainLp"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="GainMp"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="GainPp"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="DirectDamage"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="FightRandomCardType"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="HolyWord"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="AddTowerHp"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="AttrAddAfterSummon"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Items"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="ItemCount"/>
+    <tableColumn id="16" name="CdGroup" dataDxfId="15"/>
+    <tableColumn id="25" name="CdTime"/>
+    <tableColumn id="3" name="GainExp"/>
+    <tableColumn id="4" name="GainFood"/>
+    <tableColumn id="21" name="GainHealth"/>
+    <tableColumn id="20" name="GainMental"/>
+    <tableColumn id="5" name="ResourceId"/>
+    <tableColumn id="6" name="ResourceCount"/>
+    <tableColumn id="23" name="BlessId"/>
+    <tableColumn id="26" name="RandomCardCount"/>
+    <tableColumn id="24" name="RandomCardCatalog"/>
+    <tableColumn id="8" name="RandomCardRate"/>
+    <tableColumn id="7" name="DropItem"/>
+    <tableColumn id="22" name="Instruction"/>
+    <tableColumn id="9" name="FarmItemId"/>
+    <tableColumn id="10" name="FarmTime"/>
+    <tableColumn id="11" name="GainLp"/>
+    <tableColumn id="12" name="GainMp"/>
+    <tableColumn id="13" name="GainPp"/>
+    <tableColumn id="14" name="DirectDamage"/>
+    <tableColumn id="15" name="FightRandomCardType"/>
+    <tableColumn id="17" name="HolyWord"/>
+    <tableColumn id="19" name="AddTowerHp"/>
+    <tableColumn id="18" name="AttrAddAfterSummon"/>
+    <tableColumn id="27" name="Items"/>
+    <tableColumn id="28" name="ItemCount"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2657,7 +2729,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2969,11 +3041,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA123"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2985,111 +3057,115 @@
     <col min="6" max="8" width="3.75" customWidth="1"/>
     <col min="9" max="10" width="4.25" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
-    <col min="12" max="12" width="6.875" customWidth="1"/>
-    <col min="13" max="13" width="12.625" customWidth="1"/>
-    <col min="14" max="14" width="9.75" customWidth="1"/>
-    <col min="15" max="15" width="6.75" customWidth="1"/>
-    <col min="16" max="16" width="8.625" customWidth="1"/>
-    <col min="17" max="17" width="6.625" customWidth="1"/>
-    <col min="18" max="25" width="7.375" customWidth="1"/>
-    <col min="26" max="26" width="18.25" customWidth="1"/>
+    <col min="12" max="12" width="5.25" customWidth="1"/>
+    <col min="13" max="13" width="6.875" customWidth="1"/>
+    <col min="14" max="14" width="12.625" customWidth="1"/>
+    <col min="15" max="15" width="9.75" customWidth="1"/>
+    <col min="16" max="16" width="6.75" customWidth="1"/>
+    <col min="17" max="17" width="8.625" customWidth="1"/>
+    <col min="18" max="18" width="6.625" customWidth="1"/>
+    <col min="19" max="26" width="7.375" customWidth="1"/>
+    <col min="27" max="27" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="77.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="E1" s="11" t="s">
+      <c r="C1" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="I1" s="11" t="s">
+      <c r="F1" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="O1" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="P1" s="11" t="s">
+      <c r="K1" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="R1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="S1" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="U1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="V1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="W1" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="V1" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="W1" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="X1" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y1" s="12" t="s">
-        <v>47</v>
+      <c r="X1" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y1" s="20" t="s">
+        <v>44</v>
       </c>
       <c r="Z1" s="20" t="s">
-        <v>147</v>
+        <v>35</v>
       </c>
       <c r="AA1" s="21" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.15">
+        <v>117</v>
+      </c>
+      <c r="AB1" s="22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>144</v>
+      <c r="C2" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>114</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
@@ -3113,27 +3189,27 @@
         <v>0</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>105</v>
+        <v>34</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="R2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="T2" s="3" t="s">
@@ -3146,45 +3222,48 @@
         <v>0</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="AA2" s="18" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.15">
+        <v>45</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB2" s="15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>142</v>
+        <v>47</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>112</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>2</v>
@@ -3193,95 +3272,101 @@
         <v>3</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>155</v>
+        <v>125</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>71</v>
+        <v>129</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>106</v>
+        <v>29</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="P3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="R3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="S3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="T3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="T3" s="8" t="s">
+      <c r="U3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="U3" s="8" t="s">
+      <c r="V3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="V3" s="8" t="s">
-        <v>25</v>
-      </c>
       <c r="W3" s="8" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="X3" s="8" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="Y3" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z3" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="AA3" s="19" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.15">
+        <v>46</v>
+      </c>
+      <c r="Z3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA3" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB3" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>22200001</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C4" s="14">
+        <v>126</v>
+      </c>
+      <c r="C4" s="12">
         <v>4</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="12">
         <v>15</v>
       </c>
-      <c r="L4" t="s">
-        <v>139</v>
+      <c r="L4">
+        <v>1</v>
       </c>
       <c r="M4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.15">
+        <v>151</v>
+      </c>
+      <c r="N4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>22200002</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C5" s="14">
+        <v>127</v>
+      </c>
+      <c r="C5" s="12">
         <v>4</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="12">
         <v>15</v>
       </c>
-      <c r="N5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="O5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>22300001</v>
       </c>
@@ -3289,14 +3374,14 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>新手礼包</v>
       </c>
-      <c r="Z6" t="s">
-        <v>152</v>
-      </c>
       <c r="AA6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.15">
+        <v>122</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>22301311</v>
       </c>
@@ -3304,11 +3389,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>素材袋</v>
       </c>
-      <c r="N7" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="O7" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>22301312</v>
       </c>
@@ -3316,11 +3401,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>高级素材袋</v>
       </c>
-      <c r="N8" s="13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="O8" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>22301313</v>
       </c>
@@ -3328,11 +3413,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>特级素材袋</v>
       </c>
-      <c r="N9" s="13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="O9" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>22301314</v>
       </c>
@@ -3340,11 +3425,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>极品素材袋</v>
       </c>
-      <c r="N10" s="13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="O10" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>22301201</v>
       </c>
@@ -3352,14 +3437,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>蓝色卡包</v>
       </c>
-      <c r="L11" t="s">
-        <v>34</v>
+      <c r="L11">
+        <v>5</v>
       </c>
       <c r="M11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.15">
+        <v>157</v>
+      </c>
+      <c r="N11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>22301202</v>
       </c>
@@ -3367,14 +3455,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>黄色卡包</v>
       </c>
-      <c r="L12" t="s">
-        <v>34</v>
+      <c r="L12">
+        <v>5</v>
       </c>
       <c r="M12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.15">
+        <v>157</v>
+      </c>
+      <c r="N12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>22301203</v>
       </c>
@@ -3382,14 +3473,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>红色卡包</v>
       </c>
-      <c r="L13" t="s">
-        <v>34</v>
+      <c r="L13">
+        <v>5</v>
       </c>
       <c r="M13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.15">
+        <v>157</v>
+      </c>
+      <c r="N13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>22301212</v>
       </c>
@@ -3397,14 +3491,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(无)</v>
       </c>
-      <c r="L14" t="s">
-        <v>27</v>
+      <c r="L14">
+        <v>1</v>
       </c>
       <c r="M14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.15">
+        <v>131</v>
+      </c>
+      <c r="N14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>22301213</v>
       </c>
@@ -3412,14 +3509,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(水)</v>
       </c>
-      <c r="L15" t="s">
-        <v>28</v>
+      <c r="L15">
+        <v>1</v>
       </c>
       <c r="M15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.15">
+        <v>132</v>
+      </c>
+      <c r="N15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>22301214</v>
       </c>
@@ -3427,14 +3527,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(风)</v>
       </c>
-      <c r="L16" t="s">
-        <v>29</v>
+      <c r="L16">
+        <v>1</v>
       </c>
       <c r="M16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
+        <v>133</v>
+      </c>
+      <c r="N16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>22301215</v>
       </c>
@@ -3442,14 +3545,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(地)</v>
       </c>
-      <c r="L17" t="s">
-        <v>30</v>
+      <c r="L17">
+        <v>1</v>
       </c>
       <c r="M17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+      <c r="N17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>22301216</v>
       </c>
@@ -3457,14 +3563,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(火)</v>
       </c>
-      <c r="L18" t="s">
-        <v>31</v>
+      <c r="L18">
+        <v>1</v>
       </c>
       <c r="M18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
+        <v>135</v>
+      </c>
+      <c r="N18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>22301217</v>
       </c>
@@ -3472,14 +3581,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(光)</v>
       </c>
-      <c r="L19" t="s">
-        <v>32</v>
+      <c r="L19">
+        <v>1</v>
       </c>
       <c r="M19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
+        <v>136</v>
+      </c>
+      <c r="N19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>22301218</v>
       </c>
@@ -3487,14 +3599,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(暗)</v>
       </c>
-      <c r="L20" t="s">
-        <v>33</v>
+      <c r="L20">
+        <v>1</v>
       </c>
       <c r="M20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
+        <v>137</v>
+      </c>
+      <c r="N20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>22301221</v>
       </c>
@@ -3502,14 +3617,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(生物)</v>
       </c>
-      <c r="L21" t="s">
-        <v>39</v>
+      <c r="L21">
+        <v>1</v>
       </c>
       <c r="M21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
+        <v>138</v>
+      </c>
+      <c r="N21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>22301222</v>
       </c>
@@ -3517,14 +3635,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(武器)</v>
       </c>
-      <c r="L22" t="s">
-        <v>40</v>
+      <c r="L22">
+        <v>1</v>
       </c>
       <c r="M22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
+        <v>139</v>
+      </c>
+      <c r="N22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>22301223</v>
       </c>
@@ -3532,14 +3653,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(法术)</v>
       </c>
-      <c r="L23" t="s">
-        <v>41</v>
+      <c r="L23">
+        <v>1</v>
       </c>
       <c r="M23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
+        <v>140</v>
+      </c>
+      <c r="N23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>22301231</v>
       </c>
@@ -3547,14 +3671,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(恶魔)</v>
       </c>
-      <c r="L24" t="s">
-        <v>88</v>
+      <c r="L24">
+        <v>1</v>
       </c>
       <c r="M24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
+        <v>141</v>
+      </c>
+      <c r="N24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>22301232</v>
       </c>
@@ -3562,14 +3689,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(机械)</v>
       </c>
-      <c r="L25" t="s">
-        <v>89</v>
+      <c r="L25">
+        <v>1</v>
       </c>
       <c r="M25" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
+        <v>142</v>
+      </c>
+      <c r="N25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>22301233</v>
       </c>
@@ -3577,14 +3707,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(精灵)</v>
       </c>
-      <c r="L26" t="s">
-        <v>90</v>
+      <c r="L26">
+        <v>1</v>
       </c>
       <c r="M26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
+        <v>143</v>
+      </c>
+      <c r="N26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>22301234</v>
       </c>
@@ -3592,14 +3725,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(昆虫)</v>
       </c>
-      <c r="L27" t="s">
-        <v>91</v>
+      <c r="L27">
+        <v>1</v>
       </c>
       <c r="M27" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
+        <v>144</v>
+      </c>
+      <c r="N27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>22301235</v>
       </c>
@@ -3607,14 +3743,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(龙)</v>
       </c>
-      <c r="L28" t="s">
-        <v>92</v>
+      <c r="L28">
+        <v>1</v>
       </c>
       <c r="M28" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
+        <v>145</v>
+      </c>
+      <c r="N28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>22301236</v>
       </c>
@@ -3622,14 +3761,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(鸟)</v>
       </c>
-      <c r="L29" t="s">
-        <v>93</v>
+      <c r="L29">
+        <v>1</v>
       </c>
       <c r="M29" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
+        <v>146</v>
+      </c>
+      <c r="N29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>22301237</v>
       </c>
@@ -3637,14 +3779,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(爬行)</v>
       </c>
-      <c r="L30" t="s">
-        <v>94</v>
+      <c r="L30">
+        <v>1</v>
       </c>
       <c r="M30" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.15">
+        <v>147</v>
+      </c>
+      <c r="N30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>22301238</v>
       </c>
@@ -3652,14 +3797,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(人类)</v>
       </c>
-      <c r="L31" t="s">
-        <v>95</v>
+      <c r="L31">
+        <v>1</v>
       </c>
       <c r="M31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.15">
+        <v>148</v>
+      </c>
+      <c r="N31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>22301239</v>
       </c>
@@ -3667,14 +3815,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(兽人)</v>
       </c>
-      <c r="L32" t="s">
-        <v>96</v>
+      <c r="L32">
+        <v>1</v>
       </c>
       <c r="M32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.15">
+        <v>149</v>
+      </c>
+      <c r="N32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>22301240</v>
       </c>
@@ -3682,14 +3833,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(亡灵)</v>
       </c>
-      <c r="L33" t="s">
-        <v>97</v>
+      <c r="L33">
+        <v>1</v>
       </c>
       <c r="M33" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.15">
+        <v>150</v>
+      </c>
+      <c r="N33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>22301241</v>
       </c>
@@ -3697,14 +3851,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(野兽)</v>
       </c>
-      <c r="L34" t="s">
-        <v>98</v>
+      <c r="L34">
+        <v>1</v>
       </c>
       <c r="M34" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.15">
+        <v>151</v>
+      </c>
+      <c r="N34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>22301242</v>
       </c>
@@ -3712,14 +3869,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(鱼)</v>
       </c>
-      <c r="L35" t="s">
-        <v>99</v>
+      <c r="L35">
+        <v>1</v>
       </c>
       <c r="M35" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.15">
+        <v>152</v>
+      </c>
+      <c r="N35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>22301243</v>
       </c>
@@ -3727,14 +3887,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(元素)</v>
       </c>
-      <c r="L36" t="s">
-        <v>100</v>
+      <c r="L36">
+        <v>1</v>
       </c>
       <c r="M36" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.15">
+        <v>153</v>
+      </c>
+      <c r="N36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>22301244</v>
       </c>
@@ -3742,14 +3905,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(植物)</v>
       </c>
-      <c r="L37" t="s">
-        <v>101</v>
+      <c r="L37">
+        <v>1</v>
       </c>
       <c r="M37" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.15">
+        <v>154</v>
+      </c>
+      <c r="N37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>22301245</v>
       </c>
@@ -3757,14 +3923,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(地精)</v>
       </c>
-      <c r="L38" t="s">
-        <v>102</v>
+      <c r="L38">
+        <v>1</v>
       </c>
       <c r="M38" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.15">
+        <v>155</v>
+      </c>
+      <c r="N38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>22301246</v>
       </c>
@@ -3772,14 +3941,17 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>卡牌补给包(石像)</v>
       </c>
-      <c r="L39" t="s">
-        <v>103</v>
+      <c r="L39">
+        <v>1</v>
       </c>
       <c r="M39" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.15">
+        <v>156</v>
+      </c>
+      <c r="N39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>22301301</v>
       </c>
@@ -3787,11 +3959,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(绿)</v>
       </c>
-      <c r="N40" s="13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O40" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>22301302</v>
       </c>
@@ -3799,11 +3971,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(蓝)</v>
       </c>
-      <c r="N41" s="9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O41" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>22301303</v>
       </c>
@@ -3811,11 +3983,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(红)</v>
       </c>
-      <c r="N42" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O42" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>22301304</v>
       </c>
@@ -3823,11 +3995,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(紫)</v>
       </c>
-      <c r="N43" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O43" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>22301305</v>
       </c>
@@ -3835,11 +4007,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(灰)</v>
       </c>
-      <c r="N44" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>22301321</v>
       </c>
@@ -3847,11 +4019,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>素材袋(无)</v>
       </c>
-      <c r="N45" s="14" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O45" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>22301322</v>
       </c>
@@ -3859,11 +4031,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>素材袋(水)</v>
       </c>
-      <c r="N46" s="14" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O46" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>22301323</v>
       </c>
@@ -3871,11 +4043,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>素材袋(风)</v>
       </c>
-      <c r="N47" s="14" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O47" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>22301324</v>
       </c>
@@ -3883,11 +4055,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>素材袋(火)</v>
       </c>
-      <c r="N48" s="14" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O48" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>22301325</v>
       </c>
@@ -3895,11 +4067,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>素材袋(地)</v>
       </c>
-      <c r="N49" s="14" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O49" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>22301326</v>
       </c>
@@ -3907,11 +4079,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>素材袋(光)</v>
       </c>
-      <c r="N50" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O50" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>22301327</v>
       </c>
@@ -3919,11 +4091,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>素材袋(暗)</v>
       </c>
-      <c r="N51" s="10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O51" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>22301331</v>
       </c>
@@ -3931,11 +4103,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(恶魔)</v>
       </c>
-      <c r="N52" s="9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O52" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>22301332</v>
       </c>
@@ -3943,11 +4115,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(机械)</v>
       </c>
-      <c r="N53" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O53" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>22301333</v>
       </c>
@@ -3955,11 +4127,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(精灵)</v>
       </c>
-      <c r="N54" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O54" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>22301334</v>
       </c>
@@ -3967,11 +4139,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(昆虫)</v>
       </c>
-      <c r="N55" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O55" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>22301335</v>
       </c>
@@ -3979,11 +4151,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(龙)</v>
       </c>
-      <c r="N56" s="9" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O56" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>22301336</v>
       </c>
@@ -3991,11 +4163,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(鸟)</v>
       </c>
-      <c r="N57" s="9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O57" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>22301337</v>
       </c>
@@ -4003,11 +4175,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(爬行)</v>
       </c>
-      <c r="N58" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O58" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>22301338</v>
       </c>
@@ -4015,11 +4187,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(人类)</v>
       </c>
-      <c r="N59" s="9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O59" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A60">
         <v>22301339</v>
       </c>
@@ -4027,11 +4199,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(兽人)</v>
       </c>
-      <c r="N60" s="9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O60" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>22301340</v>
       </c>
@@ -4039,11 +4211,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(亡灵)</v>
       </c>
-      <c r="N61" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O61" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>22301341</v>
       </c>
@@ -4051,11 +4223,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(野兽)</v>
       </c>
-      <c r="N62" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O62" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>22301342</v>
       </c>
@@ -4063,11 +4235,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(鱼)</v>
       </c>
-      <c r="N63" s="9" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O63" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>22301343</v>
       </c>
@@ -4075,11 +4247,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(元素)</v>
       </c>
-      <c r="N64" s="9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O64" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A65">
         <v>22301344</v>
       </c>
@@ -4087,11 +4259,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(植物)</v>
       </c>
-      <c r="N65" s="9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O65" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A66">
         <v>22301345</v>
       </c>
@@ -4099,11 +4271,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(地精)</v>
       </c>
-      <c r="N66" s="9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O66" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>22301346</v>
       </c>
@@ -4111,11 +4283,11 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>资源袋(石像)</v>
       </c>
-      <c r="N67" s="9" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="O67" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A68">
         <v>22301401</v>
       </c>
@@ -4130,7 +4302,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A69">
         <v>22301402</v>
       </c>
@@ -4145,7 +4317,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A70">
         <v>22301403</v>
       </c>
@@ -4160,7 +4332,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>22301404</v>
       </c>
@@ -4175,7 +4347,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A72">
         <v>22301405</v>
       </c>
@@ -4190,7 +4362,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A73">
         <v>22301406</v>
       </c>
@@ -4205,7 +4377,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A74">
         <v>22301407</v>
       </c>
@@ -4220,7 +4392,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A75">
         <v>22301408</v>
       </c>
@@ -4235,7 +4407,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A76">
         <v>22301411</v>
       </c>
@@ -4243,7 +4415,7 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>木材补给车</v>
       </c>
-      <c r="C76" s="22"/>
+      <c r="C76" s="17"/>
       <c r="I76">
         <v>2</v>
       </c>
@@ -4251,7 +4423,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A77">
         <v>22301412</v>
       </c>
@@ -4259,7 +4431,7 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>矿石补给车</v>
       </c>
-      <c r="C77" s="22"/>
+      <c r="C77" s="17"/>
       <c r="I77">
         <v>3</v>
       </c>
@@ -4267,7 +4439,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A78">
         <v>22301413</v>
       </c>
@@ -4275,7 +4447,7 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>水银补给车</v>
       </c>
-      <c r="C78" s="22"/>
+      <c r="C78" s="17"/>
       <c r="I78">
         <v>4</v>
       </c>
@@ -4283,7 +4455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A79">
         <v>22301414</v>
       </c>
@@ -4291,7 +4463,7 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>红宝石补给车</v>
       </c>
-      <c r="C79" s="22"/>
+      <c r="C79" s="17"/>
       <c r="I79">
         <v>5</v>
       </c>
@@ -4299,7 +4471,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A80">
         <v>22301415</v>
       </c>
@@ -4307,7 +4479,7 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>硫磺补给车</v>
       </c>
-      <c r="C80" s="22"/>
+      <c r="C80" s="17"/>
       <c r="I80">
         <v>6</v>
       </c>
@@ -4315,7 +4487,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A81">
         <v>22301416</v>
       </c>
@@ -4323,7 +4495,7 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>水晶补给车</v>
       </c>
-      <c r="C81" s="22"/>
+      <c r="C81" s="17"/>
       <c r="I81">
         <v>7</v>
       </c>
@@ -4331,7 +4503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A82">
         <v>22302001</v>
       </c>
@@ -4345,11 +4517,11 @@
       <c r="D82">
         <v>15</v>
       </c>
-      <c r="S82">
+      <c r="T82">
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A83">
         <v>22302002</v>
       </c>
@@ -4363,11 +4535,11 @@
       <c r="D83">
         <v>15</v>
       </c>
-      <c r="S83">
+      <c r="T83">
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A84">
         <v>22302003</v>
       </c>
@@ -4381,11 +4553,11 @@
       <c r="D84">
         <v>15</v>
       </c>
-      <c r="S84">
+      <c r="T84">
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A85">
         <v>22302004</v>
       </c>
@@ -4399,11 +4571,11 @@
       <c r="D85">
         <v>15</v>
       </c>
-      <c r="R85">
+      <c r="S85">
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A86">
         <v>22302005</v>
       </c>
@@ -4417,11 +4589,11 @@
       <c r="D86">
         <v>15</v>
       </c>
-      <c r="R86">
+      <c r="S86">
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A87">
         <v>22302006</v>
       </c>
@@ -4435,11 +4607,11 @@
       <c r="D87">
         <v>15</v>
       </c>
-      <c r="R87">
+      <c r="S87">
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A88">
         <v>22302007</v>
       </c>
@@ -4453,11 +4625,11 @@
       <c r="D88">
         <v>15</v>
       </c>
-      <c r="T88">
+      <c r="U88">
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A89">
         <v>22302008</v>
       </c>
@@ -4471,11 +4643,11 @@
       <c r="D89">
         <v>15</v>
       </c>
-      <c r="T89">
+      <c r="U89">
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A90">
         <v>22302009</v>
       </c>
@@ -4489,11 +4661,11 @@
       <c r="D90">
         <v>15</v>
       </c>
-      <c r="T90">
+      <c r="U90">
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A91">
         <v>22302013</v>
       </c>
@@ -4507,11 +4679,11 @@
       <c r="D91">
         <v>15</v>
       </c>
-      <c r="V91">
+      <c r="W91">
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A92">
         <v>22302014</v>
       </c>
@@ -4525,11 +4697,11 @@
       <c r="D92">
         <v>15</v>
       </c>
-      <c r="V92">
+      <c r="W92">
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A93">
         <v>22302015</v>
       </c>
@@ -4543,11 +4715,11 @@
       <c r="D93">
         <v>15</v>
       </c>
-      <c r="V93">
+      <c r="W93">
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A94">
         <v>22302016</v>
       </c>
@@ -4561,11 +4733,11 @@
       <c r="D94">
         <v>15</v>
       </c>
-      <c r="U94">
+      <c r="V94">
         <v>9999</v>
       </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A95">
         <v>22302017</v>
       </c>
@@ -4579,11 +4751,11 @@
       <c r="D95">
         <v>15</v>
       </c>
-      <c r="U95">
+      <c r="V95">
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A96">
         <v>22302018</v>
       </c>
@@ -4597,15 +4769,15 @@
       <c r="D96">
         <v>15</v>
       </c>
-      <c r="W96" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="X96" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="97" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A97">
         <v>22302030</v>
       </c>
-      <c r="B97" s="13" t="str">
+      <c r="B97" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>木质修理锤</v>
       </c>
@@ -4615,15 +4787,15 @@
       <c r="D97">
         <v>15</v>
       </c>
-      <c r="X97">
+      <c r="Y97">
         <v>200</v>
       </c>
     </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A98">
         <v>22302031</v>
       </c>
-      <c r="B98" s="13" t="str">
+      <c r="B98" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>钢铁修理锤</v>
       </c>
@@ -4633,15 +4805,15 @@
       <c r="D98">
         <v>15</v>
       </c>
-      <c r="X98">
+      <c r="Y98">
         <v>500</v>
       </c>
     </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A99">
         <v>22302032</v>
       </c>
-      <c r="B99" s="13" t="str">
+      <c r="B99" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>神圣修理锤</v>
       </c>
@@ -4651,15 +4823,15 @@
       <c r="D99">
         <v>15</v>
       </c>
-      <c r="X99">
+      <c r="Y99">
         <v>1000</v>
       </c>
     </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A100">
         <v>22302101</v>
       </c>
-      <c r="B100" s="13" t="str">
+      <c r="B100" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>经验之书</v>
       </c>
@@ -4673,11 +4845,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A101">
         <v>22302102</v>
       </c>
-      <c r="B101" s="13" t="str">
+      <c r="B101" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>能量之书</v>
       </c>
@@ -4691,11 +4863,11 @@
         <v>300</v>
       </c>
     </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A102">
         <v>22302103</v>
       </c>
-      <c r="B102" s="13" t="str">
+      <c r="B102" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>攻速药水</v>
       </c>
@@ -4705,15 +4877,15 @@
       <c r="D102">
         <v>15</v>
       </c>
-      <c r="Y102" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="Z102" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="103" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A103">
         <v>22302104</v>
       </c>
-      <c r="B103" s="13" t="str">
+      <c r="B103" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>守护药水</v>
       </c>
@@ -4723,15 +4895,15 @@
       <c r="D103">
         <v>15</v>
       </c>
-      <c r="Y103" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="Z103" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="104" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A104">
         <v>22302105</v>
       </c>
-      <c r="B104" s="13" t="str">
+      <c r="B104" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>法术药水</v>
       </c>
@@ -4741,15 +4913,15 @@
       <c r="D104">
         <v>15</v>
       </c>
-      <c r="Y104" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="Z104" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="105" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A105">
         <v>22302106</v>
       </c>
-      <c r="B105" s="13" t="str">
+      <c r="B105" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>技巧药水</v>
       </c>
@@ -4759,15 +4931,15 @@
       <c r="D105">
         <v>15</v>
       </c>
-      <c r="Y105" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="Z105" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="106" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A106">
         <v>22302107</v>
       </c>
-      <c r="B106" s="13" t="str">
+      <c r="B106" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>速度药水</v>
       </c>
@@ -4777,15 +4949,15 @@
       <c r="D106">
         <v>15</v>
       </c>
-      <c r="Y106" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="Z106" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="107" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A107">
         <v>22302108</v>
       </c>
-      <c r="B107" s="13" t="str">
+      <c r="B107" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>幸运药水</v>
       </c>
@@ -4795,11 +4967,11 @@
       <c r="D107">
         <v>15</v>
       </c>
-      <c r="Y107" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="Z107" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="108" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A108">
         <v>22302109</v>
       </c>
@@ -4813,11 +4985,11 @@
       <c r="D108">
         <v>15</v>
       </c>
-      <c r="Y108" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="Z108" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="109" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A109">
         <v>22302110</v>
       </c>
@@ -4835,7 +5007,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A110">
         <v>22302111</v>
       </c>
@@ -4853,7 +5025,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A111">
         <v>22302112</v>
       </c>
@@ -4871,7 +5043,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A112">
         <v>22302113</v>
       </c>
@@ -4879,15 +5051,15 @@
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>水晶球</v>
       </c>
-      <c r="O112" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="P112" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A113">
         <v>22302114</v>
       </c>
-      <c r="B113" s="14" t="str">
+      <c r="B113" s="12" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>坐骑黑豹</v>
       </c>
@@ -4895,98 +5067,98 @@
         <v>16000009</v>
       </c>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A114">
         <v>22302115</v>
       </c>
-      <c r="B114" s="14" t="str">
+      <c r="B114" s="12" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>坐骑鹰</v>
       </c>
-      <c r="D114" s="14"/>
+      <c r="D114" s="12"/>
       <c r="K114" s="9">
         <v>16002002</v>
       </c>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A115">
         <v>22302116</v>
       </c>
-      <c r="B115" s="14" t="str">
+      <c r="B115" s="12" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>坐骑传送器</v>
       </c>
-      <c r="D115" s="14"/>
+      <c r="D115" s="12"/>
       <c r="K115" s="9">
         <v>16002002</v>
       </c>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A116">
         <v>22301501</v>
       </c>
-      <c r="B116" s="13" t="str">
+      <c r="B116" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>种子-豌豆</v>
       </c>
-      <c r="D116" s="14"/>
-      <c r="P116">
+      <c r="D116" s="12"/>
+      <c r="Q116">
         <v>22301601</v>
       </c>
-      <c r="Q116">
+      <c r="R116">
         <v>900</v>
       </c>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A117">
         <v>22301502</v>
       </c>
-      <c r="B117" s="13" t="str">
+      <c r="B117" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>种子-玉米</v>
       </c>
-      <c r="P117">
+      <c r="Q117">
         <v>22301602</v>
       </c>
-      <c r="Q117">
+      <c r="R117">
         <v>900</v>
       </c>
     </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A118">
         <v>22301503</v>
       </c>
-      <c r="B118" s="13" t="str">
+      <c r="B118" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>种子-苹果</v>
       </c>
-      <c r="P118">
+      <c r="Q118">
         <v>22301603</v>
       </c>
-      <c r="Q118">
+      <c r="R118">
         <v>900</v>
       </c>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A119">
         <v>22301504</v>
       </c>
-      <c r="B119" s="13" t="str">
+      <c r="B119" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>种子-蓝莓</v>
       </c>
-      <c r="P119">
+      <c r="Q119">
         <v>22301604</v>
       </c>
-      <c r="Q119">
+      <c r="R119">
         <v>1800</v>
       </c>
     </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A120">
         <v>22301601</v>
       </c>
-      <c r="B120" s="13" t="str">
+      <c r="B120" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>豌豆</v>
       </c>
@@ -4994,11 +5166,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A121">
         <v>22301602</v>
       </c>
-      <c r="B121" s="13" t="str">
+      <c r="B121" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>玉米</v>
       </c>
@@ -5009,23 +5181,23 @@
         <v>20</v>
       </c>
     </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A122">
         <v>22301603</v>
       </c>
-      <c r="B122" s="13" t="str">
+      <c r="B122" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>苹果</v>
       </c>
-      <c r="R122">
+      <c r="S122">
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A123">
         <v>22301604</v>
       </c>
-      <c r="B123" s="13" t="str">
+      <c r="B123" s="11" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
         <v>蓝莓</v>
       </c>
@@ -5038,74 +5210,79 @@
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="Y42:Y74 P42:X64 P40:Y41 O17:Y23 O40:O64 N11:Y16 E113:K113 N24:Y39 O7:Y10 O65:X67 N120:Y122 N116:O119 Q116:Y119 E6:Y6 E123:AA123 E112:L112 E116:K122 E114:J115 Z4:AA4 E5:AA5 N68:X79 N82:Y115 E82:K111 E7:M75 L82:M122 Z6:AA79 Z82:AA123 B42:B95 K80:AA81 E76:H81 K76:M79">
-    <cfRule type="containsBlanks" dxfId="13" priority="23">
+  <conditionalFormatting sqref="Z42:Z74 Q42:Y64 Q40:Z41 P17:Z23 P40:P64 O11:Z16 E113:K113 O24:Z39 P7:Z10 P65:Y67 O120:Z122 O116:P119 R116:Z119 E6:Z6 E123:AB123 E112:M112 E116:K122 E114:J115 AA4:AB4 E5:AB5 O68:Y79 O82:Z115 E82:K111 L82:N122 AA6:AB79 AA82:AB123 B42:B95 K80:AB81 E76:H81 K76:N79 E7:N75">
+    <cfRule type="containsBlanks" dxfId="14" priority="24">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y75:Y79">
-    <cfRule type="containsBlanks" dxfId="12" priority="17">
-      <formula>LEN(TRIM(Y75))=0</formula>
+  <conditionalFormatting sqref="Z75:Z79">
+    <cfRule type="containsBlanks" dxfId="13" priority="18">
+      <formula>LEN(TRIM(Z75))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N21:N23">
-    <cfRule type="containsBlanks" dxfId="11" priority="14">
-      <formula>LEN(TRIM(N21))=0</formula>
+  <conditionalFormatting sqref="O21:O23">
+    <cfRule type="containsBlanks" dxfId="12" priority="15">
+      <formula>LEN(TRIM(O21))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N17:N20">
-    <cfRule type="containsBlanks" dxfId="10" priority="13">
-      <formula>LEN(TRIM(N17))=0</formula>
+  <conditionalFormatting sqref="O17:O20">
+    <cfRule type="containsBlanks" dxfId="11" priority="14">
+      <formula>LEN(TRIM(O17))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O4:Y4 E4:K4">
-    <cfRule type="containsBlanks" dxfId="9" priority="12">
+  <conditionalFormatting sqref="P4:Z4 E4:K4">
+    <cfRule type="containsBlanks" dxfId="10" priority="13">
       <formula>LEN(TRIM(E4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N4">
-    <cfRule type="containsBlanks" dxfId="8" priority="11">
-      <formula>LEN(TRIM(N4))=0</formula>
+  <conditionalFormatting sqref="O4">
+    <cfRule type="containsBlanks" dxfId="9" priority="12">
+      <formula>LEN(TRIM(O4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L4:M4">
-    <cfRule type="containsBlanks" dxfId="7" priority="10">
+  <conditionalFormatting sqref="L4 N4">
+    <cfRule type="containsBlanks" dxfId="8" priority="11">
       <formula>LEN(TRIM(L4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:D14 C18:D24 C41:D123">
-    <cfRule type="containsBlanks" dxfId="6" priority="9">
+    <cfRule type="containsBlanks" dxfId="7" priority="10">
       <formula>LEN(TRIM(C7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:D17">
-    <cfRule type="containsBlanks" dxfId="5" priority="8">
+    <cfRule type="containsBlanks" dxfId="6" priority="9">
       <formula>LEN(TRIM(C15))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:D54">
-    <cfRule type="containsBlanks" dxfId="4" priority="7">
+    <cfRule type="containsBlanks" dxfId="5" priority="8">
       <formula>LEN(TRIM(C25))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:D6">
-    <cfRule type="containsBlanks" dxfId="3" priority="5">
+    <cfRule type="containsBlanks" dxfId="4" priority="6">
       <formula>LEN(TRIM(C6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="containsBlanks" dxfId="2" priority="4">
+    <cfRule type="containsBlanks" dxfId="3" priority="5">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="containsBlanks" dxfId="1" priority="3">
+    <cfRule type="containsBlanks" dxfId="2" priority="4">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I76:J81">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(I76))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M4">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(I76))=0</formula>
+      <formula>LEN(TRIM(M4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
a well levelup form effect
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/ItemConsumer.xlsx
+++ b/ConfigData/Xlsx/ItemConsumer.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -436,14 +436,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>xiaoxingmofayaoji;zhongxingmofayaoji;chushiziyuanbao;suijihuanshouka;suijiwuqika;suijimofaka</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>5;5;1;5;3;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>获得祝福</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -599,6 +591,14 @@
   </si>
   <si>
     <t>1;1;0;0;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>xiaoxingmofayaoji;zhongxingmofayaoji;suijihuanshouka;suijiwuqika;suijimofaka</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>5;5;5;3;3</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1391,16 +1391,6 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="30">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2234,6 +2224,16 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2297,7 +2297,7 @@
             <v>22301201</v>
           </cell>
           <cell r="B5" t="str">
-            <v>蓝色卡包</v>
+            <v>经典卡包</v>
           </cell>
         </row>
         <row r="6">
@@ -2305,7 +2305,7 @@
             <v>22301202</v>
           </cell>
           <cell r="B6" t="str">
-            <v>黄色卡包</v>
+            <v>经典卡包加强</v>
           </cell>
         </row>
         <row r="7">
@@ -2313,7 +2313,7 @@
             <v>22301203</v>
           </cell>
           <cell r="B7" t="str">
-            <v>红色卡包</v>
+            <v>经典卡包收藏</v>
           </cell>
         </row>
         <row r="8">
@@ -3236,42 +3236,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:AB123" totalsRowShown="0" headerRowDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:AB123" totalsRowShown="0" headerRowDxfId="28">
   <autoFilter ref="A3:AB123"/>
   <sortState ref="A4:Z122">
     <sortCondition ref="A3:A122"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="28"/>
-    <tableColumn id="2" name="~Name" dataDxfId="27">
+    <tableColumn id="1" name="Id" dataDxfId="27"/>
+    <tableColumn id="2" name="~Name" dataDxfId="26">
       <calculatedColumnFormula>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="CdGroup" dataDxfId="26"/>
-    <tableColumn id="25" name="CdTime" dataDxfId="25"/>
-    <tableColumn id="3" name="GainExp" dataDxfId="24"/>
-    <tableColumn id="4" name="GainFood" dataDxfId="23"/>
-    <tableColumn id="21" name="GainHealth" dataDxfId="22"/>
-    <tableColumn id="20" name="GainMental" dataDxfId="21"/>
-    <tableColumn id="5" name="ResourceId" dataDxfId="20"/>
-    <tableColumn id="6" name="ResourceCount" dataDxfId="19"/>
-    <tableColumn id="23" name="BlessId" dataDxfId="18"/>
-    <tableColumn id="26" name="RandomCardCount" dataDxfId="17"/>
-    <tableColumn id="24" name="RandomCardCatalog" dataDxfId="16"/>
-    <tableColumn id="8" name="RandomCardRate" dataDxfId="15"/>
-    <tableColumn id="7" name="DropItem" dataDxfId="14"/>
-    <tableColumn id="22" name="Instruction" dataDxfId="13"/>
-    <tableColumn id="9" name="FarmItemId" dataDxfId="12"/>
-    <tableColumn id="10" name="FarmTime" dataDxfId="11"/>
-    <tableColumn id="29" name="DungeonAttr" dataDxfId="1"/>
-    <tableColumn id="11" name="GainLp" dataDxfId="10"/>
-    <tableColumn id="12" name="GainMp" dataDxfId="9"/>
-    <tableColumn id="13" name="GainPp" dataDxfId="8"/>
-    <tableColumn id="14" name="DirectDamage" dataDxfId="7"/>
-    <tableColumn id="15" name="FightRandomCardType" dataDxfId="6"/>
-    <tableColumn id="17" name="HolyWord" dataDxfId="5"/>
-    <tableColumn id="19" name="AddTowerHp" dataDxfId="4"/>
-    <tableColumn id="27" name="Items" dataDxfId="3"/>
-    <tableColumn id="28" name="ItemCount" dataDxfId="2"/>
+    <tableColumn id="16" name="CdGroup" dataDxfId="25"/>
+    <tableColumn id="25" name="CdTime" dataDxfId="24"/>
+    <tableColumn id="3" name="GainExp" dataDxfId="23"/>
+    <tableColumn id="4" name="GainFood" dataDxfId="22"/>
+    <tableColumn id="21" name="GainHealth" dataDxfId="21"/>
+    <tableColumn id="20" name="GainMental" dataDxfId="20"/>
+    <tableColumn id="5" name="ResourceId" dataDxfId="19"/>
+    <tableColumn id="6" name="ResourceCount" dataDxfId="18"/>
+    <tableColumn id="23" name="BlessId" dataDxfId="17"/>
+    <tableColumn id="26" name="RandomCardCount" dataDxfId="16"/>
+    <tableColumn id="24" name="RandomCardCatalog" dataDxfId="15"/>
+    <tableColumn id="8" name="RandomCardRate" dataDxfId="14"/>
+    <tableColumn id="7" name="DropItem" dataDxfId="13"/>
+    <tableColumn id="22" name="Instruction" dataDxfId="12"/>
+    <tableColumn id="9" name="FarmItemId" dataDxfId="11"/>
+    <tableColumn id="10" name="FarmTime" dataDxfId="10"/>
+    <tableColumn id="29" name="DungeonAttr" dataDxfId="9"/>
+    <tableColumn id="11" name="GainLp" dataDxfId="8"/>
+    <tableColumn id="12" name="GainMp" dataDxfId="7"/>
+    <tableColumn id="13" name="GainPp" dataDxfId="6"/>
+    <tableColumn id="14" name="DirectDamage" dataDxfId="5"/>
+    <tableColumn id="15" name="FightRandomCardType" dataDxfId="4"/>
+    <tableColumn id="17" name="HolyWord" dataDxfId="3"/>
+    <tableColumn id="19" name="AddTowerHp" dataDxfId="2"/>
+    <tableColumn id="27" name="Items" dataDxfId="1"/>
+    <tableColumn id="28" name="ItemCount" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3600,8 +3600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100:D100"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3657,10 +3657,10 @@
         <v>14</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M1" s="14" t="s">
         <v>66</v>
@@ -3681,7 +3681,7 @@
         <v>16</v>
       </c>
       <c r="S1" s="14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="T1" s="16" t="s">
         <v>19</v>
@@ -3767,7 +3767,7 @@
         <v>0</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="T2" s="6" t="s">
         <v>0</v>
@@ -3829,13 +3829,13 @@
         <v>3</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>29</v>
@@ -3853,7 +3853,7 @@
         <v>5</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="T3" s="7" t="s">
         <v>6</v>
@@ -3888,7 +3888,7 @@
         <v>22200001</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C4" s="9">
         <v>4</v>
@@ -3907,7 +3907,7 @@
         <v>1</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="N4" s="9" t="s">
         <v>101</v>
@@ -3932,7 +3932,7 @@
         <v>22200002</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C5" s="9">
         <v>4</v>
@@ -3951,7 +3951,7 @@
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
       <c r="O5" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
@@ -4000,10 +4000,10 @@
       <c r="Y6" s="9"/>
       <c r="Z6" s="9"/>
       <c r="AA6" s="9" t="s">
-        <v>113</v>
+        <v>158</v>
       </c>
       <c r="AB6" s="9" t="s">
-        <v>114</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.15">
@@ -4160,7 +4160,7 @@
       </c>
       <c r="B11" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>蓝色卡包</v>
+        <v>经典卡包</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -4175,7 +4175,7 @@
         <v>5</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="N11" s="9" t="s">
         <v>26</v>
@@ -4201,7 +4201,7 @@
       </c>
       <c r="B12" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>黄色卡包</v>
+        <v>经典卡包加强</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -4216,7 +4216,7 @@
         <v>5</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="N12" s="9" t="s">
         <v>27</v>
@@ -4242,7 +4242,7 @@
       </c>
       <c r="B13" s="9" t="str">
         <f>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</f>
-        <v>红色卡包</v>
+        <v>经典卡包收藏</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -4257,7 +4257,7 @@
         <v>5</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="N13" s="9" t="s">
         <v>28</v>
@@ -4298,7 +4298,7 @@
         <v>1</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="N14" s="9" t="s">
         <v>26</v>
@@ -4339,7 +4339,7 @@
         <v>1</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="N15" s="9" t="s">
         <v>26</v>
@@ -4380,7 +4380,7 @@
         <v>1</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="N16" s="9" t="s">
         <v>26</v>
@@ -4421,7 +4421,7 @@
         <v>1</v>
       </c>
       <c r="M17" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N17" s="9" t="s">
         <v>26</v>
@@ -4462,7 +4462,7 @@
         <v>1</v>
       </c>
       <c r="M18" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N18" s="9" t="s">
         <v>26</v>
@@ -4503,7 +4503,7 @@
         <v>1</v>
       </c>
       <c r="M19" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N19" s="9" t="s">
         <v>26</v>
@@ -4544,7 +4544,7 @@
         <v>1</v>
       </c>
       <c r="M20" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="N20" s="9" t="s">
         <v>26</v>
@@ -4585,7 +4585,7 @@
         <v>1</v>
       </c>
       <c r="M21" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="N21" s="9" t="s">
         <v>26</v>
@@ -4626,7 +4626,7 @@
         <v>1</v>
       </c>
       <c r="M22" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="N22" s="9" t="s">
         <v>26</v>
@@ -4667,7 +4667,7 @@
         <v>1</v>
       </c>
       <c r="M23" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="N23" s="9" t="s">
         <v>26</v>
@@ -4708,7 +4708,7 @@
         <v>1</v>
       </c>
       <c r="M24" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N24" s="9" t="s">
         <v>50</v>
@@ -4749,7 +4749,7 @@
         <v>1</v>
       </c>
       <c r="M25" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="N25" s="9" t="s">
         <v>51</v>
@@ -4790,7 +4790,7 @@
         <v>1</v>
       </c>
       <c r="M26" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="N26" s="9" t="s">
         <v>52</v>
@@ -4831,7 +4831,7 @@
         <v>1</v>
       </c>
       <c r="M27" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="N27" s="9" t="s">
         <v>53</v>
@@ -4872,7 +4872,7 @@
         <v>1</v>
       </c>
       <c r="M28" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="N28" s="9" t="s">
         <v>54</v>
@@ -4913,7 +4913,7 @@
         <v>1</v>
       </c>
       <c r="M29" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="N29" s="9" t="s">
         <v>55</v>
@@ -4954,7 +4954,7 @@
         <v>1</v>
       </c>
       <c r="M30" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="N30" s="9" t="s">
         <v>56</v>
@@ -4995,7 +4995,7 @@
         <v>1</v>
       </c>
       <c r="M31" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="N31" s="9" t="s">
         <v>57</v>
@@ -5036,7 +5036,7 @@
         <v>1</v>
       </c>
       <c r="M32" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="N32" s="9" t="s">
         <v>58</v>
@@ -5077,7 +5077,7 @@
         <v>1</v>
       </c>
       <c r="M33" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="N33" s="9" t="s">
         <v>59</v>
@@ -5118,7 +5118,7 @@
         <v>1</v>
       </c>
       <c r="M34" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="N34" s="9" t="s">
         <v>60</v>
@@ -5159,7 +5159,7 @@
         <v>1</v>
       </c>
       <c r="M35" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="N35" s="9" t="s">
         <v>61</v>
@@ -5200,7 +5200,7 @@
         <v>1</v>
       </c>
       <c r="M36" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="N36" s="9" t="s">
         <v>62</v>
@@ -5241,7 +5241,7 @@
         <v>1</v>
       </c>
       <c r="M37" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="N37" s="9" t="s">
         <v>63</v>
@@ -5282,7 +5282,7 @@
         <v>1</v>
       </c>
       <c r="M38" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="N38" s="9" t="s">
         <v>64</v>
@@ -5323,7 +5323,7 @@
         <v>1</v>
       </c>
       <c r="M39" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="N39" s="9" t="s">
         <v>65</v>
@@ -7762,7 +7762,7 @@
       <c r="Q102" s="9"/>
       <c r="R102" s="9"/>
       <c r="S102" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="T102" s="9"/>
       <c r="U102" s="9"/>
@@ -7799,7 +7799,7 @@
       <c r="Q103" s="9"/>
       <c r="R103" s="9"/>
       <c r="S103" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="T103" s="9"/>
       <c r="U103" s="9"/>
@@ -7836,7 +7836,7 @@
       <c r="Q104" s="9"/>
       <c r="R104" s="9"/>
       <c r="S104" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="T104" s="9"/>
       <c r="U104" s="9"/>
@@ -7873,7 +7873,7 @@
       <c r="Q105" s="9"/>
       <c r="R105" s="9"/>
       <c r="S105" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="T105" s="9"/>
       <c r="U105" s="9"/>
@@ -7910,7 +7910,7 @@
       <c r="Q106" s="9"/>
       <c r="R106" s="9"/>
       <c r="S106" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="T106" s="9"/>
       <c r="U106" s="9"/>
@@ -7947,7 +7947,7 @@
       <c r="Q107" s="9"/>
       <c r="R107" s="9"/>
       <c r="S107" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="T107" s="9"/>
       <c r="U107" s="9"/>
@@ -7984,7 +7984,7 @@
       <c r="Q108" s="9"/>
       <c r="R108" s="9"/>
       <c r="S108" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="T108" s="9"/>
       <c r="U108" s="9"/>
@@ -8566,7 +8566,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="D4:AB4 C5:AB123">
-    <cfRule type="containsBlanks" dxfId="0" priority="26">
+    <cfRule type="containsBlanks" dxfId="29" priority="26">
       <formula>LEN(TRIM(C4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
balance the quest exp
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/ItemConsumer.xlsx
+++ b/ConfigData/Xlsx/ItemConsumer.xlsx
@@ -594,11 +594,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>xiaoxingmofayaoji;zhongxingmofayaoji;suijihuanshouka;suijiwuqika;suijimofaka</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>5;5;5;3;3</t>
+    <t>jinbi;xiaoxingmofayaoji;zhongxingmofayaoji;suijihuanshouka;suijiwuqika;suijimofaka</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>2;5;5;5;3;3</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -3600,7 +3600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
farm need ep to harvest not time
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/ItemConsumer.xlsx
+++ b/ConfigData/Xlsx/ItemConsumer.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{ECE9F9DD-17FA-49C3-BB83-079D9C8DC66A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -44,10 +45,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>FarmTime</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>GainLp</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -88,10 +85,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>产出时间</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>string</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -599,13 +592,21 @@
   </si>
   <si>
     <t>2;5;5;5;3;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>产出需求</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>FarmEnergy</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3236,42 +3237,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:AB123" totalsRowShown="0" headerRowDxfId="28">
-  <autoFilter ref="A3:AB123"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表2" displayName="表2" ref="A3:AB123" totalsRowShown="0" headerRowDxfId="28">
+  <autoFilter ref="A3:AB123" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState ref="A4:Z122">
     <sortCondition ref="A3:A122"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="27"/>
-    <tableColumn id="2" name="~Name" dataDxfId="26">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="~Name" dataDxfId="26">
       <calculatedColumnFormula>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="CdGroup" dataDxfId="25"/>
-    <tableColumn id="25" name="CdTime" dataDxfId="24"/>
-    <tableColumn id="3" name="GainExp" dataDxfId="23"/>
-    <tableColumn id="4" name="GainFood" dataDxfId="22"/>
-    <tableColumn id="21" name="GainHealth" dataDxfId="21"/>
-    <tableColumn id="20" name="GainMental" dataDxfId="20"/>
-    <tableColumn id="5" name="ResourceId" dataDxfId="19"/>
-    <tableColumn id="6" name="ResourceCount" dataDxfId="18"/>
-    <tableColumn id="23" name="BlessId" dataDxfId="17"/>
-    <tableColumn id="26" name="RandomCardCount" dataDxfId="16"/>
-    <tableColumn id="24" name="RandomCardCatalog" dataDxfId="15"/>
-    <tableColumn id="8" name="RandomCardRate" dataDxfId="14"/>
-    <tableColumn id="7" name="DropItem" dataDxfId="13"/>
-    <tableColumn id="22" name="Instruction" dataDxfId="12"/>
-    <tableColumn id="9" name="FarmItemId" dataDxfId="11"/>
-    <tableColumn id="10" name="FarmTime" dataDxfId="10"/>
-    <tableColumn id="29" name="DungeonAttr" dataDxfId="9"/>
-    <tableColumn id="11" name="GainLp" dataDxfId="8"/>
-    <tableColumn id="12" name="GainMp" dataDxfId="7"/>
-    <tableColumn id="13" name="GainPp" dataDxfId="6"/>
-    <tableColumn id="14" name="DirectDamage" dataDxfId="5"/>
-    <tableColumn id="15" name="FightRandomCardType" dataDxfId="4"/>
-    <tableColumn id="17" name="HolyWord" dataDxfId="3"/>
-    <tableColumn id="19" name="AddTowerHp" dataDxfId="2"/>
-    <tableColumn id="27" name="Items" dataDxfId="1"/>
-    <tableColumn id="28" name="ItemCount" dataDxfId="0"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="CdGroup" dataDxfId="25"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="CdTime" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="GainExp" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="GainFood" dataDxfId="22"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="GainHealth" dataDxfId="21"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="GainMental" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="ResourceId" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="ResourceCount" dataDxfId="18"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="BlessId" dataDxfId="17"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="RandomCardCount" dataDxfId="16"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="RandomCardCatalog" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="RandomCardRate" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="DropItem" dataDxfId="13"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Instruction" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="FarmItemId" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="FarmEnergy" dataDxfId="10"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="DungeonAttr" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="GainLp" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="GainMp" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="GainPp" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="DirectDamage" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="FightRandomCardType" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="HolyWord" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="AddTowerHp" dataDxfId="2"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Items" dataDxfId="1"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="ItemCount" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3597,11 +3598,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AA6" sqref="AA6"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="R119" sqref="R119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3627,88 +3628,88 @@
   <sheetData>
     <row r="1" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="F1" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="S1" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="T1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z1" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA1" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="P1" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q1" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="T1" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z1" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA1" s="17" t="s">
-        <v>108</v>
-      </c>
       <c r="AB1" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.15">
@@ -3716,13 +3717,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
@@ -3746,19 +3747,19 @@
         <v>0</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>0</v>
@@ -3767,7 +3768,7 @@
         <v>0</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="T2" s="6" t="s">
         <v>0</v>
@@ -3785,42 +3786,42 @@
         <v>0</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AB2" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>2</v>
@@ -3829,58 +3830,58 @@
         <v>3</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="R3" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="T3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="T3" s="7" t="s">
+      <c r="U3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="U3" s="8" t="s">
+      <c r="V3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="V3" s="8" t="s">
+      <c r="W3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="W3" s="8" t="s">
-        <v>9</v>
-      </c>
       <c r="X3" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="Y3" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Z3" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="AA3" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB3" s="13" t="s">
         <v>107</v>
-      </c>
-      <c r="AB3" s="13" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.15">
@@ -3888,7 +3889,7 @@
         <v>22200001</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C4" s="9">
         <v>4</v>
@@ -3907,10 +3908,10 @@
         <v>1</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="O4" s="9"/>
       <c r="P4" s="9"/>
@@ -3932,7 +3933,7 @@
         <v>22200002</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C5" s="9">
         <v>4</v>
@@ -3951,7 +3952,7 @@
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
       <c r="O5" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
@@ -4000,10 +4001,10 @@
       <c r="Y6" s="9"/>
       <c r="Z6" s="9"/>
       <c r="AA6" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AB6" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.15">
@@ -4027,7 +4028,7 @@
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
       <c r="O7" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
@@ -4064,7 +4065,7 @@
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
       <c r="O8" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
@@ -4101,7 +4102,7 @@
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
       <c r="O9" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
@@ -4138,7 +4139,7 @@
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
       <c r="O10" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
@@ -4175,10 +4176,10 @@
         <v>5</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O11" s="9"/>
       <c r="P11" s="9"/>
@@ -4216,10 +4217,10 @@
         <v>5</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
@@ -4257,10 +4258,10 @@
         <v>5</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
@@ -4298,10 +4299,10 @@
         <v>1</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O14" s="9"/>
       <c r="P14" s="9"/>
@@ -4339,10 +4340,10 @@
         <v>1</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O15" s="9"/>
       <c r="P15" s="9"/>
@@ -4380,10 +4381,10 @@
         <v>1</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O16" s="9"/>
       <c r="P16" s="9"/>
@@ -4421,10 +4422,10 @@
         <v>1</v>
       </c>
       <c r="M17" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O17" s="9"/>
       <c r="P17" s="9"/>
@@ -4462,10 +4463,10 @@
         <v>1</v>
       </c>
       <c r="M18" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O18" s="9"/>
       <c r="P18" s="9"/>
@@ -4503,10 +4504,10 @@
         <v>1</v>
       </c>
       <c r="M19" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O19" s="9"/>
       <c r="P19" s="9"/>
@@ -4544,10 +4545,10 @@
         <v>1</v>
       </c>
       <c r="M20" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O20" s="9"/>
       <c r="P20" s="9"/>
@@ -4585,10 +4586,10 @@
         <v>1</v>
       </c>
       <c r="M21" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O21" s="9"/>
       <c r="P21" s="9"/>
@@ -4626,10 +4627,10 @@
         <v>1</v>
       </c>
       <c r="M22" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O22" s="9"/>
       <c r="P22" s="9"/>
@@ -4667,10 +4668,10 @@
         <v>1</v>
       </c>
       <c r="M23" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O23" s="9"/>
       <c r="P23" s="9"/>
@@ -4708,10 +4709,10 @@
         <v>1</v>
       </c>
       <c r="M24" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O24" s="9"/>
       <c r="P24" s="9"/>
@@ -4749,10 +4750,10 @@
         <v>1</v>
       </c>
       <c r="M25" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="O25" s="9"/>
       <c r="P25" s="9"/>
@@ -4790,10 +4791,10 @@
         <v>1</v>
       </c>
       <c r="M26" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="N26" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="O26" s="9"/>
       <c r="P26" s="9"/>
@@ -4831,10 +4832,10 @@
         <v>1</v>
       </c>
       <c r="M27" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="N27" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O27" s="9"/>
       <c r="P27" s="9"/>
@@ -4872,10 +4873,10 @@
         <v>1</v>
       </c>
       <c r="M28" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="N28" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O28" s="9"/>
       <c r="P28" s="9"/>
@@ -4913,10 +4914,10 @@
         <v>1</v>
       </c>
       <c r="M29" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="N29" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O29" s="9"/>
       <c r="P29" s="9"/>
@@ -4954,10 +4955,10 @@
         <v>1</v>
       </c>
       <c r="M30" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="N30" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O30" s="9"/>
       <c r="P30" s="9"/>
@@ -4995,10 +4996,10 @@
         <v>1</v>
       </c>
       <c r="M31" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="N31" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O31" s="9"/>
       <c r="P31" s="9"/>
@@ -5036,10 +5037,10 @@
         <v>1</v>
       </c>
       <c r="M32" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="N32" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="O32" s="9"/>
       <c r="P32" s="9"/>
@@ -5077,10 +5078,10 @@
         <v>1</v>
       </c>
       <c r="M33" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="N33" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O33" s="9"/>
       <c r="P33" s="9"/>
@@ -5118,10 +5119,10 @@
         <v>1</v>
       </c>
       <c r="M34" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="N34" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O34" s="9"/>
       <c r="P34" s="9"/>
@@ -5159,10 +5160,10 @@
         <v>1</v>
       </c>
       <c r="M35" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="N35" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O35" s="9"/>
       <c r="P35" s="9"/>
@@ -5200,10 +5201,10 @@
         <v>1</v>
       </c>
       <c r="M36" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="N36" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O36" s="9"/>
       <c r="P36" s="9"/>
@@ -5241,10 +5242,10 @@
         <v>1</v>
       </c>
       <c r="M37" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="N37" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="O37" s="9"/>
       <c r="P37" s="9"/>
@@ -5282,10 +5283,10 @@
         <v>1</v>
       </c>
       <c r="M38" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="N38" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O38" s="9"/>
       <c r="P38" s="9"/>
@@ -5323,10 +5324,10 @@
         <v>1</v>
       </c>
       <c r="M39" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="N39" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O39" s="9"/>
       <c r="P39" s="9"/>
@@ -5364,7 +5365,7 @@
       <c r="M40" s="9"/>
       <c r="N40" s="9"/>
       <c r="O40" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P40" s="9"/>
       <c r="Q40" s="9"/>
@@ -5401,7 +5402,7 @@
       <c r="M41" s="9"/>
       <c r="N41" s="9"/>
       <c r="O41" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="P41" s="9"/>
       <c r="Q41" s="9"/>
@@ -5438,7 +5439,7 @@
       <c r="M42" s="9"/>
       <c r="N42" s="9"/>
       <c r="O42" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P42" s="9"/>
       <c r="Q42" s="9"/>
@@ -5475,7 +5476,7 @@
       <c r="M43" s="9"/>
       <c r="N43" s="9"/>
       <c r="O43" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P43" s="9"/>
       <c r="Q43" s="9"/>
@@ -5512,7 +5513,7 @@
       <c r="M44" s="9"/>
       <c r="N44" s="9"/>
       <c r="O44" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P44" s="9"/>
       <c r="Q44" s="9"/>
@@ -5549,7 +5550,7 @@
       <c r="M45" s="9"/>
       <c r="N45" s="9"/>
       <c r="O45" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="P45" s="9"/>
       <c r="Q45" s="9"/>
@@ -5586,7 +5587,7 @@
       <c r="M46" s="9"/>
       <c r="N46" s="9"/>
       <c r="O46" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P46" s="9"/>
       <c r="Q46" s="9"/>
@@ -5623,7 +5624,7 @@
       <c r="M47" s="9"/>
       <c r="N47" s="9"/>
       <c r="O47" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P47" s="9"/>
       <c r="Q47" s="9"/>
@@ -5660,7 +5661,7 @@
       <c r="M48" s="9"/>
       <c r="N48" s="9"/>
       <c r="O48" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="P48" s="9"/>
       <c r="Q48" s="9"/>
@@ -5697,7 +5698,7 @@
       <c r="M49" s="9"/>
       <c r="N49" s="9"/>
       <c r="O49" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="P49" s="9"/>
       <c r="Q49" s="9"/>
@@ -5734,7 +5735,7 @@
       <c r="M50" s="9"/>
       <c r="N50" s="9"/>
       <c r="O50" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="P50" s="9"/>
       <c r="Q50" s="9"/>
@@ -5771,7 +5772,7 @@
       <c r="M51" s="9"/>
       <c r="N51" s="9"/>
       <c r="O51" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="P51" s="9"/>
       <c r="Q51" s="9"/>
@@ -5808,7 +5809,7 @@
       <c r="M52" s="9"/>
       <c r="N52" s="9"/>
       <c r="O52" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="P52" s="9"/>
       <c r="Q52" s="9"/>
@@ -5845,7 +5846,7 @@
       <c r="M53" s="9"/>
       <c r="N53" s="9"/>
       <c r="O53" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="P53" s="9"/>
       <c r="Q53" s="9"/>
@@ -5882,7 +5883,7 @@
       <c r="M54" s="9"/>
       <c r="N54" s="9"/>
       <c r="O54" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P54" s="9"/>
       <c r="Q54" s="9"/>
@@ -5919,7 +5920,7 @@
       <c r="M55" s="9"/>
       <c r="N55" s="9"/>
       <c r="O55" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="P55" s="9"/>
       <c r="Q55" s="9"/>
@@ -5956,7 +5957,7 @@
       <c r="M56" s="9"/>
       <c r="N56" s="9"/>
       <c r="O56" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="P56" s="9"/>
       <c r="Q56" s="9"/>
@@ -5993,7 +5994,7 @@
       <c r="M57" s="9"/>
       <c r="N57" s="9"/>
       <c r="O57" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P57" s="9"/>
       <c r="Q57" s="9"/>
@@ -6030,7 +6031,7 @@
       <c r="M58" s="9"/>
       <c r="N58" s="9"/>
       <c r="O58" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P58" s="9"/>
       <c r="Q58" s="9"/>
@@ -6067,7 +6068,7 @@
       <c r="M59" s="9"/>
       <c r="N59" s="9"/>
       <c r="O59" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="P59" s="9"/>
       <c r="Q59" s="9"/>
@@ -6104,7 +6105,7 @@
       <c r="M60" s="9"/>
       <c r="N60" s="9"/>
       <c r="O60" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="P60" s="9"/>
       <c r="Q60" s="9"/>
@@ -6141,7 +6142,7 @@
       <c r="M61" s="9"/>
       <c r="N61" s="9"/>
       <c r="O61" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="P61" s="9"/>
       <c r="Q61" s="9"/>
@@ -6178,7 +6179,7 @@
       <c r="M62" s="9"/>
       <c r="N62" s="9"/>
       <c r="O62" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="P62" s="9"/>
       <c r="Q62" s="9"/>
@@ -6215,7 +6216,7 @@
       <c r="M63" s="9"/>
       <c r="N63" s="9"/>
       <c r="O63" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="P63" s="9"/>
       <c r="Q63" s="9"/>
@@ -6252,7 +6253,7 @@
       <c r="M64" s="9"/>
       <c r="N64" s="9"/>
       <c r="O64" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="P64" s="9"/>
       <c r="Q64" s="9"/>
@@ -6289,7 +6290,7 @@
       <c r="M65" s="9"/>
       <c r="N65" s="9"/>
       <c r="O65" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="P65" s="9"/>
       <c r="Q65" s="9"/>
@@ -6326,7 +6327,7 @@
       <c r="M66" s="9"/>
       <c r="N66" s="9"/>
       <c r="O66" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="P66" s="9"/>
       <c r="Q66" s="9"/>
@@ -6363,7 +6364,7 @@
       <c r="M67" s="9"/>
       <c r="N67" s="9"/>
       <c r="O67" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="P67" s="9"/>
       <c r="Q67" s="9"/>
@@ -7534,7 +7535,7 @@
       <c r="W96" s="9"/>
       <c r="X96" s="9"/>
       <c r="Y96" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Z96" s="9"/>
       <c r="AA96" s="9"/>
@@ -7762,7 +7763,7 @@
       <c r="Q102" s="9"/>
       <c r="R102" s="9"/>
       <c r="S102" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="T102" s="9"/>
       <c r="U102" s="9"/>
@@ -7799,7 +7800,7 @@
       <c r="Q103" s="9"/>
       <c r="R103" s="9"/>
       <c r="S103" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="T103" s="9"/>
       <c r="U103" s="9"/>
@@ -7836,7 +7837,7 @@
       <c r="Q104" s="9"/>
       <c r="R104" s="9"/>
       <c r="S104" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="T104" s="9"/>
       <c r="U104" s="9"/>
@@ -7873,7 +7874,7 @@
       <c r="Q105" s="9"/>
       <c r="R105" s="9"/>
       <c r="S105" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="T105" s="9"/>
       <c r="U105" s="9"/>
@@ -7910,7 +7911,7 @@
       <c r="Q106" s="9"/>
       <c r="R106" s="9"/>
       <c r="S106" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="T106" s="9"/>
       <c r="U106" s="9"/>
@@ -7947,7 +7948,7 @@
       <c r="Q107" s="9"/>
       <c r="R107" s="9"/>
       <c r="S107" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="T107" s="9"/>
       <c r="U107" s="9"/>
@@ -7984,7 +7985,7 @@
       <c r="Q108" s="9"/>
       <c r="R108" s="9"/>
       <c r="S108" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="T108" s="9"/>
       <c r="U108" s="9"/>
@@ -8129,7 +8130,7 @@
       <c r="N112" s="9"/>
       <c r="O112" s="9"/>
       <c r="P112" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q112" s="9"/>
       <c r="R112" s="9"/>
@@ -8281,7 +8282,7 @@
         <v>22301601</v>
       </c>
       <c r="R116" s="9">
-        <v>900</v>
+        <v>10</v>
       </c>
       <c r="S116" s="9"/>
       <c r="T116" s="9"/>
@@ -8320,7 +8321,7 @@
         <v>22301602</v>
       </c>
       <c r="R117" s="9">
-        <v>900</v>
+        <v>10</v>
       </c>
       <c r="S117" s="9"/>
       <c r="T117" s="9"/>
@@ -8359,7 +8360,7 @@
         <v>22301603</v>
       </c>
       <c r="R118" s="9">
-        <v>900</v>
+        <v>10</v>
       </c>
       <c r="S118" s="9"/>
       <c r="T118" s="9"/>
@@ -8398,7 +8399,7 @@
         <v>22301604</v>
       </c>
       <c r="R119" s="9">
-        <v>1800</v>
+        <v>20</v>
       </c>
       <c r="S119" s="9"/>
       <c r="T119" s="9"/>

</xml_diff>

<commit_message>
fix the card bag bug
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/ItemConsumer.xlsx
+++ b/ConfigData/Xlsx/ItemConsumer.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FFB329C1-70B2-45F9-B27A-90FC7F67DC8C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="144">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -120,18 +121,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>0;840;150;10;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0;720;250;30;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>0;600;350;50;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>RandomCardRate</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -212,54 +201,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>0;840;150;10;11</t>
-  </si>
-  <si>
-    <t>0;840;150;10;12</t>
-  </si>
-  <si>
-    <t>0;840;150;10;13</t>
-  </si>
-  <si>
-    <t>0;840;150;10;14</t>
-  </si>
-  <si>
-    <t>0;840;150;10;15</t>
-  </si>
-  <si>
-    <t>0;840;150;10;16</t>
-  </si>
-  <si>
-    <t>0;840;150;10;17</t>
-  </si>
-  <si>
-    <t>0;840;150;10;18</t>
-  </si>
-  <si>
-    <t>0;840;150;10;19</t>
-  </si>
-  <si>
-    <t>0;840;150;10;20</t>
-  </si>
-  <si>
-    <t>0;840;150;10;21</t>
-  </si>
-  <si>
-    <t>0;840;150;10;22</t>
-  </si>
-  <si>
-    <t>0;840;150;10;23</t>
-  </si>
-  <si>
-    <t>0;840;150;10;24</t>
-  </si>
-  <si>
-    <t>0;840;150;10;25</t>
-  </si>
-  <si>
-    <t>0;840;150;10;26</t>
-  </si>
-  <si>
     <t>随机卡规则</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -598,13 +539,25 @@
   </si>
   <si>
     <t>holyman</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>500;340;140;10;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>300;420;235;30;15</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>200;400;315;60;25</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1407,16 +1360,6 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="31">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2279,76 +2222,18 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3445,43 +3330,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:AC135" totalsRowShown="0" headerRowDxfId="30">
-  <autoFilter ref="A3:AC135"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表2" displayName="表2" ref="A3:AC135" totalsRowShown="0" headerRowDxfId="29">
+  <autoFilter ref="A3:AC135" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState ref="A4:AA126">
     <sortCondition ref="A3:A126"/>
   </sortState>
   <tableColumns count="29">
-    <tableColumn id="1" name="Id" dataDxfId="29"/>
-    <tableColumn id="2" name="~Name" dataDxfId="28">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="~Name" dataDxfId="27">
       <calculatedColumnFormula>LOOKUP(表2[[#This Row],[Id]],[1]其他!$A:$A,[1]其他!$B:$B)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="CdGroup" dataDxfId="27"/>
-    <tableColumn id="25" name="CdTime" dataDxfId="26"/>
-    <tableColumn id="3" name="GainExp" dataDxfId="25"/>
-    <tableColumn id="4" name="GainFood" dataDxfId="24"/>
-    <tableColumn id="21" name="GainHealth" dataDxfId="23"/>
-    <tableColumn id="20" name="GainMental" dataDxfId="22"/>
-    <tableColumn id="5" name="ResourceId" dataDxfId="21"/>
-    <tableColumn id="6" name="ResourceCount" dataDxfId="20"/>
-    <tableColumn id="23" name="BlessId" dataDxfId="19"/>
-    <tableColumn id="18" name="BuildPoint" dataDxfId="18"/>
-    <tableColumn id="26" name="RandomCardCount" dataDxfId="17"/>
-    <tableColumn id="24" name="RandomCardCatalog" dataDxfId="16"/>
-    <tableColumn id="8" name="RandomCardRate" dataDxfId="15"/>
-    <tableColumn id="7" name="DropItem" dataDxfId="14"/>
-    <tableColumn id="22" name="Instruction" dataDxfId="13"/>
-    <tableColumn id="9" name="FarmItemId" dataDxfId="12"/>
-    <tableColumn id="10" name="FarmEnergy" dataDxfId="11"/>
-    <tableColumn id="29" name="DungeonAttr" dataDxfId="10"/>
-    <tableColumn id="11" name="GainLp" dataDxfId="9"/>
-    <tableColumn id="12" name="GainMp" dataDxfId="8"/>
-    <tableColumn id="13" name="GainPp" dataDxfId="7"/>
-    <tableColumn id="14" name="DirectDamage" dataDxfId="6"/>
-    <tableColumn id="15" name="FightRandomCardType" dataDxfId="5"/>
-    <tableColumn id="17" name="HolyWord" dataDxfId="4"/>
-    <tableColumn id="19" name="AddTowerHp" dataDxfId="3"/>
-    <tableColumn id="27" name="Items" dataDxfId="2"/>
-    <tableColumn id="28" name="ItemCount" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="CdGroup" dataDxfId="26"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="CdTime" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="GainExp" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="GainFood" dataDxfId="23"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="GainHealth" dataDxfId="22"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="GainMental" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="ResourceId" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="ResourceCount" dataDxfId="19"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="BlessId" dataDxfId="18"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="BuildPoint" dataDxfId="17"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="RandomCardCount" dataDxfId="16"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="RandomCardCatalog" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="RandomCardRate" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="DropItem" dataDxfId="13"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Instruction" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="FarmItemId" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="FarmEnergy" dataDxfId="10"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="DungeonAttr" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="GainLp" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="GainMp" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="GainPp" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="DirectDamage" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="FightRandomCardType" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="HolyWord" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="AddTowerHp" dataDxfId="2"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Items" dataDxfId="1"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="ItemCount" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3495,7 +3380,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -3807,11 +3692,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="Z92" sqref="Z92"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3847,22 +3732,22 @@
         <v>10</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>11</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>12</v>
@@ -3871,34 +3756,34 @@
         <v>13</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="N1" s="14" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="O1" s="14" t="s">
         <v>23</v>
       </c>
       <c r="P1" s="14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Q1" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="R1" s="14" t="s">
         <v>14</v>
       </c>
       <c r="S1" s="14" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="T1" s="14" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="U1" s="16" t="s">
         <v>17</v>
@@ -3916,16 +3801,16 @@
         <v>21</v>
       </c>
       <c r="Z1" s="16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="AA1" s="16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AB1" s="17" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="AC1" s="18" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.15">
@@ -3936,10 +3821,10 @@
         <v>15</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>0</v>
@@ -3963,22 +3848,22 @@
         <v>0</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="P2" s="2" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>0</v>
@@ -3987,7 +3872,7 @@
         <v>0</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="U2" s="6" t="s">
         <v>0</v>
@@ -4005,16 +3890,16 @@
         <v>0</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="AC2" s="12" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.15">
@@ -4022,25 +3907,25 @@
         <v>16</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="H3" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>2</v>
@@ -4049,34 +3934,34 @@
         <v>3</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="R3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="U3" s="7" t="s">
         <v>5</v>
@@ -4094,16 +3979,16 @@
         <v>22</v>
       </c>
       <c r="Z3" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AA3" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="AB3" s="13" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="AC3" s="13" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.15">
@@ -4111,7 +3996,7 @@
         <v>22200001</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="C4" s="9">
         <v>4</v>
@@ -4131,10 +4016,10 @@
         <v>1</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
@@ -4156,7 +4041,7 @@
         <v>22200002</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="C5" s="9">
         <v>4</v>
@@ -4176,7 +4061,7 @@
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
       <c r="P5" s="9" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="Q5" s="9"/>
       <c r="R5" s="9"/>
@@ -4226,10 +4111,10 @@
       <c r="Z6" s="9"/>
       <c r="AA6" s="9"/>
       <c r="AB6" s="9" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="AC6" s="9" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.15">
@@ -4254,7 +4139,7 @@
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
       <c r="P7" s="9" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="Q7" s="9"/>
       <c r="R7" s="9"/>
@@ -4292,7 +4177,7 @@
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
       <c r="P8" s="9" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="Q8" s="9"/>
       <c r="R8" s="9"/>
@@ -4330,7 +4215,7 @@
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
       <c r="P9" s="9" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="Q9" s="9"/>
       <c r="R9" s="9"/>
@@ -4368,7 +4253,7 @@
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
       <c r="P10" s="9" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="Q10" s="9"/>
       <c r="R10" s="9"/>
@@ -4406,10 +4291,10 @@
         <v>5</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
@@ -4448,10 +4333,10 @@
         <v>5</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="O12" s="9" t="s">
-        <v>25</v>
+        <v>142</v>
       </c>
       <c r="P12" s="9"/>
       <c r="Q12" s="9"/>
@@ -4490,10 +4375,10 @@
         <v>5</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="O13" s="9" t="s">
-        <v>26</v>
+        <v>143</v>
       </c>
       <c r="P13" s="9"/>
       <c r="Q13" s="9"/>
@@ -4532,10 +4417,10 @@
         <v>1</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="P14" s="9"/>
       <c r="Q14" s="9"/>
@@ -4574,10 +4459,10 @@
         <v>1</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="P15" s="9"/>
       <c r="Q15" s="9"/>
@@ -4616,10 +4501,10 @@
         <v>1</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="O16" s="9" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="P16" s="9"/>
       <c r="Q16" s="9"/>
@@ -4658,10 +4543,10 @@
         <v>1</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="P17" s="9"/>
       <c r="Q17" s="9"/>
@@ -4700,10 +4585,10 @@
         <v>1</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="P18" s="9"/>
       <c r="Q18" s="9"/>
@@ -4742,10 +4627,10 @@
         <v>1</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="O19" s="9" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="P19" s="9"/>
       <c r="Q19" s="9"/>
@@ -4784,10 +4669,10 @@
         <v>1</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="O20" s="9" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="P20" s="9"/>
       <c r="Q20" s="9"/>
@@ -4826,10 +4711,10 @@
         <v>1</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="O21" s="9" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="P21" s="9"/>
       <c r="Q21" s="9"/>
@@ -4868,10 +4753,10 @@
         <v>1</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="O22" s="9" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="P22" s="9"/>
       <c r="Q22" s="9"/>
@@ -4910,10 +4795,10 @@
         <v>1</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="O23" s="9" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="P23" s="9"/>
       <c r="Q23" s="9"/>
@@ -4952,10 +4837,10 @@
         <v>1</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="O24" s="9" t="s">
-        <v>47</v>
+        <v>141</v>
       </c>
       <c r="P24" s="9"/>
       <c r="Q24" s="9"/>
@@ -4994,10 +4879,10 @@
         <v>1</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="O25" s="9" t="s">
-        <v>48</v>
+        <v>141</v>
       </c>
       <c r="P25" s="9"/>
       <c r="Q25" s="9"/>
@@ -5036,10 +4921,10 @@
         <v>1</v>
       </c>
       <c r="N26" s="9" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="O26" s="9" t="s">
-        <v>49</v>
+        <v>141</v>
       </c>
       <c r="P26" s="9"/>
       <c r="Q26" s="9"/>
@@ -5078,10 +4963,10 @@
         <v>1</v>
       </c>
       <c r="N27" s="9" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="O27" s="9" t="s">
-        <v>50</v>
+        <v>141</v>
       </c>
       <c r="P27" s="9"/>
       <c r="Q27" s="9"/>
@@ -5120,10 +5005,10 @@
         <v>1</v>
       </c>
       <c r="N28" s="9" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="O28" s="9" t="s">
-        <v>51</v>
+        <v>141</v>
       </c>
       <c r="P28" s="9"/>
       <c r="Q28" s="9"/>
@@ -5162,10 +5047,10 @@
         <v>1</v>
       </c>
       <c r="N29" s="9" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="O29" s="9" t="s">
-        <v>52</v>
+        <v>141</v>
       </c>
       <c r="P29" s="9"/>
       <c r="Q29" s="9"/>
@@ -5204,10 +5089,10 @@
         <v>1</v>
       </c>
       <c r="N30" s="9" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="O30" s="9" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
       <c r="P30" s="9"/>
       <c r="Q30" s="9"/>
@@ -5246,10 +5131,10 @@
         <v>1</v>
       </c>
       <c r="N31" s="9" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="O31" s="9" t="s">
-        <v>54</v>
+        <v>141</v>
       </c>
       <c r="P31" s="9"/>
       <c r="Q31" s="9"/>
@@ -5288,10 +5173,10 @@
         <v>1</v>
       </c>
       <c r="N32" s="9" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="O32" s="9" t="s">
-        <v>55</v>
+        <v>141</v>
       </c>
       <c r="P32" s="9"/>
       <c r="Q32" s="9"/>
@@ -5330,10 +5215,10 @@
         <v>1</v>
       </c>
       <c r="N33" s="9" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="O33" s="9" t="s">
-        <v>56</v>
+        <v>141</v>
       </c>
       <c r="P33" s="9"/>
       <c r="Q33" s="9"/>
@@ -5372,10 +5257,10 @@
         <v>1</v>
       </c>
       <c r="N34" s="9" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="O34" s="9" t="s">
-        <v>57</v>
+        <v>141</v>
       </c>
       <c r="P34" s="9"/>
       <c r="Q34" s="9"/>
@@ -5414,10 +5299,10 @@
         <v>1</v>
       </c>
       <c r="N35" s="9" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="O35" s="9" t="s">
-        <v>58</v>
+        <v>141</v>
       </c>
       <c r="P35" s="9"/>
       <c r="Q35" s="9"/>
@@ -5456,10 +5341,10 @@
         <v>1</v>
       </c>
       <c r="N36" s="9" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="O36" s="9" t="s">
-        <v>59</v>
+        <v>141</v>
       </c>
       <c r="P36" s="9"/>
       <c r="Q36" s="9"/>
@@ -5498,10 +5383,10 @@
         <v>1</v>
       </c>
       <c r="N37" s="9" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="O37" s="9" t="s">
-        <v>60</v>
+        <v>141</v>
       </c>
       <c r="P37" s="9"/>
       <c r="Q37" s="9"/>
@@ -5540,10 +5425,10 @@
         <v>1</v>
       </c>
       <c r="N38" s="9" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="O38" s="9" t="s">
-        <v>61</v>
+        <v>141</v>
       </c>
       <c r="P38" s="9"/>
       <c r="Q38" s="9"/>
@@ -5582,10 +5467,10 @@
         <v>1</v>
       </c>
       <c r="N39" s="9" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="O39" s="9" t="s">
-        <v>62</v>
+        <v>141</v>
       </c>
       <c r="P39" s="9"/>
       <c r="Q39" s="9"/>
@@ -5624,7 +5509,7 @@
       <c r="N40" s="9"/>
       <c r="O40" s="9"/>
       <c r="P40" s="9" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="Q40" s="9"/>
       <c r="R40" s="9"/>
@@ -5662,7 +5547,7 @@
       <c r="N41" s="9"/>
       <c r="O41" s="9"/>
       <c r="P41" s="9" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="Q41" s="9"/>
       <c r="R41" s="9"/>
@@ -5700,7 +5585,7 @@
       <c r="N42" s="9"/>
       <c r="O42" s="9"/>
       <c r="P42" s="9" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="Q42" s="9"/>
       <c r="R42" s="9"/>
@@ -5738,7 +5623,7 @@
       <c r="N43" s="9"/>
       <c r="O43" s="9"/>
       <c r="P43" s="9" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="Q43" s="9"/>
       <c r="R43" s="9"/>
@@ -5776,7 +5661,7 @@
       <c r="N44" s="9"/>
       <c r="O44" s="9"/>
       <c r="P44" s="9" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="Q44" s="9"/>
       <c r="R44" s="9"/>
@@ -5814,7 +5699,7 @@
       <c r="N45" s="9"/>
       <c r="O45" s="9"/>
       <c r="P45" s="9" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="Q45" s="9"/>
       <c r="R45" s="9"/>
@@ -5852,7 +5737,7 @@
       <c r="N46" s="9"/>
       <c r="O46" s="9"/>
       <c r="P46" s="9" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="Q46" s="9"/>
       <c r="R46" s="9"/>
@@ -5890,7 +5775,7 @@
       <c r="N47" s="9"/>
       <c r="O47" s="9"/>
       <c r="P47" s="9" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="Q47" s="9"/>
       <c r="R47" s="9"/>
@@ -5928,7 +5813,7 @@
       <c r="N48" s="9"/>
       <c r="O48" s="9"/>
       <c r="P48" s="9" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="Q48" s="9"/>
       <c r="R48" s="9"/>
@@ -5966,7 +5851,7 @@
       <c r="N49" s="9"/>
       <c r="O49" s="9"/>
       <c r="P49" s="9" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="Q49" s="9"/>
       <c r="R49" s="9"/>
@@ -6004,7 +5889,7 @@
       <c r="N50" s="9"/>
       <c r="O50" s="9"/>
       <c r="P50" s="9" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="Q50" s="9"/>
       <c r="R50" s="9"/>
@@ -6042,7 +5927,7 @@
       <c r="N51" s="9"/>
       <c r="O51" s="9"/>
       <c r="P51" s="9" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="Q51" s="9"/>
       <c r="R51" s="9"/>
@@ -6080,7 +5965,7 @@
       <c r="N52" s="9"/>
       <c r="O52" s="9"/>
       <c r="P52" s="9" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="Q52" s="9"/>
       <c r="R52" s="9"/>
@@ -6118,7 +6003,7 @@
       <c r="N53" s="9"/>
       <c r="O53" s="9"/>
       <c r="P53" s="9" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="Q53" s="9"/>
       <c r="R53" s="9"/>
@@ -6156,7 +6041,7 @@
       <c r="N54" s="9"/>
       <c r="O54" s="9"/>
       <c r="P54" s="9" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="Q54" s="9"/>
       <c r="R54" s="9"/>
@@ -6194,7 +6079,7 @@
       <c r="N55" s="9"/>
       <c r="O55" s="9"/>
       <c r="P55" s="9" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="Q55" s="9"/>
       <c r="R55" s="9"/>
@@ -6232,7 +6117,7 @@
       <c r="N56" s="9"/>
       <c r="O56" s="9"/>
       <c r="P56" s="9" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="Q56" s="9"/>
       <c r="R56" s="9"/>
@@ -6270,7 +6155,7 @@
       <c r="N57" s="9"/>
       <c r="O57" s="9"/>
       <c r="P57" s="9" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="Q57" s="9"/>
       <c r="R57" s="9"/>
@@ -6308,7 +6193,7 @@
       <c r="N58" s="9"/>
       <c r="O58" s="9"/>
       <c r="P58" s="9" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="Q58" s="9"/>
       <c r="R58" s="9"/>
@@ -6346,7 +6231,7 @@
       <c r="N59" s="9"/>
       <c r="O59" s="9"/>
       <c r="P59" s="9" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="Q59" s="9"/>
       <c r="R59" s="9"/>
@@ -6384,7 +6269,7 @@
       <c r="N60" s="9"/>
       <c r="O60" s="9"/>
       <c r="P60" s="9" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="Q60" s="9"/>
       <c r="R60" s="9"/>
@@ -6422,7 +6307,7 @@
       <c r="N61" s="9"/>
       <c r="O61" s="9"/>
       <c r="P61" s="9" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="Q61" s="9"/>
       <c r="R61" s="9"/>
@@ -6460,7 +6345,7 @@
       <c r="N62" s="9"/>
       <c r="O62" s="9"/>
       <c r="P62" s="9" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="Q62" s="9"/>
       <c r="R62" s="9"/>
@@ -7660,7 +7545,7 @@
       <c r="X91" s="9"/>
       <c r="Y91" s="9"/>
       <c r="Z91" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="AA91" s="9"/>
       <c r="AB91" s="9"/>
@@ -7702,7 +7587,7 @@
       <c r="X92" s="9"/>
       <c r="Y92" s="9"/>
       <c r="Z92" s="9" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="AA92" s="9"/>
       <c r="AB92" s="9"/>
@@ -7936,7 +7821,7 @@
       <c r="R98" s="9"/>
       <c r="S98" s="9"/>
       <c r="T98" s="9" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="U98" s="9"/>
       <c r="V98" s="9"/>
@@ -7974,7 +7859,7 @@
       <c r="R99" s="9"/>
       <c r="S99" s="9"/>
       <c r="T99" s="9" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="U99" s="9"/>
       <c r="V99" s="9"/>
@@ -8012,7 +7897,7 @@
       <c r="R100" s="9"/>
       <c r="S100" s="9"/>
       <c r="T100" s="9" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="U100" s="9"/>
       <c r="V100" s="9"/>
@@ -8050,7 +7935,7 @@
       <c r="R101" s="9"/>
       <c r="S101" s="9"/>
       <c r="T101" s="9" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="U101" s="9"/>
       <c r="V101" s="9"/>
@@ -8088,7 +7973,7 @@
       <c r="R102" s="9"/>
       <c r="S102" s="9"/>
       <c r="T102" s="9" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="U102" s="9"/>
       <c r="V102" s="9"/>
@@ -8126,7 +8011,7 @@
       <c r="R103" s="9"/>
       <c r="S103" s="9"/>
       <c r="T103" s="9" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="U103" s="9"/>
       <c r="V103" s="9"/>
@@ -8164,7 +8049,7 @@
       <c r="R104" s="9"/>
       <c r="S104" s="9"/>
       <c r="T104" s="9" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="U104" s="9"/>
       <c r="V104" s="9"/>
@@ -8313,7 +8198,7 @@
       <c r="O108" s="9"/>
       <c r="P108" s="9"/>
       <c r="Q108" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="R108" s="9"/>
       <c r="S108" s="9"/>
@@ -9376,7 +9261,7 @@
       <c r="N135" s="20"/>
       <c r="O135" s="20"/>
       <c r="P135" s="20" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="Q135" s="20"/>
       <c r="R135" s="20"/>
@@ -9395,7 +9280,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="D4:AC4 C5:AC135">
-    <cfRule type="containsBlanks" dxfId="0" priority="26">
+    <cfRule type="containsBlanks" dxfId="30" priority="26">
       <formula>LEN(TRIM(C4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>